<commit_message>
Asset List Up To Date
</commit_message>
<xml_diff>
--- a/Algemeen/Asset List Game-Lab 1.xlsx
+++ b/Algemeen/Asset List Game-Lab 1.xlsx
@@ -1135,17 +1135,17 @@
     <t>| Main Character_3.6 | Main Character_3.7 | Main Character_3.8 | Main Character_3.9 | Enemy_4.1 | Enemy_4.2 | Enemy_4.3|</t>
   </si>
   <si>
-    <t>Artist Points Behaald: 131 / 250</t>
-  </si>
-  <si>
-    <t>Development Points Behaald: 230 / 250</t>
+    <t>Development Points Behaald: 230 / 375</t>
+  </si>
+  <si>
+    <t>Artist Points Behaald: 185 / 375</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1181,8 +1181,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="13">
+  <fills count="14">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1253,6 +1260,11 @@
         <fgColor rgb="FFFFC7CE"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -1263,12 +1275,13 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1338,9 +1351,13 @@
     <xf numFmtId="0" fontId="4" fillId="12" borderId="0" xfId="2" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="3">
+  <cellStyles count="4">
     <cellStyle name="Goed" xfId="1" builtinId="26"/>
+    <cellStyle name="Neutraal" xfId="3" builtinId="28"/>
     <cellStyle name="Ongeldig" xfId="2" builtinId="27"/>
     <cellStyle name="Standaard" xfId="0" builtinId="0"/>
   </cellStyles>
@@ -1654,7 +1671,7 @@
   <dimension ref="A1:R595"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="J1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K29" sqref="K29"/>
+      <selection activeCell="N15" sqref="N15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1866,10 +1883,10 @@
       <c r="I4" s="3" t="s">
         <v>151</v>
       </c>
-      <c r="J4" s="1" t="s">
-        <v>224</v>
-      </c>
-      <c r="K4" s="1" t="s">
+      <c r="J4" s="22" t="s">
+        <v>360</v>
+      </c>
+      <c r="K4" s="25" t="s">
         <v>225</v>
       </c>
       <c r="L4" s="1" t="s">
@@ -1920,9 +1937,9 @@
         <v>152</v>
       </c>
       <c r="J5" s="22" t="s">
-        <v>360</v>
-      </c>
-      <c r="K5" s="1" t="s">
+        <v>231</v>
+      </c>
+      <c r="K5" s="25" t="s">
         <v>234</v>
       </c>
       <c r="L5" s="1" t="s">
@@ -1957,11 +1974,11 @@
       <c r="I6" s="3" t="s">
         <v>73</v>
       </c>
-      <c r="J6" s="1" t="s">
-        <v>258</v>
-      </c>
-      <c r="K6" s="1" t="s">
-        <v>237</v>
+      <c r="J6" s="22" t="s">
+        <v>235</v>
+      </c>
+      <c r="K6" s="22" t="s">
+        <v>350</v>
       </c>
       <c r="L6" s="1" t="s">
         <v>245</v>
@@ -2011,7 +2028,7 @@
         <v>75</v>
       </c>
       <c r="J7" s="22" t="s">
-        <v>231</v>
+        <v>236</v>
       </c>
       <c r="K7" s="22" t="s">
         <v>254</v>
@@ -2063,12 +2080,6 @@
       <c r="I8" s="3" t="s">
         <v>150</v>
       </c>
-      <c r="J8" s="22" t="s">
-        <v>235</v>
-      </c>
-      <c r="K8" s="22" t="s">
-        <v>350</v>
-      </c>
       <c r="L8" s="1" t="s">
         <v>247</v>
       </c>
@@ -2116,9 +2127,6 @@
       <c r="I9" s="3" t="s">
         <v>134</v>
       </c>
-      <c r="J9" s="22" t="s">
-        <v>236</v>
-      </c>
       <c r="L9" s="1" t="s">
         <v>248</v>
       </c>
@@ -2239,7 +2247,7 @@
       <c r="I12" s="3" t="s">
         <v>95</v>
       </c>
-      <c r="L12" s="1" t="s">
+      <c r="L12" s="25" t="s">
         <v>251</v>
       </c>
       <c r="O12" s="1" t="s">
@@ -2315,13 +2323,13 @@
       <c r="I14" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="L14" s="1" t="s">
+      <c r="L14" s="22" t="s">
         <v>253</v>
       </c>
       <c r="O14" s="1" t="s">
         <v>358</v>
       </c>
-      <c r="Q14" s="1" t="s">
+      <c r="Q14" s="22" t="s">
         <v>321</v>
       </c>
     </row>
@@ -2448,6 +2456,9 @@
       <c r="I19" s="3" t="s">
         <v>364</v>
       </c>
+      <c r="L19" s="22" t="s">
+        <v>237</v>
+      </c>
       <c r="Q19" s="1" t="s">
         <v>356</v>
       </c>
@@ -2474,6 +2485,9 @@
       <c r="I20" s="3" t="s">
         <v>365</v>
       </c>
+      <c r="L20" s="25" t="s">
+        <v>224</v>
+      </c>
     </row>
     <row r="21" spans="1:18" x14ac:dyDescent="0.25">
       <c r="H21" s="3" t="s">
@@ -2482,32 +2496,8 @@
       <c r="I21" s="3" t="s">
         <v>370</v>
       </c>
-      <c r="J21" s="21" t="s">
-        <v>222</v>
-      </c>
-      <c r="K21" s="21" t="s">
-        <v>222</v>
-      </c>
-      <c r="L21" s="21" t="s">
-        <v>222</v>
-      </c>
-      <c r="M21" s="21" t="s">
-        <v>222</v>
-      </c>
-      <c r="N21" s="21" t="s">
-        <v>222</v>
-      </c>
-      <c r="O21" s="21" t="s">
-        <v>222</v>
-      </c>
-      <c r="P21" s="21" t="s">
-        <v>222</v>
-      </c>
-      <c r="Q21" s="21" t="s">
-        <v>222</v>
-      </c>
-      <c r="R21" s="21" t="s">
-        <v>222</v>
+      <c r="L21" s="25" t="s">
+        <v>258</v>
       </c>
     </row>
     <row r="22" spans="1:18" x14ac:dyDescent="0.25">
@@ -2532,33 +2522,6 @@
       <c r="I22" s="3" t="s">
         <v>371</v>
       </c>
-      <c r="J22" s="22" t="s">
-        <v>226</v>
-      </c>
-      <c r="K22" s="1" t="s">
-        <v>238</v>
-      </c>
-      <c r="L22" s="1" t="s">
-        <v>256</v>
-      </c>
-      <c r="M22" s="1" t="s">
-        <v>265</v>
-      </c>
-      <c r="N22" s="1" t="s">
-        <v>278</v>
-      </c>
-      <c r="O22" s="1" t="s">
-        <v>292</v>
-      </c>
-      <c r="P22" s="1" t="s">
-        <v>306</v>
-      </c>
-      <c r="Q22" s="1" t="s">
-        <v>327</v>
-      </c>
-      <c r="R22" s="1" t="s">
-        <v>333</v>
-      </c>
     </row>
     <row r="23" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A23" s="5" t="s">
@@ -2582,33 +2545,6 @@
       <c r="I23" s="3" t="s">
         <v>366</v>
       </c>
-      <c r="J23" s="22" t="s">
-        <v>227</v>
-      </c>
-      <c r="K23" s="22" t="s">
-        <v>239</v>
-      </c>
-      <c r="L23" s="1" t="s">
-        <v>257</v>
-      </c>
-      <c r="M23" s="1" t="s">
-        <v>266</v>
-      </c>
-      <c r="N23" s="1" t="s">
-        <v>279</v>
-      </c>
-      <c r="O23" s="1" t="s">
-        <v>293</v>
-      </c>
-      <c r="P23" s="1" t="s">
-        <v>307</v>
-      </c>
-      <c r="Q23" s="22" t="s">
-        <v>328</v>
-      </c>
-      <c r="R23" s="1" t="s">
-        <v>334</v>
-      </c>
     </row>
     <row r="24" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A24" s="5" t="s">
@@ -2632,33 +2568,6 @@
       <c r="I24" s="3" t="s">
         <v>367</v>
       </c>
-      <c r="J24" s="22" t="s">
-        <v>228</v>
-      </c>
-      <c r="K24" s="22" t="s">
-        <v>240</v>
-      </c>
-      <c r="L24" s="1" t="s">
-        <v>255</v>
-      </c>
-      <c r="M24" s="22" t="s">
-        <v>267</v>
-      </c>
-      <c r="N24" s="1" t="s">
-        <v>280</v>
-      </c>
-      <c r="O24" s="1" t="s">
-        <v>294</v>
-      </c>
-      <c r="P24" s="1" t="s">
-        <v>308</v>
-      </c>
-      <c r="Q24" s="1" t="s">
-        <v>329</v>
-      </c>
-      <c r="R24" s="1" t="s">
-        <v>335</v>
-      </c>
     </row>
     <row r="25" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A25" s="5" t="s">
@@ -2681,30 +2590,6 @@
       </c>
       <c r="I25" s="5" t="s">
         <v>368</v>
-      </c>
-      <c r="J25" s="22" t="s">
-        <v>229</v>
-      </c>
-      <c r="K25" s="22" t="s">
-        <v>241</v>
-      </c>
-      <c r="M25" s="1" t="s">
-        <v>268</v>
-      </c>
-      <c r="N25" s="1" t="s">
-        <v>281</v>
-      </c>
-      <c r="O25" s="1" t="s">
-        <v>295</v>
-      </c>
-      <c r="P25" s="1" t="s">
-        <v>309</v>
-      </c>
-      <c r="Q25" s="1" t="s">
-        <v>330</v>
-      </c>
-      <c r="R25" s="1" t="s">
-        <v>336</v>
       </c>
     </row>
     <row r="26" spans="1:18" x14ac:dyDescent="0.25">
@@ -2715,29 +2600,32 @@
       <c r="I26" s="5" t="s">
         <v>369</v>
       </c>
-      <c r="J26" s="22" t="s">
-        <v>230</v>
-      </c>
-      <c r="K26" s="22" t="s">
-        <v>242</v>
-      </c>
-      <c r="M26" s="1" t="s">
-        <v>269</v>
-      </c>
-      <c r="N26" s="1" t="s">
-        <v>274</v>
-      </c>
-      <c r="O26" s="1" t="s">
-        <v>296</v>
-      </c>
-      <c r="P26" s="1" t="s">
-        <v>310</v>
-      </c>
-      <c r="Q26" s="1" t="s">
-        <v>331</v>
-      </c>
-      <c r="R26" s="1" t="s">
-        <v>337</v>
+      <c r="J26" s="21" t="s">
+        <v>222</v>
+      </c>
+      <c r="K26" s="21" t="s">
+        <v>222</v>
+      </c>
+      <c r="L26" s="21" t="s">
+        <v>222</v>
+      </c>
+      <c r="M26" s="21" t="s">
+        <v>222</v>
+      </c>
+      <c r="N26" s="21" t="s">
+        <v>222</v>
+      </c>
+      <c r="O26" s="21" t="s">
+        <v>222</v>
+      </c>
+      <c r="P26" s="21" t="s">
+        <v>222</v>
+      </c>
+      <c r="Q26" s="21" t="s">
+        <v>222</v>
+      </c>
+      <c r="R26" s="21" t="s">
+        <v>222</v>
       </c>
     </row>
     <row r="27" spans="1:18" x14ac:dyDescent="0.25">
@@ -2757,17 +2645,32 @@
         <v>3</v>
       </c>
       <c r="I27" s="19"/>
+      <c r="J27" s="22" t="s">
+        <v>226</v>
+      </c>
+      <c r="K27" s="22" t="s">
+        <v>239</v>
+      </c>
+      <c r="L27" s="1" t="s">
+        <v>238</v>
+      </c>
+      <c r="M27" s="1" t="s">
+        <v>265</v>
+      </c>
       <c r="N27" s="1" t="s">
-        <v>275</v>
+        <v>278</v>
       </c>
       <c r="O27" s="1" t="s">
-        <v>297</v>
+        <v>292</v>
+      </c>
+      <c r="P27" s="1" t="s">
+        <v>306</v>
       </c>
       <c r="Q27" s="1" t="s">
-        <v>332</v>
+        <v>327</v>
       </c>
       <c r="R27" s="1" t="s">
-        <v>338</v>
+        <v>333</v>
       </c>
     </row>
     <row r="28" spans="1:18" x14ac:dyDescent="0.25">
@@ -2787,11 +2690,32 @@
         <v>3</v>
       </c>
       <c r="I28" s="19"/>
+      <c r="J28" s="22" t="s">
+        <v>227</v>
+      </c>
+      <c r="K28" s="22" t="s">
+        <v>240</v>
+      </c>
+      <c r="L28" s="1" t="s">
+        <v>256</v>
+      </c>
+      <c r="M28" s="1" t="s">
+        <v>266</v>
+      </c>
       <c r="N28" s="1" t="s">
-        <v>276</v>
+        <v>279</v>
+      </c>
+      <c r="O28" s="1" t="s">
+        <v>293</v>
+      </c>
+      <c r="P28" s="1" t="s">
+        <v>307</v>
+      </c>
+      <c r="Q28" s="22" t="s">
+        <v>328</v>
       </c>
       <c r="R28" s="1" t="s">
-        <v>339</v>
+        <v>334</v>
       </c>
     </row>
     <row r="29" spans="1:18" x14ac:dyDescent="0.25">
@@ -2811,11 +2735,32 @@
         <v>3</v>
       </c>
       <c r="I29" s="19"/>
+      <c r="J29" s="22" t="s">
+        <v>228</v>
+      </c>
+      <c r="K29" s="22" t="s">
+        <v>241</v>
+      </c>
+      <c r="L29" s="1" t="s">
+        <v>257</v>
+      </c>
+      <c r="M29" s="22" t="s">
+        <v>267</v>
+      </c>
       <c r="N29" s="1" t="s">
-        <v>277</v>
+        <v>280</v>
+      </c>
+      <c r="O29" s="1" t="s">
+        <v>294</v>
+      </c>
+      <c r="P29" s="1" t="s">
+        <v>308</v>
+      </c>
+      <c r="Q29" s="1" t="s">
+        <v>329</v>
       </c>
       <c r="R29" s="1" t="s">
-        <v>340</v>
+        <v>335</v>
       </c>
     </row>
     <row r="30" spans="1:18" x14ac:dyDescent="0.25">
@@ -2835,12 +2780,57 @@
         <v>3</v>
       </c>
       <c r="I30" s="19"/>
+      <c r="J30" s="22" t="s">
+        <v>229</v>
+      </c>
+      <c r="K30" s="22" t="s">
+        <v>242</v>
+      </c>
+      <c r="L30" s="1" t="s">
+        <v>255</v>
+      </c>
+      <c r="M30" s="1" t="s">
+        <v>268</v>
+      </c>
+      <c r="N30" s="1" t="s">
+        <v>281</v>
+      </c>
+      <c r="O30" s="1" t="s">
+        <v>295</v>
+      </c>
+      <c r="P30" s="1" t="s">
+        <v>309</v>
+      </c>
+      <c r="Q30" s="1" t="s">
+        <v>330</v>
+      </c>
+      <c r="R30" s="1" t="s">
+        <v>336</v>
+      </c>
     </row>
     <row r="31" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B31" s="16"/>
       <c r="I31" s="19"/>
-      <c r="J31" s="24" t="s">
-        <v>373</v>
+      <c r="J31" s="22" t="s">
+        <v>230</v>
+      </c>
+      <c r="M31" s="1" t="s">
+        <v>269</v>
+      </c>
+      <c r="N31" s="1" t="s">
+        <v>274</v>
+      </c>
+      <c r="O31" s="1" t="s">
+        <v>296</v>
+      </c>
+      <c r="P31" s="1" t="s">
+        <v>310</v>
+      </c>
+      <c r="Q31" s="1" t="s">
+        <v>331</v>
+      </c>
+      <c r="R31" s="1" t="s">
+        <v>337</v>
       </c>
     </row>
     <row r="32" spans="1:18" x14ac:dyDescent="0.25">
@@ -2861,11 +2851,20 @@
       </c>
       <c r="H32" s="19"/>
       <c r="I32" s="19"/>
-      <c r="J32" s="24" t="s">
-        <v>372</v>
-      </c>
-    </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="N32" s="1" t="s">
+        <v>275</v>
+      </c>
+      <c r="O32" s="1" t="s">
+        <v>297</v>
+      </c>
+      <c r="Q32" s="1" t="s">
+        <v>332</v>
+      </c>
+      <c r="R32" s="1" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="33" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A33" s="5" t="s">
         <v>59</v>
       </c>
@@ -2883,9 +2882,14 @@
       </c>
       <c r="H33" s="19"/>
       <c r="I33" s="19"/>
-      <c r="J33" s="23"/>
-    </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="N33" s="1" t="s">
+        <v>276</v>
+      </c>
+      <c r="R33" s="1" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="34" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A34" s="5" t="s">
         <v>59</v>
       </c>
@@ -2903,8 +2907,14 @@
       </c>
       <c r="H34" s="19"/>
       <c r="I34" s="19"/>
-    </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="N34" s="1" t="s">
+        <v>277</v>
+      </c>
+      <c r="R34" s="1" t="s">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="35" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A35" s="5" t="s">
         <v>59</v>
       </c>
@@ -2923,11 +2933,14 @@
       <c r="H35" s="19"/>
       <c r="I35" s="19"/>
     </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:18" x14ac:dyDescent="0.25">
       <c r="H36" s="19"/>
       <c r="I36" s="19"/>
-    </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J36" s="24" t="s">
+        <v>372</v>
+      </c>
+    </row>
+    <row r="37" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A37" s="5" t="s">
         <v>41</v>
       </c>
@@ -2945,8 +2958,11 @@
       </c>
       <c r="H37" s="19"/>
       <c r="I37" s="19"/>
-    </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J37" s="24" t="s">
+        <v>373</v>
+      </c>
+    </row>
+    <row r="38" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A38" s="5" t="s">
         <v>41</v>
       </c>
@@ -2963,8 +2979,9 @@
         <v>4</v>
       </c>
       <c r="I38" s="19"/>
-    </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J38" s="23"/>
+    </row>
+    <row r="39" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A39" s="5" t="s">
         <v>41</v>
       </c>
@@ -2982,7 +2999,7 @@
       </c>
       <c r="I39" s="19"/>
     </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A40" s="5" t="s">
         <v>41</v>
       </c>
@@ -3000,7 +3017,7 @@
       </c>
       <c r="I40" s="2"/>
     </row>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A42" s="5" t="s">
         <v>68</v>
       </c>
@@ -3017,7 +3034,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A43" s="5" t="s">
         <v>68</v>
       </c>
@@ -3034,7 +3051,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A44" s="5" t="s">
         <v>68</v>
       </c>
@@ -3051,7 +3068,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A45" s="5" t="s">
         <v>68</v>
       </c>
@@ -3068,7 +3085,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="47" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A47" s="5" t="s">
         <v>72</v>
       </c>
@@ -3085,7 +3102,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="48" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A48" s="5" t="s">
         <v>72</v>
       </c>

</xml_diff>

<commit_message>
Asset List En Scripting
</commit_message>
<xml_diff>
--- a/Algemeen/Asset List Game-Lab 1.xlsx
+++ b/Algemeen/Asset List Game-Lab 1.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12588"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12585"/>
   </bookViews>
   <sheets>
     <sheet name="Blad1" sheetId="1" r:id="rId1"/>
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1533" uniqueCount="374">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1535" uniqueCount="376">
   <si>
     <t>ID Code</t>
   </si>
@@ -1135,10 +1135,16 @@
     <t>| Main Character_3.6 | Main Character_3.7 | Main Character_3.8 | Main Character_3.9 | Enemy_4.1 | Enemy_4.2 | Enemy_4.3|</t>
   </si>
   <si>
-    <t>Development Points Behaald: 230 / 375</t>
-  </si>
-  <si>
-    <t>Artist Points Behaald: 232 / 375</t>
+    <t>Artist Points Behaald: 232 / 500</t>
+  </si>
+  <si>
+    <t>Development Points: 340 / 500</t>
+  </si>
+  <si>
+    <t>190 Fahrettin | 105 Sven | 45 Rief</t>
+  </si>
+  <si>
+    <t>Anthony | Michiel | Roos</t>
   </si>
 </sst>
 </file>
@@ -1671,31 +1677,31 @@
   <dimension ref="A1:R595"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="J1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K12" sqref="K12"/>
+      <selection activeCell="K34" sqref="K34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="26.44140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.44140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.88671875" style="4" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.88671875" style="4" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.109375" style="4" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.6640625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="18.6640625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="123.33203125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="36.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="27.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="27.109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="30.44140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="28.5546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="30.44140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="28.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="17" max="18" width="30.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="26.42578125" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.42578125" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.85546875" style="4" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.85546875" style="4" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.140625" style="4" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="18.7109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="123.28515625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="32.140625" style="1" customWidth="1"/>
+    <col min="11" max="11" width="27.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="27.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="30.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="28.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="30.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="28.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="17" max="18" width="30.42578125" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1751,7 +1757,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
         <v>55</v>
       </c>
@@ -1805,7 +1811,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
         <v>55</v>
       </c>
@@ -1858,7 +1864,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
         <v>55</v>
       </c>
@@ -1911,7 +1917,7 @@
         <v>341</v>
       </c>
     </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
         <v>55</v>
       </c>
@@ -1964,7 +1970,7 @@
         <v>342</v>
       </c>
     </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
       <c r="G6" s="10" t="s">
         <v>16</v>
       </c>
@@ -1999,7 +2005,7 @@
         <v>343</v>
       </c>
     </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
         <v>56</v>
       </c>
@@ -2049,7 +2055,7 @@
         <v>345</v>
       </c>
     </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
         <v>56</v>
       </c>
@@ -2096,7 +2102,7 @@
         <v>346</v>
       </c>
     </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
         <v>56</v>
       </c>
@@ -2143,7 +2149,7 @@
         <v>349</v>
       </c>
     </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
         <v>56</v>
       </c>
@@ -2190,7 +2196,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
       <c r="H11" s="3" t="s">
         <v>27</v>
       </c>
@@ -2219,7 +2225,7 @@
         <v>363</v>
       </c>
     </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A12" s="5" t="s">
         <v>57</v>
       </c>
@@ -2260,7 +2266,7 @@
         <v>353</v>
       </c>
     </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A13" s="5" t="s">
         <v>57</v>
       </c>
@@ -2301,7 +2307,7 @@
         <v>351</v>
       </c>
     </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A14" s="5" t="s">
         <v>57</v>
       </c>
@@ -2333,7 +2339,7 @@
         <v>321</v>
       </c>
     </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A15" s="5" t="s">
         <v>57</v>
       </c>
@@ -2362,7 +2368,7 @@
         <v>322</v>
       </c>
     </row>
-    <row r="16" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:18" x14ac:dyDescent="0.25">
       <c r="H16" s="3" t="s">
         <v>61</v>
       </c>
@@ -2376,7 +2382,7 @@
         <v>323</v>
       </c>
     </row>
-    <row r="17" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A17" s="5" t="s">
         <v>58</v>
       </c>
@@ -2405,7 +2411,7 @@
         <v>324</v>
       </c>
     </row>
-    <row r="18" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A18" s="5" t="s">
         <v>58</v>
       </c>
@@ -2434,7 +2440,7 @@
         <v>325</v>
       </c>
     </row>
-    <row r="19" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A19" s="5" t="s">
         <v>58</v>
       </c>
@@ -2463,7 +2469,7 @@
         <v>356</v>
       </c>
     </row>
-    <row r="20" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A20" s="5" t="s">
         <v>58</v>
       </c>
@@ -2489,7 +2495,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="21" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:18" x14ac:dyDescent="0.25">
       <c r="H21" s="3" t="s">
         <v>166</v>
       </c>
@@ -2500,7 +2506,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="22" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A22" s="5" t="s">
         <v>65</v>
       </c>
@@ -2523,7 +2529,7 @@
         <v>371</v>
       </c>
     </row>
-    <row r="23" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A23" s="5" t="s">
         <v>65</v>
       </c>
@@ -2546,7 +2552,7 @@
         <v>366</v>
       </c>
     </row>
-    <row r="24" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A24" s="5" t="s">
         <v>65</v>
       </c>
@@ -2569,7 +2575,7 @@
         <v>367</v>
       </c>
     </row>
-    <row r="25" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A25" s="5" t="s">
         <v>65</v>
       </c>
@@ -2592,7 +2598,7 @@
         <v>368</v>
       </c>
     </row>
-    <row r="26" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B26" s="16"/>
       <c r="H26" s="3" t="s">
         <v>166</v>
@@ -2628,7 +2634,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="27" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A27" s="5" t="s">
         <v>71</v>
       </c>
@@ -2673,7 +2679,7 @@
         <v>333</v>
       </c>
     </row>
-    <row r="28" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A28" s="5" t="s">
         <v>71</v>
       </c>
@@ -2718,7 +2724,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="29" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A29" s="5" t="s">
         <v>71</v>
       </c>
@@ -2763,7 +2769,7 @@
         <v>335</v>
       </c>
     </row>
-    <row r="30" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A30" s="5" t="s">
         <v>71</v>
       </c>
@@ -2789,10 +2795,10 @@
       <c r="L30" s="1" t="s">
         <v>255</v>
       </c>
-      <c r="M30" s="1" t="s">
+      <c r="M30" s="22" t="s">
         <v>268</v>
       </c>
-      <c r="N30" s="1" t="s">
+      <c r="N30" s="22" t="s">
         <v>281</v>
       </c>
       <c r="O30" s="1" t="s">
@@ -2808,19 +2814,19 @@
         <v>336</v>
       </c>
     </row>
-    <row r="31" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B31" s="16"/>
       <c r="I31" s="19"/>
       <c r="J31" s="22" t="s">
         <v>230</v>
       </c>
-      <c r="M31" s="1" t="s">
+      <c r="M31" s="22" t="s">
         <v>269</v>
       </c>
-      <c r="N31" s="1" t="s">
+      <c r="N31" s="22" t="s">
         <v>274</v>
       </c>
-      <c r="O31" s="1" t="s">
+      <c r="O31" s="22" t="s">
         <v>296</v>
       </c>
       <c r="P31" s="1" t="s">
@@ -2833,7 +2839,7 @@
         <v>337</v>
       </c>
     </row>
-    <row r="32" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A32" s="5" t="s">
         <v>59</v>
       </c>
@@ -2857,14 +2863,14 @@
       <c r="O32" s="1" t="s">
         <v>297</v>
       </c>
-      <c r="Q32" s="1" t="s">
+      <c r="Q32" s="22" t="s">
         <v>332</v>
       </c>
       <c r="R32" s="1" t="s">
         <v>338</v>
       </c>
     </row>
-    <row r="33" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A33" s="5" t="s">
         <v>59</v>
       </c>
@@ -2889,7 +2895,7 @@
         <v>339</v>
       </c>
     </row>
-    <row r="34" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A34" s="5" t="s">
         <v>59</v>
       </c>
@@ -2907,6 +2913,9 @@
       </c>
       <c r="H34" s="19"/>
       <c r="I34" s="19"/>
+      <c r="J34" s="24" t="s">
+        <v>373</v>
+      </c>
       <c r="N34" s="1" t="s">
         <v>277</v>
       </c>
@@ -2914,7 +2923,7 @@
         <v>340</v>
       </c>
     </row>
-    <row r="35" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A35" s="5" t="s">
         <v>59</v>
       </c>
@@ -2932,15 +2941,18 @@
       </c>
       <c r="H35" s="19"/>
       <c r="I35" s="19"/>
-    </row>
-    <row r="36" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="J35" s="1" t="s">
+        <v>374</v>
+      </c>
+    </row>
+    <row r="36" spans="1:18" x14ac:dyDescent="0.25">
       <c r="H36" s="19"/>
       <c r="I36" s="19"/>
       <c r="J36" s="24" t="s">
         <v>372</v>
       </c>
     </row>
-    <row r="37" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A37" s="5" t="s">
         <v>41</v>
       </c>
@@ -2958,11 +2970,11 @@
       </c>
       <c r="H37" s="19"/>
       <c r="I37" s="19"/>
-      <c r="J37" s="24" t="s">
-        <v>373</v>
-      </c>
-    </row>
-    <row r="38" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="J37" s="1" t="s">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="38" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A38" s="5" t="s">
         <v>41</v>
       </c>
@@ -2981,7 +2993,7 @@
       <c r="I38" s="19"/>
       <c r="J38" s="23"/>
     </row>
-    <row r="39" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A39" s="5" t="s">
         <v>41</v>
       </c>
@@ -2999,7 +3011,7 @@
       </c>
       <c r="I39" s="19"/>
     </row>
-    <row r="40" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A40" s="5" t="s">
         <v>41</v>
       </c>
@@ -3017,7 +3029,7 @@
       </c>
       <c r="I40" s="2"/>
     </row>
-    <row r="42" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A42" s="5" t="s">
         <v>68</v>
       </c>
@@ -3034,7 +3046,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="43" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A43" s="5" t="s">
         <v>68</v>
       </c>
@@ -3051,7 +3063,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="44" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A44" s="5" t="s">
         <v>68</v>
       </c>
@@ -3068,7 +3080,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="45" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A45" s="5" t="s">
         <v>68</v>
       </c>
@@ -3085,7 +3097,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="47" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A47" s="5" t="s">
         <v>72</v>
       </c>
@@ -3102,7 +3114,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="48" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A48" s="5" t="s">
         <v>72</v>
       </c>
@@ -3119,7 +3131,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A49" s="5" t="s">
         <v>72</v>
       </c>
@@ -3136,7 +3148,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A50" s="5" t="s">
         <v>72</v>
       </c>
@@ -3153,7 +3165,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A52" s="5" t="s">
         <v>69</v>
       </c>
@@ -3170,7 +3182,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A53" s="5" t="s">
         <v>69</v>
       </c>
@@ -3187,7 +3199,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A54" s="5" t="s">
         <v>69</v>
       </c>
@@ -3204,7 +3216,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A55" s="5" t="s">
         <v>69</v>
       </c>
@@ -3221,10 +3233,10 @@
         <v>3</v>
       </c>
     </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B56" s="16"/>
     </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A57" s="5" t="s">
         <v>70</v>
       </c>
@@ -3241,7 +3253,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A58" s="5" t="s">
         <v>70</v>
       </c>
@@ -3258,7 +3270,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A59" s="5" t="s">
         <v>70</v>
       </c>
@@ -3275,7 +3287,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A60" s="5" t="s">
         <v>70</v>
       </c>
@@ -3292,7 +3304,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A62" s="5" t="s">
         <v>154</v>
       </c>
@@ -3309,7 +3321,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A63" s="5" t="s">
         <v>154</v>
       </c>
@@ -3326,7 +3338,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A64" s="5" t="s">
         <v>154</v>
       </c>
@@ -3343,7 +3355,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A65" s="5" t="s">
         <v>154</v>
       </c>
@@ -3360,7 +3372,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A67" s="5" t="s">
         <v>155</v>
       </c>
@@ -3377,7 +3389,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A68" s="5" t="s">
         <v>155</v>
       </c>
@@ -3394,7 +3406,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A69" s="5" t="s">
         <v>155</v>
       </c>
@@ -3411,7 +3423,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A70" s="5" t="s">
         <v>155</v>
       </c>
@@ -3428,7 +3440,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A71" s="5" t="s">
         <v>155</v>
       </c>
@@ -3445,7 +3457,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="72" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A72" s="5" t="s">
         <v>155</v>
       </c>
@@ -3462,10 +3474,10 @@
         <v>5</v>
       </c>
     </row>
-    <row r="73" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B73" s="16"/>
     </row>
-    <row r="74" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A74" s="5" t="s">
         <v>156</v>
       </c>
@@ -3482,7 +3494,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="75" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A75" s="5" t="s">
         <v>156</v>
       </c>
@@ -3499,7 +3511,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="76" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A76" s="5" t="s">
         <v>156</v>
       </c>
@@ -3516,7 +3528,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="77" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A77" s="5" t="s">
         <v>156</v>
       </c>
@@ -3533,7 +3545,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="79" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A79" s="5" t="s">
         <v>157</v>
       </c>
@@ -3550,7 +3562,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="80" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A80" s="5" t="s">
         <v>157</v>
       </c>
@@ -3567,7 +3579,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="81" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A81" s="5" t="s">
         <v>157</v>
       </c>
@@ -3584,7 +3596,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="82" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A82" s="5" t="s">
         <v>157</v>
       </c>
@@ -3601,7 +3613,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="84" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A84" s="5" t="s">
         <v>158</v>
       </c>
@@ -3618,7 +3630,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="85" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A85" s="5" t="s">
         <v>158</v>
       </c>
@@ -3635,7 +3647,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="86" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A86" s="5" t="s">
         <v>158</v>
       </c>
@@ -3652,7 +3664,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="87" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A87" s="5" t="s">
         <v>158</v>
       </c>
@@ -3669,7 +3681,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="89" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A89" s="5" t="s">
         <v>159</v>
       </c>
@@ -3686,7 +3698,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="90" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A90" s="5" t="s">
         <v>159</v>
       </c>
@@ -3703,7 +3715,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="91" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A91" s="5" t="s">
         <v>159</v>
       </c>
@@ -3720,7 +3732,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="92" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A92" s="5" t="s">
         <v>159</v>
       </c>
@@ -3737,7 +3749,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="94" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A94" s="5" t="s">
         <v>160</v>
       </c>
@@ -3754,7 +3766,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="95" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A95" s="5" t="s">
         <v>160</v>
       </c>
@@ -3771,7 +3783,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="96" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A96" s="5" t="s">
         <v>160</v>
       </c>
@@ -3788,7 +3800,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="97" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A97" s="5" t="s">
         <v>160</v>
       </c>
@@ -3805,7 +3817,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="99" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A99" s="5" t="s">
         <v>161</v>
       </c>
@@ -3822,7 +3834,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="100" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A100" s="5" t="s">
         <v>161</v>
       </c>
@@ -3839,7 +3851,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="101" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A101" s="5" t="s">
         <v>161</v>
       </c>
@@ -3856,7 +3868,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="102" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A102" s="5" t="s">
         <v>161</v>
       </c>
@@ -3873,7 +3885,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="104" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A104" s="5" t="s">
         <v>162</v>
       </c>
@@ -3890,7 +3902,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="105" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A105" s="5" t="s">
         <v>162</v>
       </c>
@@ -3907,7 +3919,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="106" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A106" s="5" t="s">
         <v>162</v>
       </c>
@@ -3924,7 +3936,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="107" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A107" s="5" t="s">
         <v>162</v>
       </c>
@@ -3941,10 +3953,10 @@
         <v>4</v>
       </c>
     </row>
-    <row r="108" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B108" s="16"/>
     </row>
-    <row r="109" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A109" s="5" t="s">
         <v>163</v>
       </c>
@@ -3961,7 +3973,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="110" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A110" s="5" t="s">
         <v>163</v>
       </c>
@@ -3978,7 +3990,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="111" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A111" s="5" t="s">
         <v>163</v>
       </c>
@@ -3995,7 +4007,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="112" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A112" s="5" t="s">
         <v>163</v>
       </c>
@@ -4012,10 +4024,10 @@
         <v>7</v>
       </c>
     </row>
-    <row r="113" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B113" s="16"/>
     </row>
-    <row r="114" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A114" s="5" t="s">
         <v>74</v>
       </c>
@@ -4032,7 +4044,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="115" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A115" s="5" t="s">
         <v>74</v>
       </c>
@@ -4049,7 +4061,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="116" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A116" s="5" t="s">
         <v>74</v>
       </c>
@@ -4066,7 +4078,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="117" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A117" s="5" t="s">
         <v>74</v>
       </c>
@@ -4083,10 +4095,10 @@
         <v>3</v>
       </c>
     </row>
-    <row r="118" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B118" s="16"/>
     </row>
-    <row r="119" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A119" s="5" t="s">
         <v>36</v>
       </c>
@@ -4103,7 +4115,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="120" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A120" s="5" t="s">
         <v>36</v>
       </c>
@@ -4120,7 +4132,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="121" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A121" s="5" t="s">
         <v>36</v>
       </c>
@@ -4137,7 +4149,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="122" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A122" s="5" t="s">
         <v>36</v>
       </c>
@@ -4154,12 +4166,12 @@
         <v>8</v>
       </c>
     </row>
-    <row r="123" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="123" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A123" s="4"/>
       <c r="B123" s="4"/>
       <c r="C123"/>
     </row>
-    <row r="124" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A124" s="5" t="s">
         <v>165</v>
       </c>
@@ -4176,7 +4188,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="125" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="125" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A125" s="5" t="s">
         <v>165</v>
       </c>
@@ -4193,7 +4205,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="126" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="126" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A126" s="5" t="s">
         <v>165</v>
       </c>
@@ -4210,7 +4222,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="127" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="127" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A127" s="5" t="s">
         <v>165</v>
       </c>
@@ -4227,7 +4239,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="129" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="129" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A129" s="5" t="s">
         <v>76</v>
       </c>
@@ -4244,7 +4256,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="130" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="130" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A130" s="5" t="s">
         <v>76</v>
       </c>
@@ -4261,7 +4273,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="131" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="131" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A131" s="5" t="s">
         <v>76</v>
       </c>
@@ -4278,7 +4290,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="132" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="132" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A132" s="5" t="s">
         <v>76</v>
       </c>
@@ -4295,11 +4307,11 @@
         <v>5</v>
       </c>
     </row>
-    <row r="133" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="133" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B133" s="16"/>
       <c r="G133" s="15"/>
     </row>
-    <row r="134" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="134" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A134" s="5" t="s">
         <v>48</v>
       </c>
@@ -4317,7 +4329,7 @@
       </c>
       <c r="G134" s="15"/>
     </row>
-    <row r="135" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="135" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A135" s="5" t="s">
         <v>48</v>
       </c>
@@ -4335,7 +4347,7 @@
       </c>
       <c r="G135" s="15"/>
     </row>
-    <row r="136" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="136" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A136" s="5" t="s">
         <v>48</v>
       </c>
@@ -4353,7 +4365,7 @@
       </c>
       <c r="G136" s="15"/>
     </row>
-    <row r="137" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="137" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A137" s="5" t="s">
         <v>48</v>
       </c>
@@ -4371,10 +4383,10 @@
       </c>
       <c r="G137" s="15"/>
     </row>
-    <row r="138" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="138" spans="1:7" x14ac:dyDescent="0.25">
       <c r="G138" s="15"/>
     </row>
-    <row r="139" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="139" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A139" s="5" t="s">
         <v>153</v>
       </c>
@@ -4392,7 +4404,7 @@
       </c>
       <c r="G139" s="15"/>
     </row>
-    <row r="140" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="140" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A140" s="5" t="s">
         <v>153</v>
       </c>
@@ -4410,7 +4422,7 @@
       </c>
       <c r="G140" s="15"/>
     </row>
-    <row r="141" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="141" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A141" s="5" t="s">
         <v>153</v>
       </c>
@@ -4428,7 +4440,7 @@
       </c>
       <c r="G141" s="15"/>
     </row>
-    <row r="142" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="142" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A142" s="5" t="s">
         <v>153</v>
       </c>
@@ -4446,7 +4458,7 @@
       </c>
       <c r="G142" s="15"/>
     </row>
-    <row r="143" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="143" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A143" s="5" t="s">
         <v>153</v>
       </c>
@@ -4464,7 +4476,7 @@
       </c>
       <c r="G143" s="15"/>
     </row>
-    <row r="144" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="144" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A144" s="5" t="s">
         <v>153</v>
       </c>
@@ -4482,7 +4494,7 @@
       </c>
       <c r="G144" s="15"/>
     </row>
-    <row r="145" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="145" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A145" s="5" t="s">
         <v>153</v>
       </c>
@@ -4500,10 +4512,10 @@
       </c>
       <c r="G145" s="15"/>
     </row>
-    <row r="146" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="146" spans="1:7" x14ac:dyDescent="0.25">
       <c r="G146" s="15"/>
     </row>
-    <row r="147" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="147" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A147" s="5" t="s">
         <v>77</v>
       </c>
@@ -4521,7 +4533,7 @@
       </c>
       <c r="G147" s="15"/>
     </row>
-    <row r="148" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="148" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A148" s="5" t="s">
         <v>77</v>
       </c>
@@ -4539,7 +4551,7 @@
       </c>
       <c r="G148" s="15"/>
     </row>
-    <row r="149" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="149" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A149" s="5" t="s">
         <v>77</v>
       </c>
@@ -4557,7 +4569,7 @@
       </c>
       <c r="G149" s="15"/>
     </row>
-    <row r="150" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="150" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A150" s="5" t="s">
         <v>77</v>
       </c>
@@ -4575,7 +4587,7 @@
       </c>
       <c r="G150" s="15"/>
     </row>
-    <row r="151" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="151" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A151" s="5" t="s">
         <v>77</v>
       </c>
@@ -4593,7 +4605,7 @@
       </c>
       <c r="G151" s="15"/>
     </row>
-    <row r="152" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="152" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A152" s="5" t="s">
         <v>77</v>
       </c>
@@ -4611,7 +4623,7 @@
       </c>
       <c r="G152" s="15"/>
     </row>
-    <row r="153" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="153" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A153" s="5" t="s">
         <v>77</v>
       </c>
@@ -4629,7 +4641,7 @@
       </c>
       <c r="G153" s="15"/>
     </row>
-    <row r="154" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="154" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A154" s="5" t="s">
         <v>77</v>
       </c>
@@ -4647,10 +4659,10 @@
       </c>
       <c r="G154" s="15"/>
     </row>
-    <row r="155" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="155" spans="1:7" x14ac:dyDescent="0.25">
       <c r="G155" s="15"/>
     </row>
-    <row r="156" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="156" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A156" s="5" t="s">
         <v>78</v>
       </c>
@@ -4667,7 +4679,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="157" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="157" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A157" s="5" t="s">
         <v>78</v>
       </c>
@@ -4684,7 +4696,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="158" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="158" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A158" s="5" t="s">
         <v>78</v>
       </c>
@@ -4701,7 +4713,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="159" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="159" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A159" s="5" t="s">
         <v>78</v>
       </c>
@@ -4718,7 +4730,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="160" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="160" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A160" s="5" t="s">
         <v>78</v>
       </c>
@@ -4735,7 +4747,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="161" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="161" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A161" s="5" t="s">
         <v>78</v>
       </c>
@@ -4752,7 +4764,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="162" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="162" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A162" s="5" t="s">
         <v>78</v>
       </c>
@@ -4769,7 +4781,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="163" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="163" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A163" s="5" t="s">
         <v>78</v>
       </c>
@@ -4786,7 +4798,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="165" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="165" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A165" s="5" t="s">
         <v>79</v>
       </c>
@@ -4803,7 +4815,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="166" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="166" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A166" s="5" t="s">
         <v>79</v>
       </c>
@@ -4820,7 +4832,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="167" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="167" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A167" s="5" t="s">
         <v>79</v>
       </c>
@@ -4837,7 +4849,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="168" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="168" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A168" s="5" t="s">
         <v>79</v>
       </c>
@@ -4854,7 +4866,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="169" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="169" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A169" s="5" t="s">
         <v>79</v>
       </c>
@@ -4871,7 +4883,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="170" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="170" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A170" s="5" t="s">
         <v>79</v>
       </c>
@@ -4888,7 +4900,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="171" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="171" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A171" s="5" t="s">
         <v>79</v>
       </c>
@@ -4905,7 +4917,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="172" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="172" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A172" s="5" t="s">
         <v>79</v>
       </c>
@@ -4922,7 +4934,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="174" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="174" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A174" s="5" t="s">
         <v>80</v>
       </c>
@@ -4939,7 +4951,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="175" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="175" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A175" s="5" t="s">
         <v>80</v>
       </c>
@@ -4956,7 +4968,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="176" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="176" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A176" s="5" t="s">
         <v>80</v>
       </c>
@@ -4973,7 +4985,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="177" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="177" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A177" s="5" t="s">
         <v>80</v>
       </c>
@@ -4990,7 +5002,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="178" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="178" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A178" s="5" t="s">
         <v>80</v>
       </c>
@@ -5007,7 +5019,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="179" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="179" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A179" s="5" t="s">
         <v>80</v>
       </c>
@@ -5024,7 +5036,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="180" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="180" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A180" s="5" t="s">
         <v>80</v>
       </c>
@@ -5041,7 +5053,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="181" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="181" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A181" s="5" t="s">
         <v>80</v>
       </c>
@@ -5058,7 +5070,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="183" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="183" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A183" s="5" t="s">
         <v>81</v>
       </c>
@@ -5075,7 +5087,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="184" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="184" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A184" s="5" t="s">
         <v>81</v>
       </c>
@@ -5092,7 +5104,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="185" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="185" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A185" s="5" t="s">
         <v>81</v>
       </c>
@@ -5109,7 +5121,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="186" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="186" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A186" s="5" t="s">
         <v>81</v>
       </c>
@@ -5126,7 +5138,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="187" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="187" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A187" s="5" t="s">
         <v>81</v>
       </c>
@@ -5143,7 +5155,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="188" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="188" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A188" s="5" t="s">
         <v>81</v>
       </c>
@@ -5160,7 +5172,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="189" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="189" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A189" s="5" t="s">
         <v>81</v>
       </c>
@@ -5177,7 +5189,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="190" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="190" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A190" s="5" t="s">
         <v>81</v>
       </c>
@@ -5194,7 +5206,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="192" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="192" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A192" s="5" t="s">
         <v>82</v>
       </c>
@@ -5211,7 +5223,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="193" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="193" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A193" s="5" t="s">
         <v>82</v>
       </c>
@@ -5228,7 +5240,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="194" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="194" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A194" s="5" t="s">
         <v>82</v>
       </c>
@@ -5245,7 +5257,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="195" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="195" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A195" s="5" t="s">
         <v>82</v>
       </c>
@@ -5262,7 +5274,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="196" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="196" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A196" s="5" t="s">
         <v>82</v>
       </c>
@@ -5279,7 +5291,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="197" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="197" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A197" s="5" t="s">
         <v>82</v>
       </c>
@@ -5296,7 +5308,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="198" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="198" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A198" s="5" t="s">
         <v>82</v>
       </c>
@@ -5313,7 +5325,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="199" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="199" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A199" s="5" t="s">
         <v>82</v>
       </c>
@@ -5330,7 +5342,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="201" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="201" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A201" s="5" t="s">
         <v>37</v>
       </c>
@@ -5347,7 +5359,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="202" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="202" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A202" s="5" t="s">
         <v>37</v>
       </c>
@@ -5364,7 +5376,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="203" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="203" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A203" s="5" t="s">
         <v>37</v>
       </c>
@@ -5381,7 +5393,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="204" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="204" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A204" s="5" t="s">
         <v>37</v>
       </c>
@@ -5398,7 +5410,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="206" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="206" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A206" s="5" t="s">
         <v>40</v>
       </c>
@@ -5415,7 +5427,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="207" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="207" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A207" s="5" t="s">
         <v>40</v>
       </c>
@@ -5432,7 +5444,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="208" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="208" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A208" s="5" t="s">
         <v>40</v>
       </c>
@@ -5449,7 +5461,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="209" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="209" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A209" s="5" t="s">
         <v>40</v>
       </c>
@@ -5466,7 +5478,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="211" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="211" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A211" s="5" t="s">
         <v>83</v>
       </c>
@@ -5483,7 +5495,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="212" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="212" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A212" s="5" t="s">
         <v>83</v>
       </c>
@@ -5500,7 +5512,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="213" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="213" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A213" s="5" t="s">
         <v>83</v>
       </c>
@@ -5517,7 +5529,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="214" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="214" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A214" s="5" t="s">
         <v>83</v>
       </c>
@@ -5534,7 +5546,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="216" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="216" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A216" s="5" t="s">
         <v>85</v>
       </c>
@@ -5551,7 +5563,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="217" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="217" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A217" s="5" t="s">
         <v>85</v>
       </c>
@@ -5568,7 +5580,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="218" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="218" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A218" s="5" t="s">
         <v>85</v>
       </c>
@@ -5585,7 +5597,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="219" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="219" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A219" s="5" t="s">
         <v>85</v>
       </c>
@@ -5602,7 +5614,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="220" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="220" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A220" s="5" t="s">
         <v>85</v>
       </c>
@@ -5619,7 +5631,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="222" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="222" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A222" s="5" t="s">
         <v>86</v>
       </c>
@@ -5636,7 +5648,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="223" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="223" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A223" s="5" t="s">
         <v>86</v>
       </c>
@@ -5653,7 +5665,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="224" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="224" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A224" s="5" t="s">
         <v>86</v>
       </c>
@@ -5670,7 +5682,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="225" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="225" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A225" s="5" t="s">
         <v>86</v>
       </c>
@@ -5687,7 +5699,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="227" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="227" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A227" s="5" t="s">
         <v>87</v>
       </c>
@@ -5704,7 +5716,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="228" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="228" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A228" s="5" t="s">
         <v>87</v>
       </c>
@@ -5721,7 +5733,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="229" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="229" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A229" s="5" t="s">
         <v>87</v>
       </c>
@@ -5738,7 +5750,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="230" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="230" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A230" s="5" t="s">
         <v>87</v>
       </c>
@@ -5755,7 +5767,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="232" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="232" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A232" s="5" t="s">
         <v>88</v>
       </c>
@@ -5772,7 +5784,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="233" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="233" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A233" s="5" t="s">
         <v>88</v>
       </c>
@@ -5789,7 +5801,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="234" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="234" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A234" s="5" t="s">
         <v>88</v>
       </c>
@@ -5806,7 +5818,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="235" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="235" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A235" s="5" t="s">
         <v>88</v>
       </c>
@@ -5823,7 +5835,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="237" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="237" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A237" s="5" t="s">
         <v>89</v>
       </c>
@@ -5840,7 +5852,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="238" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="238" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A238" s="5" t="s">
         <v>89</v>
       </c>
@@ -5857,7 +5869,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="239" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="239" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A239" s="5" t="s">
         <v>89</v>
       </c>
@@ -5874,7 +5886,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="240" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="240" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A240" s="5" t="s">
         <v>89</v>
       </c>
@@ -5891,7 +5903,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="242" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="242" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A242" s="5" t="s">
         <v>90</v>
       </c>
@@ -5908,7 +5920,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="243" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="243" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A243" s="5" t="s">
         <v>90</v>
       </c>
@@ -5925,7 +5937,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="244" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="244" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A244" s="5" t="s">
         <v>90</v>
       </c>
@@ -5942,7 +5954,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="245" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="245" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A245" s="5" t="s">
         <v>90</v>
       </c>
@@ -5959,7 +5971,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="246" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="246" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A246" s="5" t="s">
         <v>90</v>
       </c>
@@ -5976,7 +5988,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="248" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="248" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A248" s="5" t="s">
         <v>91</v>
       </c>
@@ -5993,7 +6005,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="249" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="249" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A249" s="5" t="s">
         <v>91</v>
       </c>
@@ -6010,7 +6022,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="250" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="250" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A250" s="5" t="s">
         <v>91</v>
       </c>
@@ -6027,7 +6039,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="251" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="251" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A251" s="5" t="s">
         <v>91</v>
       </c>
@@ -6044,7 +6056,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="253" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="253" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A253" s="5" t="s">
         <v>92</v>
       </c>
@@ -6061,7 +6073,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="254" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="254" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A254" s="5" t="s">
         <v>92</v>
       </c>
@@ -6078,7 +6090,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="255" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="255" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A255" s="5" t="s">
         <v>92</v>
       </c>
@@ -6095,7 +6107,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="256" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="256" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A256" s="5" t="s">
         <v>92</v>
       </c>
@@ -6112,7 +6124,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="258" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="258" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A258" s="5" t="s">
         <v>93</v>
       </c>
@@ -6129,7 +6141,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="259" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="259" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A259" s="5" t="s">
         <v>93</v>
       </c>
@@ -6146,7 +6158,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="260" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="260" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A260" s="5" t="s">
         <v>93</v>
       </c>
@@ -6163,7 +6175,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="261" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="261" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A261" s="5" t="s">
         <v>93</v>
       </c>
@@ -6180,7 +6192,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="263" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="263" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A263" s="5" t="s">
         <v>94</v>
       </c>
@@ -6197,7 +6209,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="264" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="264" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A264" s="5" t="s">
         <v>94</v>
       </c>
@@ -6214,7 +6226,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="265" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="265" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A265" s="5" t="s">
         <v>94</v>
       </c>
@@ -6231,7 +6243,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="266" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="266" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A266" s="5" t="s">
         <v>94</v>
       </c>
@@ -6248,7 +6260,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="268" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="268" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A268" s="5" t="s">
         <v>96</v>
       </c>
@@ -6265,7 +6277,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="269" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="269" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A269" s="5" t="s">
         <v>96</v>
       </c>
@@ -6282,7 +6294,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="270" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="270" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A270" s="5" t="s">
         <v>96</v>
       </c>
@@ -6299,7 +6311,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="271" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="271" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A271" s="5" t="s">
         <v>96</v>
       </c>
@@ -6316,7 +6328,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="273" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="273" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A273" s="5" t="s">
         <v>97</v>
       </c>
@@ -6333,7 +6345,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="274" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="274" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A274" s="5" t="s">
         <v>97</v>
       </c>
@@ -6350,7 +6362,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="275" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="275" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A275" s="5" t="s">
         <v>97</v>
       </c>
@@ -6367,7 +6379,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="276" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="276" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A276" s="5" t="s">
         <v>97</v>
       </c>
@@ -6384,12 +6396,12 @@
         <v>10</v>
       </c>
     </row>
-    <row r="277" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="277" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A277" s="4"/>
       <c r="B277" s="4"/>
       <c r="C277" s="4"/>
     </row>
-    <row r="278" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="278" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A278" s="5" t="s">
         <v>144</v>
       </c>
@@ -6406,7 +6418,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="279" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="279" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A279" s="5" t="s">
         <v>144</v>
       </c>
@@ -6423,7 +6435,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="280" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="280" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A280" s="5" t="s">
         <v>144</v>
       </c>
@@ -6440,7 +6452,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="281" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="281" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A281" s="5" t="s">
         <v>144</v>
       </c>
@@ -6457,7 +6469,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="282" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="282" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A282" s="5" t="s">
         <v>144</v>
       </c>
@@ -6474,7 +6486,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="283" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="283" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A283" s="5" t="s">
         <v>144</v>
       </c>
@@ -6491,7 +6503,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="284" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="284" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A284" s="5" t="s">
         <v>144</v>
       </c>
@@ -6508,7 +6520,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="285" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="285" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A285" s="5" t="s">
         <v>144</v>
       </c>
@@ -6525,7 +6537,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="287" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="287" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A287" s="5" t="s">
         <v>145</v>
       </c>
@@ -6542,7 +6554,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="288" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="288" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A288" s="5" t="s">
         <v>145</v>
       </c>
@@ -6560,7 +6572,7 @@
       </c>
       <c r="F288" s="2"/>
     </row>
-    <row r="289" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="289" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A289" s="5" t="s">
         <v>145</v>
       </c>
@@ -6577,7 +6589,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="290" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="290" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A290" s="5" t="s">
         <v>145</v>
       </c>
@@ -6594,7 +6606,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="291" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="291" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A291" s="5" t="s">
         <v>145</v>
       </c>
@@ -6611,7 +6623,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="292" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="292" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A292" s="5" t="s">
         <v>145</v>
       </c>
@@ -6628,7 +6640,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="293" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="293" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A293" s="5" t="s">
         <v>145</v>
       </c>
@@ -6645,7 +6657,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="294" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="294" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A294" s="5" t="s">
         <v>145</v>
       </c>
@@ -6662,7 +6674,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="296" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="296" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A296" s="5" t="s">
         <v>146</v>
       </c>
@@ -6679,7 +6691,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="297" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="297" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A297" s="5" t="s">
         <v>146</v>
       </c>
@@ -6696,7 +6708,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="298" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="298" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A298" s="5" t="s">
         <v>146</v>
       </c>
@@ -6713,7 +6725,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="299" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="299" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A299" s="5" t="s">
         <v>146</v>
       </c>
@@ -6730,7 +6742,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="300" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="300" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A300" s="5" t="s">
         <v>146</v>
       </c>
@@ -6747,7 +6759,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="301" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="301" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A301" s="5" t="s">
         <v>146</v>
       </c>
@@ -6764,7 +6776,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="302" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="302" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A302" s="5" t="s">
         <v>146</v>
       </c>
@@ -6781,7 +6793,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="303" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="303" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A303" s="5" t="s">
         <v>146</v>
       </c>
@@ -6798,7 +6810,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="305" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="305" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A305" s="5" t="s">
         <v>147</v>
       </c>
@@ -6815,7 +6827,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="306" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="306" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A306" s="5" t="s">
         <v>147</v>
       </c>
@@ -6832,7 +6844,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="307" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="307" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A307" s="5" t="s">
         <v>147</v>
       </c>
@@ -6849,7 +6861,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="308" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="308" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A308" s="5" t="s">
         <v>147</v>
       </c>
@@ -6866,7 +6878,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="309" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="309" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A309" s="5" t="s">
         <v>147</v>
       </c>
@@ -6883,7 +6895,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="310" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="310" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A310" s="5" t="s">
         <v>147</v>
       </c>
@@ -6900,7 +6912,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="311" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="311" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A311" s="5" t="s">
         <v>147</v>
       </c>
@@ -6917,7 +6929,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="312" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="312" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A312" s="5" t="s">
         <v>147</v>
       </c>
@@ -6934,7 +6946,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="314" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="314" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A314" s="5" t="s">
         <v>148</v>
       </c>
@@ -6951,7 +6963,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="315" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="315" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A315" s="5" t="s">
         <v>148</v>
       </c>
@@ -6968,7 +6980,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="316" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="316" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A316" s="5" t="s">
         <v>148</v>
       </c>
@@ -6985,7 +6997,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="317" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="317" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A317" s="5" t="s">
         <v>148</v>
       </c>
@@ -7002,7 +7014,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="318" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="318" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A318" s="5" t="s">
         <v>148</v>
       </c>
@@ -7019,7 +7031,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="319" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="319" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A319" s="5" t="s">
         <v>148</v>
       </c>
@@ -7036,7 +7048,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="320" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="320" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A320" s="5" t="s">
         <v>148</v>
       </c>
@@ -7053,7 +7065,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="321" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="321" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A321" s="5" t="s">
         <v>148</v>
       </c>
@@ -7070,7 +7082,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="323" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="323" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A323" s="5" t="s">
         <v>44</v>
       </c>
@@ -7087,7 +7099,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="324" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="324" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A324" s="5" t="s">
         <v>44</v>
       </c>
@@ -7104,7 +7116,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="325" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="325" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A325" s="5" t="s">
         <v>44</v>
       </c>
@@ -7121,7 +7133,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="326" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="326" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A326" s="5" t="s">
         <v>44</v>
       </c>
@@ -7138,7 +7150,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="328" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="328" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A328" s="5" t="s">
         <v>45</v>
       </c>
@@ -7155,7 +7167,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="329" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="329" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A329" s="5" t="s">
         <v>45</v>
       </c>
@@ -7172,7 +7184,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="330" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="330" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A330" s="5" t="s">
         <v>45</v>
       </c>
@@ -7189,7 +7201,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="331" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="331" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A331" s="5" t="s">
         <v>45</v>
       </c>
@@ -7206,7 +7218,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="333" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="333" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A333" s="5" t="s">
         <v>98</v>
       </c>
@@ -7223,7 +7235,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="334" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="334" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A334" s="5" t="s">
         <v>98</v>
       </c>
@@ -7240,7 +7252,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="335" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="335" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A335" s="5" t="s">
         <v>98</v>
       </c>
@@ -7257,7 +7269,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="336" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="336" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A336" s="5" t="s">
         <v>98</v>
       </c>
@@ -7274,7 +7286,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="338" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="338" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A338" s="5" t="s">
         <v>99</v>
       </c>
@@ -7291,7 +7303,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="339" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="339" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A339" s="5" t="s">
         <v>99</v>
       </c>
@@ -7308,7 +7320,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="340" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="340" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A340" s="5" t="s">
         <v>99</v>
       </c>
@@ -7325,7 +7337,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="341" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="341" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A341" s="5" t="s">
         <v>99</v>
       </c>
@@ -7342,7 +7354,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="343" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="343" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A343" s="5" t="s">
         <v>100</v>
       </c>
@@ -7359,7 +7371,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="344" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="344" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A344" s="5" t="s">
         <v>100</v>
       </c>
@@ -7376,7 +7388,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="345" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="345" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A345" s="5" t="s">
         <v>100</v>
       </c>
@@ -7393,7 +7405,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="346" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="346" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A346" s="5" t="s">
         <v>100</v>
       </c>
@@ -7410,7 +7422,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="348" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="348" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A348" s="5" t="s">
         <v>101</v>
       </c>
@@ -7427,7 +7439,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="349" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="349" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A349" s="5" t="s">
         <v>101</v>
       </c>
@@ -7444,7 +7456,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="350" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="350" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A350" s="5" t="s">
         <v>101</v>
       </c>
@@ -7461,7 +7473,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="351" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="351" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A351" s="5" t="s">
         <v>101</v>
       </c>
@@ -7478,7 +7490,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="353" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="353" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A353" s="5" t="s">
         <v>102</v>
       </c>
@@ -7495,7 +7507,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="354" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="354" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A354" s="5" t="s">
         <v>102</v>
       </c>
@@ -7512,7 +7524,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="355" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="355" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A355" s="5" t="s">
         <v>102</v>
       </c>
@@ -7529,7 +7541,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="356" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="356" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A356" s="5" t="s">
         <v>102</v>
       </c>
@@ -7546,7 +7558,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="358" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="358" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A358" s="5" t="s">
         <v>103</v>
       </c>
@@ -7563,7 +7575,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="359" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="359" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A359" s="5" t="s">
         <v>103</v>
       </c>
@@ -7580,7 +7592,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="360" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="360" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A360" s="5" t="s">
         <v>103</v>
       </c>
@@ -7597,7 +7609,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="361" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="361" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A361" s="5" t="s">
         <v>103</v>
       </c>
@@ -7614,7 +7626,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="363" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="363" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A363" s="5" t="s">
         <v>104</v>
       </c>
@@ -7631,7 +7643,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="364" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="364" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A364" s="5" t="s">
         <v>104</v>
       </c>
@@ -7648,7 +7660,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="365" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="365" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A365" s="5" t="s">
         <v>104</v>
       </c>
@@ -7665,7 +7677,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="366" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="366" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A366" s="5" t="s">
         <v>104</v>
       </c>
@@ -7682,7 +7694,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="368" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="368" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A368" s="5" t="s">
         <v>106</v>
       </c>
@@ -7699,7 +7711,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="369" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="369" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A369" s="5" t="s">
         <v>106</v>
       </c>
@@ -7716,7 +7728,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="370" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="370" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A370" s="5" t="s">
         <v>106</v>
       </c>
@@ -7733,7 +7745,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="371" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="371" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A371" s="5" t="s">
         <v>106</v>
       </c>
@@ -7750,7 +7762,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="372" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="372" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A372" s="5" t="s">
         <v>106</v>
       </c>
@@ -7767,7 +7779,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="374" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="374" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A374" s="5" t="s">
         <v>107</v>
       </c>
@@ -7784,7 +7796,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="375" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="375" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A375" s="5" t="s">
         <v>107</v>
       </c>
@@ -7801,7 +7813,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="376" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="376" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A376" s="5" t="s">
         <v>107</v>
       </c>
@@ -7818,7 +7830,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="377" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="377" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A377" s="5" t="s">
         <v>107</v>
       </c>
@@ -7835,7 +7847,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="378" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="378" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A378" s="5" t="s">
         <v>107</v>
       </c>
@@ -7852,7 +7864,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="380" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="380" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A380" s="5" t="s">
         <v>108</v>
       </c>
@@ -7869,7 +7881,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="381" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="381" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A381" s="5" t="s">
         <v>108</v>
       </c>
@@ -7886,7 +7898,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="382" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="382" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A382" s="5" t="s">
         <v>108</v>
       </c>
@@ -7903,7 +7915,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="383" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="383" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A383" s="5" t="s">
         <v>108</v>
       </c>
@@ -7920,7 +7932,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="384" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="384" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A384" s="5" t="s">
         <v>108</v>
       </c>
@@ -7937,7 +7949,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="386" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="386" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A386" s="5" t="s">
         <v>109</v>
       </c>
@@ -7954,7 +7966,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="387" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="387" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A387" s="5" t="s">
         <v>109</v>
       </c>
@@ -7971,7 +7983,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="388" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="388" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A388" s="5" t="s">
         <v>109</v>
       </c>
@@ -7988,7 +8000,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="389" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="389" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A389" s="5" t="s">
         <v>109</v>
       </c>
@@ -8005,7 +8017,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="390" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="390" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A390" s="5" t="s">
         <v>109</v>
       </c>
@@ -8022,12 +8034,12 @@
         <v>2</v>
       </c>
     </row>
-    <row r="391" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="391" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A391" s="4"/>
       <c r="B391" s="4"/>
       <c r="C391" s="4"/>
     </row>
-    <row r="392" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="392" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A392" s="5" t="s">
         <v>110</v>
       </c>
@@ -8044,7 +8056,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="393" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="393" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A393" s="5" t="s">
         <v>110</v>
       </c>
@@ -8061,7 +8073,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="394" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="394" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A394" s="5" t="s">
         <v>110</v>
       </c>
@@ -8078,7 +8090,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="395" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="395" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A395" s="5" t="s">
         <v>110</v>
       </c>
@@ -8095,7 +8107,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="397" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="397" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A397" s="5" t="s">
         <v>111</v>
       </c>
@@ -8112,7 +8124,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="398" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="398" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A398" s="5" t="s">
         <v>111</v>
       </c>
@@ -8129,7 +8141,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="399" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="399" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A399" s="5" t="s">
         <v>111</v>
       </c>
@@ -8146,7 +8158,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="400" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="400" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A400" s="5" t="s">
         <v>111</v>
       </c>
@@ -8163,7 +8175,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="402" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="402" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A402" s="5" t="s">
         <v>112</v>
       </c>
@@ -8180,7 +8192,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="403" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="403" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A403" s="5" t="s">
         <v>112</v>
       </c>
@@ -8197,7 +8209,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="404" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="404" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A404" s="5" t="s">
         <v>112</v>
       </c>
@@ -8214,7 +8226,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="405" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="405" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A405" s="5" t="s">
         <v>112</v>
       </c>
@@ -8231,7 +8243,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="407" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="407" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A407" s="5" t="s">
         <v>113</v>
       </c>
@@ -8248,7 +8260,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="408" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="408" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A408" s="5" t="s">
         <v>113</v>
       </c>
@@ -8265,7 +8277,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="409" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="409" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A409" s="5" t="s">
         <v>113</v>
       </c>
@@ -8282,7 +8294,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="410" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="410" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A410" s="5" t="s">
         <v>113</v>
       </c>
@@ -8299,7 +8311,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="412" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="412" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A412" s="5" t="s">
         <v>114</v>
       </c>
@@ -8316,7 +8328,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="413" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="413" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A413" s="5" t="s">
         <v>114</v>
       </c>
@@ -8333,7 +8345,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="414" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="414" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A414" s="5" t="s">
         <v>114</v>
       </c>
@@ -8350,7 +8362,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="415" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="415" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A415" s="5" t="s">
         <v>114</v>
       </c>
@@ -8367,7 +8379,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="417" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="417" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A417" s="5" t="s">
         <v>116</v>
       </c>
@@ -8384,7 +8396,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="418" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="418" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A418" s="5" t="s">
         <v>116</v>
       </c>
@@ -8401,7 +8413,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="420" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="420" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A420" s="5" t="s">
         <v>117</v>
       </c>
@@ -8418,7 +8430,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="421" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="421" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A421" s="5" t="s">
         <v>117</v>
       </c>
@@ -8435,7 +8447,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="423" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="423" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A423" s="5" t="s">
         <v>118</v>
       </c>
@@ -8452,7 +8464,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="424" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="424" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A424" s="5" t="s">
         <v>118</v>
       </c>
@@ -8469,7 +8481,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="426" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="426" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A426" s="5" t="s">
         <v>119</v>
       </c>
@@ -8486,7 +8498,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="427" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="427" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A427" s="5" t="s">
         <v>119</v>
       </c>
@@ -8503,7 +8515,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="429" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="429" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A429" s="5" t="s">
         <v>120</v>
       </c>
@@ -8520,7 +8532,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="430" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="430" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A430" s="5" t="s">
         <v>120</v>
       </c>
@@ -8537,7 +8549,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="432" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="432" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A432" s="5" t="s">
         <v>121</v>
       </c>
@@ -8554,7 +8566,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="433" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="433" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A433" s="5" t="s">
         <v>121</v>
       </c>
@@ -8571,7 +8583,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="435" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="435" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A435" s="5" t="s">
         <v>122</v>
       </c>
@@ -8588,7 +8600,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="436" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="436" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A436" s="5" t="s">
         <v>122</v>
       </c>
@@ -8605,7 +8617,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="438" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="438" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A438" s="5" t="s">
         <v>123</v>
       </c>
@@ -8622,7 +8634,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="439" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="439" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A439" s="5" t="s">
         <v>123</v>
       </c>
@@ -8639,7 +8651,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="441" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="441" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A441" s="5" t="s">
         <v>124</v>
       </c>
@@ -8656,7 +8668,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="442" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="442" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A442" s="5" t="s">
         <v>124</v>
       </c>
@@ -8673,7 +8685,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="444" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="444" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A444" s="5" t="s">
         <v>125</v>
       </c>
@@ -8690,7 +8702,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="445" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="445" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A445" s="5" t="s">
         <v>125</v>
       </c>
@@ -8707,7 +8719,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="447" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="447" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A447" s="5" t="s">
         <v>126</v>
       </c>
@@ -8724,7 +8736,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="448" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="448" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A448" s="5" t="s">
         <v>126</v>
       </c>
@@ -8741,7 +8753,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="450" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="450" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A450" s="5" t="s">
         <v>127</v>
       </c>
@@ -8758,7 +8770,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="451" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="451" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A451" s="5" t="s">
         <v>127</v>
       </c>
@@ -8775,7 +8787,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="453" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="453" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A453" s="5" t="s">
         <v>128</v>
       </c>
@@ -8792,7 +8804,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="454" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="454" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A454" s="5" t="s">
         <v>128</v>
       </c>
@@ -8809,7 +8821,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="456" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="456" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A456" s="5" t="s">
         <v>129</v>
       </c>
@@ -8826,7 +8838,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="457" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="457" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A457" s="5" t="s">
         <v>129</v>
       </c>
@@ -8843,7 +8855,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="459" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="459" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A459" s="5" t="s">
         <v>130</v>
       </c>
@@ -8860,7 +8872,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="461" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="461" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A461" s="5" t="s">
         <v>131</v>
       </c>
@@ -8877,7 +8889,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="463" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="463" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A463" s="5" t="s">
         <v>132</v>
       </c>
@@ -8894,7 +8906,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="465" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="465" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A465" s="5" t="s">
         <v>133</v>
       </c>
@@ -8911,7 +8923,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="466" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="466" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A466" s="5" t="s">
         <v>133</v>
       </c>
@@ -8928,7 +8940,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="468" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="468" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A468" s="5" t="s">
         <v>167</v>
       </c>
@@ -8946,7 +8958,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="469" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="469" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A469" s="5" t="s">
         <v>168</v>
       </c>
@@ -8963,7 +8975,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="470" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="470" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A470" s="5" t="s">
         <v>169</v>
       </c>
@@ -8980,7 +8992,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="471" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="471" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A471" s="5" t="s">
         <v>170</v>
       </c>
@@ -8997,7 +9009,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="472" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="472" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A472" s="5" t="s">
         <v>171</v>
       </c>
@@ -9014,7 +9026,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="473" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="473" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A473" s="5" t="s">
         <v>172</v>
       </c>
@@ -9031,7 +9043,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="474" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="474" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A474" s="5" t="s">
         <v>173</v>
       </c>
@@ -9048,7 +9060,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="475" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="475" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A475" s="5" t="s">
         <v>174</v>
       </c>
@@ -9065,7 +9077,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="476" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="476" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A476" s="5" t="s">
         <v>175</v>
       </c>
@@ -9082,7 +9094,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="478" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="478" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A478" s="5" t="s">
         <v>177</v>
       </c>
@@ -9099,7 +9111,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="479" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="479" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A479" s="5" t="s">
         <v>178</v>
       </c>
@@ -9116,7 +9128,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="480" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="480" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A480" s="5" t="s">
         <v>179</v>
       </c>
@@ -9133,7 +9145,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="481" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="481" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A481" s="5" t="s">
         <v>180</v>
       </c>
@@ -9150,7 +9162,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="482" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="482" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A482" s="5" t="s">
         <v>181</v>
       </c>
@@ -9167,7 +9179,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="483" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="483" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A483" s="5" t="s">
         <v>182</v>
       </c>
@@ -9184,7 +9196,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="484" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="484" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A484" s="4"/>
       <c r="B484" s="4"/>
       <c r="C484"/>
@@ -9192,7 +9204,7 @@
       <c r="E484" s="1"/>
       <c r="F484" s="1"/>
     </row>
-    <row r="485" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="485" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A485" s="5" t="s">
         <v>183</v>
       </c>
@@ -9213,7 +9225,7 @@
       <c r="H485" s="1"/>
       <c r="I485" s="1"/>
     </row>
-    <row r="486" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="486" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A486" s="5" t="s">
         <v>184</v>
       </c>
@@ -9234,7 +9246,7 @@
       <c r="H486" s="1"/>
       <c r="I486" s="1"/>
     </row>
-    <row r="487" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="487" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A487" s="5" t="s">
         <v>185</v>
       </c>
@@ -9255,7 +9267,7 @@
       <c r="H487" s="1"/>
       <c r="I487" s="1"/>
     </row>
-    <row r="488" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="488" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A488" s="5" t="s">
         <v>186</v>
       </c>
@@ -9276,7 +9288,7 @@
       <c r="H488" s="1"/>
       <c r="I488" s="1"/>
     </row>
-    <row r="489" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="489" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A489" s="5" t="s">
         <v>187</v>
       </c>
@@ -9297,7 +9309,7 @@
       <c r="H489" s="1"/>
       <c r="I489" s="1"/>
     </row>
-    <row r="490" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="490" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A490" s="5" t="s">
         <v>188</v>
       </c>
@@ -9318,7 +9330,7 @@
       <c r="H490" s="1"/>
       <c r="I490" s="1"/>
     </row>
-    <row r="491" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="491" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A491" s="5" t="s">
         <v>189</v>
       </c>
@@ -9339,7 +9351,7 @@
       <c r="H491" s="1"/>
       <c r="I491" s="1"/>
     </row>
-    <row r="492" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="492" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A492" s="5" t="s">
         <v>190</v>
       </c>
@@ -9360,7 +9372,7 @@
       <c r="H492" s="1"/>
       <c r="I492" s="1"/>
     </row>
-    <row r="493" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="493" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A493" s="5" t="s">
         <v>191</v>
       </c>
@@ -9379,11 +9391,11 @@
       <c r="F493" s="1"/>
       <c r="G493" s="1"/>
     </row>
-    <row r="494" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="494" spans="1:9" x14ac:dyDescent="0.25">
       <c r="F494" s="1"/>
       <c r="G494" s="1"/>
     </row>
-    <row r="495" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="495" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A495" s="5" t="s">
         <v>192</v>
       </c>
@@ -9402,7 +9414,7 @@
       <c r="F495" s="1"/>
       <c r="G495" s="1"/>
     </row>
-    <row r="496" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="496" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A496" s="5" t="s">
         <v>193</v>
       </c>
@@ -9421,7 +9433,7 @@
       <c r="F496" s="1"/>
       <c r="G496" s="1"/>
     </row>
-    <row r="497" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="497" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A497" s="5" t="s">
         <v>194</v>
       </c>
@@ -9439,7 +9451,7 @@
       </c>
       <c r="G497" s="1"/>
     </row>
-    <row r="498" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="498" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A498" s="5" t="s">
         <v>195</v>
       </c>
@@ -9456,7 +9468,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="499" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="499" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A499" s="5" t="s">
         <v>196</v>
       </c>
@@ -9474,7 +9486,7 @@
       </c>
       <c r="F499" s="1"/>
     </row>
-    <row r="500" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="500" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A500" s="5" t="s">
         <v>197</v>
       </c>
@@ -9492,7 +9504,7 @@
       </c>
       <c r="F500" s="1"/>
     </row>
-    <row r="501" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="501" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A501" s="5" t="s">
         <v>198</v>
       </c>
@@ -9510,7 +9522,7 @@
       </c>
       <c r="F501" s="1"/>
     </row>
-    <row r="502" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="502" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A502" s="5" t="s">
         <v>199</v>
       </c>
@@ -9527,7 +9539,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="503" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="503" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A503" s="5" t="s">
         <v>200</v>
       </c>
@@ -9544,7 +9556,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="505" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="505" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A505" s="5" t="s">
         <v>201</v>
       </c>
@@ -9561,7 +9573,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="506" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="506" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A506" s="5" t="s">
         <v>202</v>
       </c>
@@ -9578,7 +9590,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="507" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="507" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A507" s="5" t="s">
         <v>203</v>
       </c>
@@ -9595,7 +9607,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="508" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="508" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A508" s="5" t="s">
         <v>204</v>
       </c>
@@ -9612,7 +9624,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="509" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="509" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A509" s="5" t="s">
         <v>205</v>
       </c>
@@ -9629,7 +9641,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="510" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="510" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A510" s="5" t="s">
         <v>206</v>
       </c>
@@ -9646,7 +9658,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="511" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="511" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A511" s="5" t="s">
         <v>207</v>
       </c>
@@ -9663,7 +9675,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="512" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="512" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A512" s="5" t="s">
         <v>208</v>
       </c>
@@ -9680,7 +9692,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="513" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="513" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A513" s="5" t="s">
         <v>209</v>
       </c>
@@ -9697,7 +9709,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="514" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="514" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A514" s="5" t="s">
         <v>210</v>
       </c>
@@ -9714,7 +9726,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="515" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="515" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A515" s="5" t="s">
         <v>211</v>
       </c>
@@ -9731,7 +9743,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="516" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="516" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A516" s="5" t="s">
         <v>212</v>
       </c>
@@ -9748,7 +9760,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="517" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="517" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A517" s="5" t="s">
         <v>213</v>
       </c>
@@ -9765,7 +9777,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="518" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="518" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A518" s="5" t="s">
         <v>214</v>
       </c>
@@ -9782,7 +9794,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="520" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="520" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A520" s="5" t="s">
         <v>215</v>
       </c>
@@ -9799,7 +9811,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="521" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="521" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A521" s="5" t="s">
         <v>216</v>
       </c>
@@ -9816,7 +9828,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="522" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="522" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A522" s="5" t="s">
         <v>217</v>
       </c>
@@ -9833,7 +9845,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="523" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="523" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A523" s="5" t="s">
         <v>218</v>
       </c>
@@ -9850,7 +9862,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="524" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="524" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A524" s="5" t="s">
         <v>219</v>
       </c>
@@ -9867,7 +9879,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="525" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="525" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A525" s="5" t="s">
         <v>220</v>
       </c>
@@ -9884,55 +9896,55 @@
         <v>1</v>
       </c>
     </row>
-    <row r="526" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="526" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D526" s="4">
         <f>SUM(D2:D525)</f>
         <v>2310</v>
       </c>
     </row>
-    <row r="578" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="578" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A578" s="19"/>
     </row>
-    <row r="582" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="582" spans="1:6" x14ac:dyDescent="0.25">
       <c r="F582"/>
     </row>
-    <row r="583" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="583" spans="1:6" x14ac:dyDescent="0.25">
       <c r="F583"/>
     </row>
-    <row r="584" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="584" spans="1:6" x14ac:dyDescent="0.25">
       <c r="F584"/>
     </row>
-    <row r="585" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="585" spans="1:6" x14ac:dyDescent="0.25">
       <c r="F585"/>
     </row>
-    <row r="586" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="586" spans="1:6" x14ac:dyDescent="0.25">
       <c r="F586"/>
     </row>
-    <row r="587" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="587" spans="1:6" x14ac:dyDescent="0.25">
       <c r="F587"/>
     </row>
-    <row r="588" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="588" spans="1:6" x14ac:dyDescent="0.25">
       <c r="F588"/>
     </row>
-    <row r="589" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="589" spans="1:6" x14ac:dyDescent="0.25">
       <c r="F589"/>
     </row>
-    <row r="590" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="590" spans="1:6" x14ac:dyDescent="0.25">
       <c r="F590"/>
     </row>
-    <row r="591" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="591" spans="1:6" x14ac:dyDescent="0.25">
       <c r="F591"/>
     </row>
-    <row r="592" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="592" spans="1:6" x14ac:dyDescent="0.25">
       <c r="F592"/>
     </row>
-    <row r="593" spans="6:6" x14ac:dyDescent="0.3">
+    <row r="593" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F593"/>
     </row>
-    <row r="594" spans="6:6" x14ac:dyDescent="0.3">
+    <row r="594" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F594"/>
     </row>
-    <row r="595" spans="6:6" x14ac:dyDescent="0.3">
+    <row r="595" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F595"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Unity Secenes in elkaar gezet en asset list up to date
</commit_message>
<xml_diff>
--- a/Algemeen/Asset List Game-Lab 1.xlsx
+++ b/Algemeen/Asset List Game-Lab 1.xlsx
@@ -1141,10 +1141,10 @@
     <t>Anthony | Michiel | Roos</t>
   </si>
   <si>
-    <t>225 Fahrettin | 105 Sven | 70 Rief</t>
-  </si>
-  <si>
-    <t>Development Points: 400 / 500</t>
+    <t>225 Fahrettin | 145 Sven | 70 Rief</t>
+  </si>
+  <si>
+    <t>Development Points: 440 / 500</t>
   </si>
 </sst>
 </file>
@@ -1677,7 +1677,7 @@
   <dimension ref="A1:R595"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="J1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K34" sqref="K34"/>
+      <selection activeCell="K35" sqref="K35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2705,7 +2705,7 @@
       <c r="L28" s="22" t="s">
         <v>256</v>
       </c>
-      <c r="M28" s="1" t="s">
+      <c r="M28" s="22" t="s">
         <v>266</v>
       </c>
       <c r="N28" s="1" t="s">

</xml_diff>

<commit_message>
Asset List Up To Date en Mini fix in uren register
</commit_message>
<xml_diff>
--- a/Algemeen/Asset List Game-Lab 1.xlsx
+++ b/Algemeen/Asset List Game-Lab 1.xlsx
@@ -1141,10 +1141,10 @@
     <t>Anthony | Michiel | Roos</t>
   </si>
   <si>
-    <t>225 Fahrettin | 145 Sven | 70 Rief</t>
-  </si>
-  <si>
-    <t>Development Points: 440 / 500</t>
+    <t>Development Points: 460 / 500</t>
+  </si>
+  <si>
+    <t>245 Fahrettin | 145 Sven | 70 Rief</t>
   </si>
 </sst>
 </file>
@@ -1677,7 +1677,7 @@
   <dimension ref="A1:R595"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="J1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K35" sqref="K35"/>
+      <selection activeCell="K33" sqref="K33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2663,7 +2663,7 @@
       <c r="M27" s="1" t="s">
         <v>265</v>
       </c>
-      <c r="N27" s="1" t="s">
+      <c r="N27" s="22" t="s">
         <v>278</v>
       </c>
       <c r="O27" s="1" t="s">
@@ -2711,7 +2711,7 @@
       <c r="N28" s="1" t="s">
         <v>279</v>
       </c>
-      <c r="O28" s="1" t="s">
+      <c r="O28" s="22" t="s">
         <v>293</v>
       </c>
       <c r="P28" s="1" t="s">
@@ -2914,7 +2914,7 @@
       <c r="H34" s="19"/>
       <c r="I34" s="19"/>
       <c r="J34" s="24" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="N34" s="1" t="s">
         <v>277</v>
@@ -2942,7 +2942,7 @@
       <c r="H35" s="19"/>
       <c r="I35" s="19"/>
       <c r="J35" s="1" t="s">
-        <v>374</v>
+        <v>375</v>
       </c>
     </row>
     <row r="36" spans="1:18" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Up To Date Asset List
</commit_message>
<xml_diff>
--- a/Algemeen/Asset List Game-Lab 1.xlsx
+++ b/Algemeen/Asset List Game-Lab 1.xlsx
@@ -1141,10 +1141,10 @@
     <t>Anthony | Michiel | Roos</t>
   </si>
   <si>
-    <t>Development Points: 460 / 500</t>
-  </si>
-  <si>
-    <t>245 Fahrettin | 145 Sven | 70 Rief</t>
+    <t>Development Points: 510 / 500</t>
+  </si>
+  <si>
+    <t>245 Fahrettin | 145 Sven | 120 Rief</t>
   </si>
 </sst>
 </file>
@@ -1677,7 +1677,7 @@
   <dimension ref="A1:R595"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="J1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K33" sqref="K33"/>
+      <selection activeCell="K20" sqref="K20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2747,7 +2747,7 @@
       <c r="K29" s="22" t="s">
         <v>241</v>
       </c>
-      <c r="L29" s="1" t="s">
+      <c r="L29" s="22" t="s">
         <v>257</v>
       </c>
       <c r="M29" s="22" t="s">
@@ -2913,7 +2913,7 @@
       </c>
       <c r="H34" s="19"/>
       <c r="I34" s="19"/>
-      <c r="J34" s="24" t="s">
+      <c r="J34" s="22" t="s">
         <v>374</v>
       </c>
       <c r="N34" s="1" t="s">

</xml_diff>

<commit_message>
Asset list update & hud concept
</commit_message>
<xml_diff>
--- a/Algemeen/Asset List Game-Lab 1.xlsx
+++ b/Algemeen/Asset List Game-Lab 1.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12585"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12588"/>
   </bookViews>
   <sheets>
     <sheet name="Blad1" sheetId="1" r:id="rId1"/>
@@ -1135,16 +1135,16 @@
     <t>| Main Character_3.6 | Main Character_3.7 | Main Character_3.8 | Main Character_3.9 | Enemy_4.1 | Enemy_4.2 | Enemy_4.3|</t>
   </si>
   <si>
-    <t>Artist Points Behaald: 232 / 500</t>
-  </si>
-  <si>
-    <t>Anthony | Michiel | Roos</t>
-  </si>
-  <si>
-    <t>Development Points: 510 / 500</t>
-  </si>
-  <si>
-    <t>245 Fahrettin | 145 Sven | 120 Rief</t>
+    <t xml:space="preserve">240 Anthony | 46 Michiel | 106 Roos </t>
+  </si>
+  <si>
+    <t>245 Fahrettin | 145 Sven | 125 Rief</t>
+  </si>
+  <si>
+    <t>Artist Points Behaald: 392 / 625</t>
+  </si>
+  <si>
+    <t>Development Points: 510 / 625</t>
   </si>
 </sst>
 </file>
@@ -1195,7 +1195,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="14">
+  <fills count="15">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1271,6 +1271,12 @@
         <fgColor rgb="FFFFEB9C"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -1287,7 +1293,7 @@
     <xf numFmtId="0" fontId="4" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1358,6 +1364,15 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="14" borderId="0" xfId="3" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="14" borderId="0" xfId="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1676,32 +1691,32 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R595"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="J1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K20" sqref="K20"/>
+    <sheetView tabSelected="1" topLeftCell="I10" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="K34" sqref="K34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="26.42578125" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.42578125" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.85546875" style="4" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.85546875" style="4" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.140625" style="4" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.7109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="18.7109375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="123.28515625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="32.140625" style="1" customWidth="1"/>
-    <col min="11" max="11" width="27.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="27.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="30.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="28.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="30.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="28.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="17" max="18" width="30.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="26.44140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.44140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.88671875" style="4" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.88671875" style="4" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.109375" style="4" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.6640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="18.6640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="123.33203125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="32.109375" style="1" customWidth="1"/>
+    <col min="11" max="11" width="27.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="27.109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="30.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="28.5546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="30.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="28.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="17" max="18" width="30.44140625" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1757,7 +1772,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A2" s="5" t="s">
         <v>55</v>
       </c>
@@ -1811,7 +1826,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A3" s="5" t="s">
         <v>55</v>
       </c>
@@ -1864,7 +1879,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A4" s="5" t="s">
         <v>55</v>
       </c>
@@ -1898,7 +1913,7 @@
       <c r="L4" s="1" t="s">
         <v>243</v>
       </c>
-      <c r="M4" s="1" t="s">
+      <c r="M4" s="22" t="s">
         <v>233</v>
       </c>
       <c r="N4" s="20" t="s">
@@ -1917,7 +1932,7 @@
         <v>341</v>
       </c>
     </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A5" s="5" t="s">
         <v>55</v>
       </c>
@@ -1970,7 +1985,7 @@
         <v>342</v>
       </c>
     </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:18" x14ac:dyDescent="0.3">
       <c r="G6" s="10" t="s">
         <v>16</v>
       </c>
@@ -2005,7 +2020,7 @@
         <v>343</v>
       </c>
     </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A7" s="5" t="s">
         <v>56</v>
       </c>
@@ -2055,7 +2070,7 @@
         <v>345</v>
       </c>
     </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A8" s="5" t="s">
         <v>56</v>
       </c>
@@ -2083,7 +2098,7 @@
       <c r="L8" s="1" t="s">
         <v>247</v>
       </c>
-      <c r="M8" s="1" t="s">
+      <c r="M8" s="27" t="s">
         <v>262</v>
       </c>
       <c r="N8" s="1" t="s">
@@ -2102,7 +2117,7 @@
         <v>346</v>
       </c>
     </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A9" s="5" t="s">
         <v>56</v>
       </c>
@@ -2149,7 +2164,7 @@
         <v>349</v>
       </c>
     </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A10" s="5" t="s">
         <v>56</v>
       </c>
@@ -2196,7 +2211,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:18" x14ac:dyDescent="0.3">
       <c r="H11" s="3" t="s">
         <v>27</v>
       </c>
@@ -2225,7 +2240,7 @@
         <v>363</v>
       </c>
     </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A12" s="5" t="s">
         <v>57</v>
       </c>
@@ -2247,10 +2262,10 @@
       <c r="I12" s="3" t="s">
         <v>95</v>
       </c>
-      <c r="L12" s="25" t="s">
+      <c r="L12" s="26" t="s">
         <v>251</v>
       </c>
-      <c r="M12" s="25" t="s">
+      <c r="M12" s="26" t="s">
         <v>225</v>
       </c>
       <c r="O12" s="1" t="s">
@@ -2266,7 +2281,7 @@
         <v>353</v>
       </c>
     </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A13" s="5" t="s">
         <v>57</v>
       </c>
@@ -2291,7 +2306,7 @@
       <c r="L13" s="22" t="s">
         <v>252</v>
       </c>
-      <c r="M13" s="25" t="s">
+      <c r="M13" s="26" t="s">
         <v>234</v>
       </c>
       <c r="O13" s="1" t="s">
@@ -2303,11 +2318,11 @@
       <c r="Q13" s="1" t="s">
         <v>320</v>
       </c>
-      <c r="R13" s="22" t="s">
+      <c r="R13" s="28" t="s">
         <v>351</v>
       </c>
     </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A14" s="5" t="s">
         <v>57</v>
       </c>
@@ -2339,7 +2354,7 @@
         <v>321</v>
       </c>
     </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A15" s="5" t="s">
         <v>57</v>
       </c>
@@ -2368,7 +2383,7 @@
         <v>322</v>
       </c>
     </row>
-    <row r="16" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:18" x14ac:dyDescent="0.3">
       <c r="H16" s="3" t="s">
         <v>61</v>
       </c>
@@ -2382,7 +2397,7 @@
         <v>323</v>
       </c>
     </row>
-    <row r="17" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A17" s="5" t="s">
         <v>58</v>
       </c>
@@ -2411,7 +2426,7 @@
         <v>324</v>
       </c>
     </row>
-    <row r="18" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A18" s="5" t="s">
         <v>58</v>
       </c>
@@ -2440,7 +2455,7 @@
         <v>325</v>
       </c>
     </row>
-    <row r="19" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A19" s="5" t="s">
         <v>58</v>
       </c>
@@ -2469,7 +2484,7 @@
         <v>356</v>
       </c>
     </row>
-    <row r="20" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A20" s="5" t="s">
         <v>58</v>
       </c>
@@ -2491,11 +2506,11 @@
       <c r="I20" s="3" t="s">
         <v>365</v>
       </c>
-      <c r="L20" s="25" t="s">
+      <c r="L20" s="26" t="s">
         <v>224</v>
       </c>
     </row>
-    <row r="21" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:18" x14ac:dyDescent="0.3">
       <c r="H21" s="3" t="s">
         <v>166</v>
       </c>
@@ -2506,7 +2521,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="22" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A22" s="5" t="s">
         <v>65</v>
       </c>
@@ -2529,7 +2544,7 @@
         <v>371</v>
       </c>
     </row>
-    <row r="23" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A23" s="5" t="s">
         <v>65</v>
       </c>
@@ -2552,7 +2567,7 @@
         <v>366</v>
       </c>
     </row>
-    <row r="24" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A24" s="5" t="s">
         <v>65</v>
       </c>
@@ -2575,7 +2590,7 @@
         <v>367</v>
       </c>
     </row>
-    <row r="25" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A25" s="5" t="s">
         <v>65</v>
       </c>
@@ -2598,7 +2613,7 @@
         <v>368</v>
       </c>
     </row>
-    <row r="26" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:18" x14ac:dyDescent="0.3">
       <c r="B26" s="16"/>
       <c r="H26" s="3" t="s">
         <v>166</v>
@@ -2634,7 +2649,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="27" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A27" s="5" t="s">
         <v>71</v>
       </c>
@@ -2679,7 +2694,7 @@
         <v>333</v>
       </c>
     </row>
-    <row r="28" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A28" s="5" t="s">
         <v>71</v>
       </c>
@@ -2708,7 +2723,7 @@
       <c r="M28" s="22" t="s">
         <v>266</v>
       </c>
-      <c r="N28" s="1" t="s">
+      <c r="N28" s="22" t="s">
         <v>279</v>
       </c>
       <c r="O28" s="22" t="s">
@@ -2724,7 +2739,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="29" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A29" s="5" t="s">
         <v>71</v>
       </c>
@@ -2769,7 +2784,7 @@
         <v>335</v>
       </c>
     </row>
-    <row r="30" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A30" s="5" t="s">
         <v>71</v>
       </c>
@@ -2814,7 +2829,7 @@
         <v>336</v>
       </c>
     </row>
-    <row r="31" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:18" x14ac:dyDescent="0.3">
       <c r="B31" s="16"/>
       <c r="I31" s="19"/>
       <c r="J31" s="22" t="s">
@@ -2839,7 +2854,7 @@
         <v>337</v>
       </c>
     </row>
-    <row r="32" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A32" s="5" t="s">
         <v>59</v>
       </c>
@@ -2870,7 +2885,7 @@
         <v>338</v>
       </c>
     </row>
-    <row r="33" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A33" s="5" t="s">
         <v>59</v>
       </c>
@@ -2895,7 +2910,7 @@
         <v>339</v>
       </c>
     </row>
-    <row r="34" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A34" s="5" t="s">
         <v>59</v>
       </c>
@@ -2913,8 +2928,8 @@
       </c>
       <c r="H34" s="19"/>
       <c r="I34" s="19"/>
-      <c r="J34" s="22" t="s">
-        <v>374</v>
+      <c r="J34" s="24" t="s">
+        <v>375</v>
       </c>
       <c r="N34" s="1" t="s">
         <v>277</v>
@@ -2923,7 +2938,7 @@
         <v>340</v>
       </c>
     </row>
-    <row r="35" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A35" s="5" t="s">
         <v>59</v>
       </c>
@@ -2942,17 +2957,17 @@
       <c r="H35" s="19"/>
       <c r="I35" s="19"/>
       <c r="J35" s="1" t="s">
-        <v>375</v>
-      </c>
-    </row>
-    <row r="36" spans="1:18" x14ac:dyDescent="0.25">
+        <v>373</v>
+      </c>
+    </row>
+    <row r="36" spans="1:18" x14ac:dyDescent="0.3">
       <c r="H36" s="19"/>
       <c r="I36" s="19"/>
       <c r="J36" s="24" t="s">
-        <v>372</v>
-      </c>
-    </row>
-    <row r="37" spans="1:18" x14ac:dyDescent="0.25">
+        <v>374</v>
+      </c>
+    </row>
+    <row r="37" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A37" s="5" t="s">
         <v>41</v>
       </c>
@@ -2971,10 +2986,10 @@
       <c r="H37" s="19"/>
       <c r="I37" s="19"/>
       <c r="J37" s="1" t="s">
-        <v>373</v>
-      </c>
-    </row>
-    <row r="38" spans="1:18" x14ac:dyDescent="0.25">
+        <v>372</v>
+      </c>
+    </row>
+    <row r="38" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A38" s="5" t="s">
         <v>41</v>
       </c>
@@ -2993,7 +3008,7 @@
       <c r="I38" s="19"/>
       <c r="J38" s="23"/>
     </row>
-    <row r="39" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A39" s="5" t="s">
         <v>41</v>
       </c>
@@ -3011,7 +3026,7 @@
       </c>
       <c r="I39" s="19"/>
     </row>
-    <row r="40" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A40" s="5" t="s">
         <v>41</v>
       </c>
@@ -3029,7 +3044,7 @@
       </c>
       <c r="I40" s="2"/>
     </row>
-    <row r="42" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A42" s="5" t="s">
         <v>68</v>
       </c>
@@ -3046,7 +3061,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="43" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A43" s="5" t="s">
         <v>68</v>
       </c>
@@ -3063,7 +3078,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="44" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A44" s="5" t="s">
         <v>68</v>
       </c>
@@ -3080,7 +3095,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="45" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A45" s="5" t="s">
         <v>68</v>
       </c>
@@ -3097,7 +3112,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="47" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A47" s="5" t="s">
         <v>72</v>
       </c>
@@ -3114,7 +3129,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="48" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A48" s="5" t="s">
         <v>72</v>
       </c>
@@ -3131,7 +3146,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A49" s="5" t="s">
         <v>72</v>
       </c>
@@ -3148,7 +3163,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A50" s="5" t="s">
         <v>72</v>
       </c>
@@ -3165,7 +3180,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A52" s="5" t="s">
         <v>69</v>
       </c>
@@ -3182,7 +3197,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A53" s="5" t="s">
         <v>69</v>
       </c>
@@ -3199,7 +3214,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A54" s="5" t="s">
         <v>69</v>
       </c>
@@ -3216,7 +3231,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A55" s="5" t="s">
         <v>69</v>
       </c>
@@ -3233,10 +3248,10 @@
         <v>3</v>
       </c>
     </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B56" s="16"/>
     </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A57" s="5" t="s">
         <v>70</v>
       </c>
@@ -3253,7 +3268,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A58" s="5" t="s">
         <v>70</v>
       </c>
@@ -3270,7 +3285,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A59" s="5" t="s">
         <v>70</v>
       </c>
@@ -3287,7 +3302,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A60" s="5" t="s">
         <v>70</v>
       </c>
@@ -3304,7 +3319,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A62" s="5" t="s">
         <v>154</v>
       </c>
@@ -3321,7 +3336,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A63" s="5" t="s">
         <v>154</v>
       </c>
@@ -3338,7 +3353,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A64" s="5" t="s">
         <v>154</v>
       </c>
@@ -3355,7 +3370,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A65" s="5" t="s">
         <v>154</v>
       </c>
@@ -3372,7 +3387,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A67" s="5" t="s">
         <v>155</v>
       </c>
@@ -3389,7 +3404,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A68" s="5" t="s">
         <v>155</v>
       </c>
@@ -3406,7 +3421,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A69" s="5" t="s">
         <v>155</v>
       </c>
@@ -3423,7 +3438,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A70" s="5" t="s">
         <v>155</v>
       </c>
@@ -3440,7 +3455,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A71" s="5" t="s">
         <v>155</v>
       </c>
@@ -3457,7 +3472,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A72" s="5" t="s">
         <v>155</v>
       </c>
@@ -3474,10 +3489,10 @@
         <v>5</v>
       </c>
     </row>
-    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B73" s="16"/>
     </row>
-    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A74" s="5" t="s">
         <v>156</v>
       </c>
@@ -3494,7 +3509,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="75" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A75" s="5" t="s">
         <v>156</v>
       </c>
@@ -3511,7 +3526,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="76" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A76" s="5" t="s">
         <v>156</v>
       </c>
@@ -3528,7 +3543,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="77" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A77" s="5" t="s">
         <v>156</v>
       </c>
@@ -3545,7 +3560,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="79" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A79" s="5" t="s">
         <v>157</v>
       </c>
@@ -3562,7 +3577,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="80" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A80" s="5" t="s">
         <v>157</v>
       </c>
@@ -3579,7 +3594,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="81" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A81" s="5" t="s">
         <v>157</v>
       </c>
@@ -3596,7 +3611,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="82" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A82" s="5" t="s">
         <v>157</v>
       </c>
@@ -3613,7 +3628,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="84" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A84" s="5" t="s">
         <v>158</v>
       </c>
@@ -3630,7 +3645,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="85" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A85" s="5" t="s">
         <v>158</v>
       </c>
@@ -3647,7 +3662,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="86" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A86" s="5" t="s">
         <v>158</v>
       </c>
@@ -3664,7 +3679,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="87" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A87" s="5" t="s">
         <v>158</v>
       </c>
@@ -3681,7 +3696,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="89" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A89" s="5" t="s">
         <v>159</v>
       </c>
@@ -3698,7 +3713,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="90" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A90" s="5" t="s">
         <v>159</v>
       </c>
@@ -3715,7 +3730,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="91" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A91" s="5" t="s">
         <v>159</v>
       </c>
@@ -3732,7 +3747,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="92" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A92" s="5" t="s">
         <v>159</v>
       </c>
@@ -3749,7 +3764,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="94" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A94" s="5" t="s">
         <v>160</v>
       </c>
@@ -3766,7 +3781,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="95" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A95" s="5" t="s">
         <v>160</v>
       </c>
@@ -3783,7 +3798,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="96" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A96" s="5" t="s">
         <v>160</v>
       </c>
@@ -3800,7 +3815,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="97" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A97" s="5" t="s">
         <v>160</v>
       </c>
@@ -3817,7 +3832,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="99" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A99" s="5" t="s">
         <v>161</v>
       </c>
@@ -3834,7 +3849,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="100" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A100" s="5" t="s">
         <v>161</v>
       </c>
@@ -3851,7 +3866,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="101" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A101" s="5" t="s">
         <v>161</v>
       </c>
@@ -3868,7 +3883,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="102" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A102" s="5" t="s">
         <v>161</v>
       </c>
@@ -3885,7 +3900,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="104" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A104" s="5" t="s">
         <v>162</v>
       </c>
@@ -3902,7 +3917,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="105" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A105" s="5" t="s">
         <v>162</v>
       </c>
@@ -3919,7 +3934,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="106" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A106" s="5" t="s">
         <v>162</v>
       </c>
@@ -3936,7 +3951,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="107" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A107" s="5" t="s">
         <v>162</v>
       </c>
@@ -3953,10 +3968,10 @@
         <v>4</v>
       </c>
     </row>
-    <row r="108" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B108" s="16"/>
     </row>
-    <row r="109" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A109" s="5" t="s">
         <v>163</v>
       </c>
@@ -3973,7 +3988,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="110" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A110" s="5" t="s">
         <v>163</v>
       </c>
@@ -3990,7 +4005,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="111" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A111" s="5" t="s">
         <v>163</v>
       </c>
@@ -4007,7 +4022,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="112" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A112" s="5" t="s">
         <v>163</v>
       </c>
@@ -4024,10 +4039,10 @@
         <v>7</v>
       </c>
     </row>
-    <row r="113" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B113" s="16"/>
     </row>
-    <row r="114" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A114" s="5" t="s">
         <v>74</v>
       </c>
@@ -4044,7 +4059,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="115" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A115" s="5" t="s">
         <v>74</v>
       </c>
@@ -4061,7 +4076,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="116" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A116" s="5" t="s">
         <v>74</v>
       </c>
@@ -4078,7 +4093,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="117" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A117" s="5" t="s">
         <v>74</v>
       </c>
@@ -4095,10 +4110,10 @@
         <v>3</v>
       </c>
     </row>
-    <row r="118" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B118" s="16"/>
     </row>
-    <row r="119" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A119" s="5" t="s">
         <v>36</v>
       </c>
@@ -4115,7 +4130,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="120" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A120" s="5" t="s">
         <v>36</v>
       </c>
@@ -4132,7 +4147,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="121" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A121" s="5" t="s">
         <v>36</v>
       </c>
@@ -4149,7 +4164,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="122" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A122" s="5" t="s">
         <v>36</v>
       </c>
@@ -4166,12 +4181,12 @@
         <v>8</v>
       </c>
     </row>
-    <row r="123" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A123" s="4"/>
       <c r="B123" s="4"/>
       <c r="C123"/>
     </row>
-    <row r="124" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A124" s="5" t="s">
         <v>165</v>
       </c>
@@ -4188,7 +4203,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="125" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A125" s="5" t="s">
         <v>165</v>
       </c>
@@ -4205,7 +4220,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="126" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A126" s="5" t="s">
         <v>165</v>
       </c>
@@ -4222,7 +4237,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="127" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A127" s="5" t="s">
         <v>165</v>
       </c>
@@ -4239,7 +4254,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="129" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A129" s="5" t="s">
         <v>76</v>
       </c>
@@ -4256,7 +4271,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="130" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A130" s="5" t="s">
         <v>76</v>
       </c>
@@ -4273,7 +4288,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="131" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A131" s="5" t="s">
         <v>76</v>
       </c>
@@ -4290,7 +4305,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="132" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A132" s="5" t="s">
         <v>76</v>
       </c>
@@ -4307,11 +4322,11 @@
         <v>5</v>
       </c>
     </row>
-    <row r="133" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B133" s="16"/>
       <c r="G133" s="15"/>
     </row>
-    <row r="134" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A134" s="5" t="s">
         <v>48</v>
       </c>
@@ -4329,7 +4344,7 @@
       </c>
       <c r="G134" s="15"/>
     </row>
-    <row r="135" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A135" s="5" t="s">
         <v>48</v>
       </c>
@@ -4347,7 +4362,7 @@
       </c>
       <c r="G135" s="15"/>
     </row>
-    <row r="136" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A136" s="5" t="s">
         <v>48</v>
       </c>
@@ -4365,7 +4380,7 @@
       </c>
       <c r="G136" s="15"/>
     </row>
-    <row r="137" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A137" s="5" t="s">
         <v>48</v>
       </c>
@@ -4383,10 +4398,10 @@
       </c>
       <c r="G137" s="15"/>
     </row>
-    <row r="138" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:7" x14ac:dyDescent="0.3">
       <c r="G138" s="15"/>
     </row>
-    <row r="139" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A139" s="5" t="s">
         <v>153</v>
       </c>
@@ -4404,7 +4419,7 @@
       </c>
       <c r="G139" s="15"/>
     </row>
-    <row r="140" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A140" s="5" t="s">
         <v>153</v>
       </c>
@@ -4422,7 +4437,7 @@
       </c>
       <c r="G140" s="15"/>
     </row>
-    <row r="141" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A141" s="5" t="s">
         <v>153</v>
       </c>
@@ -4440,7 +4455,7 @@
       </c>
       <c r="G141" s="15"/>
     </row>
-    <row r="142" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A142" s="5" t="s">
         <v>153</v>
       </c>
@@ -4458,7 +4473,7 @@
       </c>
       <c r="G142" s="15"/>
     </row>
-    <row r="143" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A143" s="5" t="s">
         <v>153</v>
       </c>
@@ -4476,7 +4491,7 @@
       </c>
       <c r="G143" s="15"/>
     </row>
-    <row r="144" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A144" s="5" t="s">
         <v>153</v>
       </c>
@@ -4494,7 +4509,7 @@
       </c>
       <c r="G144" s="15"/>
     </row>
-    <row r="145" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A145" s="5" t="s">
         <v>153</v>
       </c>
@@ -4512,10 +4527,10 @@
       </c>
       <c r="G145" s="15"/>
     </row>
-    <row r="146" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:7" x14ac:dyDescent="0.3">
       <c r="G146" s="15"/>
     </row>
-    <row r="147" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A147" s="5" t="s">
         <v>77</v>
       </c>
@@ -4533,7 +4548,7 @@
       </c>
       <c r="G147" s="15"/>
     </row>
-    <row r="148" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A148" s="5" t="s">
         <v>77</v>
       </c>
@@ -4551,7 +4566,7 @@
       </c>
       <c r="G148" s="15"/>
     </row>
-    <row r="149" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A149" s="5" t="s">
         <v>77</v>
       </c>
@@ -4569,7 +4584,7 @@
       </c>
       <c r="G149" s="15"/>
     </row>
-    <row r="150" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A150" s="5" t="s">
         <v>77</v>
       </c>
@@ -4587,7 +4602,7 @@
       </c>
       <c r="G150" s="15"/>
     </row>
-    <row r="151" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A151" s="5" t="s">
         <v>77</v>
       </c>
@@ -4605,7 +4620,7 @@
       </c>
       <c r="G151" s="15"/>
     </row>
-    <row r="152" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A152" s="5" t="s">
         <v>77</v>
       </c>
@@ -4623,7 +4638,7 @@
       </c>
       <c r="G152" s="15"/>
     </row>
-    <row r="153" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A153" s="5" t="s">
         <v>77</v>
       </c>
@@ -4641,7 +4656,7 @@
       </c>
       <c r="G153" s="15"/>
     </row>
-    <row r="154" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A154" s="5" t="s">
         <v>77</v>
       </c>
@@ -4659,10 +4674,10 @@
       </c>
       <c r="G154" s="15"/>
     </row>
-    <row r="155" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:7" x14ac:dyDescent="0.3">
       <c r="G155" s="15"/>
     </row>
-    <row r="156" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A156" s="5" t="s">
         <v>78</v>
       </c>
@@ -4679,7 +4694,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="157" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A157" s="5" t="s">
         <v>78</v>
       </c>
@@ -4696,7 +4711,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="158" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A158" s="5" t="s">
         <v>78</v>
       </c>
@@ -4713,7 +4728,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="159" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A159" s="5" t="s">
         <v>78</v>
       </c>
@@ -4730,7 +4745,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="160" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A160" s="5" t="s">
         <v>78</v>
       </c>
@@ -4747,7 +4762,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="161" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A161" s="5" t="s">
         <v>78</v>
       </c>
@@ -4764,7 +4779,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="162" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A162" s="5" t="s">
         <v>78</v>
       </c>
@@ -4781,7 +4796,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="163" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A163" s="5" t="s">
         <v>78</v>
       </c>
@@ -4798,7 +4813,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="165" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A165" s="5" t="s">
         <v>79</v>
       </c>
@@ -4815,7 +4830,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="166" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A166" s="5" t="s">
         <v>79</v>
       </c>
@@ -4832,7 +4847,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="167" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A167" s="5" t="s">
         <v>79</v>
       </c>
@@ -4849,7 +4864,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="168" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A168" s="5" t="s">
         <v>79</v>
       </c>
@@ -4866,7 +4881,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="169" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A169" s="5" t="s">
         <v>79</v>
       </c>
@@ -4883,7 +4898,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="170" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A170" s="5" t="s">
         <v>79</v>
       </c>
@@ -4900,7 +4915,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="171" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A171" s="5" t="s">
         <v>79</v>
       </c>
@@ -4917,7 +4932,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="172" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A172" s="5" t="s">
         <v>79</v>
       </c>
@@ -4934,7 +4949,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="174" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A174" s="5" t="s">
         <v>80</v>
       </c>
@@ -4951,7 +4966,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="175" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A175" s="5" t="s">
         <v>80</v>
       </c>
@@ -4968,7 +4983,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="176" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A176" s="5" t="s">
         <v>80</v>
       </c>
@@ -4985,7 +5000,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="177" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A177" s="5" t="s">
         <v>80</v>
       </c>
@@ -5002,7 +5017,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="178" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A178" s="5" t="s">
         <v>80</v>
       </c>
@@ -5019,7 +5034,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="179" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A179" s="5" t="s">
         <v>80</v>
       </c>
@@ -5036,7 +5051,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="180" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A180" s="5" t="s">
         <v>80</v>
       </c>
@@ -5053,7 +5068,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="181" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A181" s="5" t="s">
         <v>80</v>
       </c>
@@ -5070,7 +5085,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="183" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A183" s="5" t="s">
         <v>81</v>
       </c>
@@ -5087,7 +5102,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="184" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A184" s="5" t="s">
         <v>81</v>
       </c>
@@ -5104,7 +5119,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="185" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A185" s="5" t="s">
         <v>81</v>
       </c>
@@ -5121,7 +5136,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="186" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A186" s="5" t="s">
         <v>81</v>
       </c>
@@ -5138,7 +5153,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="187" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A187" s="5" t="s">
         <v>81</v>
       </c>
@@ -5155,7 +5170,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="188" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A188" s="5" t="s">
         <v>81</v>
       </c>
@@ -5172,7 +5187,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="189" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A189" s="5" t="s">
         <v>81</v>
       </c>
@@ -5189,7 +5204,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="190" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A190" s="5" t="s">
         <v>81</v>
       </c>
@@ -5206,7 +5221,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="192" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A192" s="5" t="s">
         <v>82</v>
       </c>
@@ -5223,7 +5238,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="193" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A193" s="5" t="s">
         <v>82</v>
       </c>
@@ -5240,7 +5255,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="194" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A194" s="5" t="s">
         <v>82</v>
       </c>
@@ -5257,7 +5272,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="195" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A195" s="5" t="s">
         <v>82</v>
       </c>
@@ -5274,7 +5289,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="196" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A196" s="5" t="s">
         <v>82</v>
       </c>
@@ -5291,7 +5306,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="197" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A197" s="5" t="s">
         <v>82</v>
       </c>
@@ -5308,7 +5323,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="198" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="198" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A198" s="5" t="s">
         <v>82</v>
       </c>
@@ -5325,7 +5340,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="199" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="199" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A199" s="5" t="s">
         <v>82</v>
       </c>
@@ -5342,7 +5357,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="201" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="201" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A201" s="5" t="s">
         <v>37</v>
       </c>
@@ -5359,7 +5374,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="202" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="202" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A202" s="5" t="s">
         <v>37</v>
       </c>
@@ -5376,7 +5391,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="203" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="203" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A203" s="5" t="s">
         <v>37</v>
       </c>
@@ -5393,7 +5408,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="204" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="204" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A204" s="5" t="s">
         <v>37</v>
       </c>
@@ -5410,7 +5425,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="206" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="206" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A206" s="5" t="s">
         <v>40</v>
       </c>
@@ -5427,7 +5442,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="207" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="207" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A207" s="5" t="s">
         <v>40</v>
       </c>
@@ -5444,7 +5459,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="208" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="208" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A208" s="5" t="s">
         <v>40</v>
       </c>
@@ -5461,7 +5476,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="209" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="209" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A209" s="5" t="s">
         <v>40</v>
       </c>
@@ -5478,7 +5493,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="211" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="211" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A211" s="5" t="s">
         <v>83</v>
       </c>
@@ -5495,7 +5510,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="212" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="212" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A212" s="5" t="s">
         <v>83</v>
       </c>
@@ -5512,7 +5527,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="213" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="213" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A213" s="5" t="s">
         <v>83</v>
       </c>
@@ -5529,7 +5544,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="214" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="214" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A214" s="5" t="s">
         <v>83</v>
       </c>
@@ -5546,7 +5561,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="216" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="216" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A216" s="5" t="s">
         <v>85</v>
       </c>
@@ -5563,7 +5578,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="217" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="217" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A217" s="5" t="s">
         <v>85</v>
       </c>
@@ -5580,7 +5595,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="218" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="218" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A218" s="5" t="s">
         <v>85</v>
       </c>
@@ -5597,7 +5612,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="219" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="219" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A219" s="5" t="s">
         <v>85</v>
       </c>
@@ -5614,7 +5629,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="220" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="220" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A220" s="5" t="s">
         <v>85</v>
       </c>
@@ -5631,7 +5646,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="222" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="222" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A222" s="5" t="s">
         <v>86</v>
       </c>
@@ -5648,7 +5663,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="223" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="223" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A223" s="5" t="s">
         <v>86</v>
       </c>
@@ -5665,7 +5680,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="224" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="224" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A224" s="5" t="s">
         <v>86</v>
       </c>
@@ -5682,7 +5697,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="225" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="225" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A225" s="5" t="s">
         <v>86</v>
       </c>
@@ -5699,7 +5714,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="227" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="227" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A227" s="5" t="s">
         <v>87</v>
       </c>
@@ -5716,7 +5731,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="228" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="228" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A228" s="5" t="s">
         <v>87</v>
       </c>
@@ -5733,7 +5748,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="229" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="229" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A229" s="5" t="s">
         <v>87</v>
       </c>
@@ -5750,7 +5765,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="230" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="230" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A230" s="5" t="s">
         <v>87</v>
       </c>
@@ -5767,7 +5782,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="232" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="232" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A232" s="5" t="s">
         <v>88</v>
       </c>
@@ -5784,7 +5799,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="233" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="233" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A233" s="5" t="s">
         <v>88</v>
       </c>
@@ -5801,7 +5816,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="234" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="234" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A234" s="5" t="s">
         <v>88</v>
       </c>
@@ -5818,7 +5833,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="235" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="235" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A235" s="5" t="s">
         <v>88</v>
       </c>
@@ -5835,7 +5850,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="237" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="237" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A237" s="5" t="s">
         <v>89</v>
       </c>
@@ -5852,7 +5867,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="238" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="238" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A238" s="5" t="s">
         <v>89</v>
       </c>
@@ -5869,7 +5884,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="239" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="239" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A239" s="5" t="s">
         <v>89</v>
       </c>
@@ -5886,7 +5901,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="240" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="240" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A240" s="5" t="s">
         <v>89</v>
       </c>
@@ -5903,7 +5918,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="242" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="242" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A242" s="5" t="s">
         <v>90</v>
       </c>
@@ -5920,7 +5935,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="243" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="243" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A243" s="5" t="s">
         <v>90</v>
       </c>
@@ -5937,7 +5952,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="244" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="244" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A244" s="5" t="s">
         <v>90</v>
       </c>
@@ -5954,7 +5969,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="245" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="245" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A245" s="5" t="s">
         <v>90</v>
       </c>
@@ -5971,7 +5986,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="246" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="246" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A246" s="5" t="s">
         <v>90</v>
       </c>
@@ -5988,7 +6003,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="248" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="248" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A248" s="5" t="s">
         <v>91</v>
       </c>
@@ -6005,7 +6020,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="249" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="249" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A249" s="5" t="s">
         <v>91</v>
       </c>
@@ -6022,7 +6037,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="250" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="250" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A250" s="5" t="s">
         <v>91</v>
       </c>
@@ -6039,7 +6054,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="251" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="251" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A251" s="5" t="s">
         <v>91</v>
       </c>
@@ -6056,7 +6071,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="253" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="253" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A253" s="5" t="s">
         <v>92</v>
       </c>
@@ -6073,7 +6088,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="254" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="254" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A254" s="5" t="s">
         <v>92</v>
       </c>
@@ -6090,7 +6105,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="255" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="255" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A255" s="5" t="s">
         <v>92</v>
       </c>
@@ -6107,7 +6122,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="256" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="256" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A256" s="5" t="s">
         <v>92</v>
       </c>
@@ -6124,7 +6139,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="258" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="258" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A258" s="5" t="s">
         <v>93</v>
       </c>
@@ -6141,7 +6156,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="259" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="259" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A259" s="5" t="s">
         <v>93</v>
       </c>
@@ -6158,7 +6173,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="260" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="260" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A260" s="5" t="s">
         <v>93</v>
       </c>
@@ -6175,7 +6190,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="261" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="261" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A261" s="5" t="s">
         <v>93</v>
       </c>
@@ -6192,7 +6207,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="263" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="263" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A263" s="5" t="s">
         <v>94</v>
       </c>
@@ -6209,7 +6224,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="264" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="264" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A264" s="5" t="s">
         <v>94</v>
       </c>
@@ -6226,7 +6241,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="265" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="265" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A265" s="5" t="s">
         <v>94</v>
       </c>
@@ -6243,7 +6258,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="266" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="266" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A266" s="5" t="s">
         <v>94</v>
       </c>
@@ -6260,7 +6275,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="268" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="268" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A268" s="5" t="s">
         <v>96</v>
       </c>
@@ -6277,7 +6292,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="269" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="269" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A269" s="5" t="s">
         <v>96</v>
       </c>
@@ -6294,7 +6309,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="270" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="270" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A270" s="5" t="s">
         <v>96</v>
       </c>
@@ -6311,7 +6326,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="271" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="271" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A271" s="5" t="s">
         <v>96</v>
       </c>
@@ -6328,7 +6343,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="273" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="273" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A273" s="5" t="s">
         <v>97</v>
       </c>
@@ -6345,7 +6360,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="274" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="274" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A274" s="5" t="s">
         <v>97</v>
       </c>
@@ -6362,7 +6377,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="275" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="275" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A275" s="5" t="s">
         <v>97</v>
       </c>
@@ -6379,7 +6394,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="276" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="276" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A276" s="5" t="s">
         <v>97</v>
       </c>
@@ -6396,12 +6411,12 @@
         <v>10</v>
       </c>
     </row>
-    <row r="277" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="277" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A277" s="4"/>
       <c r="B277" s="4"/>
       <c r="C277" s="4"/>
     </row>
-    <row r="278" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="278" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A278" s="5" t="s">
         <v>144</v>
       </c>
@@ -6418,7 +6433,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="279" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="279" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A279" s="5" t="s">
         <v>144</v>
       </c>
@@ -6435,7 +6450,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="280" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="280" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A280" s="5" t="s">
         <v>144</v>
       </c>
@@ -6452,7 +6467,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="281" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="281" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A281" s="5" t="s">
         <v>144</v>
       </c>
@@ -6469,7 +6484,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="282" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="282" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A282" s="5" t="s">
         <v>144</v>
       </c>
@@ -6486,7 +6501,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="283" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="283" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A283" s="5" t="s">
         <v>144</v>
       </c>
@@ -6503,7 +6518,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="284" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="284" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A284" s="5" t="s">
         <v>144</v>
       </c>
@@ -6520,7 +6535,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="285" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="285" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A285" s="5" t="s">
         <v>144</v>
       </c>
@@ -6537,7 +6552,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="287" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="287" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A287" s="5" t="s">
         <v>145</v>
       </c>
@@ -6554,7 +6569,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="288" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="288" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A288" s="5" t="s">
         <v>145</v>
       </c>
@@ -6572,7 +6587,7 @@
       </c>
       <c r="F288" s="2"/>
     </row>
-    <row r="289" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="289" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A289" s="5" t="s">
         <v>145</v>
       </c>
@@ -6589,7 +6604,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="290" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="290" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A290" s="5" t="s">
         <v>145</v>
       </c>
@@ -6606,7 +6621,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="291" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="291" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A291" s="5" t="s">
         <v>145</v>
       </c>
@@ -6623,7 +6638,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="292" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="292" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A292" s="5" t="s">
         <v>145</v>
       </c>
@@ -6640,7 +6655,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="293" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="293" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A293" s="5" t="s">
         <v>145</v>
       </c>
@@ -6657,7 +6672,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="294" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="294" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A294" s="5" t="s">
         <v>145</v>
       </c>
@@ -6674,7 +6689,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="296" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="296" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A296" s="5" t="s">
         <v>146</v>
       </c>
@@ -6691,7 +6706,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="297" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="297" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A297" s="5" t="s">
         <v>146</v>
       </c>
@@ -6708,7 +6723,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="298" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="298" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A298" s="5" t="s">
         <v>146</v>
       </c>
@@ -6725,7 +6740,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="299" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="299" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A299" s="5" t="s">
         <v>146</v>
       </c>
@@ -6742,7 +6757,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="300" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="300" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A300" s="5" t="s">
         <v>146</v>
       </c>
@@ -6759,7 +6774,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="301" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="301" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A301" s="5" t="s">
         <v>146</v>
       </c>
@@ -6776,7 +6791,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="302" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="302" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A302" s="5" t="s">
         <v>146</v>
       </c>
@@ -6793,7 +6808,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="303" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="303" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A303" s="5" t="s">
         <v>146</v>
       </c>
@@ -6810,7 +6825,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="305" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="305" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A305" s="5" t="s">
         <v>147</v>
       </c>
@@ -6827,7 +6842,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="306" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="306" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A306" s="5" t="s">
         <v>147</v>
       </c>
@@ -6844,7 +6859,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="307" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="307" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A307" s="5" t="s">
         <v>147</v>
       </c>
@@ -6861,7 +6876,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="308" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="308" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A308" s="5" t="s">
         <v>147</v>
       </c>
@@ -6878,7 +6893,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="309" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="309" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A309" s="5" t="s">
         <v>147</v>
       </c>
@@ -6895,7 +6910,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="310" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="310" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A310" s="5" t="s">
         <v>147</v>
       </c>
@@ -6912,7 +6927,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="311" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="311" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A311" s="5" t="s">
         <v>147</v>
       </c>
@@ -6929,7 +6944,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="312" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="312" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A312" s="5" t="s">
         <v>147</v>
       </c>
@@ -6946,7 +6961,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="314" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="314" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A314" s="5" t="s">
         <v>148</v>
       </c>
@@ -6963,7 +6978,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="315" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="315" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A315" s="5" t="s">
         <v>148</v>
       </c>
@@ -6980,7 +6995,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="316" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="316" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A316" s="5" t="s">
         <v>148</v>
       </c>
@@ -6997,7 +7012,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="317" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="317" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A317" s="5" t="s">
         <v>148</v>
       </c>
@@ -7014,7 +7029,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="318" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="318" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A318" s="5" t="s">
         <v>148</v>
       </c>
@@ -7031,7 +7046,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="319" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="319" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A319" s="5" t="s">
         <v>148</v>
       </c>
@@ -7048,7 +7063,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="320" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="320" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A320" s="5" t="s">
         <v>148</v>
       </c>
@@ -7065,7 +7080,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="321" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="321" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A321" s="5" t="s">
         <v>148</v>
       </c>
@@ -7082,7 +7097,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="323" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="323" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A323" s="5" t="s">
         <v>44</v>
       </c>
@@ -7099,7 +7114,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="324" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="324" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A324" s="5" t="s">
         <v>44</v>
       </c>
@@ -7116,7 +7131,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="325" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="325" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A325" s="5" t="s">
         <v>44</v>
       </c>
@@ -7133,7 +7148,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="326" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="326" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A326" s="5" t="s">
         <v>44</v>
       </c>
@@ -7150,7 +7165,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="328" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="328" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A328" s="5" t="s">
         <v>45</v>
       </c>
@@ -7167,7 +7182,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="329" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="329" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A329" s="5" t="s">
         <v>45</v>
       </c>
@@ -7184,7 +7199,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="330" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="330" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A330" s="5" t="s">
         <v>45</v>
       </c>
@@ -7201,7 +7216,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="331" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="331" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A331" s="5" t="s">
         <v>45</v>
       </c>
@@ -7218,7 +7233,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="333" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="333" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A333" s="5" t="s">
         <v>98</v>
       </c>
@@ -7235,7 +7250,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="334" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="334" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A334" s="5" t="s">
         <v>98</v>
       </c>
@@ -7252,7 +7267,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="335" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="335" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A335" s="5" t="s">
         <v>98</v>
       </c>
@@ -7269,7 +7284,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="336" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="336" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A336" s="5" t="s">
         <v>98</v>
       </c>
@@ -7286,7 +7301,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="338" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="338" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A338" s="5" t="s">
         <v>99</v>
       </c>
@@ -7303,7 +7318,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="339" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="339" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A339" s="5" t="s">
         <v>99</v>
       </c>
@@ -7320,7 +7335,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="340" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="340" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A340" s="5" t="s">
         <v>99</v>
       </c>
@@ -7337,7 +7352,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="341" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="341" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A341" s="5" t="s">
         <v>99</v>
       </c>
@@ -7354,7 +7369,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="343" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="343" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A343" s="5" t="s">
         <v>100</v>
       </c>
@@ -7371,7 +7386,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="344" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="344" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A344" s="5" t="s">
         <v>100</v>
       </c>
@@ -7388,7 +7403,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="345" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="345" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A345" s="5" t="s">
         <v>100</v>
       </c>
@@ -7405,7 +7420,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="346" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="346" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A346" s="5" t="s">
         <v>100</v>
       </c>
@@ -7422,7 +7437,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="348" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="348" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A348" s="5" t="s">
         <v>101</v>
       </c>
@@ -7439,7 +7454,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="349" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="349" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A349" s="5" t="s">
         <v>101</v>
       </c>
@@ -7456,7 +7471,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="350" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="350" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A350" s="5" t="s">
         <v>101</v>
       </c>
@@ -7473,7 +7488,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="351" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="351" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A351" s="5" t="s">
         <v>101</v>
       </c>
@@ -7490,7 +7505,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="353" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="353" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A353" s="5" t="s">
         <v>102</v>
       </c>
@@ -7507,7 +7522,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="354" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="354" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A354" s="5" t="s">
         <v>102</v>
       </c>
@@ -7524,7 +7539,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="355" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="355" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A355" s="5" t="s">
         <v>102</v>
       </c>
@@ -7541,7 +7556,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="356" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="356" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A356" s="5" t="s">
         <v>102</v>
       </c>
@@ -7558,7 +7573,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="358" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="358" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A358" s="5" t="s">
         <v>103</v>
       </c>
@@ -7575,7 +7590,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="359" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="359" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A359" s="5" t="s">
         <v>103</v>
       </c>
@@ -7592,7 +7607,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="360" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="360" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A360" s="5" t="s">
         <v>103</v>
       </c>
@@ -7609,7 +7624,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="361" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="361" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A361" s="5" t="s">
         <v>103</v>
       </c>
@@ -7626,7 +7641,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="363" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="363" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A363" s="5" t="s">
         <v>104</v>
       </c>
@@ -7643,7 +7658,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="364" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="364" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A364" s="5" t="s">
         <v>104</v>
       </c>
@@ -7660,7 +7675,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="365" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="365" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A365" s="5" t="s">
         <v>104</v>
       </c>
@@ -7677,7 +7692,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="366" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="366" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A366" s="5" t="s">
         <v>104</v>
       </c>
@@ -7694,7 +7709,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="368" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="368" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A368" s="5" t="s">
         <v>106</v>
       </c>
@@ -7711,7 +7726,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="369" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="369" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A369" s="5" t="s">
         <v>106</v>
       </c>
@@ -7728,7 +7743,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="370" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="370" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A370" s="5" t="s">
         <v>106</v>
       </c>
@@ -7745,7 +7760,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="371" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="371" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A371" s="5" t="s">
         <v>106</v>
       </c>
@@ -7762,7 +7777,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="372" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="372" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A372" s="5" t="s">
         <v>106</v>
       </c>
@@ -7779,7 +7794,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="374" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="374" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A374" s="5" t="s">
         <v>107</v>
       </c>
@@ -7796,7 +7811,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="375" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="375" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A375" s="5" t="s">
         <v>107</v>
       </c>
@@ -7813,7 +7828,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="376" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="376" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A376" s="5" t="s">
         <v>107</v>
       </c>
@@ -7830,7 +7845,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="377" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="377" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A377" s="5" t="s">
         <v>107</v>
       </c>
@@ -7847,7 +7862,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="378" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="378" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A378" s="5" t="s">
         <v>107</v>
       </c>
@@ -7864,7 +7879,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="380" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="380" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A380" s="5" t="s">
         <v>108</v>
       </c>
@@ -7881,7 +7896,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="381" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="381" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A381" s="5" t="s">
         <v>108</v>
       </c>
@@ -7898,7 +7913,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="382" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="382" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A382" s="5" t="s">
         <v>108</v>
       </c>
@@ -7915,7 +7930,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="383" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="383" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A383" s="5" t="s">
         <v>108</v>
       </c>
@@ -7932,7 +7947,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="384" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="384" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A384" s="5" t="s">
         <v>108</v>
       </c>
@@ -7949,7 +7964,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="386" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="386" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A386" s="5" t="s">
         <v>109</v>
       </c>
@@ -7966,7 +7981,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="387" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="387" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A387" s="5" t="s">
         <v>109</v>
       </c>
@@ -7983,7 +7998,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="388" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="388" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A388" s="5" t="s">
         <v>109</v>
       </c>
@@ -8000,7 +8015,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="389" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="389" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A389" s="5" t="s">
         <v>109</v>
       </c>
@@ -8017,7 +8032,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="390" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="390" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A390" s="5" t="s">
         <v>109</v>
       </c>
@@ -8034,12 +8049,12 @@
         <v>2</v>
       </c>
     </row>
-    <row r="391" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="391" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A391" s="4"/>
       <c r="B391" s="4"/>
       <c r="C391" s="4"/>
     </row>
-    <row r="392" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="392" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A392" s="5" t="s">
         <v>110</v>
       </c>
@@ -8056,7 +8071,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="393" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="393" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A393" s="5" t="s">
         <v>110</v>
       </c>
@@ -8073,7 +8088,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="394" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="394" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A394" s="5" t="s">
         <v>110</v>
       </c>
@@ -8090,7 +8105,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="395" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="395" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A395" s="5" t="s">
         <v>110</v>
       </c>
@@ -8107,7 +8122,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="397" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="397" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A397" s="5" t="s">
         <v>111</v>
       </c>
@@ -8124,7 +8139,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="398" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="398" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A398" s="5" t="s">
         <v>111</v>
       </c>
@@ -8141,7 +8156,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="399" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="399" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A399" s="5" t="s">
         <v>111</v>
       </c>
@@ -8158,7 +8173,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="400" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="400" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A400" s="5" t="s">
         <v>111</v>
       </c>
@@ -8175,7 +8190,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="402" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="402" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A402" s="5" t="s">
         <v>112</v>
       </c>
@@ -8192,7 +8207,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="403" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="403" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A403" s="5" t="s">
         <v>112</v>
       </c>
@@ -8209,7 +8224,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="404" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="404" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A404" s="5" t="s">
         <v>112</v>
       </c>
@@ -8226,7 +8241,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="405" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="405" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A405" s="5" t="s">
         <v>112</v>
       </c>
@@ -8243,7 +8258,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="407" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="407" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A407" s="5" t="s">
         <v>113</v>
       </c>
@@ -8260,7 +8275,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="408" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="408" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A408" s="5" t="s">
         <v>113</v>
       </c>
@@ -8277,7 +8292,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="409" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="409" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A409" s="5" t="s">
         <v>113</v>
       </c>
@@ -8294,7 +8309,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="410" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="410" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A410" s="5" t="s">
         <v>113</v>
       </c>
@@ -8311,7 +8326,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="412" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="412" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A412" s="5" t="s">
         <v>114</v>
       </c>
@@ -8328,7 +8343,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="413" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="413" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A413" s="5" t="s">
         <v>114</v>
       </c>
@@ -8345,7 +8360,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="414" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="414" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A414" s="5" t="s">
         <v>114</v>
       </c>
@@ -8362,7 +8377,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="415" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="415" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A415" s="5" t="s">
         <v>114</v>
       </c>
@@ -8379,7 +8394,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="417" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="417" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A417" s="5" t="s">
         <v>116</v>
       </c>
@@ -8396,7 +8411,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="418" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="418" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A418" s="5" t="s">
         <v>116</v>
       </c>
@@ -8413,7 +8428,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="420" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="420" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A420" s="5" t="s">
         <v>117</v>
       </c>
@@ -8430,7 +8445,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="421" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="421" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A421" s="5" t="s">
         <v>117</v>
       </c>
@@ -8447,7 +8462,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="423" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="423" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A423" s="5" t="s">
         <v>118</v>
       </c>
@@ -8464,7 +8479,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="424" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="424" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A424" s="5" t="s">
         <v>118</v>
       </c>
@@ -8481,7 +8496,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="426" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="426" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A426" s="5" t="s">
         <v>119</v>
       </c>
@@ -8498,7 +8513,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="427" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="427" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A427" s="5" t="s">
         <v>119</v>
       </c>
@@ -8515,7 +8530,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="429" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="429" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A429" s="5" t="s">
         <v>120</v>
       </c>
@@ -8532,7 +8547,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="430" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="430" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A430" s="5" t="s">
         <v>120</v>
       </c>
@@ -8549,7 +8564,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="432" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="432" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A432" s="5" t="s">
         <v>121</v>
       </c>
@@ -8566,7 +8581,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="433" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="433" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A433" s="5" t="s">
         <v>121</v>
       </c>
@@ -8583,7 +8598,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="435" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="435" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A435" s="5" t="s">
         <v>122</v>
       </c>
@@ -8600,7 +8615,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="436" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="436" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A436" s="5" t="s">
         <v>122</v>
       </c>
@@ -8617,7 +8632,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="438" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="438" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A438" s="5" t="s">
         <v>123</v>
       </c>
@@ -8634,7 +8649,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="439" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="439" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A439" s="5" t="s">
         <v>123</v>
       </c>
@@ -8651,7 +8666,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="441" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="441" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A441" s="5" t="s">
         <v>124</v>
       </c>
@@ -8668,7 +8683,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="442" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="442" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A442" s="5" t="s">
         <v>124</v>
       </c>
@@ -8685,7 +8700,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="444" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="444" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A444" s="5" t="s">
         <v>125</v>
       </c>
@@ -8702,7 +8717,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="445" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="445" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A445" s="5" t="s">
         <v>125</v>
       </c>
@@ -8719,7 +8734,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="447" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="447" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A447" s="5" t="s">
         <v>126</v>
       </c>
@@ -8736,7 +8751,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="448" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="448" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A448" s="5" t="s">
         <v>126</v>
       </c>
@@ -8753,7 +8768,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="450" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="450" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A450" s="5" t="s">
         <v>127</v>
       </c>
@@ -8770,7 +8785,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="451" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="451" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A451" s="5" t="s">
         <v>127</v>
       </c>
@@ -8787,7 +8802,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="453" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="453" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A453" s="5" t="s">
         <v>128</v>
       </c>
@@ -8804,7 +8819,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="454" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="454" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A454" s="5" t="s">
         <v>128</v>
       </c>
@@ -8821,7 +8836,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="456" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="456" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A456" s="5" t="s">
         <v>129</v>
       </c>
@@ -8838,7 +8853,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="457" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="457" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A457" s="5" t="s">
         <v>129</v>
       </c>
@@ -8855,7 +8870,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="459" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="459" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A459" s="5" t="s">
         <v>130</v>
       </c>
@@ -8872,7 +8887,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="461" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="461" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A461" s="5" t="s">
         <v>131</v>
       </c>
@@ -8889,7 +8904,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="463" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="463" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A463" s="5" t="s">
         <v>132</v>
       </c>
@@ -8906,7 +8921,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="465" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="465" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A465" s="5" t="s">
         <v>133</v>
       </c>
@@ -8923,7 +8938,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="466" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="466" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A466" s="5" t="s">
         <v>133</v>
       </c>
@@ -8940,7 +8955,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="468" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="468" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A468" s="5" t="s">
         <v>167</v>
       </c>
@@ -8958,7 +8973,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="469" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="469" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A469" s="5" t="s">
         <v>168</v>
       </c>
@@ -8975,7 +8990,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="470" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="470" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A470" s="5" t="s">
         <v>169</v>
       </c>
@@ -8992,7 +9007,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="471" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="471" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A471" s="5" t="s">
         <v>170</v>
       </c>
@@ -9009,7 +9024,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="472" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="472" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A472" s="5" t="s">
         <v>171</v>
       </c>
@@ -9026,7 +9041,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="473" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="473" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A473" s="5" t="s">
         <v>172</v>
       </c>
@@ -9043,7 +9058,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="474" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="474" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A474" s="5" t="s">
         <v>173</v>
       </c>
@@ -9060,7 +9075,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="475" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="475" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A475" s="5" t="s">
         <v>174</v>
       </c>
@@ -9077,7 +9092,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="476" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="476" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A476" s="5" t="s">
         <v>175</v>
       </c>
@@ -9094,7 +9109,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="478" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="478" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A478" s="5" t="s">
         <v>177</v>
       </c>
@@ -9111,7 +9126,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="479" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="479" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A479" s="5" t="s">
         <v>178</v>
       </c>
@@ -9128,7 +9143,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="480" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="480" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A480" s="5" t="s">
         <v>179</v>
       </c>
@@ -9145,7 +9160,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="481" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="481" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A481" s="5" t="s">
         <v>180</v>
       </c>
@@ -9162,7 +9177,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="482" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="482" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A482" s="5" t="s">
         <v>181</v>
       </c>
@@ -9179,7 +9194,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="483" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="483" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A483" s="5" t="s">
         <v>182</v>
       </c>
@@ -9196,7 +9211,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="484" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="484" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A484" s="4"/>
       <c r="B484" s="4"/>
       <c r="C484"/>
@@ -9204,7 +9219,7 @@
       <c r="E484" s="1"/>
       <c r="F484" s="1"/>
     </row>
-    <row r="485" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="485" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A485" s="5" t="s">
         <v>183</v>
       </c>
@@ -9225,7 +9240,7 @@
       <c r="H485" s="1"/>
       <c r="I485" s="1"/>
     </row>
-    <row r="486" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="486" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A486" s="5" t="s">
         <v>184</v>
       </c>
@@ -9246,7 +9261,7 @@
       <c r="H486" s="1"/>
       <c r="I486" s="1"/>
     </row>
-    <row r="487" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="487" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A487" s="5" t="s">
         <v>185</v>
       </c>
@@ -9267,7 +9282,7 @@
       <c r="H487" s="1"/>
       <c r="I487" s="1"/>
     </row>
-    <row r="488" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="488" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A488" s="5" t="s">
         <v>186</v>
       </c>
@@ -9288,7 +9303,7 @@
       <c r="H488" s="1"/>
       <c r="I488" s="1"/>
     </row>
-    <row r="489" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="489" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A489" s="5" t="s">
         <v>187</v>
       </c>
@@ -9309,7 +9324,7 @@
       <c r="H489" s="1"/>
       <c r="I489" s="1"/>
     </row>
-    <row r="490" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="490" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A490" s="5" t="s">
         <v>188</v>
       </c>
@@ -9330,7 +9345,7 @@
       <c r="H490" s="1"/>
       <c r="I490" s="1"/>
     </row>
-    <row r="491" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="491" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A491" s="5" t="s">
         <v>189</v>
       </c>
@@ -9351,7 +9366,7 @@
       <c r="H491" s="1"/>
       <c r="I491" s="1"/>
     </row>
-    <row r="492" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="492" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A492" s="5" t="s">
         <v>190</v>
       </c>
@@ -9372,7 +9387,7 @@
       <c r="H492" s="1"/>
       <c r="I492" s="1"/>
     </row>
-    <row r="493" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="493" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A493" s="5" t="s">
         <v>191</v>
       </c>
@@ -9391,11 +9406,11 @@
       <c r="F493" s="1"/>
       <c r="G493" s="1"/>
     </row>
-    <row r="494" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="494" spans="1:9" x14ac:dyDescent="0.3">
       <c r="F494" s="1"/>
       <c r="G494" s="1"/>
     </row>
-    <row r="495" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="495" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A495" s="5" t="s">
         <v>192</v>
       </c>
@@ -9414,7 +9429,7 @@
       <c r="F495" s="1"/>
       <c r="G495" s="1"/>
     </row>
-    <row r="496" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="496" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A496" s="5" t="s">
         <v>193</v>
       </c>
@@ -9433,7 +9448,7 @@
       <c r="F496" s="1"/>
       <c r="G496" s="1"/>
     </row>
-    <row r="497" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="497" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A497" s="5" t="s">
         <v>194</v>
       </c>
@@ -9451,7 +9466,7 @@
       </c>
       <c r="G497" s="1"/>
     </row>
-    <row r="498" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="498" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A498" s="5" t="s">
         <v>195</v>
       </c>
@@ -9468,7 +9483,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="499" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="499" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A499" s="5" t="s">
         <v>196</v>
       </c>
@@ -9486,7 +9501,7 @@
       </c>
       <c r="F499" s="1"/>
     </row>
-    <row r="500" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="500" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A500" s="5" t="s">
         <v>197</v>
       </c>
@@ -9504,7 +9519,7 @@
       </c>
       <c r="F500" s="1"/>
     </row>
-    <row r="501" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="501" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A501" s="5" t="s">
         <v>198</v>
       </c>
@@ -9522,7 +9537,7 @@
       </c>
       <c r="F501" s="1"/>
     </row>
-    <row r="502" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="502" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A502" s="5" t="s">
         <v>199</v>
       </c>
@@ -9539,7 +9554,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="503" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="503" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A503" s="5" t="s">
         <v>200</v>
       </c>
@@ -9556,7 +9571,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="505" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="505" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A505" s="5" t="s">
         <v>201</v>
       </c>
@@ -9573,7 +9588,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="506" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="506" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A506" s="5" t="s">
         <v>202</v>
       </c>
@@ -9590,7 +9605,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="507" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="507" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A507" s="5" t="s">
         <v>203</v>
       </c>
@@ -9607,7 +9622,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="508" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="508" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A508" s="5" t="s">
         <v>204</v>
       </c>
@@ -9624,7 +9639,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="509" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="509" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A509" s="5" t="s">
         <v>205</v>
       </c>
@@ -9641,7 +9656,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="510" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="510" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A510" s="5" t="s">
         <v>206</v>
       </c>
@@ -9658,7 +9673,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="511" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="511" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A511" s="5" t="s">
         <v>207</v>
       </c>
@@ -9675,7 +9690,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="512" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="512" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A512" s="5" t="s">
         <v>208</v>
       </c>
@@ -9692,7 +9707,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="513" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="513" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A513" s="5" t="s">
         <v>209</v>
       </c>
@@ -9709,7 +9724,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="514" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="514" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A514" s="5" t="s">
         <v>210</v>
       </c>
@@ -9726,7 +9741,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="515" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="515" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A515" s="5" t="s">
         <v>211</v>
       </c>
@@ -9743,7 +9758,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="516" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="516" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A516" s="5" t="s">
         <v>212</v>
       </c>
@@ -9760,7 +9775,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="517" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="517" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A517" s="5" t="s">
         <v>213</v>
       </c>
@@ -9777,7 +9792,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="518" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="518" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A518" s="5" t="s">
         <v>214</v>
       </c>
@@ -9794,7 +9809,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="520" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="520" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A520" s="5" t="s">
         <v>215</v>
       </c>
@@ -9811,7 +9826,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="521" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="521" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A521" s="5" t="s">
         <v>216</v>
       </c>
@@ -9828,7 +9843,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="522" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="522" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A522" s="5" t="s">
         <v>217</v>
       </c>
@@ -9845,7 +9860,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="523" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="523" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A523" s="5" t="s">
         <v>218</v>
       </c>
@@ -9862,7 +9877,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="524" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="524" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A524" s="5" t="s">
         <v>219</v>
       </c>
@@ -9879,7 +9894,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="525" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="525" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A525" s="5" t="s">
         <v>220</v>
       </c>
@@ -9896,55 +9911,55 @@
         <v>1</v>
       </c>
     </row>
-    <row r="526" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="526" spans="1:5" x14ac:dyDescent="0.3">
       <c r="D526" s="4">
         <f>SUM(D2:D525)</f>
         <v>2310</v>
       </c>
     </row>
-    <row r="578" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="578" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A578" s="19"/>
     </row>
-    <row r="582" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="582" spans="1:6" x14ac:dyDescent="0.3">
       <c r="F582"/>
     </row>
-    <row r="583" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="583" spans="1:6" x14ac:dyDescent="0.3">
       <c r="F583"/>
     </row>
-    <row r="584" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="584" spans="1:6" x14ac:dyDescent="0.3">
       <c r="F584"/>
     </row>
-    <row r="585" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="585" spans="1:6" x14ac:dyDescent="0.3">
       <c r="F585"/>
     </row>
-    <row r="586" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="586" spans="1:6" x14ac:dyDescent="0.3">
       <c r="F586"/>
     </row>
-    <row r="587" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="587" spans="1:6" x14ac:dyDescent="0.3">
       <c r="F587"/>
     </row>
-    <row r="588" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="588" spans="1:6" x14ac:dyDescent="0.3">
       <c r="F588"/>
     </row>
-    <row r="589" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="589" spans="1:6" x14ac:dyDescent="0.3">
       <c r="F589"/>
     </row>
-    <row r="590" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="590" spans="1:6" x14ac:dyDescent="0.3">
       <c r="F590"/>
     </row>
-    <row r="591" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="591" spans="1:6" x14ac:dyDescent="0.3">
       <c r="F591"/>
     </row>
-    <row r="592" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="592" spans="1:6" x14ac:dyDescent="0.3">
       <c r="F592"/>
     </row>
-    <row r="593" spans="6:6" x14ac:dyDescent="0.25">
+    <row r="593" spans="6:6" x14ac:dyDescent="0.3">
       <c r="F593"/>
     </row>
-    <row r="594" spans="6:6" x14ac:dyDescent="0.25">
+    <row r="594" spans="6:6" x14ac:dyDescent="0.3">
       <c r="F594"/>
     </row>
-    <row r="595" spans="6:6" x14ac:dyDescent="0.25">
+    <row r="595" spans="6:6" x14ac:dyDescent="0.3">
       <c r="F595"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updates Unity en Asset List
</commit_message>
<xml_diff>
--- a/Algemeen/Asset List Game-Lab 1.xlsx
+++ b/Algemeen/Asset List Game-Lab 1.xlsx
@@ -1138,9 +1138,6 @@
     <t>lvlDesign_Schuur_4 (27)</t>
   </si>
   <si>
-    <t>Artist Points Behaald: 456 / 625</t>
-  </si>
-  <si>
     <t xml:space="preserve"> Anthony |  Michiel |  Roos </t>
   </si>
   <si>
@@ -1148,6 +1145,9 @@
   </si>
   <si>
     <t>Development Points: 515 / 625</t>
+  </si>
+  <si>
+    <t>Artist Points Behaald: 464 / 625</t>
   </si>
 </sst>
 </file>
@@ -1689,7 +1689,7 @@
   <dimension ref="A1:R594"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="J1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="N23" sqref="N23"/>
+      <selection activeCell="M16" sqref="M16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2098,7 +2098,7 @@
       <c r="M8" s="25" t="s">
         <v>261</v>
       </c>
-      <c r="N8" s="1" t="s">
+      <c r="N8" s="22" t="s">
         <v>361</v>
       </c>
       <c r="O8" s="1" t="s">
@@ -2186,7 +2186,7 @@
       <c r="I10" s="3" t="s">
         <v>84</v>
       </c>
-      <c r="L10" s="1" t="s">
+      <c r="L10" s="22" t="s">
         <v>248</v>
       </c>
       <c r="M10" s="22" t="s">
@@ -2926,7 +2926,7 @@
       <c r="H34" s="19"/>
       <c r="I34" s="19"/>
       <c r="J34" s="23" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="N34" s="1" t="s">
         <v>276</v>
@@ -2961,7 +2961,7 @@
       <c r="H36" s="19"/>
       <c r="I36" s="19"/>
       <c r="J36" s="23" t="s">
-        <v>373</v>
+        <v>376</v>
       </c>
     </row>
     <row r="37" spans="1:18" x14ac:dyDescent="0.25">
@@ -2983,7 +2983,7 @@
       <c r="H37" s="19"/>
       <c r="I37" s="19"/>
       <c r="J37" s="1" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
     </row>
     <row r="38" spans="1:18" x14ac:dyDescent="0.25">
@@ -3004,7 +3004,7 @@
       </c>
       <c r="I38" s="19"/>
       <c r="J38" s="1" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
     </row>
     <row r="39" spans="1:18" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Asset list update en scene 0
</commit_message>
<xml_diff>
--- a/Algemeen/Asset List Game-Lab 1.xlsx
+++ b/Algemeen/Asset List Game-Lab 1.xlsx
@@ -1147,7 +1147,7 @@
     <t>Development Points: 515 / 625</t>
   </si>
   <si>
-    <t>Artist Points Behaald: 464 / 625</t>
+    <t>Artist Points Behaald: 344 / 625</t>
   </si>
 </sst>
 </file>
@@ -1689,7 +1689,7 @@
   <dimension ref="A1:R594"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="J1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="M16" sqref="M16"/>
+      <selection activeCell="N19" sqref="N19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2048,7 +2048,7 @@
       <c r="L7" s="22" t="s">
         <v>245</v>
       </c>
-      <c r="M7" s="1" t="s">
+      <c r="M7" s="22" t="s">
         <v>260</v>
       </c>
       <c r="N7" s="1" t="s">

</xml_diff>

<commit_message>
Items Toegevoegd aan item xml document
</commit_message>
<xml_diff>
--- a/Algemeen/Asset List Game-Lab 1.xlsx
+++ b/Algemeen/Asset List Game-Lab 1.xlsx
@@ -10,14 +10,14 @@
     <sheet name="Blad1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Blad1!$A$1:$F$605</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Blad1!$A$1:$F$604</definedName>
   </definedNames>
   <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1533" uniqueCount="377">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1530" uniqueCount="377">
   <si>
     <t>ID Code</t>
   </si>
@@ -1132,9 +1132,6 @@
     <t>| Main Character_3.6 | Main Character_3.7 | Main Character_3.8 | Main Character_3.9 | Enemy_4.1 | Enemy_4.2 | Enemy_4.3|</t>
   </si>
   <si>
-    <t>245 Fahrettin | 145 Sven | 125 Rief</t>
-  </si>
-  <si>
     <t>lvlDesign_Schuur_4 (27)</t>
   </si>
   <si>
@@ -1144,10 +1141,13 @@
     <t xml:space="preserve"> Fahrettin</t>
   </si>
   <si>
-    <t>Development Points: 515 / 625</t>
-  </si>
-  <si>
-    <t>Artist Points Behaald: 344 / 625</t>
+    <t>Artist Points Behaald: 352 / 625</t>
+  </si>
+  <si>
+    <t>Development Points: 590 / 625</t>
+  </si>
+  <si>
+    <t>320 Fahrettin | 145 Sven | 125 Rief</t>
   </si>
 </sst>
 </file>
@@ -1296,7 +1296,7 @@
     <xf numFmtId="0" fontId="4" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1367,9 +1367,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="14" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="14" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1686,10 +1683,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:R594"/>
+  <dimension ref="A1:R593"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="J1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="M19" sqref="M19"/>
+      <selection activeCell="P18" sqref="P18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2139,7 +2136,7 @@
       <c r="I9" s="3" t="s">
         <v>134</v>
       </c>
-      <c r="L9" s="1" t="s">
+      <c r="L9" s="22" t="s">
         <v>247</v>
       </c>
       <c r="M9" s="22" t="s">
@@ -2263,7 +2260,7 @@
         <v>250</v>
       </c>
       <c r="M12" s="22" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="O12" s="1" t="s">
         <v>354</v>
@@ -2315,7 +2312,7 @@
       <c r="Q13" s="1" t="s">
         <v>319</v>
       </c>
-      <c r="R13" s="26" t="s">
+      <c r="R13" s="22" t="s">
         <v>350</v>
       </c>
     </row>
@@ -2804,7 +2801,7 @@
       <c r="K30" s="22" t="s">
         <v>241</v>
       </c>
-      <c r="L30" s="1" t="s">
+      <c r="L30" s="22" t="s">
         <v>254</v>
       </c>
       <c r="M30" s="22" t="s">
@@ -2928,7 +2925,7 @@
       <c r="J34" s="23" t="s">
         <v>375</v>
       </c>
-      <c r="N34" s="1" t="s">
+      <c r="N34" s="22" t="s">
         <v>276</v>
       </c>
       <c r="R34" s="1" t="s">
@@ -2954,14 +2951,14 @@
       <c r="H35" s="19"/>
       <c r="I35" s="19"/>
       <c r="J35" s="1" t="s">
-        <v>371</v>
+        <v>376</v>
       </c>
     </row>
     <row r="36" spans="1:18" x14ac:dyDescent="0.25">
       <c r="H36" s="19"/>
       <c r="I36" s="19"/>
       <c r="J36" s="23" t="s">
-        <v>376</v>
+        <v>374</v>
       </c>
     </row>
     <row r="37" spans="1:18" x14ac:dyDescent="0.25">
@@ -2983,7 +2980,7 @@
       <c r="H37" s="19"/>
       <c r="I37" s="19"/>
       <c r="J37" s="1" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
     </row>
     <row r="38" spans="1:18" x14ac:dyDescent="0.25">
@@ -3004,7 +3001,7 @@
       </c>
       <c r="I38" s="19"/>
       <c r="J38" s="1" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
     </row>
     <row r="39" spans="1:18" x14ac:dyDescent="0.25">
@@ -7844,35 +7841,35 @@
         <v>3</v>
       </c>
     </row>
-    <row r="377" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A377" s="5" t="s">
-        <v>107</v>
-      </c>
-      <c r="B377" s="13" t="s">
-        <v>17</v>
-      </c>
-      <c r="C377" s="1" t="s">
+    <row r="378" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A378" s="5" t="s">
+        <v>108</v>
+      </c>
+      <c r="B378" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="C378" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="D377" s="4">
-        <v>1</v>
-      </c>
-      <c r="E377" s="4">
-        <v>3</v>
+      <c r="D378" s="4">
+        <v>1</v>
+      </c>
+      <c r="E378" s="4">
+        <v>4</v>
       </c>
     </row>
     <row r="379" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A379" s="5" t="s">
         <v>108</v>
       </c>
-      <c r="B379" s="7" t="s">
-        <v>13</v>
+      <c r="B379" s="8" t="s">
+        <v>18</v>
       </c>
       <c r="C379" s="1" t="s">
         <v>52</v>
       </c>
       <c r="D379" s="4">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E379" s="4">
         <v>4</v>
@@ -7882,8 +7879,8 @@
       <c r="A380" s="5" t="s">
         <v>108</v>
       </c>
-      <c r="B380" s="8" t="s">
-        <v>18</v>
+      <c r="B380" s="17" t="s">
+        <v>15</v>
       </c>
       <c r="C380" s="1" t="s">
         <v>52</v>
@@ -7899,14 +7896,14 @@
       <c r="A381" s="5" t="s">
         <v>108</v>
       </c>
-      <c r="B381" s="17" t="s">
-        <v>15</v>
+      <c r="B381" s="9" t="s">
+        <v>50</v>
       </c>
       <c r="C381" s="1" t="s">
         <v>52</v>
       </c>
       <c r="D381" s="4">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E381" s="4">
         <v>4</v>
@@ -7916,48 +7913,48 @@
       <c r="A382" s="5" t="s">
         <v>108</v>
       </c>
-      <c r="B382" s="9" t="s">
-        <v>50</v>
+      <c r="B382" s="13" t="s">
+        <v>17</v>
       </c>
       <c r="C382" s="1" t="s">
         <v>52</v>
       </c>
       <c r="D382" s="4">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E382" s="4">
         <v>4</v>
       </c>
     </row>
-    <row r="383" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A383" s="5" t="s">
-        <v>108</v>
-      </c>
-      <c r="B383" s="13" t="s">
-        <v>17</v>
-      </c>
-      <c r="C383" s="1" t="s">
+    <row r="384" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A384" s="5" t="s">
+        <v>109</v>
+      </c>
+      <c r="B384" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="C384" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="D383" s="4">
-        <v>1</v>
-      </c>
-      <c r="E383" s="4">
-        <v>4</v>
+      <c r="D384" s="4">
+        <v>1</v>
+      </c>
+      <c r="E384" s="4">
+        <v>2</v>
       </c>
     </row>
     <row r="385" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A385" s="5" t="s">
         <v>109</v>
       </c>
-      <c r="B385" s="7" t="s">
-        <v>13</v>
+      <c r="B385" s="8" t="s">
+        <v>18</v>
       </c>
       <c r="C385" s="1" t="s">
         <v>52</v>
       </c>
       <c r="D385" s="4">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E385" s="4">
         <v>2</v>
@@ -7967,8 +7964,8 @@
       <c r="A386" s="5" t="s">
         <v>109</v>
       </c>
-      <c r="B386" s="8" t="s">
-        <v>18</v>
+      <c r="B386" s="17" t="s">
+        <v>15</v>
       </c>
       <c r="C386" s="1" t="s">
         <v>52</v>
@@ -7984,14 +7981,14 @@
       <c r="A387" s="5" t="s">
         <v>109</v>
       </c>
-      <c r="B387" s="17" t="s">
-        <v>15</v>
+      <c r="B387" s="9" t="s">
+        <v>50</v>
       </c>
       <c r="C387" s="1" t="s">
         <v>52</v>
       </c>
       <c r="D387" s="4">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E387" s="4">
         <v>2</v>
@@ -8001,53 +7998,53 @@
       <c r="A388" s="5" t="s">
         <v>109</v>
       </c>
-      <c r="B388" s="9" t="s">
-        <v>50</v>
+      <c r="B388" s="13" t="s">
+        <v>17</v>
       </c>
       <c r="C388" s="1" t="s">
         <v>52</v>
       </c>
       <c r="D388" s="4">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="E388" s="4">
         <v>2</v>
       </c>
     </row>
     <row r="389" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A389" s="5" t="s">
-        <v>109</v>
-      </c>
-      <c r="B389" s="13" t="s">
-        <v>17</v>
-      </c>
-      <c r="C389" s="1" t="s">
+      <c r="A389" s="4"/>
+      <c r="B389" s="4"/>
+      <c r="C389" s="4"/>
+    </row>
+    <row r="390" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A390" s="5" t="s">
+        <v>110</v>
+      </c>
+      <c r="B390" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="C390" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="D389" s="4">
-        <v>1</v>
-      </c>
-      <c r="E389" s="4">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="390" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A390" s="4"/>
-      <c r="B390" s="4"/>
-      <c r="C390" s="4"/>
+      <c r="D390" s="4">
+        <v>1</v>
+      </c>
+      <c r="E390" s="4">
+        <v>5</v>
+      </c>
     </row>
     <row r="391" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A391" s="5" t="s">
         <v>110</v>
       </c>
-      <c r="B391" s="7" t="s">
-        <v>13</v>
+      <c r="B391" s="8" t="s">
+        <v>18</v>
       </c>
       <c r="C391" s="1" t="s">
         <v>52</v>
       </c>
       <c r="D391" s="4">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E391" s="4">
         <v>5</v>
@@ -8057,8 +8054,8 @@
       <c r="A392" s="5" t="s">
         <v>110</v>
       </c>
-      <c r="B392" s="8" t="s">
-        <v>18</v>
+      <c r="B392" s="17" t="s">
+        <v>15</v>
       </c>
       <c r="C392" s="1" t="s">
         <v>52</v>
@@ -8074,48 +8071,48 @@
       <c r="A393" s="5" t="s">
         <v>110</v>
       </c>
-      <c r="B393" s="17" t="s">
-        <v>15</v>
+      <c r="B393" s="9" t="s">
+        <v>50</v>
       </c>
       <c r="C393" s="1" t="s">
         <v>52</v>
       </c>
       <c r="D393" s="4">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E393" s="4">
         <v>5</v>
       </c>
     </row>
-    <row r="394" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A394" s="5" t="s">
-        <v>110</v>
-      </c>
-      <c r="B394" s="9" t="s">
-        <v>50</v>
-      </c>
-      <c r="C394" s="1" t="s">
+    <row r="395" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A395" s="5" t="s">
+        <v>111</v>
+      </c>
+      <c r="B395" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="C395" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="D394" s="4">
-        <v>4</v>
-      </c>
-      <c r="E394" s="4">
-        <v>5</v>
+      <c r="D395" s="4">
+        <v>1</v>
+      </c>
+      <c r="E395" s="4">
+        <v>4</v>
       </c>
     </row>
     <row r="396" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A396" s="5" t="s">
         <v>111</v>
       </c>
-      <c r="B396" s="7" t="s">
-        <v>13</v>
+      <c r="B396" s="8" t="s">
+        <v>18</v>
       </c>
       <c r="C396" s="1" t="s">
         <v>52</v>
       </c>
       <c r="D396" s="4">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E396" s="4">
         <v>4</v>
@@ -8125,8 +8122,8 @@
       <c r="A397" s="5" t="s">
         <v>111</v>
       </c>
-      <c r="B397" s="8" t="s">
-        <v>18</v>
+      <c r="B397" s="17" t="s">
+        <v>15</v>
       </c>
       <c r="C397" s="1" t="s">
         <v>52</v>
@@ -8142,8 +8139,8 @@
       <c r="A398" s="5" t="s">
         <v>111</v>
       </c>
-      <c r="B398" s="17" t="s">
-        <v>15</v>
+      <c r="B398" s="9" t="s">
+        <v>50</v>
       </c>
       <c r="C398" s="1" t="s">
         <v>52</v>
@@ -8155,20 +8152,20 @@
         <v>4</v>
       </c>
     </row>
-    <row r="399" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A399" s="5" t="s">
-        <v>111</v>
-      </c>
-      <c r="B399" s="9" t="s">
-        <v>50</v>
-      </c>
-      <c r="C399" s="1" t="s">
+    <row r="400" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A400" s="5" t="s">
+        <v>112</v>
+      </c>
+      <c r="B400" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="C400" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="D399" s="4">
-        <v>3</v>
-      </c>
-      <c r="E399" s="4">
+      <c r="D400" s="4">
+        <v>1</v>
+      </c>
+      <c r="E400" s="4">
         <v>4</v>
       </c>
     </row>
@@ -8176,14 +8173,14 @@
       <c r="A401" s="5" t="s">
         <v>112</v>
       </c>
-      <c r="B401" s="7" t="s">
-        <v>13</v>
+      <c r="B401" s="8" t="s">
+        <v>18</v>
       </c>
       <c r="C401" s="1" t="s">
         <v>52</v>
       </c>
       <c r="D401" s="4">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E401" s="4">
         <v>4</v>
@@ -8193,8 +8190,8 @@
       <c r="A402" s="5" t="s">
         <v>112</v>
       </c>
-      <c r="B402" s="8" t="s">
-        <v>18</v>
+      <c r="B402" s="17" t="s">
+        <v>15</v>
       </c>
       <c r="C402" s="1" t="s">
         <v>52</v>
@@ -8210,8 +8207,8 @@
       <c r="A403" s="5" t="s">
         <v>112</v>
       </c>
-      <c r="B403" s="17" t="s">
-        <v>15</v>
+      <c r="B403" s="9" t="s">
+        <v>50</v>
       </c>
       <c r="C403" s="1" t="s">
         <v>52</v>
@@ -8223,20 +8220,20 @@
         <v>4</v>
       </c>
     </row>
-    <row r="404" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A404" s="5" t="s">
-        <v>112</v>
-      </c>
-      <c r="B404" s="9" t="s">
-        <v>50</v>
-      </c>
-      <c r="C404" s="1" t="s">
+    <row r="405" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A405" s="5" t="s">
+        <v>113</v>
+      </c>
+      <c r="B405" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="C405" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="D404" s="4">
-        <v>3</v>
-      </c>
-      <c r="E404" s="4">
+      <c r="D405" s="4">
+        <v>1</v>
+      </c>
+      <c r="E405" s="4">
         <v>4</v>
       </c>
     </row>
@@ -8244,14 +8241,14 @@
       <c r="A406" s="5" t="s">
         <v>113</v>
       </c>
-      <c r="B406" s="7" t="s">
-        <v>13</v>
+      <c r="B406" s="8" t="s">
+        <v>18</v>
       </c>
       <c r="C406" s="1" t="s">
         <v>52</v>
       </c>
       <c r="D406" s="4">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E406" s="4">
         <v>4</v>
@@ -8261,8 +8258,8 @@
       <c r="A407" s="5" t="s">
         <v>113</v>
       </c>
-      <c r="B407" s="8" t="s">
-        <v>18</v>
+      <c r="B407" s="17" t="s">
+        <v>15</v>
       </c>
       <c r="C407" s="1" t="s">
         <v>52</v>
@@ -8278,8 +8275,8 @@
       <c r="A408" s="5" t="s">
         <v>113</v>
       </c>
-      <c r="B408" s="17" t="s">
-        <v>15</v>
+      <c r="B408" s="9" t="s">
+        <v>50</v>
       </c>
       <c r="C408" s="1" t="s">
         <v>52</v>
@@ -8291,20 +8288,20 @@
         <v>4</v>
       </c>
     </row>
-    <row r="409" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A409" s="5" t="s">
-        <v>113</v>
-      </c>
-      <c r="B409" s="9" t="s">
-        <v>50</v>
-      </c>
-      <c r="C409" s="1" t="s">
+    <row r="410" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A410" s="5" t="s">
+        <v>114</v>
+      </c>
+      <c r="B410" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="C410" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="D409" s="4">
-        <v>3</v>
-      </c>
-      <c r="E409" s="4">
+      <c r="D410" s="4">
+        <v>1</v>
+      </c>
+      <c r="E410" s="4">
         <v>4</v>
       </c>
     </row>
@@ -8312,14 +8309,14 @@
       <c r="A411" s="5" t="s">
         <v>114</v>
       </c>
-      <c r="B411" s="7" t="s">
-        <v>13</v>
+      <c r="B411" s="8" t="s">
+        <v>18</v>
       </c>
       <c r="C411" s="1" t="s">
         <v>52</v>
       </c>
       <c r="D411" s="4">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E411" s="4">
         <v>4</v>
@@ -8329,8 +8326,8 @@
       <c r="A412" s="5" t="s">
         <v>114</v>
       </c>
-      <c r="B412" s="8" t="s">
-        <v>18</v>
+      <c r="B412" s="17" t="s">
+        <v>15</v>
       </c>
       <c r="C412" s="1" t="s">
         <v>52</v>
@@ -8346,8 +8343,8 @@
       <c r="A413" s="5" t="s">
         <v>114</v>
       </c>
-      <c r="B413" s="17" t="s">
-        <v>15</v>
+      <c r="B413" s="9" t="s">
+        <v>50</v>
       </c>
       <c r="C413" s="1" t="s">
         <v>52</v>
@@ -8359,54 +8356,54 @@
         <v>4</v>
       </c>
     </row>
-    <row r="414" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A414" s="5" t="s">
-        <v>114</v>
-      </c>
-      <c r="B414" s="9" t="s">
-        <v>50</v>
-      </c>
-      <c r="C414" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="D414" s="4">
-        <v>3</v>
-      </c>
-      <c r="E414" s="4">
-        <v>4</v>
+    <row r="415" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A415" s="5" t="s">
+        <v>116</v>
+      </c>
+      <c r="B415" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="C415" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="D415" s="4">
+        <v>1</v>
+      </c>
+      <c r="E415" s="4">
+        <v>10</v>
       </c>
     </row>
     <row r="416" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A416" s="5" t="s">
         <v>116</v>
       </c>
-      <c r="B416" s="7" t="s">
-        <v>13</v>
+      <c r="B416" s="9" t="s">
+        <v>19</v>
       </c>
       <c r="C416" s="1" t="s">
         <v>54</v>
       </c>
       <c r="D416" s="4">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E416" s="4">
         <v>10</v>
       </c>
     </row>
-    <row r="417" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A417" s="5" t="s">
-        <v>116</v>
-      </c>
-      <c r="B417" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="C417" s="1" t="s">
+    <row r="418" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A418" s="5" t="s">
+        <v>117</v>
+      </c>
+      <c r="B418" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="C418" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="D417" s="4">
-        <v>2</v>
-      </c>
-      <c r="E417" s="4">
+      <c r="D418" s="4">
+        <v>1</v>
+      </c>
+      <c r="E418" s="4">
         <v>10</v>
       </c>
     </row>
@@ -8414,33 +8411,33 @@
       <c r="A419" s="5" t="s">
         <v>117</v>
       </c>
-      <c r="B419" s="7" t="s">
-        <v>13</v>
+      <c r="B419" s="9" t="s">
+        <v>19</v>
       </c>
       <c r="C419" s="1" t="s">
         <v>54</v>
       </c>
       <c r="D419" s="4">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E419" s="4">
         <v>10</v>
       </c>
     </row>
-    <row r="420" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A420" s="5" t="s">
-        <v>117</v>
-      </c>
-      <c r="B420" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="C420" s="1" t="s">
+    <row r="421" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A421" s="5" t="s">
+        <v>118</v>
+      </c>
+      <c r="B421" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="C421" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="D420" s="4">
-        <v>2</v>
-      </c>
-      <c r="E420" s="4">
+      <c r="D421" s="4">
+        <v>1</v>
+      </c>
+      <c r="E421" s="4">
         <v>10</v>
       </c>
     </row>
@@ -8448,135 +8445,135 @@
       <c r="A422" s="5" t="s">
         <v>118</v>
       </c>
-      <c r="B422" s="7" t="s">
-        <v>13</v>
+      <c r="B422" s="9" t="s">
+        <v>19</v>
       </c>
       <c r="C422" s="1" t="s">
         <v>54</v>
       </c>
       <c r="D422" s="4">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E422" s="4">
         <v>10</v>
       </c>
     </row>
-    <row r="423" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A423" s="5" t="s">
-        <v>118</v>
-      </c>
-      <c r="B423" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="C423" s="1" t="s">
+    <row r="424" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A424" s="5" t="s">
+        <v>119</v>
+      </c>
+      <c r="B424" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="C424" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="D423" s="4">
-        <v>2</v>
-      </c>
-      <c r="E423" s="4">
-        <v>10</v>
+      <c r="D424" s="4">
+        <v>1</v>
+      </c>
+      <c r="E424" s="4">
+        <v>4</v>
       </c>
     </row>
     <row r="425" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A425" s="5" t="s">
         <v>119</v>
       </c>
-      <c r="B425" s="7" t="s">
-        <v>13</v>
+      <c r="B425" s="9" t="s">
+        <v>19</v>
       </c>
       <c r="C425" s="1" t="s">
         <v>54</v>
       </c>
       <c r="D425" s="4">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E425" s="4">
         <v>4</v>
       </c>
     </row>
-    <row r="426" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A426" s="5" t="s">
-        <v>119</v>
-      </c>
-      <c r="B426" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="C426" s="1" t="s">
+    <row r="427" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A427" s="5" t="s">
+        <v>120</v>
+      </c>
+      <c r="B427" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="C427" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="D426" s="4">
-        <v>2</v>
-      </c>
-      <c r="E426" s="4">
-        <v>4</v>
+      <c r="D427" s="4">
+        <v>1</v>
+      </c>
+      <c r="E427" s="4">
+        <v>10</v>
       </c>
     </row>
     <row r="428" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A428" s="5" t="s">
         <v>120</v>
       </c>
-      <c r="B428" s="7" t="s">
-        <v>13</v>
+      <c r="B428" s="9" t="s">
+        <v>19</v>
       </c>
       <c r="C428" s="1" t="s">
         <v>54</v>
       </c>
       <c r="D428" s="4">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E428" s="4">
         <v>10</v>
       </c>
     </row>
-    <row r="429" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A429" s="5" t="s">
-        <v>120</v>
-      </c>
-      <c r="B429" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="C429" s="1" t="s">
+    <row r="430" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A430" s="5" t="s">
+        <v>121</v>
+      </c>
+      <c r="B430" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="C430" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="D429" s="4">
-        <v>2</v>
-      </c>
-      <c r="E429" s="4">
-        <v>10</v>
+      <c r="D430" s="4">
+        <v>1</v>
+      </c>
+      <c r="E430" s="4">
+        <v>1</v>
       </c>
     </row>
     <row r="431" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A431" s="5" t="s">
         <v>121</v>
       </c>
-      <c r="B431" s="7" t="s">
-        <v>13</v>
+      <c r="B431" s="9" t="s">
+        <v>19</v>
       </c>
       <c r="C431" s="1" t="s">
         <v>54</v>
       </c>
       <c r="D431" s="4">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E431" s="4">
         <v>1</v>
       </c>
     </row>
-    <row r="432" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A432" s="5" t="s">
-        <v>121</v>
-      </c>
-      <c r="B432" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="C432" s="1" t="s">
+    <row r="433" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A433" s="5" t="s">
+        <v>122</v>
+      </c>
+      <c r="B433" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="C433" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="D432" s="4">
-        <v>2</v>
-      </c>
-      <c r="E432" s="4">
+      <c r="D433" s="4">
+        <v>1</v>
+      </c>
+      <c r="E433" s="4">
         <v>1</v>
       </c>
     </row>
@@ -8584,101 +8581,101 @@
       <c r="A434" s="5" t="s">
         <v>122</v>
       </c>
-      <c r="B434" s="7" t="s">
-        <v>13</v>
+      <c r="B434" s="9" t="s">
+        <v>19</v>
       </c>
       <c r="C434" s="1" t="s">
         <v>54</v>
       </c>
       <c r="D434" s="4">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E434" s="4">
         <v>1</v>
       </c>
     </row>
-    <row r="435" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A435" s="5" t="s">
-        <v>122</v>
-      </c>
-      <c r="B435" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="C435" s="1" t="s">
+    <row r="436" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A436" s="5" t="s">
+        <v>123</v>
+      </c>
+      <c r="B436" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="C436" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="D435" s="4">
-        <v>2</v>
-      </c>
-      <c r="E435" s="4">
-        <v>1</v>
+      <c r="D436" s="4">
+        <v>1</v>
+      </c>
+      <c r="E436" s="4">
+        <v>7</v>
       </c>
     </row>
     <row r="437" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A437" s="5" t="s">
         <v>123</v>
       </c>
-      <c r="B437" s="7" t="s">
-        <v>13</v>
+      <c r="B437" s="9" t="s">
+        <v>19</v>
       </c>
       <c r="C437" s="1" t="s">
         <v>54</v>
       </c>
       <c r="D437" s="4">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E437" s="4">
         <v>7</v>
       </c>
     </row>
-    <row r="438" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A438" s="5" t="s">
-        <v>123</v>
-      </c>
-      <c r="B438" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="C438" s="1" t="s">
+    <row r="439" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A439" s="5" t="s">
+        <v>124</v>
+      </c>
+      <c r="B439" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="C439" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="D438" s="4">
-        <v>2</v>
-      </c>
-      <c r="E438" s="4">
-        <v>7</v>
+      <c r="D439" s="4">
+        <v>1</v>
+      </c>
+      <c r="E439" s="4">
+        <v>10</v>
       </c>
     </row>
     <row r="440" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A440" s="5" t="s">
         <v>124</v>
       </c>
-      <c r="B440" s="7" t="s">
-        <v>13</v>
+      <c r="B440" s="9" t="s">
+        <v>19</v>
       </c>
       <c r="C440" s="1" t="s">
         <v>54</v>
       </c>
       <c r="D440" s="4">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="E440" s="4">
         <v>10</v>
       </c>
     </row>
-    <row r="441" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A441" s="5" t="s">
-        <v>124</v>
-      </c>
-      <c r="B441" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="C441" s="1" t="s">
+    <row r="442" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A442" s="5" t="s">
+        <v>125</v>
+      </c>
+      <c r="B442" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="C442" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="D441" s="4">
-        <v>4</v>
-      </c>
-      <c r="E441" s="4">
+      <c r="D442" s="4">
+        <v>1</v>
+      </c>
+      <c r="E442" s="4">
         <v>10</v>
       </c>
     </row>
@@ -8686,33 +8683,33 @@
       <c r="A443" s="5" t="s">
         <v>125</v>
       </c>
-      <c r="B443" s="7" t="s">
-        <v>13</v>
+      <c r="B443" s="9" t="s">
+        <v>19</v>
       </c>
       <c r="C443" s="1" t="s">
         <v>54</v>
       </c>
       <c r="D443" s="4">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="E443" s="4">
         <v>10</v>
       </c>
     </row>
-    <row r="444" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A444" s="5" t="s">
-        <v>125</v>
-      </c>
-      <c r="B444" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="C444" s="1" t="s">
+    <row r="445" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A445" s="5" t="s">
+        <v>126</v>
+      </c>
+      <c r="B445" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="C445" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="D444" s="4">
-        <v>4</v>
-      </c>
-      <c r="E444" s="4">
+      <c r="D445" s="4">
+        <v>1</v>
+      </c>
+      <c r="E445" s="4">
         <v>10</v>
       </c>
     </row>
@@ -8720,33 +8717,33 @@
       <c r="A446" s="5" t="s">
         <v>126</v>
       </c>
-      <c r="B446" s="7" t="s">
-        <v>13</v>
+      <c r="B446" s="9" t="s">
+        <v>19</v>
       </c>
       <c r="C446" s="1" t="s">
         <v>54</v>
       </c>
       <c r="D446" s="4">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="E446" s="4">
         <v>10</v>
       </c>
     </row>
-    <row r="447" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A447" s="5" t="s">
-        <v>126</v>
-      </c>
-      <c r="B447" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="C447" s="1" t="s">
+    <row r="448" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A448" s="5" t="s">
+        <v>127</v>
+      </c>
+      <c r="B448" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="C448" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="D447" s="4">
-        <v>4</v>
-      </c>
-      <c r="E447" s="4">
+      <c r="D448" s="4">
+        <v>1</v>
+      </c>
+      <c r="E448" s="4">
         <v>10</v>
       </c>
     </row>
@@ -8754,192 +8751,193 @@
       <c r="A449" s="5" t="s">
         <v>127</v>
       </c>
-      <c r="B449" s="7" t="s">
-        <v>13</v>
+      <c r="B449" s="9" t="s">
+        <v>19</v>
       </c>
       <c r="C449" s="1" t="s">
         <v>54</v>
       </c>
       <c r="D449" s="4">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="E449" s="4">
         <v>10</v>
       </c>
     </row>
-    <row r="450" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A450" s="5" t="s">
-        <v>127</v>
-      </c>
-      <c r="B450" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="C450" s="1" t="s">
+    <row r="451" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A451" s="5" t="s">
+        <v>128</v>
+      </c>
+      <c r="B451" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="C451" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="D450" s="4">
-        <v>4</v>
-      </c>
-      <c r="E450" s="4">
-        <v>10</v>
+      <c r="D451" s="4">
+        <v>1</v>
+      </c>
+      <c r="E451" s="4">
+        <v>8</v>
       </c>
     </row>
     <row r="452" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A452" s="5" t="s">
         <v>128</v>
       </c>
-      <c r="B452" s="7" t="s">
-        <v>13</v>
+      <c r="B452" s="9" t="s">
+        <v>19</v>
       </c>
       <c r="C452" s="1" t="s">
         <v>54</v>
       </c>
       <c r="D452" s="4">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E452" s="4">
         <v>8</v>
       </c>
     </row>
-    <row r="453" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A453" s="5" t="s">
-        <v>128</v>
-      </c>
-      <c r="B453" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="C453" s="1" t="s">
+    <row r="454" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A454" s="5" t="s">
+        <v>129</v>
+      </c>
+      <c r="B454" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="C454" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="D453" s="4">
-        <v>3</v>
-      </c>
-      <c r="E453" s="4">
-        <v>8</v>
+      <c r="D454" s="4">
+        <v>1</v>
+      </c>
+      <c r="E454" s="4">
+        <v>7</v>
       </c>
     </row>
     <row r="455" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A455" s="5" t="s">
         <v>129</v>
       </c>
-      <c r="B455" s="7" t="s">
-        <v>13</v>
+      <c r="B455" s="9" t="s">
+        <v>19</v>
       </c>
       <c r="C455" s="1" t="s">
         <v>54</v>
       </c>
       <c r="D455" s="4">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="E455" s="4">
         <v>7</v>
       </c>
     </row>
-    <row r="456" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A456" s="5" t="s">
-        <v>129</v>
-      </c>
-      <c r="B456" s="9" t="s">
+    <row r="457" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A457" s="5" t="s">
+        <v>130</v>
+      </c>
+      <c r="B457" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="C456" s="1" t="s">
+      <c r="C457" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="D456" s="4">
+      <c r="D457" s="4">
+        <v>2</v>
+      </c>
+      <c r="E457" s="4">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="459" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A459" s="5" t="s">
+        <v>131</v>
+      </c>
+      <c r="B459" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="C459" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="D459" s="4">
+        <v>2</v>
+      </c>
+      <c r="E459" s="4">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="461" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A461" s="5" t="s">
+        <v>132</v>
+      </c>
+      <c r="B461" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="C461" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="D461" s="4">
+        <v>2</v>
+      </c>
+      <c r="E461" s="4">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="463" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A463" s="5" t="s">
+        <v>133</v>
+      </c>
+      <c r="B463" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="C463" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="D463" s="4">
+        <v>1</v>
+      </c>
+      <c r="E463" s="4">
         <v>6</v>
-      </c>
-      <c r="E456" s="4">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="458" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A458" s="5" t="s">
-        <v>130</v>
-      </c>
-      <c r="B458" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="C458" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="D458" s="4">
-        <v>2</v>
-      </c>
-      <c r="E458" s="4">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="460" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A460" s="5" t="s">
-        <v>131</v>
-      </c>
-      <c r="B460" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="C460" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="D460" s="4">
-        <v>2</v>
-      </c>
-      <c r="E460" s="4">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="462" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A462" s="5" t="s">
-        <v>132</v>
-      </c>
-      <c r="B462" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="C462" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="D462" s="4">
-        <v>2</v>
-      </c>
-      <c r="E462" s="4">
-        <v>7</v>
       </c>
     </row>
     <row r="464" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A464" s="5" t="s">
         <v>133</v>
       </c>
-      <c r="B464" s="7" t="s">
-        <v>13</v>
+      <c r="B464" s="9" t="s">
+        <v>19</v>
       </c>
       <c r="C464" s="1" t="s">
         <v>54</v>
       </c>
       <c r="D464" s="4">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E464" s="4">
         <v>6</v>
       </c>
     </row>
-    <row r="465" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A465" s="5" t="s">
-        <v>133</v>
-      </c>
-      <c r="B465" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="C465" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="D465" s="4">
-        <v>2</v>
-      </c>
-      <c r="E465" s="4">
-        <v>6</v>
+    <row r="466" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A466" s="5" t="s">
+        <v>167</v>
+      </c>
+      <c r="B466" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="C466" s="1" t="s">
+        <v>176</v>
+      </c>
+      <c r="D466" s="4">
+        <f>6*2.5</f>
+        <v>15</v>
+      </c>
+      <c r="E466" s="4">
+        <v>10</v>
       </c>
     </row>
     <row r="467" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A467" s="5" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="B467" s="12" t="s">
         <v>20</v>
@@ -8948,8 +8946,7 @@
         <v>176</v>
       </c>
       <c r="D467" s="4">
-        <f>6*2.5</f>
-        <v>15</v>
+        <v>40</v>
       </c>
       <c r="E467" s="4">
         <v>10</v>
@@ -8957,7 +8954,7 @@
     </row>
     <row r="468" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A468" s="5" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="B468" s="12" t="s">
         <v>20</v>
@@ -8966,7 +8963,7 @@
         <v>176</v>
       </c>
       <c r="D468" s="4">
-        <v>40</v>
+        <v>15</v>
       </c>
       <c r="E468" s="4">
         <v>10</v>
@@ -8974,7 +8971,7 @@
     </row>
     <row r="469" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A469" s="5" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="B469" s="12" t="s">
         <v>20</v>
@@ -8983,15 +8980,15 @@
         <v>176</v>
       </c>
       <c r="D469" s="4">
-        <v>15</v>
+        <v>5</v>
       </c>
       <c r="E469" s="4">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="470" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A470" s="5" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="B470" s="12" t="s">
         <v>20</v>
@@ -9008,7 +9005,7 @@
     </row>
     <row r="471" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A471" s="5" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="B471" s="12" t="s">
         <v>20</v>
@@ -9017,7 +9014,7 @@
         <v>176</v>
       </c>
       <c r="D471" s="4">
-        <v>5</v>
+        <v>25</v>
       </c>
       <c r="E471" s="4">
         <v>5</v>
@@ -9025,7 +9022,7 @@
     </row>
     <row r="472" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A472" s="5" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="B472" s="12" t="s">
         <v>20</v>
@@ -9034,15 +9031,15 @@
         <v>176</v>
       </c>
       <c r="D472" s="4">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="E472" s="4">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="473" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A473" s="5" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="B473" s="12" t="s">
         <v>20</v>
@@ -9051,7 +9048,7 @@
         <v>176</v>
       </c>
       <c r="D473" s="4">
-        <v>30</v>
+        <v>40</v>
       </c>
       <c r="E473" s="4">
         <v>7</v>
@@ -9059,7 +9056,7 @@
     </row>
     <row r="474" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A474" s="5" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="B474" s="12" t="s">
         <v>20</v>
@@ -9068,32 +9065,32 @@
         <v>176</v>
       </c>
       <c r="D474" s="4">
-        <v>40</v>
+        <v>5</v>
       </c>
       <c r="E474" s="4">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="475" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A475" s="5" t="s">
-        <v>175</v>
-      </c>
-      <c r="B475" s="12" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="476" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A476" s="5" t="s">
+        <v>177</v>
+      </c>
+      <c r="B476" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="C475" s="1" t="s">
+      <c r="C476" s="1" t="s">
         <v>176</v>
       </c>
-      <c r="D475" s="4">
-        <v>5</v>
-      </c>
-      <c r="E475" s="4">
-        <v>5</v>
+      <c r="D476" s="4">
+        <v>30</v>
+      </c>
+      <c r="E476" s="4">
+        <v>8</v>
       </c>
     </row>
     <row r="477" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A477" s="5" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="B477" s="12" t="s">
         <v>20</v>
@@ -9102,15 +9099,15 @@
         <v>176</v>
       </c>
       <c r="D477" s="4">
-        <v>30</v>
+        <v>5</v>
       </c>
       <c r="E477" s="4">
-        <v>8</v>
+        <v>1</v>
       </c>
     </row>
     <row r="478" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A478" s="5" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="B478" s="12" t="s">
         <v>20</v>
@@ -9119,15 +9116,15 @@
         <v>176</v>
       </c>
       <c r="D478" s="4">
-        <v>5</v>
+        <v>25</v>
       </c>
       <c r="E478" s="4">
-        <v>1</v>
+        <v>8</v>
       </c>
     </row>
     <row r="479" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A479" s="5" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="B479" s="12" t="s">
         <v>20</v>
@@ -9136,7 +9133,7 @@
         <v>176</v>
       </c>
       <c r="D479" s="4">
-        <v>25</v>
+        <v>35</v>
       </c>
       <c r="E479" s="4">
         <v>8</v>
@@ -9144,7 +9141,7 @@
     </row>
     <row r="480" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A480" s="5" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="B480" s="12" t="s">
         <v>20</v>
@@ -9153,15 +9150,15 @@
         <v>176</v>
       </c>
       <c r="D480" s="4">
-        <v>35</v>
+        <v>5</v>
       </c>
       <c r="E480" s="4">
-        <v>8</v>
+        <v>1</v>
       </c>
     </row>
     <row r="481" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A481" s="5" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="B481" s="12" t="s">
         <v>20</v>
@@ -9177,33 +9174,37 @@
       </c>
     </row>
     <row r="482" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A482" s="5" t="s">
-        <v>182</v>
-      </c>
-      <c r="B482" s="12" t="s">
+      <c r="A482" s="4"/>
+      <c r="B482" s="4"/>
+      <c r="C482"/>
+      <c r="D482" s="1"/>
+      <c r="E482" s="1"/>
+      <c r="F482" s="1"/>
+    </row>
+    <row r="483" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A483" s="5" t="s">
+        <v>183</v>
+      </c>
+      <c r="B483" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="C482" s="1" t="s">
+      <c r="C483" s="1" t="s">
         <v>176</v>
       </c>
-      <c r="D482" s="4">
-        <v>5</v>
-      </c>
-      <c r="E482" s="4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="483" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A483" s="4"/>
-      <c r="B483" s="4"/>
-      <c r="C483"/>
-      <c r="D483" s="1"/>
-      <c r="E483" s="1"/>
+      <c r="D483" s="4">
+        <v>15</v>
+      </c>
+      <c r="E483" s="4">
+        <v>7</v>
+      </c>
       <c r="F483" s="1"/>
+      <c r="G483" s="1"/>
+      <c r="H483" s="1"/>
+      <c r="I483" s="1"/>
     </row>
     <row r="484" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A484" s="5" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="B484" s="12" t="s">
         <v>20</v>
@@ -9224,7 +9225,7 @@
     </row>
     <row r="485" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A485" s="5" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="B485" s="12" t="s">
         <v>20</v>
@@ -9233,10 +9234,10 @@
         <v>176</v>
       </c>
       <c r="D485" s="4">
-        <v>15</v>
+        <v>25</v>
       </c>
       <c r="E485" s="4">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="F485" s="1"/>
       <c r="G485" s="1"/>
@@ -9245,7 +9246,7 @@
     </row>
     <row r="486" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A486" s="5" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="B486" s="12" t="s">
         <v>20</v>
@@ -9254,10 +9255,10 @@
         <v>176</v>
       </c>
       <c r="D486" s="4">
-        <v>25</v>
+        <v>50</v>
       </c>
       <c r="E486" s="4">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F486" s="1"/>
       <c r="G486" s="1"/>
@@ -9266,7 +9267,7 @@
     </row>
     <row r="487" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A487" s="5" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="B487" s="12" t="s">
         <v>20</v>
@@ -9275,10 +9276,10 @@
         <v>176</v>
       </c>
       <c r="D487" s="4">
-        <v>50</v>
+        <v>15</v>
       </c>
       <c r="E487" s="4">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="F487" s="1"/>
       <c r="G487" s="1"/>
@@ -9287,7 +9288,7 @@
     </row>
     <row r="488" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A488" s="5" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="B488" s="12" t="s">
         <v>20</v>
@@ -9308,7 +9309,7 @@
     </row>
     <row r="489" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A489" s="5" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="B489" s="12" t="s">
         <v>20</v>
@@ -9317,7 +9318,7 @@
         <v>176</v>
       </c>
       <c r="D489" s="4">
-        <v>15</v>
+        <v>25</v>
       </c>
       <c r="E489" s="4">
         <v>5</v>
@@ -9329,7 +9330,7 @@
     </row>
     <row r="490" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A490" s="5" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="B490" s="12" t="s">
         <v>20</v>
@@ -9338,10 +9339,10 @@
         <v>176</v>
       </c>
       <c r="D490" s="4">
-        <v>25</v>
+        <v>10</v>
       </c>
       <c r="E490" s="4">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="F490" s="1"/>
       <c r="G490" s="1"/>
@@ -9350,7 +9351,7 @@
     </row>
     <row r="491" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A491" s="5" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="B491" s="12" t="s">
         <v>20</v>
@@ -9359,42 +9360,40 @@
         <v>176</v>
       </c>
       <c r="D491" s="4">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="E491" s="4">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="F491" s="1"/>
       <c r="G491" s="1"/>
-      <c r="H491" s="1"/>
-      <c r="I491" s="1"/>
     </row>
     <row r="492" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A492" s="5" t="s">
-        <v>191</v>
-      </c>
-      <c r="B492" s="12" t="s">
-        <v>20</v>
-      </c>
-      <c r="C492" s="1" t="s">
-        <v>176</v>
-      </c>
-      <c r="D492" s="4">
-        <v>15</v>
-      </c>
-      <c r="E492" s="4">
-        <v>7</v>
-      </c>
       <c r="F492" s="1"/>
       <c r="G492" s="1"/>
     </row>
     <row r="493" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A493" s="5" t="s">
+        <v>192</v>
+      </c>
+      <c r="B493" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="C493" s="1" t="s">
+        <v>176</v>
+      </c>
+      <c r="D493" s="4">
+        <v>15</v>
+      </c>
+      <c r="E493" s="4">
+        <v>6</v>
+      </c>
       <c r="F493" s="1"/>
       <c r="G493" s="1"/>
     </row>
     <row r="494" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A494" s="5" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="B494" s="12" t="s">
         <v>20</v>
@@ -9413,7 +9412,7 @@
     </row>
     <row r="495" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A495" s="5" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="B495" s="12" t="s">
         <v>20</v>
@@ -9422,17 +9421,16 @@
         <v>176</v>
       </c>
       <c r="D495" s="4">
-        <v>15</v>
+        <v>25</v>
       </c>
       <c r="E495" s="4">
-        <v>6</v>
-      </c>
-      <c r="F495" s="1"/>
+        <v>7</v>
+      </c>
       <c r="G495" s="1"/>
     </row>
     <row r="496" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A496" s="5" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="B496" s="12" t="s">
         <v>20</v>
@@ -9441,16 +9439,15 @@
         <v>176</v>
       </c>
       <c r="D496" s="4">
-        <v>25</v>
+        <v>15</v>
       </c>
       <c r="E496" s="4">
-        <v>7</v>
-      </c>
-      <c r="G496" s="1"/>
+        <v>1</v>
+      </c>
     </row>
     <row r="497" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A497" s="5" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="B497" s="12" t="s">
         <v>20</v>
@@ -9464,10 +9461,11 @@
       <c r="E497" s="4">
         <v>1</v>
       </c>
+      <c r="F497" s="1"/>
     </row>
     <row r="498" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A498" s="5" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="B498" s="12" t="s">
         <v>20</v>
@@ -9476,16 +9474,16 @@
         <v>176</v>
       </c>
       <c r="D498" s="4">
-        <v>15</v>
+        <v>25</v>
       </c>
       <c r="E498" s="4">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="F498" s="1"/>
     </row>
     <row r="499" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A499" s="5" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="B499" s="12" t="s">
         <v>20</v>
@@ -9494,7 +9492,7 @@
         <v>176</v>
       </c>
       <c r="D499" s="4">
-        <v>25</v>
+        <v>10</v>
       </c>
       <c r="E499" s="4">
         <v>5</v>
@@ -9503,7 +9501,7 @@
     </row>
     <row r="500" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A500" s="5" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="B500" s="12" t="s">
         <v>20</v>
@@ -9512,16 +9510,15 @@
         <v>176</v>
       </c>
       <c r="D500" s="4">
-        <v>10</v>
+        <v>50</v>
       </c>
       <c r="E500" s="4">
-        <v>5</v>
-      </c>
-      <c r="F500" s="1"/>
+        <v>7</v>
+      </c>
     </row>
     <row r="501" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A501" s="5" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="B501" s="12" t="s">
         <v>20</v>
@@ -9530,32 +9527,32 @@
         <v>176</v>
       </c>
       <c r="D501" s="4">
-        <v>50</v>
+        <v>30</v>
       </c>
       <c r="E501" s="4">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="502" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A502" s="5" t="s">
-        <v>200</v>
-      </c>
-      <c r="B502" s="12" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="503" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A503" s="5" t="s">
+        <v>201</v>
+      </c>
+      <c r="B503" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="C502" s="1" t="s">
+      <c r="C503" s="1" t="s">
         <v>176</v>
       </c>
-      <c r="D502" s="4">
-        <v>30</v>
-      </c>
-      <c r="E502" s="4">
-        <v>2</v>
+      <c r="D503" s="4">
+        <v>10</v>
+      </c>
+      <c r="E503" s="4">
+        <v>6</v>
       </c>
     </row>
     <row r="504" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A504" s="5" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="B504" s="12" t="s">
         <v>20</v>
@@ -9564,15 +9561,15 @@
         <v>176</v>
       </c>
       <c r="D504" s="4">
-        <v>10</v>
+        <v>50</v>
       </c>
       <c r="E504" s="4">
-        <v>6</v>
+        <v>8</v>
       </c>
     </row>
     <row r="505" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A505" s="5" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="B505" s="12" t="s">
         <v>20</v>
@@ -9581,15 +9578,15 @@
         <v>176</v>
       </c>
       <c r="D505" s="4">
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="E505" s="4">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="506" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A506" s="5" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="B506" s="12" t="s">
         <v>20</v>
@@ -9598,15 +9595,15 @@
         <v>176</v>
       </c>
       <c r="D506" s="4">
-        <v>40</v>
+        <v>15</v>
       </c>
       <c r="E506" s="4">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="507" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A507" s="5" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="B507" s="12" t="s">
         <v>20</v>
@@ -9615,15 +9612,15 @@
         <v>176</v>
       </c>
       <c r="D507" s="4">
-        <v>15</v>
+        <v>40</v>
       </c>
       <c r="E507" s="4">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="508" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A508" s="5" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="B508" s="12" t="s">
         <v>20</v>
@@ -9632,15 +9629,15 @@
         <v>176</v>
       </c>
       <c r="D508" s="4">
-        <v>40</v>
+        <v>5</v>
       </c>
       <c r="E508" s="4">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="509" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A509" s="5" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="B509" s="12" t="s">
         <v>20</v>
@@ -9657,7 +9654,7 @@
     </row>
     <row r="510" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A510" s="5" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="B510" s="12" t="s">
         <v>20</v>
@@ -9666,15 +9663,15 @@
         <v>176</v>
       </c>
       <c r="D510" s="4">
-        <v>5</v>
+        <v>50</v>
       </c>
       <c r="E510" s="4">
-        <v>1</v>
+        <v>8</v>
       </c>
     </row>
     <row r="511" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A511" s="5" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="B511" s="12" t="s">
         <v>20</v>
@@ -9683,15 +9680,15 @@
         <v>176</v>
       </c>
       <c r="D511" s="4">
-        <v>50</v>
+        <v>15</v>
       </c>
       <c r="E511" s="4">
-        <v>8</v>
+        <v>4</v>
       </c>
     </row>
     <row r="512" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A512" s="5" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="B512" s="12" t="s">
         <v>20</v>
@@ -9700,15 +9697,15 @@
         <v>176</v>
       </c>
       <c r="D512" s="4">
-        <v>15</v>
+        <v>5</v>
       </c>
       <c r="E512" s="4">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="513" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A513" s="5" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="B513" s="12" t="s">
         <v>20</v>
@@ -9717,15 +9714,15 @@
         <v>176</v>
       </c>
       <c r="D513" s="4">
-        <v>5</v>
+        <v>25</v>
       </c>
       <c r="E513" s="4">
-        <v>1</v>
+        <v>6</v>
       </c>
     </row>
     <row r="514" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A514" s="5" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="B514" s="12" t="s">
         <v>20</v>
@@ -9734,15 +9731,15 @@
         <v>176</v>
       </c>
       <c r="D514" s="4">
-        <v>25</v>
+        <v>5</v>
       </c>
       <c r="E514" s="4">
-        <v>6</v>
+        <v>1</v>
       </c>
     </row>
     <row r="515" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A515" s="5" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="B515" s="12" t="s">
         <v>20</v>
@@ -9751,15 +9748,15 @@
         <v>176</v>
       </c>
       <c r="D515" s="4">
+        <v>40</v>
+      </c>
+      <c r="E515" s="4">
         <v>5</v>
-      </c>
-      <c r="E515" s="4">
-        <v>1</v>
       </c>
     </row>
     <row r="516" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A516" s="5" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="B516" s="12" t="s">
         <v>20</v>
@@ -9768,32 +9765,32 @@
         <v>176</v>
       </c>
       <c r="D516" s="4">
-        <v>40</v>
+        <v>25</v>
       </c>
       <c r="E516" s="4">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="517" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A517" s="5" t="s">
-        <v>214</v>
-      </c>
-      <c r="B517" s="12" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="518" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A518" s="5" t="s">
+        <v>215</v>
+      </c>
+      <c r="B518" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="C517" s="1" t="s">
+      <c r="C518" s="1" t="s">
         <v>176</v>
       </c>
-      <c r="D517" s="4">
-        <v>25</v>
-      </c>
-      <c r="E517" s="4">
-        <v>3</v>
+      <c r="D518" s="4">
+        <v>10</v>
+      </c>
+      <c r="E518" s="4">
+        <v>8</v>
       </c>
     </row>
     <row r="519" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A519" s="5" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="B519" s="12" t="s">
         <v>20</v>
@@ -9810,7 +9807,7 @@
     </row>
     <row r="520" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A520" s="5" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="B520" s="12" t="s">
         <v>20</v>
@@ -9827,7 +9824,7 @@
     </row>
     <row r="521" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A521" s="5" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="B521" s="12" t="s">
         <v>20</v>
@@ -9836,15 +9833,15 @@
         <v>176</v>
       </c>
       <c r="D521" s="4">
-        <v>10</v>
+        <v>50</v>
       </c>
       <c r="E521" s="4">
-        <v>8</v>
+        <v>1</v>
       </c>
     </row>
     <row r="522" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A522" s="5" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="B522" s="12" t="s">
         <v>20</v>
@@ -9853,15 +9850,15 @@
         <v>176</v>
       </c>
       <c r="D522" s="4">
-        <v>50</v>
+        <v>10</v>
       </c>
       <c r="E522" s="4">
-        <v>1</v>
+        <v>8</v>
       </c>
     </row>
     <row r="523" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A523" s="5" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
       <c r="B523" s="12" t="s">
         <v>20</v>
@@ -9870,82 +9867,65 @@
         <v>176</v>
       </c>
       <c r="D523" s="4">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="E523" s="4">
-        <v>8</v>
+        <v>1</v>
       </c>
     </row>
     <row r="524" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A524" s="5" t="s">
-        <v>220</v>
-      </c>
-      <c r="B524" s="12" t="s">
-        <v>20</v>
-      </c>
-      <c r="C524" s="1" t="s">
-        <v>176</v>
-      </c>
       <c r="D524" s="4">
-        <v>5</v>
-      </c>
-      <c r="E524" s="4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="525" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="D525" s="4">
-        <f>SUM(D2:D524)</f>
-        <v>2305</v>
-      </c>
-    </row>
-    <row r="577" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A577" s="19"/>
-    </row>
-    <row r="581" spans="1:6" x14ac:dyDescent="0.25">
+        <f>SUM(D2:D523)</f>
+        <v>2304</v>
+      </c>
+    </row>
+    <row r="576" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A576" s="19"/>
+    </row>
+    <row r="580" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F580"/>
+    </row>
+    <row r="581" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F581"/>
     </row>
-    <row r="582" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="582" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F582"/>
     </row>
-    <row r="583" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="583" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F583"/>
     </row>
-    <row r="584" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="584" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F584"/>
     </row>
-    <row r="585" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="585" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F585"/>
     </row>
-    <row r="586" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="586" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F586"/>
     </row>
-    <row r="587" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="587" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F587"/>
     </row>
-    <row r="588" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="588" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F588"/>
     </row>
-    <row r="589" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="589" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F589"/>
     </row>
-    <row r="590" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="590" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F590"/>
     </row>
-    <row r="591" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="591" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F591"/>
     </row>
-    <row r="592" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="592" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F592"/>
     </row>
     <row r="593" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F593"/>
     </row>
-    <row r="594" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F594"/>
-    </row>
   </sheetData>
-  <autoFilter ref="A1:F605"/>
+  <autoFilter ref="A1:F604"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
Throw af en asset list geupdate
</commit_message>
<xml_diff>
--- a/Algemeen/Asset List Game-Lab 1.xlsx
+++ b/Algemeen/Asset List Game-Lab 1.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12585"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12588"/>
   </bookViews>
   <sheets>
     <sheet name="Blad1" sheetId="1" r:id="rId1"/>
@@ -1144,10 +1144,10 @@
     <t>Artist Points Behaald: 352 / 625</t>
   </si>
   <si>
-    <t>Development Points: 590 / 625</t>
-  </si>
-  <si>
-    <t>320 Fahrettin | 145 Sven | 125 Rief</t>
+    <t>320 Fahrettin | 145 Sven | 150 Rief</t>
+  </si>
+  <si>
+    <t>Development Points: 590 / 650</t>
   </si>
 </sst>
 </file>
@@ -1685,32 +1685,32 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R593"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="J1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="P18" sqref="P18"/>
+    <sheetView tabSelected="1" topLeftCell="J13" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="J35" sqref="J35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="26.42578125" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.42578125" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.85546875" style="4" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.85546875" style="4" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.140625" style="4" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.7109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="18.7109375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="123.28515625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="32.140625" style="1" customWidth="1"/>
-    <col min="11" max="11" width="27.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="27.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="30.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="28.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="30.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="28.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="17" max="18" width="30.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="26.44140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.44140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.88671875" style="4" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.88671875" style="4" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.109375" style="4" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.6640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="18.6640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="123.33203125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="32.109375" style="1" customWidth="1"/>
+    <col min="11" max="11" width="27.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="27.109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="30.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="28.5546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="30.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="28.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="17" max="18" width="30.44140625" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1766,7 +1766,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A2" s="5" t="s">
         <v>55</v>
       </c>
@@ -1820,7 +1820,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A3" s="5" t="s">
         <v>55</v>
       </c>
@@ -1873,7 +1873,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A4" s="5" t="s">
         <v>55</v>
       </c>
@@ -1926,7 +1926,7 @@
         <v>340</v>
       </c>
     </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A5" s="5" t="s">
         <v>55</v>
       </c>
@@ -1979,7 +1979,7 @@
         <v>341</v>
       </c>
     </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:18" x14ac:dyDescent="0.3">
       <c r="G6" s="10" t="s">
         <v>16</v>
       </c>
@@ -2014,7 +2014,7 @@
         <v>342</v>
       </c>
     </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A7" s="5" t="s">
         <v>56</v>
       </c>
@@ -2064,7 +2064,7 @@
         <v>344</v>
       </c>
     </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A8" s="5" t="s">
         <v>56</v>
       </c>
@@ -2111,7 +2111,7 @@
         <v>345</v>
       </c>
     </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A9" s="5" t="s">
         <v>56</v>
       </c>
@@ -2158,7 +2158,7 @@
         <v>348</v>
       </c>
     </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A10" s="5" t="s">
         <v>56</v>
       </c>
@@ -2205,7 +2205,7 @@
         <v>351</v>
       </c>
     </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:18" x14ac:dyDescent="0.3">
       <c r="H11" s="3" t="s">
         <v>27</v>
       </c>
@@ -2234,7 +2234,7 @@
         <v>362</v>
       </c>
     </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A12" s="5" t="s">
         <v>57</v>
       </c>
@@ -2275,7 +2275,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A13" s="5" t="s">
         <v>57</v>
       </c>
@@ -2316,7 +2316,7 @@
         <v>350</v>
       </c>
     </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A14" s="5" t="s">
         <v>57</v>
       </c>
@@ -2348,7 +2348,7 @@
         <v>320</v>
       </c>
     </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A15" s="5" t="s">
         <v>57</v>
       </c>
@@ -2377,7 +2377,7 @@
         <v>321</v>
       </c>
     </row>
-    <row r="16" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:18" x14ac:dyDescent="0.3">
       <c r="H16" s="3" t="s">
         <v>61</v>
       </c>
@@ -2391,7 +2391,7 @@
         <v>322</v>
       </c>
     </row>
-    <row r="17" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A17" s="5" t="s">
         <v>58</v>
       </c>
@@ -2420,7 +2420,7 @@
         <v>323</v>
       </c>
     </row>
-    <row r="18" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A18" s="5" t="s">
         <v>58</v>
       </c>
@@ -2449,7 +2449,7 @@
         <v>324</v>
       </c>
     </row>
-    <row r="19" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A19" s="5" t="s">
         <v>58</v>
       </c>
@@ -2478,7 +2478,7 @@
         <v>355</v>
       </c>
     </row>
-    <row r="20" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A20" s="5" t="s">
         <v>58</v>
       </c>
@@ -2504,7 +2504,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="21" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:18" x14ac:dyDescent="0.3">
       <c r="H21" s="3" t="s">
         <v>166</v>
       </c>
@@ -2515,7 +2515,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="22" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A22" s="5" t="s">
         <v>65</v>
       </c>
@@ -2538,7 +2538,7 @@
         <v>370</v>
       </c>
     </row>
-    <row r="23" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A23" s="5" t="s">
         <v>65</v>
       </c>
@@ -2561,7 +2561,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="24" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A24" s="5" t="s">
         <v>65</v>
       </c>
@@ -2584,7 +2584,7 @@
         <v>366</v>
       </c>
     </row>
-    <row r="25" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A25" s="5" t="s">
         <v>65</v>
       </c>
@@ -2607,7 +2607,7 @@
         <v>367</v>
       </c>
     </row>
-    <row r="26" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:18" x14ac:dyDescent="0.3">
       <c r="B26" s="16"/>
       <c r="H26" s="3" t="s">
         <v>166</v>
@@ -2643,7 +2643,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="27" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A27" s="5" t="s">
         <v>71</v>
       </c>
@@ -2688,7 +2688,7 @@
         <v>332</v>
       </c>
     </row>
-    <row r="28" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A28" s="5" t="s">
         <v>71</v>
       </c>
@@ -2733,7 +2733,7 @@
         <v>333</v>
       </c>
     </row>
-    <row r="29" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A29" s="5" t="s">
         <v>71</v>
       </c>
@@ -2762,7 +2762,7 @@
       <c r="M29" s="22" t="s">
         <v>266</v>
       </c>
-      <c r="N29" s="1" t="s">
+      <c r="N29" s="22" t="s">
         <v>279</v>
       </c>
       <c r="O29" s="1" t="s">
@@ -2778,7 +2778,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="30" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A30" s="5" t="s">
         <v>71</v>
       </c>
@@ -2823,7 +2823,7 @@
         <v>335</v>
       </c>
     </row>
-    <row r="31" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:18" x14ac:dyDescent="0.3">
       <c r="B31" s="16"/>
       <c r="I31" s="19"/>
       <c r="J31" s="22" t="s">
@@ -2848,7 +2848,7 @@
         <v>336</v>
       </c>
     </row>
-    <row r="32" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A32" s="5" t="s">
         <v>59</v>
       </c>
@@ -2879,7 +2879,7 @@
         <v>337</v>
       </c>
     </row>
-    <row r="33" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A33" s="5" t="s">
         <v>59</v>
       </c>
@@ -2904,7 +2904,7 @@
         <v>338</v>
       </c>
     </row>
-    <row r="34" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A34" s="5" t="s">
         <v>59</v>
       </c>
@@ -2923,7 +2923,7 @@
       <c r="H34" s="19"/>
       <c r="I34" s="19"/>
       <c r="J34" s="23" t="s">
-        <v>375</v>
+        <v>376</v>
       </c>
       <c r="N34" s="22" t="s">
         <v>276</v>
@@ -2932,7 +2932,7 @@
         <v>339</v>
       </c>
     </row>
-    <row r="35" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A35" s="5" t="s">
         <v>59</v>
       </c>
@@ -2951,17 +2951,17 @@
       <c r="H35" s="19"/>
       <c r="I35" s="19"/>
       <c r="J35" s="1" t="s">
-        <v>376</v>
-      </c>
-    </row>
-    <row r="36" spans="1:18" x14ac:dyDescent="0.25">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="36" spans="1:18" x14ac:dyDescent="0.3">
       <c r="H36" s="19"/>
       <c r="I36" s="19"/>
       <c r="J36" s="23" t="s">
         <v>374</v>
       </c>
     </row>
-    <row r="37" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A37" s="5" t="s">
         <v>41</v>
       </c>
@@ -2983,7 +2983,7 @@
         <v>372</v>
       </c>
     </row>
-    <row r="38" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A38" s="5" t="s">
         <v>41</v>
       </c>
@@ -3004,7 +3004,7 @@
         <v>373</v>
       </c>
     </row>
-    <row r="39" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A39" s="5" t="s">
         <v>41</v>
       </c>
@@ -3022,7 +3022,7 @@
       </c>
       <c r="I39" s="19"/>
     </row>
-    <row r="40" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A40" s="5" t="s">
         <v>41</v>
       </c>
@@ -3040,7 +3040,7 @@
       </c>
       <c r="I40" s="2"/>
     </row>
-    <row r="42" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A42" s="5" t="s">
         <v>68</v>
       </c>
@@ -3057,7 +3057,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="43" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A43" s="5" t="s">
         <v>68</v>
       </c>
@@ -3074,7 +3074,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="44" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A44" s="5" t="s">
         <v>68</v>
       </c>
@@ -3091,7 +3091,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="45" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A45" s="5" t="s">
         <v>68</v>
       </c>
@@ -3108,7 +3108,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="47" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A47" s="5" t="s">
         <v>72</v>
       </c>
@@ -3125,7 +3125,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="48" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A48" s="5" t="s">
         <v>72</v>
       </c>
@@ -3142,7 +3142,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A49" s="5" t="s">
         <v>72</v>
       </c>
@@ -3159,7 +3159,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A50" s="5" t="s">
         <v>72</v>
       </c>
@@ -3176,7 +3176,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A52" s="5" t="s">
         <v>69</v>
       </c>
@@ -3193,7 +3193,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A53" s="5" t="s">
         <v>69</v>
       </c>
@@ -3210,7 +3210,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A54" s="5" t="s">
         <v>69</v>
       </c>
@@ -3227,7 +3227,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A55" s="5" t="s">
         <v>69</v>
       </c>
@@ -3244,10 +3244,10 @@
         <v>3</v>
       </c>
     </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B56" s="16"/>
     </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A57" s="5" t="s">
         <v>70</v>
       </c>
@@ -3264,7 +3264,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A58" s="5" t="s">
         <v>70</v>
       </c>
@@ -3281,7 +3281,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A59" s="5" t="s">
         <v>70</v>
       </c>
@@ -3298,7 +3298,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A60" s="5" t="s">
         <v>70</v>
       </c>
@@ -3315,7 +3315,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A62" s="5" t="s">
         <v>154</v>
       </c>
@@ -3332,7 +3332,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A63" s="5" t="s">
         <v>154</v>
       </c>
@@ -3349,7 +3349,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A64" s="5" t="s">
         <v>154</v>
       </c>
@@ -3366,7 +3366,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A65" s="5" t="s">
         <v>154</v>
       </c>
@@ -3383,7 +3383,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A67" s="5" t="s">
         <v>155</v>
       </c>
@@ -3400,7 +3400,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A68" s="5" t="s">
         <v>155</v>
       </c>
@@ -3417,7 +3417,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A69" s="5" t="s">
         <v>155</v>
       </c>
@@ -3434,7 +3434,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A70" s="5" t="s">
         <v>155</v>
       </c>
@@ -3451,7 +3451,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A71" s="5" t="s">
         <v>155</v>
       </c>
@@ -3468,7 +3468,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A72" s="5" t="s">
         <v>155</v>
       </c>
@@ -3485,10 +3485,10 @@
         <v>5</v>
       </c>
     </row>
-    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B73" s="16"/>
     </row>
-    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A74" s="5" t="s">
         <v>156</v>
       </c>
@@ -3505,7 +3505,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="75" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A75" s="5" t="s">
         <v>156</v>
       </c>
@@ -3522,7 +3522,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="76" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A76" s="5" t="s">
         <v>156</v>
       </c>
@@ -3539,7 +3539,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="77" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A77" s="5" t="s">
         <v>156</v>
       </c>
@@ -3556,7 +3556,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="79" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A79" s="5" t="s">
         <v>157</v>
       </c>
@@ -3573,7 +3573,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="80" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A80" s="5" t="s">
         <v>157</v>
       </c>
@@ -3590,7 +3590,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="81" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A81" s="5" t="s">
         <v>157</v>
       </c>
@@ -3607,7 +3607,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="82" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A82" s="5" t="s">
         <v>157</v>
       </c>
@@ -3624,7 +3624,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="84" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A84" s="5" t="s">
         <v>158</v>
       </c>
@@ -3641,7 +3641,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="85" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A85" s="5" t="s">
         <v>158</v>
       </c>
@@ -3658,7 +3658,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="86" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A86" s="5" t="s">
         <v>158</v>
       </c>
@@ -3675,7 +3675,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="87" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A87" s="5" t="s">
         <v>158</v>
       </c>
@@ -3692,7 +3692,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="89" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A89" s="5" t="s">
         <v>159</v>
       </c>
@@ -3709,7 +3709,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="90" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A90" s="5" t="s">
         <v>159</v>
       </c>
@@ -3726,7 +3726,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="91" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A91" s="5" t="s">
         <v>159</v>
       </c>
@@ -3743,7 +3743,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="92" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A92" s="5" t="s">
         <v>159</v>
       </c>
@@ -3760,7 +3760,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="94" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A94" s="5" t="s">
         <v>160</v>
       </c>
@@ -3777,7 +3777,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="95" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A95" s="5" t="s">
         <v>160</v>
       </c>
@@ -3794,7 +3794,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="96" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A96" s="5" t="s">
         <v>160</v>
       </c>
@@ -3811,7 +3811,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="97" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A97" s="5" t="s">
         <v>160</v>
       </c>
@@ -3828,7 +3828,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="99" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A99" s="5" t="s">
         <v>161</v>
       </c>
@@ -3845,7 +3845,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="100" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A100" s="5" t="s">
         <v>161</v>
       </c>
@@ -3862,7 +3862,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="101" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A101" s="5" t="s">
         <v>161</v>
       </c>
@@ -3879,7 +3879,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="102" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A102" s="5" t="s">
         <v>161</v>
       </c>
@@ -3896,7 +3896,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="104" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A104" s="5" t="s">
         <v>162</v>
       </c>
@@ -3913,7 +3913,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="105" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A105" s="5" t="s">
         <v>162</v>
       </c>
@@ -3930,7 +3930,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="106" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A106" s="5" t="s">
         <v>162</v>
       </c>
@@ -3947,7 +3947,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="107" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A107" s="5" t="s">
         <v>162</v>
       </c>
@@ -3964,10 +3964,10 @@
         <v>4</v>
       </c>
     </row>
-    <row r="108" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B108" s="16"/>
     </row>
-    <row r="109" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A109" s="5" t="s">
         <v>163</v>
       </c>
@@ -3984,7 +3984,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="110" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A110" s="5" t="s">
         <v>163</v>
       </c>
@@ -4001,7 +4001,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="111" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A111" s="5" t="s">
         <v>163</v>
       </c>
@@ -4018,7 +4018,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="112" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A112" s="5" t="s">
         <v>163</v>
       </c>
@@ -4035,10 +4035,10 @@
         <v>7</v>
       </c>
     </row>
-    <row r="113" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B113" s="16"/>
     </row>
-    <row r="114" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A114" s="5" t="s">
         <v>74</v>
       </c>
@@ -4055,7 +4055,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="115" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A115" s="5" t="s">
         <v>74</v>
       </c>
@@ -4072,7 +4072,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="116" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A116" s="5" t="s">
         <v>74</v>
       </c>
@@ -4089,7 +4089,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="117" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A117" s="5" t="s">
         <v>74</v>
       </c>
@@ -4106,10 +4106,10 @@
         <v>3</v>
       </c>
     </row>
-    <row r="118" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B118" s="16"/>
     </row>
-    <row r="119" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A119" s="5" t="s">
         <v>36</v>
       </c>
@@ -4126,7 +4126,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="120" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A120" s="5" t="s">
         <v>36</v>
       </c>
@@ -4143,7 +4143,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="121" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A121" s="5" t="s">
         <v>36</v>
       </c>
@@ -4160,7 +4160,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="122" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A122" s="5" t="s">
         <v>36</v>
       </c>
@@ -4177,12 +4177,12 @@
         <v>8</v>
       </c>
     </row>
-    <row r="123" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A123" s="4"/>
       <c r="B123" s="4"/>
       <c r="C123"/>
     </row>
-    <row r="124" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A124" s="5" t="s">
         <v>165</v>
       </c>
@@ -4199,7 +4199,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="125" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A125" s="5" t="s">
         <v>165</v>
       </c>
@@ -4216,7 +4216,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="126" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A126" s="5" t="s">
         <v>165</v>
       </c>
@@ -4233,7 +4233,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="127" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A127" s="5" t="s">
         <v>165</v>
       </c>
@@ -4250,7 +4250,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="129" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A129" s="5" t="s">
         <v>76</v>
       </c>
@@ -4267,7 +4267,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="130" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A130" s="5" t="s">
         <v>76</v>
       </c>
@@ -4284,7 +4284,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="131" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A131" s="5" t="s">
         <v>76</v>
       </c>
@@ -4301,7 +4301,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="132" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A132" s="5" t="s">
         <v>76</v>
       </c>
@@ -4318,11 +4318,11 @@
         <v>5</v>
       </c>
     </row>
-    <row r="133" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B133" s="16"/>
       <c r="G133" s="15"/>
     </row>
-    <row r="134" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A134" s="5" t="s">
         <v>48</v>
       </c>
@@ -4340,7 +4340,7 @@
       </c>
       <c r="G134" s="15"/>
     </row>
-    <row r="135" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A135" s="5" t="s">
         <v>48</v>
       </c>
@@ -4358,7 +4358,7 @@
       </c>
       <c r="G135" s="15"/>
     </row>
-    <row r="136" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A136" s="5" t="s">
         <v>48</v>
       </c>
@@ -4376,7 +4376,7 @@
       </c>
       <c r="G136" s="15"/>
     </row>
-    <row r="137" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A137" s="5" t="s">
         <v>48</v>
       </c>
@@ -4394,10 +4394,10 @@
       </c>
       <c r="G137" s="15"/>
     </row>
-    <row r="138" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:7" x14ac:dyDescent="0.3">
       <c r="G138" s="15"/>
     </row>
-    <row r="139" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A139" s="5" t="s">
         <v>153</v>
       </c>
@@ -4415,7 +4415,7 @@
       </c>
       <c r="G139" s="15"/>
     </row>
-    <row r="140" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A140" s="5" t="s">
         <v>153</v>
       </c>
@@ -4433,7 +4433,7 @@
       </c>
       <c r="G140" s="15"/>
     </row>
-    <row r="141" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A141" s="5" t="s">
         <v>153</v>
       </c>
@@ -4451,7 +4451,7 @@
       </c>
       <c r="G141" s="15"/>
     </row>
-    <row r="142" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A142" s="5" t="s">
         <v>153</v>
       </c>
@@ -4469,7 +4469,7 @@
       </c>
       <c r="G142" s="15"/>
     </row>
-    <row r="143" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A143" s="5" t="s">
         <v>153</v>
       </c>
@@ -4487,7 +4487,7 @@
       </c>
       <c r="G143" s="15"/>
     </row>
-    <row r="144" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A144" s="5" t="s">
         <v>153</v>
       </c>
@@ -4505,7 +4505,7 @@
       </c>
       <c r="G144" s="15"/>
     </row>
-    <row r="145" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A145" s="5" t="s">
         <v>153</v>
       </c>
@@ -4523,10 +4523,10 @@
       </c>
       <c r="G145" s="15"/>
     </row>
-    <row r="146" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:7" x14ac:dyDescent="0.3">
       <c r="G146" s="15"/>
     </row>
-    <row r="147" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A147" s="5" t="s">
         <v>77</v>
       </c>
@@ -4544,7 +4544,7 @@
       </c>
       <c r="G147" s="15"/>
     </row>
-    <row r="148" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A148" s="5" t="s">
         <v>77</v>
       </c>
@@ -4562,7 +4562,7 @@
       </c>
       <c r="G148" s="15"/>
     </row>
-    <row r="149" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A149" s="5" t="s">
         <v>77</v>
       </c>
@@ -4580,7 +4580,7 @@
       </c>
       <c r="G149" s="15"/>
     </row>
-    <row r="150" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A150" s="5" t="s">
         <v>77</v>
       </c>
@@ -4598,7 +4598,7 @@
       </c>
       <c r="G150" s="15"/>
     </row>
-    <row r="151" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A151" s="5" t="s">
         <v>77</v>
       </c>
@@ -4616,7 +4616,7 @@
       </c>
       <c r="G151" s="15"/>
     </row>
-    <row r="152" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A152" s="5" t="s">
         <v>77</v>
       </c>
@@ -4634,7 +4634,7 @@
       </c>
       <c r="G152" s="15"/>
     </row>
-    <row r="153" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A153" s="5" t="s">
         <v>77</v>
       </c>
@@ -4652,7 +4652,7 @@
       </c>
       <c r="G153" s="15"/>
     </row>
-    <row r="154" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A154" s="5" t="s">
         <v>77</v>
       </c>
@@ -4670,10 +4670,10 @@
       </c>
       <c r="G154" s="15"/>
     </row>
-    <row r="155" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:7" x14ac:dyDescent="0.3">
       <c r="G155" s="15"/>
     </row>
-    <row r="156" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A156" s="5" t="s">
         <v>78</v>
       </c>
@@ -4690,7 +4690,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="157" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A157" s="5" t="s">
         <v>78</v>
       </c>
@@ -4707,7 +4707,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="158" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A158" s="5" t="s">
         <v>78</v>
       </c>
@@ -4724,7 +4724,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="159" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A159" s="5" t="s">
         <v>78</v>
       </c>
@@ -4741,7 +4741,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="160" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A160" s="5" t="s">
         <v>78</v>
       </c>
@@ -4758,7 +4758,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="161" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A161" s="5" t="s">
         <v>78</v>
       </c>
@@ -4775,7 +4775,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="162" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A162" s="5" t="s">
         <v>78</v>
       </c>
@@ -4792,7 +4792,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="163" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A163" s="5" t="s">
         <v>78</v>
       </c>
@@ -4809,7 +4809,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="165" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A165" s="5" t="s">
         <v>79</v>
       </c>
@@ -4826,7 +4826,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="166" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A166" s="5" t="s">
         <v>79</v>
       </c>
@@ -4843,7 +4843,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="167" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A167" s="5" t="s">
         <v>79</v>
       </c>
@@ -4860,7 +4860,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="168" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A168" s="5" t="s">
         <v>79</v>
       </c>
@@ -4877,7 +4877,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="169" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A169" s="5" t="s">
         <v>79</v>
       </c>
@@ -4894,7 +4894,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="170" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A170" s="5" t="s">
         <v>79</v>
       </c>
@@ -4911,7 +4911,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="171" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A171" s="5" t="s">
         <v>79</v>
       </c>
@@ -4928,7 +4928,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="172" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A172" s="5" t="s">
         <v>79</v>
       </c>
@@ -4945,7 +4945,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="174" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A174" s="5" t="s">
         <v>80</v>
       </c>
@@ -4962,7 +4962,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="175" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A175" s="5" t="s">
         <v>80</v>
       </c>
@@ -4979,7 +4979,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="176" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A176" s="5" t="s">
         <v>80</v>
       </c>
@@ -4996,7 +4996,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="177" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A177" s="5" t="s">
         <v>80</v>
       </c>
@@ -5013,7 +5013,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="178" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A178" s="5" t="s">
         <v>80</v>
       </c>
@@ -5030,7 +5030,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="179" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A179" s="5" t="s">
         <v>80</v>
       </c>
@@ -5047,7 +5047,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="180" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A180" s="5" t="s">
         <v>80</v>
       </c>
@@ -5064,7 +5064,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="181" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A181" s="5" t="s">
         <v>80</v>
       </c>
@@ -5081,7 +5081,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="183" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A183" s="5" t="s">
         <v>81</v>
       </c>
@@ -5098,7 +5098,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="184" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A184" s="5" t="s">
         <v>81</v>
       </c>
@@ -5115,7 +5115,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="185" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A185" s="5" t="s">
         <v>81</v>
       </c>
@@ -5132,7 +5132,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="186" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A186" s="5" t="s">
         <v>81</v>
       </c>
@@ -5149,7 +5149,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="187" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A187" s="5" t="s">
         <v>81</v>
       </c>
@@ -5166,7 +5166,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="188" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A188" s="5" t="s">
         <v>81</v>
       </c>
@@ -5183,7 +5183,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="189" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A189" s="5" t="s">
         <v>81</v>
       </c>
@@ -5200,7 +5200,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="190" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A190" s="5" t="s">
         <v>81</v>
       </c>
@@ -5217,7 +5217,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="192" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A192" s="5" t="s">
         <v>82</v>
       </c>
@@ -5234,7 +5234,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="193" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A193" s="5" t="s">
         <v>82</v>
       </c>
@@ -5251,7 +5251,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="194" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A194" s="5" t="s">
         <v>82</v>
       </c>
@@ -5268,7 +5268,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="195" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A195" s="5" t="s">
         <v>82</v>
       </c>
@@ -5285,7 +5285,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="196" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A196" s="5" t="s">
         <v>82</v>
       </c>
@@ -5302,7 +5302,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="197" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A197" s="5" t="s">
         <v>82</v>
       </c>
@@ -5319,7 +5319,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="198" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="198" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A198" s="5" t="s">
         <v>82</v>
       </c>
@@ -5336,7 +5336,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="199" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="199" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A199" s="5" t="s">
         <v>82</v>
       </c>
@@ -5353,7 +5353,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="201" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="201" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A201" s="5" t="s">
         <v>37</v>
       </c>
@@ -5370,7 +5370,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="202" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="202" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A202" s="5" t="s">
         <v>37</v>
       </c>
@@ -5387,7 +5387,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="203" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="203" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A203" s="5" t="s">
         <v>37</v>
       </c>
@@ -5404,7 +5404,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="204" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="204" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A204" s="5" t="s">
         <v>37</v>
       </c>
@@ -5421,7 +5421,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="206" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="206" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A206" s="5" t="s">
         <v>40</v>
       </c>
@@ -5438,7 +5438,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="207" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="207" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A207" s="5" t="s">
         <v>40</v>
       </c>
@@ -5455,7 +5455,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="208" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="208" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A208" s="5" t="s">
         <v>40</v>
       </c>
@@ -5472,7 +5472,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="209" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="209" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A209" s="5" t="s">
         <v>40</v>
       </c>
@@ -5489,7 +5489,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="211" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="211" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A211" s="5" t="s">
         <v>83</v>
       </c>
@@ -5506,7 +5506,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="212" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="212" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A212" s="5" t="s">
         <v>83</v>
       </c>
@@ -5523,7 +5523,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="213" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="213" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A213" s="5" t="s">
         <v>83</v>
       </c>
@@ -5540,7 +5540,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="214" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="214" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A214" s="5" t="s">
         <v>83</v>
       </c>
@@ -5557,7 +5557,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="216" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="216" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A216" s="5" t="s">
         <v>85</v>
       </c>
@@ -5574,7 +5574,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="217" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="217" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A217" s="5" t="s">
         <v>85</v>
       </c>
@@ -5591,7 +5591,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="218" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="218" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A218" s="5" t="s">
         <v>85</v>
       </c>
@@ -5608,7 +5608,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="219" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="219" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A219" s="5" t="s">
         <v>85</v>
       </c>
@@ -5625,7 +5625,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="221" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="221" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A221" s="5" t="s">
         <v>86</v>
       </c>
@@ -5642,7 +5642,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="222" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="222" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A222" s="5" t="s">
         <v>86</v>
       </c>
@@ -5659,7 +5659,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="223" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="223" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A223" s="5" t="s">
         <v>86</v>
       </c>
@@ -5676,7 +5676,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="224" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="224" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A224" s="5" t="s">
         <v>86</v>
       </c>
@@ -5693,7 +5693,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="226" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="226" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A226" s="5" t="s">
         <v>87</v>
       </c>
@@ -5710,7 +5710,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="227" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="227" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A227" s="5" t="s">
         <v>87</v>
       </c>
@@ -5727,7 +5727,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="228" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="228" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A228" s="5" t="s">
         <v>87</v>
       </c>
@@ -5744,7 +5744,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="229" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="229" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A229" s="5" t="s">
         <v>87</v>
       </c>
@@ -5761,7 +5761,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="231" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="231" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A231" s="5" t="s">
         <v>88</v>
       </c>
@@ -5778,7 +5778,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="232" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="232" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A232" s="5" t="s">
         <v>88</v>
       </c>
@@ -5795,7 +5795,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="233" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="233" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A233" s="5" t="s">
         <v>88</v>
       </c>
@@ -5812,7 +5812,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="234" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="234" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A234" s="5" t="s">
         <v>88</v>
       </c>
@@ -5829,7 +5829,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="236" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="236" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A236" s="5" t="s">
         <v>89</v>
       </c>
@@ -5846,7 +5846,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="237" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="237" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A237" s="5" t="s">
         <v>89</v>
       </c>
@@ -5863,7 +5863,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="238" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="238" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A238" s="5" t="s">
         <v>89</v>
       </c>
@@ -5880,7 +5880,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="239" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="239" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A239" s="5" t="s">
         <v>89</v>
       </c>
@@ -5897,7 +5897,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="241" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="241" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A241" s="5" t="s">
         <v>90</v>
       </c>
@@ -5914,7 +5914,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="242" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="242" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A242" s="5" t="s">
         <v>90</v>
       </c>
@@ -5931,7 +5931,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="243" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="243" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A243" s="5" t="s">
         <v>90</v>
       </c>
@@ -5948,7 +5948,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="244" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="244" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A244" s="5" t="s">
         <v>90</v>
       </c>
@@ -5965,7 +5965,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="245" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="245" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A245" s="5" t="s">
         <v>90</v>
       </c>
@@ -5982,7 +5982,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="247" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="247" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A247" s="5" t="s">
         <v>91</v>
       </c>
@@ -5999,7 +5999,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="248" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="248" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A248" s="5" t="s">
         <v>91</v>
       </c>
@@ -6016,7 +6016,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="249" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="249" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A249" s="5" t="s">
         <v>91</v>
       </c>
@@ -6033,7 +6033,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="250" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="250" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A250" s="5" t="s">
         <v>91</v>
       </c>
@@ -6050,7 +6050,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="252" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="252" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A252" s="5" t="s">
         <v>92</v>
       </c>
@@ -6067,7 +6067,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="253" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="253" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A253" s="5" t="s">
         <v>92</v>
       </c>
@@ -6084,7 +6084,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="254" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="254" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A254" s="5" t="s">
         <v>92</v>
       </c>
@@ -6101,7 +6101,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="255" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="255" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A255" s="5" t="s">
         <v>92</v>
       </c>
@@ -6118,7 +6118,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="257" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="257" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A257" s="5" t="s">
         <v>93</v>
       </c>
@@ -6135,7 +6135,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="258" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="258" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A258" s="5" t="s">
         <v>93</v>
       </c>
@@ -6152,7 +6152,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="259" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="259" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A259" s="5" t="s">
         <v>93</v>
       </c>
@@ -6169,7 +6169,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="260" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="260" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A260" s="5" t="s">
         <v>93</v>
       </c>
@@ -6186,7 +6186,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="262" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="262" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A262" s="5" t="s">
         <v>94</v>
       </c>
@@ -6203,7 +6203,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="263" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="263" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A263" s="5" t="s">
         <v>94</v>
       </c>
@@ -6220,7 +6220,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="264" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="264" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A264" s="5" t="s">
         <v>94</v>
       </c>
@@ -6237,7 +6237,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="265" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="265" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A265" s="5" t="s">
         <v>94</v>
       </c>
@@ -6254,7 +6254,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="267" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="267" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A267" s="5" t="s">
         <v>96</v>
       </c>
@@ -6271,7 +6271,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="268" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="268" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A268" s="5" t="s">
         <v>96</v>
       </c>
@@ -6288,7 +6288,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="269" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="269" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A269" s="5" t="s">
         <v>96</v>
       </c>
@@ -6305,7 +6305,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="270" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="270" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A270" s="5" t="s">
         <v>96</v>
       </c>
@@ -6322,7 +6322,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="272" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="272" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A272" s="5" t="s">
         <v>97</v>
       </c>
@@ -6339,7 +6339,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="273" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="273" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A273" s="5" t="s">
         <v>97</v>
       </c>
@@ -6356,7 +6356,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="274" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="274" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A274" s="5" t="s">
         <v>97</v>
       </c>
@@ -6373,7 +6373,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="275" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="275" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A275" s="5" t="s">
         <v>97</v>
       </c>
@@ -6390,12 +6390,12 @@
         <v>10</v>
       </c>
     </row>
-    <row r="276" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="276" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A276" s="4"/>
       <c r="B276" s="4"/>
       <c r="C276" s="4"/>
     </row>
-    <row r="277" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="277" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A277" s="5" t="s">
         <v>144</v>
       </c>
@@ -6412,7 +6412,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="278" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="278" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A278" s="5" t="s">
         <v>144</v>
       </c>
@@ -6429,7 +6429,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="279" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="279" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A279" s="5" t="s">
         <v>144</v>
       </c>
@@ -6446,7 +6446,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="280" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="280" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A280" s="5" t="s">
         <v>144</v>
       </c>
@@ -6463,7 +6463,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="281" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="281" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A281" s="5" t="s">
         <v>144</v>
       </c>
@@ -6480,7 +6480,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="282" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="282" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A282" s="5" t="s">
         <v>144</v>
       </c>
@@ -6497,7 +6497,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="283" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="283" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A283" s="5" t="s">
         <v>144</v>
       </c>
@@ -6514,7 +6514,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="284" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="284" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A284" s="5" t="s">
         <v>144</v>
       </c>
@@ -6531,7 +6531,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="286" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="286" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A286" s="5" t="s">
         <v>145</v>
       </c>
@@ -6548,7 +6548,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="287" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="287" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A287" s="5" t="s">
         <v>145</v>
       </c>
@@ -6566,7 +6566,7 @@
       </c>
       <c r="F287" s="2"/>
     </row>
-    <row r="288" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="288" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A288" s="5" t="s">
         <v>145</v>
       </c>
@@ -6583,7 +6583,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="289" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="289" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A289" s="5" t="s">
         <v>145</v>
       </c>
@@ -6600,7 +6600,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="290" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="290" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A290" s="5" t="s">
         <v>145</v>
       </c>
@@ -6617,7 +6617,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="291" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="291" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A291" s="5" t="s">
         <v>145</v>
       </c>
@@ -6634,7 +6634,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="292" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="292" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A292" s="5" t="s">
         <v>145</v>
       </c>
@@ -6651,7 +6651,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="293" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="293" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A293" s="5" t="s">
         <v>145</v>
       </c>
@@ -6668,7 +6668,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="295" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="295" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A295" s="5" t="s">
         <v>146</v>
       </c>
@@ -6685,7 +6685,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="296" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="296" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A296" s="5" t="s">
         <v>146</v>
       </c>
@@ -6702,7 +6702,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="297" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="297" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A297" s="5" t="s">
         <v>146</v>
       </c>
@@ -6719,7 +6719,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="298" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="298" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A298" s="5" t="s">
         <v>146</v>
       </c>
@@ -6736,7 +6736,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="299" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="299" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A299" s="5" t="s">
         <v>146</v>
       </c>
@@ -6753,7 +6753,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="300" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="300" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A300" s="5" t="s">
         <v>146</v>
       </c>
@@ -6770,7 +6770,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="301" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="301" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A301" s="5" t="s">
         <v>146</v>
       </c>
@@ -6787,7 +6787,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="302" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="302" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A302" s="5" t="s">
         <v>146</v>
       </c>
@@ -6804,7 +6804,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="304" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="304" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A304" s="5" t="s">
         <v>147</v>
       </c>
@@ -6821,7 +6821,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="305" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="305" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A305" s="5" t="s">
         <v>147</v>
       </c>
@@ -6838,7 +6838,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="306" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="306" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A306" s="5" t="s">
         <v>147</v>
       </c>
@@ -6855,7 +6855,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="307" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="307" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A307" s="5" t="s">
         <v>147</v>
       </c>
@@ -6872,7 +6872,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="308" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="308" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A308" s="5" t="s">
         <v>147</v>
       </c>
@@ -6889,7 +6889,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="309" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="309" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A309" s="5" t="s">
         <v>147</v>
       </c>
@@ -6906,7 +6906,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="310" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="310" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A310" s="5" t="s">
         <v>147</v>
       </c>
@@ -6923,7 +6923,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="311" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="311" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A311" s="5" t="s">
         <v>147</v>
       </c>
@@ -6940,7 +6940,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="313" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="313" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A313" s="5" t="s">
         <v>148</v>
       </c>
@@ -6957,7 +6957,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="314" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="314" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A314" s="5" t="s">
         <v>148</v>
       </c>
@@ -6974,7 +6974,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="315" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="315" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A315" s="5" t="s">
         <v>148</v>
       </c>
@@ -6991,7 +6991,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="316" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="316" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A316" s="5" t="s">
         <v>148</v>
       </c>
@@ -7008,7 +7008,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="317" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="317" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A317" s="5" t="s">
         <v>148</v>
       </c>
@@ -7025,7 +7025,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="318" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="318" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A318" s="5" t="s">
         <v>148</v>
       </c>
@@ -7042,7 +7042,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="319" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="319" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A319" s="5" t="s">
         <v>148</v>
       </c>
@@ -7059,7 +7059,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="320" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="320" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A320" s="5" t="s">
         <v>148</v>
       </c>
@@ -7076,7 +7076,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="322" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="322" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A322" s="5" t="s">
         <v>44</v>
       </c>
@@ -7093,7 +7093,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="323" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="323" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A323" s="5" t="s">
         <v>44</v>
       </c>
@@ -7110,7 +7110,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="324" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="324" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A324" s="5" t="s">
         <v>44</v>
       </c>
@@ -7127,7 +7127,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="325" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="325" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A325" s="5" t="s">
         <v>44</v>
       </c>
@@ -7144,7 +7144,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="327" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="327" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A327" s="5" t="s">
         <v>45</v>
       </c>
@@ -7161,7 +7161,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="328" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="328" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A328" s="5" t="s">
         <v>45</v>
       </c>
@@ -7178,7 +7178,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="329" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="329" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A329" s="5" t="s">
         <v>45</v>
       </c>
@@ -7195,7 +7195,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="330" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="330" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A330" s="5" t="s">
         <v>45</v>
       </c>
@@ -7212,7 +7212,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="332" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="332" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A332" s="5" t="s">
         <v>98</v>
       </c>
@@ -7229,7 +7229,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="333" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="333" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A333" s="5" t="s">
         <v>98</v>
       </c>
@@ -7246,7 +7246,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="334" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="334" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A334" s="5" t="s">
         <v>98</v>
       </c>
@@ -7263,7 +7263,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="335" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="335" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A335" s="5" t="s">
         <v>98</v>
       </c>
@@ -7280,7 +7280,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="337" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="337" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A337" s="5" t="s">
         <v>99</v>
       </c>
@@ -7297,7 +7297,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="338" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="338" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A338" s="5" t="s">
         <v>99</v>
       </c>
@@ -7314,7 +7314,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="339" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="339" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A339" s="5" t="s">
         <v>99</v>
       </c>
@@ -7331,7 +7331,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="340" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="340" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A340" s="5" t="s">
         <v>99</v>
       </c>
@@ -7348,7 +7348,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="342" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="342" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A342" s="5" t="s">
         <v>100</v>
       </c>
@@ -7365,7 +7365,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="343" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="343" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A343" s="5" t="s">
         <v>100</v>
       </c>
@@ -7382,7 +7382,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="344" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="344" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A344" s="5" t="s">
         <v>100</v>
       </c>
@@ -7399,7 +7399,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="345" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="345" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A345" s="5" t="s">
         <v>100</v>
       </c>
@@ -7416,7 +7416,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="347" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="347" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A347" s="5" t="s">
         <v>101</v>
       </c>
@@ -7433,7 +7433,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="348" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="348" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A348" s="5" t="s">
         <v>101</v>
       </c>
@@ -7450,7 +7450,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="349" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="349" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A349" s="5" t="s">
         <v>101</v>
       </c>
@@ -7467,7 +7467,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="350" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="350" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A350" s="5" t="s">
         <v>101</v>
       </c>
@@ -7484,7 +7484,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="352" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="352" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A352" s="5" t="s">
         <v>102</v>
       </c>
@@ -7501,7 +7501,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="353" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="353" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A353" s="5" t="s">
         <v>102</v>
       </c>
@@ -7518,7 +7518,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="354" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="354" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A354" s="5" t="s">
         <v>102</v>
       </c>
@@ -7535,7 +7535,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="355" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="355" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A355" s="5" t="s">
         <v>102</v>
       </c>
@@ -7552,7 +7552,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="357" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="357" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A357" s="5" t="s">
         <v>103</v>
       </c>
@@ -7569,7 +7569,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="358" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="358" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A358" s="5" t="s">
         <v>103</v>
       </c>
@@ -7586,7 +7586,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="359" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="359" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A359" s="5" t="s">
         <v>103</v>
       </c>
@@ -7603,7 +7603,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="360" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="360" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A360" s="5" t="s">
         <v>103</v>
       </c>
@@ -7620,7 +7620,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="362" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="362" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A362" s="5" t="s">
         <v>104</v>
       </c>
@@ -7637,7 +7637,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="363" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="363" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A363" s="5" t="s">
         <v>104</v>
       </c>
@@ -7654,7 +7654,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="364" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="364" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A364" s="5" t="s">
         <v>104</v>
       </c>
@@ -7671,7 +7671,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="365" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="365" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A365" s="5" t="s">
         <v>104</v>
       </c>
@@ -7688,7 +7688,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="367" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="367" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A367" s="5" t="s">
         <v>106</v>
       </c>
@@ -7705,7 +7705,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="368" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="368" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A368" s="5" t="s">
         <v>106</v>
       </c>
@@ -7722,7 +7722,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="369" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="369" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A369" s="5" t="s">
         <v>106</v>
       </c>
@@ -7739,7 +7739,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="370" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="370" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A370" s="5" t="s">
         <v>106</v>
       </c>
@@ -7756,7 +7756,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="371" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="371" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A371" s="5" t="s">
         <v>106</v>
       </c>
@@ -7773,7 +7773,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="373" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="373" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A373" s="5" t="s">
         <v>107</v>
       </c>
@@ -7790,7 +7790,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="374" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="374" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A374" s="5" t="s">
         <v>107</v>
       </c>
@@ -7807,7 +7807,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="375" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="375" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A375" s="5" t="s">
         <v>107</v>
       </c>
@@ -7824,7 +7824,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="376" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="376" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A376" s="5" t="s">
         <v>107</v>
       </c>
@@ -7841,7 +7841,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="378" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="378" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A378" s="5" t="s">
         <v>108</v>
       </c>
@@ -7858,7 +7858,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="379" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="379" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A379" s="5" t="s">
         <v>108</v>
       </c>
@@ -7875,7 +7875,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="380" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="380" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A380" s="5" t="s">
         <v>108</v>
       </c>
@@ -7892,7 +7892,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="381" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="381" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A381" s="5" t="s">
         <v>108</v>
       </c>
@@ -7909,7 +7909,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="382" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="382" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A382" s="5" t="s">
         <v>108</v>
       </c>
@@ -7926,7 +7926,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="384" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="384" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A384" s="5" t="s">
         <v>109</v>
       </c>
@@ -7943,7 +7943,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="385" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="385" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A385" s="5" t="s">
         <v>109</v>
       </c>
@@ -7960,7 +7960,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="386" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="386" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A386" s="5" t="s">
         <v>109</v>
       </c>
@@ -7977,7 +7977,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="387" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="387" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A387" s="5" t="s">
         <v>109</v>
       </c>
@@ -7994,7 +7994,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="388" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="388" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A388" s="5" t="s">
         <v>109</v>
       </c>
@@ -8011,12 +8011,12 @@
         <v>2</v>
       </c>
     </row>
-    <row r="389" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="389" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A389" s="4"/>
       <c r="B389" s="4"/>
       <c r="C389" s="4"/>
     </row>
-    <row r="390" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="390" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A390" s="5" t="s">
         <v>110</v>
       </c>
@@ -8033,7 +8033,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="391" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="391" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A391" s="5" t="s">
         <v>110</v>
       </c>
@@ -8050,7 +8050,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="392" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="392" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A392" s="5" t="s">
         <v>110</v>
       </c>
@@ -8067,7 +8067,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="393" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="393" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A393" s="5" t="s">
         <v>110</v>
       </c>
@@ -8084,7 +8084,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="395" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="395" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A395" s="5" t="s">
         <v>111</v>
       </c>
@@ -8101,7 +8101,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="396" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="396" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A396" s="5" t="s">
         <v>111</v>
       </c>
@@ -8118,7 +8118,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="397" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="397" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A397" s="5" t="s">
         <v>111</v>
       </c>
@@ -8135,7 +8135,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="398" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="398" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A398" s="5" t="s">
         <v>111</v>
       </c>
@@ -8152,7 +8152,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="400" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="400" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A400" s="5" t="s">
         <v>112</v>
       </c>
@@ -8169,7 +8169,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="401" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="401" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A401" s="5" t="s">
         <v>112</v>
       </c>
@@ -8186,7 +8186,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="402" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="402" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A402" s="5" t="s">
         <v>112</v>
       </c>
@@ -8203,7 +8203,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="403" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="403" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A403" s="5" t="s">
         <v>112</v>
       </c>
@@ -8220,7 +8220,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="405" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="405" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A405" s="5" t="s">
         <v>113</v>
       </c>
@@ -8237,7 +8237,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="406" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="406" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A406" s="5" t="s">
         <v>113</v>
       </c>
@@ -8254,7 +8254,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="407" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="407" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A407" s="5" t="s">
         <v>113</v>
       </c>
@@ -8271,7 +8271,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="408" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="408" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A408" s="5" t="s">
         <v>113</v>
       </c>
@@ -8288,7 +8288,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="410" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="410" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A410" s="5" t="s">
         <v>114</v>
       </c>
@@ -8305,7 +8305,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="411" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="411" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A411" s="5" t="s">
         <v>114</v>
       </c>
@@ -8322,7 +8322,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="412" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="412" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A412" s="5" t="s">
         <v>114</v>
       </c>
@@ -8339,7 +8339,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="413" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="413" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A413" s="5" t="s">
         <v>114</v>
       </c>
@@ -8356,7 +8356,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="415" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="415" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A415" s="5" t="s">
         <v>116</v>
       </c>
@@ -8373,7 +8373,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="416" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="416" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A416" s="5" t="s">
         <v>116</v>
       </c>
@@ -8390,7 +8390,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="418" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="418" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A418" s="5" t="s">
         <v>117</v>
       </c>
@@ -8407,7 +8407,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="419" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="419" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A419" s="5" t="s">
         <v>117</v>
       </c>
@@ -8424,7 +8424,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="421" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="421" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A421" s="5" t="s">
         <v>118</v>
       </c>
@@ -8441,7 +8441,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="422" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="422" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A422" s="5" t="s">
         <v>118</v>
       </c>
@@ -8458,7 +8458,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="424" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="424" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A424" s="5" t="s">
         <v>119</v>
       </c>
@@ -8475,7 +8475,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="425" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="425" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A425" s="5" t="s">
         <v>119</v>
       </c>
@@ -8492,7 +8492,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="427" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="427" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A427" s="5" t="s">
         <v>120</v>
       </c>
@@ -8509,7 +8509,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="428" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="428" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A428" s="5" t="s">
         <v>120</v>
       </c>
@@ -8526,7 +8526,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="430" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="430" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A430" s="5" t="s">
         <v>121</v>
       </c>
@@ -8543,7 +8543,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="431" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="431" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A431" s="5" t="s">
         <v>121</v>
       </c>
@@ -8560,7 +8560,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="433" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="433" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A433" s="5" t="s">
         <v>122</v>
       </c>
@@ -8577,7 +8577,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="434" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="434" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A434" s="5" t="s">
         <v>122</v>
       </c>
@@ -8594,7 +8594,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="436" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="436" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A436" s="5" t="s">
         <v>123</v>
       </c>
@@ -8611,7 +8611,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="437" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="437" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A437" s="5" t="s">
         <v>123</v>
       </c>
@@ -8628,7 +8628,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="439" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="439" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A439" s="5" t="s">
         <v>124</v>
       </c>
@@ -8645,7 +8645,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="440" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="440" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A440" s="5" t="s">
         <v>124</v>
       </c>
@@ -8662,7 +8662,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="442" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="442" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A442" s="5" t="s">
         <v>125</v>
       </c>
@@ -8679,7 +8679,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="443" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="443" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A443" s="5" t="s">
         <v>125</v>
       </c>
@@ -8696,7 +8696,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="445" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="445" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A445" s="5" t="s">
         <v>126</v>
       </c>
@@ -8713,7 +8713,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="446" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="446" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A446" s="5" t="s">
         <v>126</v>
       </c>
@@ -8730,7 +8730,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="448" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="448" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A448" s="5" t="s">
         <v>127</v>
       </c>
@@ -8747,7 +8747,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="449" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="449" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A449" s="5" t="s">
         <v>127</v>
       </c>
@@ -8764,7 +8764,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="451" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="451" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A451" s="5" t="s">
         <v>128</v>
       </c>
@@ -8781,7 +8781,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="452" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="452" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A452" s="5" t="s">
         <v>128</v>
       </c>
@@ -8798,7 +8798,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="454" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="454" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A454" s="5" t="s">
         <v>129</v>
       </c>
@@ -8815,7 +8815,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="455" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="455" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A455" s="5" t="s">
         <v>129</v>
       </c>
@@ -8832,7 +8832,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="457" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="457" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A457" s="5" t="s">
         <v>130</v>
       </c>
@@ -8849,7 +8849,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="459" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="459" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A459" s="5" t="s">
         <v>131</v>
       </c>
@@ -8866,7 +8866,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="461" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="461" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A461" s="5" t="s">
         <v>132</v>
       </c>
@@ -8883,7 +8883,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="463" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="463" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A463" s="5" t="s">
         <v>133</v>
       </c>
@@ -8900,7 +8900,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="464" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="464" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A464" s="5" t="s">
         <v>133</v>
       </c>
@@ -8917,7 +8917,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="466" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="466" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A466" s="5" t="s">
         <v>167</v>
       </c>
@@ -8935,7 +8935,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="467" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="467" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A467" s="5" t="s">
         <v>168</v>
       </c>
@@ -8952,7 +8952,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="468" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="468" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A468" s="5" t="s">
         <v>169</v>
       </c>
@@ -8969,7 +8969,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="469" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="469" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A469" s="5" t="s">
         <v>170</v>
       </c>
@@ -8986,7 +8986,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="470" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="470" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A470" s="5" t="s">
         <v>171</v>
       </c>
@@ -9003,7 +9003,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="471" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="471" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A471" s="5" t="s">
         <v>172</v>
       </c>
@@ -9020,7 +9020,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="472" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="472" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A472" s="5" t="s">
         <v>173</v>
       </c>
@@ -9037,7 +9037,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="473" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="473" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A473" s="5" t="s">
         <v>174</v>
       </c>
@@ -9054,7 +9054,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="474" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="474" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A474" s="5" t="s">
         <v>175</v>
       </c>
@@ -9071,7 +9071,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="476" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="476" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A476" s="5" t="s">
         <v>177</v>
       </c>
@@ -9088,7 +9088,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="477" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="477" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A477" s="5" t="s">
         <v>178</v>
       </c>
@@ -9105,7 +9105,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="478" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="478" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A478" s="5" t="s">
         <v>179</v>
       </c>
@@ -9122,7 +9122,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="479" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="479" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A479" s="5" t="s">
         <v>180</v>
       </c>
@@ -9139,7 +9139,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="480" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="480" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A480" s="5" t="s">
         <v>181</v>
       </c>
@@ -9156,7 +9156,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="481" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="481" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A481" s="5" t="s">
         <v>182</v>
       </c>
@@ -9173,7 +9173,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="482" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="482" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A482" s="4"/>
       <c r="B482" s="4"/>
       <c r="C482"/>
@@ -9181,7 +9181,7 @@
       <c r="E482" s="1"/>
       <c r="F482" s="1"/>
     </row>
-    <row r="483" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="483" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A483" s="5" t="s">
         <v>183</v>
       </c>
@@ -9202,7 +9202,7 @@
       <c r="H483" s="1"/>
       <c r="I483" s="1"/>
     </row>
-    <row r="484" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="484" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A484" s="5" t="s">
         <v>184</v>
       </c>
@@ -9223,7 +9223,7 @@
       <c r="H484" s="1"/>
       <c r="I484" s="1"/>
     </row>
-    <row r="485" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="485" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A485" s="5" t="s">
         <v>185</v>
       </c>
@@ -9244,7 +9244,7 @@
       <c r="H485" s="1"/>
       <c r="I485" s="1"/>
     </row>
-    <row r="486" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="486" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A486" s="5" t="s">
         <v>186</v>
       </c>
@@ -9265,7 +9265,7 @@
       <c r="H486" s="1"/>
       <c r="I486" s="1"/>
     </row>
-    <row r="487" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="487" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A487" s="5" t="s">
         <v>187</v>
       </c>
@@ -9286,7 +9286,7 @@
       <c r="H487" s="1"/>
       <c r="I487" s="1"/>
     </row>
-    <row r="488" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="488" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A488" s="5" t="s">
         <v>188</v>
       </c>
@@ -9307,7 +9307,7 @@
       <c r="H488" s="1"/>
       <c r="I488" s="1"/>
     </row>
-    <row r="489" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="489" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A489" s="5" t="s">
         <v>189</v>
       </c>
@@ -9328,7 +9328,7 @@
       <c r="H489" s="1"/>
       <c r="I489" s="1"/>
     </row>
-    <row r="490" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="490" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A490" s="5" t="s">
         <v>190</v>
       </c>
@@ -9349,7 +9349,7 @@
       <c r="H490" s="1"/>
       <c r="I490" s="1"/>
     </row>
-    <row r="491" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="491" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A491" s="5" t="s">
         <v>191</v>
       </c>
@@ -9368,11 +9368,11 @@
       <c r="F491" s="1"/>
       <c r="G491" s="1"/>
     </row>
-    <row r="492" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="492" spans="1:9" x14ac:dyDescent="0.3">
       <c r="F492" s="1"/>
       <c r="G492" s="1"/>
     </row>
-    <row r="493" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="493" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A493" s="5" t="s">
         <v>192</v>
       </c>
@@ -9391,7 +9391,7 @@
       <c r="F493" s="1"/>
       <c r="G493" s="1"/>
     </row>
-    <row r="494" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="494" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A494" s="5" t="s">
         <v>193</v>
       </c>
@@ -9410,7 +9410,7 @@
       <c r="F494" s="1"/>
       <c r="G494" s="1"/>
     </row>
-    <row r="495" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="495" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A495" s="5" t="s">
         <v>194</v>
       </c>
@@ -9428,7 +9428,7 @@
       </c>
       <c r="G495" s="1"/>
     </row>
-    <row r="496" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="496" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A496" s="5" t="s">
         <v>195</v>
       </c>
@@ -9445,7 +9445,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="497" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="497" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A497" s="5" t="s">
         <v>196</v>
       </c>
@@ -9463,7 +9463,7 @@
       </c>
       <c r="F497" s="1"/>
     </row>
-    <row r="498" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="498" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A498" s="5" t="s">
         <v>197</v>
       </c>
@@ -9481,7 +9481,7 @@
       </c>
       <c r="F498" s="1"/>
     </row>
-    <row r="499" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="499" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A499" s="5" t="s">
         <v>198</v>
       </c>
@@ -9499,7 +9499,7 @@
       </c>
       <c r="F499" s="1"/>
     </row>
-    <row r="500" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="500" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A500" s="5" t="s">
         <v>199</v>
       </c>
@@ -9516,7 +9516,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="501" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="501" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A501" s="5" t="s">
         <v>200</v>
       </c>
@@ -9533,7 +9533,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="503" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="503" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A503" s="5" t="s">
         <v>201</v>
       </c>
@@ -9550,7 +9550,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="504" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="504" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A504" s="5" t="s">
         <v>202</v>
       </c>
@@ -9567,7 +9567,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="505" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="505" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A505" s="5" t="s">
         <v>203</v>
       </c>
@@ -9584,7 +9584,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="506" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="506" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A506" s="5" t="s">
         <v>204</v>
       </c>
@@ -9601,7 +9601,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="507" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="507" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A507" s="5" t="s">
         <v>205</v>
       </c>
@@ -9618,7 +9618,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="508" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="508" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A508" s="5" t="s">
         <v>206</v>
       </c>
@@ -9635,7 +9635,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="509" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="509" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A509" s="5" t="s">
         <v>207</v>
       </c>
@@ -9652,7 +9652,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="510" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="510" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A510" s="5" t="s">
         <v>208</v>
       </c>
@@ -9669,7 +9669,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="511" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="511" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A511" s="5" t="s">
         <v>209</v>
       </c>
@@ -9686,7 +9686,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="512" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="512" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A512" s="5" t="s">
         <v>210</v>
       </c>
@@ -9703,7 +9703,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="513" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="513" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A513" s="5" t="s">
         <v>211</v>
       </c>
@@ -9720,7 +9720,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="514" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="514" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A514" s="5" t="s">
         <v>212</v>
       </c>
@@ -9737,7 +9737,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="515" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="515" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A515" s="5" t="s">
         <v>213</v>
       </c>
@@ -9754,7 +9754,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="516" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="516" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A516" s="5" t="s">
         <v>214</v>
       </c>
@@ -9771,7 +9771,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="518" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="518" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A518" s="5" t="s">
         <v>215</v>
       </c>
@@ -9788,7 +9788,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="519" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="519" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A519" s="5" t="s">
         <v>216</v>
       </c>
@@ -9805,7 +9805,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="520" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="520" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A520" s="5" t="s">
         <v>217</v>
       </c>
@@ -9822,7 +9822,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="521" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="521" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A521" s="5" t="s">
         <v>218</v>
       </c>
@@ -9839,7 +9839,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="522" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="522" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A522" s="5" t="s">
         <v>219</v>
       </c>
@@ -9856,7 +9856,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="523" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="523" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A523" s="5" t="s">
         <v>220</v>
       </c>
@@ -9873,55 +9873,55 @@
         <v>1</v>
       </c>
     </row>
-    <row r="524" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="524" spans="1:5" x14ac:dyDescent="0.3">
       <c r="D524" s="4">
         <f>SUM(D2:D523)</f>
         <v>2304</v>
       </c>
     </row>
-    <row r="576" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="576" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A576" s="19"/>
     </row>
-    <row r="580" spans="6:6" x14ac:dyDescent="0.25">
+    <row r="580" spans="6:6" x14ac:dyDescent="0.3">
       <c r="F580"/>
     </row>
-    <row r="581" spans="6:6" x14ac:dyDescent="0.25">
+    <row r="581" spans="6:6" x14ac:dyDescent="0.3">
       <c r="F581"/>
     </row>
-    <row r="582" spans="6:6" x14ac:dyDescent="0.25">
+    <row r="582" spans="6:6" x14ac:dyDescent="0.3">
       <c r="F582"/>
     </row>
-    <row r="583" spans="6:6" x14ac:dyDescent="0.25">
+    <row r="583" spans="6:6" x14ac:dyDescent="0.3">
       <c r="F583"/>
     </row>
-    <row r="584" spans="6:6" x14ac:dyDescent="0.25">
+    <row r="584" spans="6:6" x14ac:dyDescent="0.3">
       <c r="F584"/>
     </row>
-    <row r="585" spans="6:6" x14ac:dyDescent="0.25">
+    <row r="585" spans="6:6" x14ac:dyDescent="0.3">
       <c r="F585"/>
     </row>
-    <row r="586" spans="6:6" x14ac:dyDescent="0.25">
+    <row r="586" spans="6:6" x14ac:dyDescent="0.3">
       <c r="F586"/>
     </row>
-    <row r="587" spans="6:6" x14ac:dyDescent="0.25">
+    <row r="587" spans="6:6" x14ac:dyDescent="0.3">
       <c r="F587"/>
     </row>
-    <row r="588" spans="6:6" x14ac:dyDescent="0.25">
+    <row r="588" spans="6:6" x14ac:dyDescent="0.3">
       <c r="F588"/>
     </row>
-    <row r="589" spans="6:6" x14ac:dyDescent="0.25">
+    <row r="589" spans="6:6" x14ac:dyDescent="0.3">
       <c r="F589"/>
     </row>
-    <row r="590" spans="6:6" x14ac:dyDescent="0.25">
+    <row r="590" spans="6:6" x14ac:dyDescent="0.3">
       <c r="F590"/>
     </row>
-    <row r="591" spans="6:6" x14ac:dyDescent="0.25">
+    <row r="591" spans="6:6" x14ac:dyDescent="0.3">
       <c r="F591"/>
     </row>
-    <row r="592" spans="6:6" x14ac:dyDescent="0.25">
+    <row r="592" spans="6:6" x14ac:dyDescent="0.3">
       <c r="F592"/>
     </row>
-    <row r="593" spans="6:6" x14ac:dyDescent="0.25">
+    <row r="593" spans="6:6" x14ac:dyDescent="0.3">
       <c r="F593"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Asset List Punten Update
</commit_message>
<xml_diff>
--- a/Algemeen/Asset List Game-Lab 1.xlsx
+++ b/Algemeen/Asset List Game-Lab 1.xlsx
@@ -1144,10 +1144,10 @@
     <t>Artist Points Behaald: 352 / 625</t>
   </si>
   <si>
-    <t>Development Points: 590 / 650</t>
-  </si>
-  <si>
     <t>320 Fahrettin | 185 Sven | 150 Rief</t>
+  </si>
+  <si>
+    <t>Development Points: 655 / 625</t>
   </si>
 </sst>
 </file>
@@ -1686,7 +1686,7 @@
   <dimension ref="A1:R593"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="J1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K21" sqref="K21"/>
+      <selection activeCell="K18" sqref="K18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2922,8 +2922,8 @@
       </c>
       <c r="H34" s="19"/>
       <c r="I34" s="19"/>
-      <c r="J34" s="23" t="s">
-        <v>375</v>
+      <c r="J34" s="22" t="s">
+        <v>376</v>
       </c>
       <c r="N34" s="22" t="s">
         <v>276</v>
@@ -2951,7 +2951,7 @@
       <c r="H35" s="19"/>
       <c r="I35" s="19"/>
       <c r="J35" s="1" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
     </row>
     <row r="36" spans="1:18" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Asset list en uren registratie 25-11-2015
</commit_message>
<xml_diff>
--- a/Algemeen/Asset List Game-Lab 1.xlsx
+++ b/Algemeen/Asset List Game-Lab 1.xlsx
@@ -1141,13 +1141,13 @@
     <t xml:space="preserve"> Fahrettin</t>
   </si>
   <si>
-    <t>Artist Points Behaald: 352 / 625</t>
-  </si>
-  <si>
     <t>320 Fahrettin | 185 Sven | 150 Rief</t>
   </si>
   <si>
     <t>Development Points: 655 / 625</t>
+  </si>
+  <si>
+    <t>Artist Points Behaald: 366 / 625</t>
   </si>
 </sst>
 </file>
@@ -1686,7 +1686,7 @@
   <dimension ref="A1:R593"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="J1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K18" sqref="K18"/>
+      <selection activeCell="J19" sqref="J19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2303,7 +2303,7 @@
       <c r="M13" s="24" t="s">
         <v>233</v>
       </c>
-      <c r="O13" s="1" t="s">
+      <c r="O13" s="22" t="s">
         <v>304</v>
       </c>
       <c r="P13" s="22" t="s">
@@ -2923,7 +2923,7 @@
       <c r="H34" s="19"/>
       <c r="I34" s="19"/>
       <c r="J34" s="22" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="N34" s="22" t="s">
         <v>276</v>
@@ -2951,14 +2951,14 @@
       <c r="H35" s="19"/>
       <c r="I35" s="19"/>
       <c r="J35" s="1" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
     </row>
     <row r="36" spans="1:18" x14ac:dyDescent="0.25">
       <c r="H36" s="19"/>
       <c r="I36" s="19"/>
       <c r="J36" s="23" t="s">
-        <v>374</v>
+        <v>376</v>
       </c>
     </row>
     <row r="37" spans="1:18" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Uren Registratie Roos Aangepast + Special moves Script Af
</commit_message>
<xml_diff>
--- a/Algemeen/Asset List Game-Lab 1.xlsx
+++ b/Algemeen/Asset List Game-Lab 1.xlsx
@@ -1141,13 +1141,13 @@
     <t xml:space="preserve"> Fahrettin</t>
   </si>
   <si>
-    <t>320 Fahrettin | 185 Sven | 150 Rief</t>
-  </si>
-  <si>
-    <t>Development Points: 655 / 625</t>
-  </si>
-  <si>
     <t>Artist Points Behaald: 366 / 625</t>
+  </si>
+  <si>
+    <t>350 Fahrettin | 185 Sven | 150 Rief</t>
+  </si>
+  <si>
+    <t>Development Points: 685 / 750</t>
   </si>
 </sst>
 </file>
@@ -1686,7 +1686,7 @@
   <dimension ref="A1:R593"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="J1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J19" sqref="J19"/>
+      <selection activeCell="N18" sqref="N18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2669,7 +2669,7 @@
       <c r="L27" s="22" t="s">
         <v>237</v>
       </c>
-      <c r="M27" s="1" t="s">
+      <c r="M27" s="22" t="s">
         <v>264</v>
       </c>
       <c r="N27" s="22" t="s">
@@ -2922,8 +2922,8 @@
       </c>
       <c r="H34" s="19"/>
       <c r="I34" s="19"/>
-      <c r="J34" s="22" t="s">
-        <v>375</v>
+      <c r="J34" s="23" t="s">
+        <v>376</v>
       </c>
       <c r="N34" s="22" t="s">
         <v>276</v>
@@ -2951,14 +2951,14 @@
       <c r="H35" s="19"/>
       <c r="I35" s="19"/>
       <c r="J35" s="1" t="s">
-        <v>374</v>
+        <v>375</v>
       </c>
     </row>
     <row r="36" spans="1:18" x14ac:dyDescent="0.25">
       <c r="H36" s="19"/>
       <c r="I36" s="19"/>
       <c r="J36" s="23" t="s">
-        <v>376</v>
+        <v>374</v>
       </c>
     </row>
     <row r="37" spans="1:18" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
XP & PlayerCalculation Bug Fixes
</commit_message>
<xml_diff>
--- a/Algemeen/Asset List Game-Lab 1.xlsx
+++ b/Algemeen/Asset List Game-Lab 1.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1539" uniqueCount="384">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1539" uniqueCount="385">
   <si>
     <t>ID Code</t>
   </si>
@@ -1144,9 +1144,6 @@
     <t>Artist Points Behaald: 366 / 625</t>
   </si>
   <si>
-    <t>Development Points: 685 / 750</t>
-  </si>
-  <si>
     <t>55 Fahrettin|55 Sven|15 Rief</t>
   </si>
   <si>
@@ -1162,13 +1159,19 @@
     <t>265 Fahrettin|185 Sven|150 Rief</t>
   </si>
   <si>
-    <t>290 Fahrettin|185 Sven|150 Rief</t>
-  </si>
-  <si>
     <t>350 Fahrettin|185 Sven|150 Rief</t>
   </si>
   <si>
     <t>350 Fahrettin|185 Sven|180 Rief</t>
+  </si>
+  <si>
+    <t>290 Fahrettin|185 Sven|165 Rief</t>
+  </si>
+  <si>
+    <t>Development Points: 715 / 750</t>
+  </si>
+  <si>
+    <t>290 Fahrettin|185 Sven|180 Rief</t>
   </si>
 </sst>
 </file>
@@ -1707,7 +1710,7 @@
   <dimension ref="A1:R593"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="J1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="P34" sqref="P34"/>
+      <selection activeCell="P35" sqref="P35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2628,31 +2631,31 @@
         <v>367</v>
       </c>
       <c r="J25" s="1" t="s">
+        <v>375</v>
+      </c>
+      <c r="K25" s="1" t="s">
         <v>376</v>
       </c>
-      <c r="K25" s="1" t="s">
+      <c r="L25" s="1" t="s">
         <v>377</v>
       </c>
-      <c r="L25" s="1" t="s">
+      <c r="M25" s="1" t="s">
         <v>378</v>
       </c>
-      <c r="M25" s="1" t="s">
+      <c r="N25" s="1" t="s">
         <v>379</v>
       </c>
-      <c r="N25" s="1" t="s">
+      <c r="O25" s="1" t="s">
+        <v>382</v>
+      </c>
+      <c r="P25" s="1" t="s">
+        <v>384</v>
+      </c>
+      <c r="Q25" s="1" t="s">
         <v>380</v>
       </c>
-      <c r="O25" s="1" t="s">
-        <v>381</v>
-      </c>
-      <c r="P25" s="1" t="s">
-        <v>381</v>
-      </c>
-      <c r="Q25" s="1" t="s">
-        <v>382</v>
-      </c>
       <c r="R25" s="1" t="s">
-        <v>382</v>
+        <v>380</v>
       </c>
     </row>
     <row r="26" spans="1:18" x14ac:dyDescent="0.25">
@@ -2971,7 +2974,7 @@
       <c r="H34" s="19"/>
       <c r="I34" s="19"/>
       <c r="J34" s="23" t="s">
-        <v>375</v>
+        <v>383</v>
       </c>
       <c r="N34" s="22" t="s">
         <v>276</v>
@@ -2999,7 +3002,7 @@
       <c r="H35" s="19"/>
       <c r="I35" s="19"/>
       <c r="J35" s="1" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
     </row>
     <row r="36" spans="1:18" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Uren Registratie 02-12-2015 & Asset List Upgrade
</commit_message>
<xml_diff>
--- a/Algemeen/Asset List Game-Lab 1.xlsx
+++ b/Algemeen/Asset List Game-Lab 1.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1539" uniqueCount="385">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1548" uniqueCount="395">
   <si>
     <t>ID Code</t>
   </si>
@@ -1135,50 +1135,80 @@
     <t>lvlDesign_Schuur_4 (27)</t>
   </si>
   <si>
-    <t xml:space="preserve"> Anthony |  Michiel |  Roos </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Fahrettin</t>
-  </si>
-  <si>
-    <t>Artist Points Behaald: 366 / 625</t>
-  </si>
-  <si>
     <t>55 Fahrettin|55 Sven|15 Rief</t>
   </si>
   <si>
-    <t>55 Fahrettin|105 Sven|45 Rief</t>
-  </si>
-  <si>
-    <t>140 Fahrettin|105 Sven|120 Rief</t>
-  </si>
-  <si>
-    <t>215 Fahrettin|145 Sven|120 Rief</t>
-  </si>
-  <si>
-    <t>265 Fahrettin|185 Sven|150 Rief</t>
-  </si>
-  <si>
-    <t>350 Fahrettin|185 Sven|150 Rief</t>
-  </si>
-  <si>
     <t>350 Fahrettin|185 Sven|180 Rief</t>
   </si>
   <si>
-    <t>290 Fahrettin|185 Sven|165 Rief</t>
-  </si>
-  <si>
     <t>Development Points: 715 / 750</t>
   </si>
   <si>
-    <t>290 Fahrettin|185 Sven|180 Rief</t>
+    <t>0 Fahrettin|50 Sven|30 Rief</t>
+  </si>
+  <si>
+    <t xml:space="preserve">32 Anthony| 0 Michiel| 16 Roos </t>
+  </si>
+  <si>
+    <t xml:space="preserve">12 Anthony| 0 Michiel| 20 Roos </t>
+  </si>
+  <si>
+    <t xml:space="preserve">61 Anthony| 51 Michiel| 74 Roos </t>
+  </si>
+  <si>
+    <t xml:space="preserve">113 Anthony| 70 Michiel| 6 Roos </t>
+  </si>
+  <si>
+    <t xml:space="preserve">27 Anthony| 26 Michiel| 0 Roos </t>
+  </si>
+  <si>
+    <t xml:space="preserve">30 Fahrettin </t>
+  </si>
+  <si>
+    <t xml:space="preserve">10 Anthony| 0 Michiel| 0 Roos </t>
+  </si>
+  <si>
+    <t xml:space="preserve">10 Anthony| 0 Michiel| 25 Roos </t>
+  </si>
+  <si>
+    <t xml:space="preserve">12 Anthony| 0 Michiel| 0 Roos </t>
+  </si>
+  <si>
+    <t>85 Fahrettin|0 Sven|75 Rief</t>
+  </si>
+  <si>
+    <t>75 Fahrettin|40 Sven|0 Rief</t>
+  </si>
+  <si>
+    <t xml:space="preserve">10 Anthony| 0 Michiel| 11 Roos </t>
+  </si>
+  <si>
+    <t xml:space="preserve">287 Anthony | 147 Michiel | 152 Roos </t>
+  </si>
+  <si>
+    <t>Artist Points Behaald: 616 / 750</t>
+  </si>
+  <si>
+    <t>25 Fahrettin|0 Sven|15 Rief</t>
+  </si>
+  <si>
+    <t>0 Fahrettin|0 Sven|15 Rief</t>
+  </si>
+  <si>
+    <t>60 Fahrettin|0 Sven|0 Rief</t>
+  </si>
+  <si>
+    <t>0 Fahrettin|0 Sven|0 Rief</t>
+  </si>
+  <si>
+    <t>50 Fahrettin|40 Sven|30 Rief</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1203,12 +1233,6 @@
     </font>
     <font>
       <sz val="11"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -1222,7 +1246,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="15">
+  <fills count="14">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1298,12 +1322,6 @@
         <fgColor rgb="FFFFEB9C"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="0"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -1317,10 +1335,10 @@
   <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1375,22 +1393,16 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="12" borderId="0" xfId="2" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="12" borderId="0" xfId="2" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="14" borderId="0" xfId="3" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="14" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="13" borderId="0" xfId="3" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1710,7 +1722,7 @@
   <dimension ref="A1:R593"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="J1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="P35" sqref="P35"/>
+      <selection activeCell="N22" sqref="N22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1724,10 +1736,9 @@
     <col min="7" max="7" width="15.7109375" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="18.7109375" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="123.28515625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="28.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="27.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="30" style="1" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="30.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="34.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="29.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="13" width="30.7109375" style="1" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="30" style="1" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="30.42578125" style="1" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="30" style="1" bestFit="1" customWidth="1"/>
@@ -1869,32 +1880,32 @@
       <c r="I3" s="5" t="s">
         <v>67</v>
       </c>
-      <c r="J3" s="21" t="s">
-        <v>221</v>
-      </c>
-      <c r="K3" s="21" t="s">
-        <v>221</v>
-      </c>
-      <c r="L3" s="21" t="s">
-        <v>221</v>
-      </c>
-      <c r="M3" s="21" t="s">
-        <v>221</v>
-      </c>
-      <c r="N3" s="21" t="s">
-        <v>221</v>
-      </c>
-      <c r="O3" s="21" t="s">
-        <v>221</v>
-      </c>
-      <c r="P3" s="21" t="s">
-        <v>221</v>
-      </c>
-      <c r="Q3" s="21" t="s">
-        <v>221</v>
-      </c>
-      <c r="R3" s="21" t="s">
-        <v>221</v>
+      <c r="J3" s="1" t="s">
+        <v>376</v>
+      </c>
+      <c r="K3" s="1" t="s">
+        <v>377</v>
+      </c>
+      <c r="L3" s="1" t="s">
+        <v>378</v>
+      </c>
+      <c r="M3" s="1" t="s">
+        <v>379</v>
+      </c>
+      <c r="N3" s="1" t="s">
+        <v>380</v>
+      </c>
+      <c r="O3" s="1" t="s">
+        <v>387</v>
+      </c>
+      <c r="P3" s="1" t="s">
+        <v>382</v>
+      </c>
+      <c r="Q3" s="1" t="s">
+        <v>383</v>
+      </c>
+      <c r="R3" s="1" t="s">
+        <v>384</v>
       </c>
     </row>
     <row r="4" spans="1:18" x14ac:dyDescent="0.25">
@@ -1922,32 +1933,32 @@
       <c r="I4" s="3" t="s">
         <v>151</v>
       </c>
-      <c r="J4" s="22" t="s">
-        <v>359</v>
-      </c>
-      <c r="K4" s="22" t="s">
-        <v>349</v>
-      </c>
-      <c r="L4" s="22" t="s">
-        <v>242</v>
-      </c>
-      <c r="M4" s="22" t="s">
-        <v>232</v>
+      <c r="J4" s="20" t="s">
+        <v>221</v>
+      </c>
+      <c r="K4" s="20" t="s">
+        <v>221</v>
+      </c>
+      <c r="L4" s="20" t="s">
+        <v>221</v>
+      </c>
+      <c r="M4" s="20" t="s">
+        <v>221</v>
       </c>
       <c r="N4" s="20" t="s">
-        <v>259</v>
-      </c>
-      <c r="O4" s="1" t="s">
-        <v>281</v>
-      </c>
-      <c r="P4" s="1" t="s">
-        <v>297</v>
-      </c>
-      <c r="Q4" s="1" t="s">
-        <v>310</v>
-      </c>
-      <c r="R4" s="1" t="s">
-        <v>340</v>
+        <v>221</v>
+      </c>
+      <c r="O4" s="20" t="s">
+        <v>221</v>
+      </c>
+      <c r="P4" s="20" t="s">
+        <v>221</v>
+      </c>
+      <c r="Q4" s="20" t="s">
+        <v>221</v>
+      </c>
+      <c r="R4" s="20" t="s">
+        <v>221</v>
       </c>
     </row>
     <row r="5" spans="1:18" x14ac:dyDescent="0.25">
@@ -1975,32 +1986,32 @@
       <c r="I5" s="3" t="s">
         <v>152</v>
       </c>
-      <c r="J5" s="22" t="s">
-        <v>230</v>
-      </c>
-      <c r="K5" s="22" t="s">
-        <v>253</v>
-      </c>
-      <c r="L5" s="22" t="s">
-        <v>243</v>
-      </c>
-      <c r="M5" s="22" t="s">
-        <v>231</v>
-      </c>
-      <c r="N5" s="1" t="s">
-        <v>269</v>
+      <c r="J5" s="21" t="s">
+        <v>359</v>
+      </c>
+      <c r="K5" s="21" t="s">
+        <v>349</v>
+      </c>
+      <c r="L5" s="21" t="s">
+        <v>242</v>
+      </c>
+      <c r="M5" s="21" t="s">
+        <v>232</v>
+      </c>
+      <c r="N5" s="23" t="s">
+        <v>259</v>
       </c>
       <c r="O5" s="1" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="P5" s="1" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="Q5" s="1" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="R5" s="1" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
     </row>
     <row r="6" spans="1:18" x14ac:dyDescent="0.25">
@@ -2013,29 +2024,32 @@
       <c r="I6" s="3" t="s">
         <v>73</v>
       </c>
-      <c r="J6" s="22" t="s">
-        <v>234</v>
-      </c>
-      <c r="L6" s="22" t="s">
-        <v>244</v>
-      </c>
-      <c r="M6" s="1" t="s">
-        <v>258</v>
-      </c>
-      <c r="N6" s="1" t="s">
-        <v>270</v>
+      <c r="J6" s="21" t="s">
+        <v>230</v>
+      </c>
+      <c r="K6" s="21" t="s">
+        <v>253</v>
+      </c>
+      <c r="L6" s="21" t="s">
+        <v>243</v>
+      </c>
+      <c r="M6" s="21" t="s">
+        <v>231</v>
+      </c>
+      <c r="N6" s="23" t="s">
+        <v>269</v>
       </c>
       <c r="O6" s="1" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="P6" s="1" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="Q6" s="1" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="R6" s="1" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
     </row>
     <row r="7" spans="1:18" x14ac:dyDescent="0.25">
@@ -2063,29 +2077,29 @@
       <c r="I7" s="3" t="s">
         <v>75</v>
       </c>
-      <c r="J7" s="22" t="s">
-        <v>235</v>
-      </c>
-      <c r="L7" s="22" t="s">
-        <v>245</v>
-      </c>
-      <c r="M7" s="22" t="s">
-        <v>260</v>
+      <c r="J7" s="21" t="s">
+        <v>234</v>
+      </c>
+      <c r="L7" s="21" t="s">
+        <v>244</v>
+      </c>
+      <c r="M7" s="23" t="s">
+        <v>258</v>
       </c>
       <c r="N7" s="1" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="O7" s="1" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="P7" s="1" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="Q7" s="1" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="R7" s="1" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
     </row>
     <row r="8" spans="1:18" x14ac:dyDescent="0.25">
@@ -2113,26 +2127,29 @@
       <c r="I8" s="3" t="s">
         <v>150</v>
       </c>
-      <c r="L8" s="22" t="s">
-        <v>246</v>
-      </c>
-      <c r="M8" s="25" t="s">
-        <v>261</v>
-      </c>
-      <c r="N8" s="22" t="s">
-        <v>361</v>
+      <c r="J8" s="21" t="s">
+        <v>235</v>
+      </c>
+      <c r="L8" s="21" t="s">
+        <v>245</v>
+      </c>
+      <c r="M8" s="21" t="s">
+        <v>260</v>
+      </c>
+      <c r="N8" s="1" t="s">
+        <v>271</v>
       </c>
       <c r="O8" s="1" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="P8" s="1" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="Q8" s="1" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="R8" s="1" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
     </row>
     <row r="9" spans="1:18" x14ac:dyDescent="0.25">
@@ -2160,26 +2177,26 @@
       <c r="I9" s="3" t="s">
         <v>134</v>
       </c>
-      <c r="L9" s="22" t="s">
-        <v>247</v>
-      </c>
-      <c r="M9" s="22" t="s">
-        <v>358</v>
-      </c>
-      <c r="N9" s="1" t="s">
-        <v>272</v>
-      </c>
-      <c r="O9" s="1" t="s">
-        <v>286</v>
+      <c r="L9" s="21" t="s">
+        <v>246</v>
+      </c>
+      <c r="M9" s="23" t="s">
+        <v>261</v>
+      </c>
+      <c r="N9" s="21" t="s">
+        <v>361</v>
+      </c>
+      <c r="O9" s="21" t="s">
+        <v>285</v>
       </c>
       <c r="P9" s="1" t="s">
-        <v>302</v>
-      </c>
-      <c r="Q9" s="22" t="s">
-        <v>315</v>
+        <v>301</v>
+      </c>
+      <c r="Q9" s="1" t="s">
+        <v>314</v>
       </c>
       <c r="R9" s="1" t="s">
-        <v>348</v>
+        <v>345</v>
       </c>
     </row>
     <row r="10" spans="1:18" x14ac:dyDescent="0.25">
@@ -2207,26 +2224,26 @@
       <c r="I10" s="3" t="s">
         <v>84</v>
       </c>
-      <c r="L10" s="22" t="s">
-        <v>248</v>
-      </c>
-      <c r="M10" s="22" t="s">
-        <v>346</v>
-      </c>
-      <c r="N10" s="22" t="s">
-        <v>290</v>
+      <c r="L10" s="21" t="s">
+        <v>247</v>
+      </c>
+      <c r="M10" s="21" t="s">
+        <v>358</v>
+      </c>
+      <c r="N10" s="1" t="s">
+        <v>272</v>
       </c>
       <c r="O10" s="1" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="P10" s="1" t="s">
-        <v>303</v>
-      </c>
-      <c r="Q10" s="22" t="s">
-        <v>316</v>
+        <v>302</v>
+      </c>
+      <c r="Q10" s="21" t="s">
+        <v>315</v>
       </c>
       <c r="R10" s="1" t="s">
-        <v>351</v>
+        <v>348</v>
       </c>
     </row>
     <row r="11" spans="1:18" x14ac:dyDescent="0.25">
@@ -2236,26 +2253,26 @@
       <c r="I11" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="L11" s="22" t="s">
-        <v>249</v>
-      </c>
-      <c r="M11" s="1" t="s">
-        <v>343</v>
-      </c>
-      <c r="N11" s="1" t="s">
-        <v>347</v>
+      <c r="L11" s="21" t="s">
+        <v>248</v>
+      </c>
+      <c r="M11" s="21" t="s">
+        <v>346</v>
+      </c>
+      <c r="N11" s="21" t="s">
+        <v>290</v>
       </c>
       <c r="O11" s="1" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="P11" s="1" t="s">
-        <v>288</v>
-      </c>
-      <c r="Q11" s="22" t="s">
-        <v>317</v>
+        <v>303</v>
+      </c>
+      <c r="Q11" s="21" t="s">
+        <v>316</v>
       </c>
       <c r="R11" s="1" t="s">
-        <v>362</v>
+        <v>351</v>
       </c>
     </row>
     <row r="12" spans="1:18" x14ac:dyDescent="0.25">
@@ -2280,23 +2297,26 @@
       <c r="I12" s="3" t="s">
         <v>95</v>
       </c>
-      <c r="L12" s="24" t="s">
-        <v>250</v>
-      </c>
-      <c r="M12" s="22" t="s">
-        <v>371</v>
+      <c r="L12" s="21" t="s">
+        <v>249</v>
+      </c>
+      <c r="M12" s="21" t="s">
+        <v>343</v>
+      </c>
+      <c r="N12" s="1" t="s">
+        <v>347</v>
       </c>
       <c r="O12" s="1" t="s">
-        <v>354</v>
-      </c>
-      <c r="P12" s="22" t="s">
-        <v>325</v>
-      </c>
-      <c r="Q12" s="22" t="s">
-        <v>318</v>
+        <v>289</v>
+      </c>
+      <c r="P12" s="1" t="s">
+        <v>288</v>
+      </c>
+      <c r="Q12" s="21" t="s">
+        <v>317</v>
       </c>
       <c r="R12" s="1" t="s">
-        <v>352</v>
+        <v>362</v>
       </c>
     </row>
     <row r="13" spans="1:18" x14ac:dyDescent="0.25">
@@ -2321,23 +2341,23 @@
       <c r="I13" s="3" t="s">
         <v>135</v>
       </c>
-      <c r="L13" s="22" t="s">
-        <v>251</v>
-      </c>
-      <c r="M13" s="24" t="s">
-        <v>233</v>
-      </c>
-      <c r="O13" s="22" t="s">
-        <v>304</v>
-      </c>
-      <c r="P13" s="22" t="s">
-        <v>356</v>
-      </c>
-      <c r="Q13" s="1" t="s">
-        <v>319</v>
-      </c>
-      <c r="R13" s="22" t="s">
-        <v>350</v>
+      <c r="L13" s="23" t="s">
+        <v>250</v>
+      </c>
+      <c r="M13" s="21" t="s">
+        <v>371</v>
+      </c>
+      <c r="O13" s="1" t="s">
+        <v>354</v>
+      </c>
+      <c r="P13" s="21" t="s">
+        <v>325</v>
+      </c>
+      <c r="Q13" s="21" t="s">
+        <v>318</v>
+      </c>
+      <c r="R13" s="1" t="s">
+        <v>352</v>
       </c>
     </row>
     <row r="14" spans="1:18" x14ac:dyDescent="0.25">
@@ -2362,14 +2382,23 @@
       <c r="I14" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="L14" s="22" t="s">
-        <v>252</v>
-      </c>
-      <c r="O14" s="22" t="s">
-        <v>357</v>
-      </c>
-      <c r="Q14" s="22" t="s">
-        <v>320</v>
+      <c r="L14" s="21" t="s">
+        <v>251</v>
+      </c>
+      <c r="M14" s="23" t="s">
+        <v>233</v>
+      </c>
+      <c r="O14" s="21" t="s">
+        <v>304</v>
+      </c>
+      <c r="P14" s="21" t="s">
+        <v>356</v>
+      </c>
+      <c r="Q14" s="1" t="s">
+        <v>319</v>
+      </c>
+      <c r="R14" s="21" t="s">
+        <v>350</v>
       </c>
     </row>
     <row r="15" spans="1:18" x14ac:dyDescent="0.25">
@@ -2394,11 +2423,14 @@
       <c r="I15" s="3" t="s">
         <v>105</v>
       </c>
-      <c r="L15" s="22" t="s">
-        <v>360</v>
-      </c>
-      <c r="Q15" s="1" t="s">
-        <v>321</v>
+      <c r="L15" s="21" t="s">
+        <v>252</v>
+      </c>
+      <c r="O15" s="21" t="s">
+        <v>357</v>
+      </c>
+      <c r="Q15" s="21" t="s">
+        <v>320</v>
       </c>
     </row>
     <row r="16" spans="1:18" x14ac:dyDescent="0.25">
@@ -2408,11 +2440,11 @@
       <c r="I16" s="3" t="s">
         <v>115</v>
       </c>
-      <c r="L16" s="22" t="s">
-        <v>262</v>
+      <c r="L16" s="21" t="s">
+        <v>360</v>
       </c>
       <c r="Q16" s="1" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
     </row>
     <row r="17" spans="1:18" x14ac:dyDescent="0.25">
@@ -2437,11 +2469,11 @@
       <c r="I17" s="3" t="s">
         <v>137</v>
       </c>
-      <c r="L17" s="22" t="s">
-        <v>263</v>
+      <c r="L17" s="21" t="s">
+        <v>262</v>
       </c>
       <c r="Q17" s="1" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
     </row>
     <row r="18" spans="1:18" x14ac:dyDescent="0.25">
@@ -2466,11 +2498,11 @@
       <c r="I18" s="3" t="s">
         <v>136</v>
       </c>
-      <c r="L18" s="22" t="s">
-        <v>353</v>
+      <c r="L18" s="21" t="s">
+        <v>263</v>
       </c>
       <c r="Q18" s="1" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
     </row>
     <row r="19" spans="1:18" x14ac:dyDescent="0.25">
@@ -2495,11 +2527,11 @@
       <c r="I19" s="3" t="s">
         <v>363</v>
       </c>
-      <c r="L19" s="22" t="s">
-        <v>236</v>
-      </c>
-      <c r="Q19" s="22" t="s">
-        <v>355</v>
+      <c r="L19" s="21" t="s">
+        <v>353</v>
+      </c>
+      <c r="Q19" s="1" t="s">
+        <v>324</v>
       </c>
     </row>
     <row r="20" spans="1:18" x14ac:dyDescent="0.25">
@@ -2524,8 +2556,11 @@
       <c r="I20" s="3" t="s">
         <v>364</v>
       </c>
-      <c r="L20" s="24" t="s">
-        <v>224</v>
+      <c r="L20" s="21" t="s">
+        <v>236</v>
+      </c>
+      <c r="Q20" s="21" t="s">
+        <v>355</v>
       </c>
     </row>
     <row r="21" spans="1:18" x14ac:dyDescent="0.25">
@@ -2535,8 +2570,8 @@
       <c r="I21" s="3" t="s">
         <v>369</v>
       </c>
-      <c r="L21" s="22" t="s">
-        <v>257</v>
+      <c r="L21" s="23" t="s">
+        <v>224</v>
       </c>
     </row>
     <row r="22" spans="1:18" x14ac:dyDescent="0.25">
@@ -2561,6 +2596,9 @@
       <c r="I22" s="3" t="s">
         <v>370</v>
       </c>
+      <c r="L22" s="21" t="s">
+        <v>257</v>
+      </c>
     </row>
     <row r="23" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A23" s="5" t="s">
@@ -2631,31 +2669,31 @@
         <v>367</v>
       </c>
       <c r="J25" s="1" t="s">
+        <v>372</v>
+      </c>
+      <c r="K25" s="1" t="s">
         <v>375</v>
       </c>
-      <c r="K25" s="1" t="s">
-        <v>376</v>
-      </c>
       <c r="L25" s="1" t="s">
-        <v>377</v>
+        <v>385</v>
       </c>
       <c r="M25" s="1" t="s">
-        <v>378</v>
+        <v>386</v>
       </c>
       <c r="N25" s="1" t="s">
-        <v>379</v>
+        <v>394</v>
       </c>
       <c r="O25" s="1" t="s">
-        <v>382</v>
+        <v>390</v>
       </c>
       <c r="P25" s="1" t="s">
-        <v>384</v>
+        <v>391</v>
       </c>
       <c r="Q25" s="1" t="s">
-        <v>380</v>
+        <v>392</v>
       </c>
       <c r="R25" s="1" t="s">
-        <v>380</v>
+        <v>393</v>
       </c>
     </row>
     <row r="26" spans="1:18" x14ac:dyDescent="0.25">
@@ -2666,31 +2704,31 @@
       <c r="I26" s="5" t="s">
         <v>368</v>
       </c>
-      <c r="J26" s="21" t="s">
+      <c r="J26" s="20" t="s">
         <v>222</v>
       </c>
-      <c r="K26" s="21" t="s">
+      <c r="K26" s="20" t="s">
         <v>222</v>
       </c>
-      <c r="L26" s="21" t="s">
+      <c r="L26" s="20" t="s">
         <v>222</v>
       </c>
-      <c r="M26" s="21" t="s">
+      <c r="M26" s="20" t="s">
         <v>222</v>
       </c>
-      <c r="N26" s="21" t="s">
+      <c r="N26" s="20" t="s">
         <v>222</v>
       </c>
-      <c r="O26" s="21" t="s">
+      <c r="O26" s="20" t="s">
         <v>222</v>
       </c>
-      <c r="P26" s="21" t="s">
+      <c r="P26" s="20" t="s">
         <v>222</v>
       </c>
-      <c r="Q26" s="21" t="s">
+      <c r="Q26" s="20" t="s">
         <v>222</v>
       </c>
-      <c r="R26" s="21" t="s">
+      <c r="R26" s="20" t="s">
         <v>222</v>
       </c>
     </row>
@@ -2711,22 +2749,22 @@
         <v>3</v>
       </c>
       <c r="I27" s="19"/>
-      <c r="J27" s="22" t="s">
+      <c r="J27" s="21" t="s">
         <v>225</v>
       </c>
-      <c r="K27" s="22" t="s">
+      <c r="K27" s="21" t="s">
         <v>238</v>
       </c>
-      <c r="L27" s="22" t="s">
+      <c r="L27" s="21" t="s">
         <v>237</v>
       </c>
-      <c r="M27" s="22" t="s">
+      <c r="M27" s="21" t="s">
         <v>264</v>
       </c>
-      <c r="N27" s="22" t="s">
+      <c r="N27" s="21" t="s">
         <v>277</v>
       </c>
-      <c r="O27" s="22" t="s">
+      <c r="O27" s="21" t="s">
         <v>291</v>
       </c>
       <c r="P27" s="1" t="s">
@@ -2756,28 +2794,28 @@
         <v>3</v>
       </c>
       <c r="I28" s="19"/>
-      <c r="J28" s="22" t="s">
+      <c r="J28" s="21" t="s">
         <v>226</v>
       </c>
-      <c r="K28" s="22" t="s">
+      <c r="K28" s="21" t="s">
         <v>239</v>
       </c>
-      <c r="L28" s="22" t="s">
+      <c r="L28" s="21" t="s">
         <v>255</v>
       </c>
-      <c r="M28" s="22" t="s">
+      <c r="M28" s="21" t="s">
         <v>265</v>
       </c>
-      <c r="N28" s="22" t="s">
+      <c r="N28" s="21" t="s">
         <v>278</v>
       </c>
-      <c r="O28" s="22" t="s">
+      <c r="O28" s="21" t="s">
         <v>292</v>
       </c>
       <c r="P28" s="1" t="s">
         <v>306</v>
       </c>
-      <c r="Q28" s="22" t="s">
+      <c r="Q28" s="21" t="s">
         <v>327</v>
       </c>
       <c r="R28" s="1" t="s">
@@ -2801,25 +2839,25 @@
         <v>3</v>
       </c>
       <c r="I29" s="19"/>
-      <c r="J29" s="22" t="s">
+      <c r="J29" s="21" t="s">
         <v>227</v>
       </c>
-      <c r="K29" s="22" t="s">
+      <c r="K29" s="21" t="s">
         <v>240</v>
       </c>
-      <c r="L29" s="22" t="s">
+      <c r="L29" s="21" t="s">
         <v>256</v>
       </c>
-      <c r="M29" s="22" t="s">
+      <c r="M29" s="21" t="s">
         <v>266</v>
       </c>
-      <c r="N29" s="22" t="s">
+      <c r="N29" s="21" t="s">
         <v>279</v>
       </c>
       <c r="O29" s="1" t="s">
         <v>293</v>
       </c>
-      <c r="P29" s="22" t="s">
+      <c r="P29" s="21" t="s">
         <v>307</v>
       </c>
       <c r="Q29" s="1" t="s">
@@ -2846,19 +2884,19 @@
         <v>3</v>
       </c>
       <c r="I30" s="19"/>
-      <c r="J30" s="22" t="s">
+      <c r="J30" s="21" t="s">
         <v>228</v>
       </c>
-      <c r="K30" s="22" t="s">
+      <c r="K30" s="21" t="s">
         <v>241</v>
       </c>
-      <c r="L30" s="22" t="s">
+      <c r="L30" s="21" t="s">
         <v>254</v>
       </c>
-      <c r="M30" s="22" t="s">
+      <c r="M30" s="21" t="s">
         <v>267</v>
       </c>
-      <c r="N30" s="22" t="s">
+      <c r="N30" s="21" t="s">
         <v>280</v>
       </c>
       <c r="O30" s="1" t="s">
@@ -2877,16 +2915,16 @@
     <row r="31" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B31" s="16"/>
       <c r="I31" s="19"/>
-      <c r="J31" s="22" t="s">
+      <c r="J31" s="21" t="s">
         <v>229</v>
       </c>
-      <c r="M31" s="22" t="s">
+      <c r="M31" s="21" t="s">
         <v>268</v>
       </c>
-      <c r="N31" s="22" t="s">
+      <c r="N31" s="21" t="s">
         <v>273</v>
       </c>
-      <c r="O31" s="22" t="s">
+      <c r="O31" s="21" t="s">
         <v>295</v>
       </c>
       <c r="P31" s="1" t="s">
@@ -2923,7 +2961,7 @@
       <c r="O32" s="1" t="s">
         <v>296</v>
       </c>
-      <c r="Q32" s="22" t="s">
+      <c r="Q32" s="21" t="s">
         <v>331</v>
       </c>
       <c r="R32" s="1" t="s">
@@ -2948,7 +2986,7 @@
       </c>
       <c r="H33" s="19"/>
       <c r="I33" s="19"/>
-      <c r="N33" s="22" t="s">
+      <c r="N33" s="21" t="s">
         <v>275</v>
       </c>
       <c r="R33" s="1" t="s">
@@ -2973,10 +3011,10 @@
       </c>
       <c r="H34" s="19"/>
       <c r="I34" s="19"/>
-      <c r="J34" s="23" t="s">
-        <v>383</v>
-      </c>
-      <c r="N34" s="22" t="s">
+      <c r="J34" s="22" t="s">
+        <v>374</v>
+      </c>
+      <c r="N34" s="21" t="s">
         <v>276</v>
       </c>
       <c r="R34" s="1" t="s">
@@ -3002,14 +3040,14 @@
       <c r="H35" s="19"/>
       <c r="I35" s="19"/>
       <c r="J35" s="1" t="s">
-        <v>381</v>
+        <v>373</v>
       </c>
     </row>
     <row r="36" spans="1:18" x14ac:dyDescent="0.25">
       <c r="H36" s="19"/>
       <c r="I36" s="19"/>
-      <c r="J36" s="23" t="s">
-        <v>374</v>
+      <c r="J36" s="22" t="s">
+        <v>389</v>
       </c>
     </row>
     <row r="37" spans="1:18" x14ac:dyDescent="0.25">
@@ -3031,7 +3069,7 @@
       <c r="H37" s="19"/>
       <c r="I37" s="19"/>
       <c r="J37" s="1" t="s">
-        <v>372</v>
+        <v>388</v>
       </c>
     </row>
     <row r="38" spans="1:18" x14ac:dyDescent="0.25">
@@ -3052,7 +3090,7 @@
       </c>
       <c r="I38" s="19"/>
       <c r="J38" s="1" t="s">
-        <v>373</v>
+        <v>381</v>
       </c>
     </row>
     <row r="39" spans="1:18" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Bugs in word gezet & Asset List Update
</commit_message>
<xml_diff>
--- a/Algemeen/Asset List Game-Lab 1.xlsx
+++ b/Algemeen/Asset List Game-Lab 1.xlsx
@@ -1180,15 +1180,6 @@
     <t>75 Fahrettin|40 Sven|0 Rief</t>
   </si>
   <si>
-    <t xml:space="preserve">10 Anthony| 0 Michiel| 11 Roos </t>
-  </si>
-  <si>
-    <t xml:space="preserve">287 Anthony | 147 Michiel | 152 Roos </t>
-  </si>
-  <si>
-    <t>Artist Points Behaald: 616 / 750</t>
-  </si>
-  <si>
     <t>25 Fahrettin|0 Sven|15 Rief</t>
   </si>
   <si>
@@ -1202,6 +1193,15 @@
   </si>
   <si>
     <t>50 Fahrettin|40 Sven|30 Rief</t>
+  </si>
+  <si>
+    <t xml:space="preserve">10 Anthony| 0 Michiel| 26 Roos </t>
+  </si>
+  <si>
+    <t xml:space="preserve">287 Anthony | 147 Michiel | 167 Roos </t>
+  </si>
+  <si>
+    <t>Artist Points Behaald: 631 / 750</t>
   </si>
 </sst>
 </file>
@@ -1722,7 +1722,7 @@
   <dimension ref="A1:R593"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="J1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="N22" sqref="N22"/>
+      <selection activeCell="M34" sqref="M34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1896,7 +1896,7 @@
         <v>380</v>
       </c>
       <c r="O3" s="1" t="s">
-        <v>387</v>
+        <v>392</v>
       </c>
       <c r="P3" s="1" t="s">
         <v>382</v>
@@ -2139,7 +2139,7 @@
       <c r="N8" s="1" t="s">
         <v>271</v>
       </c>
-      <c r="O8" s="1" t="s">
+      <c r="O8" s="21" t="s">
         <v>284</v>
       </c>
       <c r="P8" s="1" t="s">
@@ -2681,19 +2681,19 @@
         <v>386</v>
       </c>
       <c r="N25" s="1" t="s">
-        <v>394</v>
+        <v>391</v>
       </c>
       <c r="O25" s="1" t="s">
+        <v>387</v>
+      </c>
+      <c r="P25" s="1" t="s">
+        <v>388</v>
+      </c>
+      <c r="Q25" s="1" t="s">
+        <v>389</v>
+      </c>
+      <c r="R25" s="1" t="s">
         <v>390</v>
-      </c>
-      <c r="P25" s="1" t="s">
-        <v>391</v>
-      </c>
-      <c r="Q25" s="1" t="s">
-        <v>392</v>
-      </c>
-      <c r="R25" s="1" t="s">
-        <v>393</v>
       </c>
     </row>
     <row r="26" spans="1:18" x14ac:dyDescent="0.25">
@@ -3047,7 +3047,7 @@
       <c r="H36" s="19"/>
       <c r="I36" s="19"/>
       <c r="J36" s="22" t="s">
-        <v>389</v>
+        <v>394</v>
       </c>
     </row>
     <row r="37" spans="1:18" x14ac:dyDescent="0.25">
@@ -3069,7 +3069,7 @@
       <c r="H37" s="19"/>
       <c r="I37" s="19"/>
       <c r="J37" s="1" t="s">
-        <v>388</v>
+        <v>393</v>
       </c>
     </row>
     <row r="38" spans="1:18" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Asset list update & Part 2 Tutorial voor currancy en shop klaar
</commit_message>
<xml_diff>
--- a/Algemeen/Asset List Game-Lab 1.xlsx
+++ b/Algemeen/Asset List Game-Lab 1.xlsx
@@ -1138,9 +1138,6 @@
     <t>55 Fahrettin|55 Sven|15 Rief</t>
   </si>
   <si>
-    <t>Development Points: 715 / 750</t>
-  </si>
-  <si>
     <t>0 Fahrettin|50 Sven|30 Rief</t>
   </si>
   <si>
@@ -1177,9 +1174,6 @@
     <t>25 Fahrettin|0 Sven|15 Rief</t>
   </si>
   <si>
-    <t>0 Fahrettin|0 Sven|15 Rief</t>
-  </si>
-  <si>
     <t>60 Fahrettin|0 Sven|0 Rief</t>
   </si>
   <si>
@@ -1192,16 +1186,22 @@
     <t xml:space="preserve">10 Anthony| 0 Michiel| 26 Roos </t>
   </si>
   <si>
-    <t xml:space="preserve">35 Anthony| 26 Michiel| 0 Roos </t>
-  </si>
-  <si>
-    <t xml:space="preserve">295 Anthony | 147 Michiel | 167 Roos </t>
-  </si>
-  <si>
-    <t>Artist Points Behaald: 639 / 750</t>
-  </si>
-  <si>
     <t>350 Fahrettin|210 Sven|180 Rief</t>
+  </si>
+  <si>
+    <t xml:space="preserve">49 Anthony| 26 Michiel| 0 Roos </t>
+  </si>
+  <si>
+    <t xml:space="preserve">309 Anthony | 147 Michiel | 167 Roos </t>
+  </si>
+  <si>
+    <t>0 Fahrettin|25 Sven|15 Rief</t>
+  </si>
+  <si>
+    <t>Development Points: 740 / 875</t>
+  </si>
+  <si>
+    <t>Artist Points Behaald: 653 / 875</t>
   </si>
 </sst>
 </file>
@@ -1721,8 +1721,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R593"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J33" sqref="J33"/>
+    <sheetView tabSelected="1" topLeftCell="J1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="L34" sqref="L34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1881,31 +1881,31 @@
         <v>67</v>
       </c>
       <c r="J3" s="1" t="s">
+        <v>374</v>
+      </c>
+      <c r="K3" s="1" t="s">
         <v>375</v>
       </c>
-      <c r="K3" s="1" t="s">
+      <c r="L3" s="1" t="s">
         <v>376</v>
       </c>
-      <c r="L3" s="1" t="s">
+      <c r="M3" s="1" t="s">
         <v>377</v>
       </c>
-      <c r="M3" s="1" t="s">
-        <v>378</v>
-      </c>
       <c r="N3" s="1" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="O3" s="1" t="s">
-        <v>390</v>
+        <v>388</v>
       </c>
       <c r="P3" s="1" t="s">
+        <v>379</v>
+      </c>
+      <c r="Q3" s="1" t="s">
         <v>380</v>
       </c>
-      <c r="Q3" s="1" t="s">
+      <c r="R3" s="1" t="s">
         <v>381</v>
-      </c>
-      <c r="R3" s="1" t="s">
-        <v>382</v>
       </c>
     </row>
     <row r="4" spans="1:18" x14ac:dyDescent="0.25">
@@ -2086,7 +2086,7 @@
       <c r="M7" s="23" t="s">
         <v>258</v>
       </c>
-      <c r="N7" s="1" t="s">
+      <c r="N7" s="21" t="s">
         <v>270</v>
       </c>
       <c r="O7" s="1" t="s">
@@ -2672,28 +2672,28 @@
         <v>372</v>
       </c>
       <c r="K25" s="1" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="L25" s="1" t="s">
+        <v>382</v>
+      </c>
+      <c r="M25" s="1" t="s">
         <v>383</v>
       </c>
-      <c r="M25" s="1" t="s">
+      <c r="N25" s="1" t="s">
+        <v>387</v>
+      </c>
+      <c r="O25" s="1" t="s">
         <v>384</v>
       </c>
-      <c r="N25" s="1" t="s">
-        <v>389</v>
-      </c>
-      <c r="O25" s="1" t="s">
+      <c r="P25" s="1" t="s">
+        <v>392</v>
+      </c>
+      <c r="Q25" s="1" t="s">
         <v>385</v>
       </c>
-      <c r="P25" s="1" t="s">
+      <c r="R25" s="1" t="s">
         <v>386</v>
-      </c>
-      <c r="Q25" s="1" t="s">
-        <v>387</v>
-      </c>
-      <c r="R25" s="1" t="s">
-        <v>388</v>
       </c>
     </row>
     <row r="26" spans="1:18" x14ac:dyDescent="0.25">
@@ -3012,7 +3012,7 @@
       <c r="H34" s="19"/>
       <c r="I34" s="19"/>
       <c r="J34" s="22" t="s">
-        <v>373</v>
+        <v>393</v>
       </c>
       <c r="N34" s="21" t="s">
         <v>276</v>
@@ -3040,14 +3040,14 @@
       <c r="H35" s="19"/>
       <c r="I35" s="19"/>
       <c r="J35" s="1" t="s">
-        <v>394</v>
+        <v>389</v>
       </c>
     </row>
     <row r="36" spans="1:18" x14ac:dyDescent="0.25">
       <c r="H36" s="19"/>
       <c r="I36" s="19"/>
       <c r="J36" s="22" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
     </row>
     <row r="37" spans="1:18" x14ac:dyDescent="0.25">
@@ -3069,7 +3069,7 @@
       <c r="H37" s="19"/>
       <c r="I37" s="19"/>
       <c r="J37" s="1" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
     </row>
     <row r="38" spans="1:18" x14ac:dyDescent="0.25">
@@ -3090,7 +3090,7 @@
       </c>
       <c r="I38" s="19"/>
       <c r="J38" s="1" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
     </row>
     <row r="39" spans="1:18" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Asset List Update met huidige aangevinkten assets bijvoorbeeld 6/8
</commit_message>
<xml_diff>
--- a/Algemeen/Asset List Game-Lab 1.xlsx
+++ b/Algemeen/Asset List Game-Lab 1.xlsx
@@ -691,9 +691,6 @@
     <t>255 Punten Totaal</t>
   </si>
   <si>
-    <t>Characters_Sara_1 (44)</t>
-  </si>
-  <si>
     <t>Scripts_3rdPersonCC_1.1 (15)</t>
   </si>
   <si>
@@ -718,9 +715,6 @@
     <t>Armor_KnuffelSchild_4 (17)</t>
   </si>
   <si>
-    <t>Enemy_TermietSoldier_1 (43)</t>
-  </si>
-  <si>
     <t>Road_BrugKort_2 (13)</t>
   </si>
   <si>
@@ -769,9 +763,6 @@
     <t>HUD_StaminaBar_12 (5)</t>
   </si>
   <si>
-    <t>Characters_SoldierAnt_4 (51)</t>
-  </si>
-  <si>
     <t>Weapons_HoutSpeer_4 (10)</t>
   </si>
   <si>
@@ -793,18 +784,9 @@
     <t>lvlDesign_Grot_3 (29)</t>
   </si>
   <si>
-    <t>Characters_Moeder_3 (40)</t>
-  </si>
-  <si>
-    <t>Enemy_TermietGeneral_2 (37)</t>
-  </si>
-  <si>
     <t>HUD_MiniMap_13 (4)</t>
   </si>
   <si>
-    <t>Enemy_VliegendHert_3 (49)</t>
-  </si>
-  <si>
     <t>HUD_Slots_15 (2)</t>
   </si>
   <si>
@@ -826,9 +808,6 @@
     <t>Script_Enemy_4.1 (15)</t>
   </si>
   <si>
-    <t>Enemy_ZwarteWeduwe_5 (49)</t>
-  </si>
-  <si>
     <t>Object_Toolbox_14 (14)</t>
   </si>
   <si>
@@ -1189,19 +1168,40 @@
     <t>350 Fahrettin|210 Sven|180 Rief</t>
   </si>
   <si>
-    <t xml:space="preserve">49 Anthony| 26 Michiel| 0 Roos </t>
-  </si>
-  <si>
-    <t xml:space="preserve">309 Anthony | 147 Michiel | 167 Roos </t>
-  </si>
-  <si>
     <t>0 Fahrettin|25 Sven|15 Rief</t>
   </si>
   <si>
     <t>Development Points: 740 / 875</t>
   </si>
   <si>
-    <t>Artist Points Behaald: 653 / 875</t>
+    <t>Characters_SoldierAnt_4 (51) 6/8</t>
+  </si>
+  <si>
+    <t>Characters_Sara_1 (44) 5/8</t>
+  </si>
+  <si>
+    <t>Characters_Moeder_3 (40) 6/8</t>
+  </si>
+  <si>
+    <t>Enemy_VliegendHert_3 (49) 6/8</t>
+  </si>
+  <si>
+    <t>Enemy_TermietSoldier_1 (43) 6/8</t>
+  </si>
+  <si>
+    <t>Enemy_TermietGeneral_2 (37) 6/8</t>
+  </si>
+  <si>
+    <t>Enemy_ZwarteWeduwe_5 (49) 4/8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">58 Anthony| 26 Michiel| 0 Roos </t>
+  </si>
+  <si>
+    <t xml:space="preserve">318 Anthony | 147 Michiel | 167 Roos </t>
+  </si>
+  <si>
+    <t>Artist Points Behaald: 662 / 875</t>
   </si>
 </sst>
 </file>
@@ -1722,7 +1722,7 @@
   <dimension ref="A1:R593"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="J1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="L34" sqref="L34"/>
+      <selection activeCell="N21" sqref="N21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1738,8 +1738,9 @@
     <col min="9" max="9" width="123.28515625" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="34.7109375" style="1" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="29.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="12" max="13" width="30.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="30" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="30.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="31.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="32" style="1" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="30.42578125" style="1" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="30" style="1" bestFit="1" customWidth="1"/>
     <col min="17" max="18" width="30.42578125" style="1" bestFit="1" customWidth="1"/>
@@ -1881,31 +1882,31 @@
         <v>67</v>
       </c>
       <c r="J3" s="1" t="s">
+        <v>367</v>
+      </c>
+      <c r="K3" s="1" t="s">
+        <v>368</v>
+      </c>
+      <c r="L3" s="1" t="s">
+        <v>369</v>
+      </c>
+      <c r="M3" s="1" t="s">
+        <v>370</v>
+      </c>
+      <c r="N3" s="1" t="s">
+        <v>392</v>
+      </c>
+      <c r="O3" s="1" t="s">
+        <v>381</v>
+      </c>
+      <c r="P3" s="1" t="s">
+        <v>372</v>
+      </c>
+      <c r="Q3" s="1" t="s">
+        <v>373</v>
+      </c>
+      <c r="R3" s="1" t="s">
         <v>374</v>
-      </c>
-      <c r="K3" s="1" t="s">
-        <v>375</v>
-      </c>
-      <c r="L3" s="1" t="s">
-        <v>376</v>
-      </c>
-      <c r="M3" s="1" t="s">
-        <v>377</v>
-      </c>
-      <c r="N3" s="1" t="s">
-        <v>390</v>
-      </c>
-      <c r="O3" s="1" t="s">
-        <v>388</v>
-      </c>
-      <c r="P3" s="1" t="s">
-        <v>379</v>
-      </c>
-      <c r="Q3" s="1" t="s">
-        <v>380</v>
-      </c>
-      <c r="R3" s="1" t="s">
-        <v>381</v>
       </c>
     </row>
     <row r="4" spans="1:18" x14ac:dyDescent="0.25">
@@ -1987,31 +1988,31 @@
         <v>152</v>
       </c>
       <c r="J5" s="21" t="s">
-        <v>359</v>
+        <v>352</v>
       </c>
       <c r="K5" s="21" t="s">
-        <v>349</v>
+        <v>342</v>
       </c>
       <c r="L5" s="21" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="M5" s="21" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="N5" s="23" t="s">
-        <v>259</v>
+        <v>390</v>
       </c>
       <c r="O5" s="1" t="s">
-        <v>281</v>
+        <v>274</v>
       </c>
       <c r="P5" s="1" t="s">
-        <v>297</v>
+        <v>290</v>
       </c>
       <c r="Q5" s="1" t="s">
-        <v>310</v>
+        <v>303</v>
       </c>
       <c r="R5" s="1" t="s">
-        <v>340</v>
+        <v>333</v>
       </c>
     </row>
     <row r="6" spans="1:18" x14ac:dyDescent="0.25">
@@ -2025,31 +2026,31 @@
         <v>73</v>
       </c>
       <c r="J6" s="21" t="s">
+        <v>229</v>
+      </c>
+      <c r="K6" s="21" t="s">
+        <v>250</v>
+      </c>
+      <c r="L6" s="21" t="s">
+        <v>241</v>
+      </c>
+      <c r="M6" s="21" t="s">
         <v>230</v>
       </c>
-      <c r="K6" s="21" t="s">
-        <v>253</v>
-      </c>
-      <c r="L6" s="21" t="s">
-        <v>243</v>
-      </c>
-      <c r="M6" s="21" t="s">
-        <v>231</v>
-      </c>
       <c r="N6" s="23" t="s">
-        <v>269</v>
+        <v>391</v>
       </c>
       <c r="O6" s="1" t="s">
-        <v>282</v>
+        <v>275</v>
       </c>
       <c r="P6" s="1" t="s">
-        <v>298</v>
+        <v>291</v>
       </c>
       <c r="Q6" s="1" t="s">
-        <v>311</v>
+        <v>304</v>
       </c>
       <c r="R6" s="1" t="s">
-        <v>341</v>
+        <v>334</v>
       </c>
     </row>
     <row r="7" spans="1:18" x14ac:dyDescent="0.25">
@@ -2078,28 +2079,28 @@
         <v>75</v>
       </c>
       <c r="J7" s="21" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="L7" s="21" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="M7" s="23" t="s">
-        <v>258</v>
+        <v>387</v>
       </c>
       <c r="N7" s="21" t="s">
-        <v>270</v>
+        <v>263</v>
       </c>
       <c r="O7" s="1" t="s">
-        <v>283</v>
+        <v>276</v>
       </c>
       <c r="P7" s="1" t="s">
-        <v>299</v>
+        <v>292</v>
       </c>
       <c r="Q7" s="1" t="s">
-        <v>312</v>
+        <v>305</v>
       </c>
       <c r="R7" s="1" t="s">
-        <v>342</v>
+        <v>335</v>
       </c>
     </row>
     <row r="8" spans="1:18" x14ac:dyDescent="0.25">
@@ -2128,28 +2129,28 @@
         <v>150</v>
       </c>
       <c r="J8" s="21" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="L8" s="21" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="M8" s="21" t="s">
-        <v>260</v>
+        <v>255</v>
       </c>
       <c r="N8" s="1" t="s">
-        <v>271</v>
+        <v>264</v>
       </c>
       <c r="O8" s="21" t="s">
-        <v>284</v>
+        <v>277</v>
       </c>
       <c r="P8" s="1" t="s">
-        <v>300</v>
+        <v>293</v>
       </c>
       <c r="Q8" s="1" t="s">
-        <v>313</v>
+        <v>306</v>
       </c>
       <c r="R8" s="1" t="s">
-        <v>344</v>
+        <v>337</v>
       </c>
     </row>
     <row r="9" spans="1:18" x14ac:dyDescent="0.25">
@@ -2178,25 +2179,25 @@
         <v>134</v>
       </c>
       <c r="L9" s="21" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="M9" s="23" t="s">
-        <v>261</v>
+        <v>388</v>
       </c>
       <c r="N9" s="21" t="s">
-        <v>361</v>
+        <v>354</v>
       </c>
       <c r="O9" s="21" t="s">
-        <v>285</v>
+        <v>278</v>
       </c>
       <c r="P9" s="1" t="s">
-        <v>301</v>
+        <v>294</v>
       </c>
       <c r="Q9" s="1" t="s">
-        <v>314</v>
+        <v>307</v>
       </c>
       <c r="R9" s="1" t="s">
-        <v>345</v>
+        <v>338</v>
       </c>
     </row>
     <row r="10" spans="1:18" x14ac:dyDescent="0.25">
@@ -2225,25 +2226,25 @@
         <v>84</v>
       </c>
       <c r="L10" s="21" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="M10" s="21" t="s">
-        <v>358</v>
+        <v>351</v>
       </c>
       <c r="N10" s="1" t="s">
-        <v>272</v>
+        <v>265</v>
       </c>
       <c r="O10" s="1" t="s">
-        <v>286</v>
+        <v>279</v>
       </c>
       <c r="P10" s="1" t="s">
-        <v>302</v>
+        <v>295</v>
       </c>
       <c r="Q10" s="21" t="s">
-        <v>315</v>
+        <v>308</v>
       </c>
       <c r="R10" s="1" t="s">
-        <v>348</v>
+        <v>341</v>
       </c>
     </row>
     <row r="11" spans="1:18" x14ac:dyDescent="0.25">
@@ -2254,25 +2255,25 @@
         <v>63</v>
       </c>
       <c r="L11" s="21" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="M11" s="21" t="s">
-        <v>346</v>
+        <v>339</v>
       </c>
       <c r="N11" s="21" t="s">
-        <v>290</v>
+        <v>283</v>
       </c>
       <c r="O11" s="1" t="s">
-        <v>287</v>
+        <v>280</v>
       </c>
       <c r="P11" s="1" t="s">
-        <v>303</v>
+        <v>296</v>
       </c>
       <c r="Q11" s="21" t="s">
-        <v>316</v>
+        <v>309</v>
       </c>
       <c r="R11" s="1" t="s">
-        <v>351</v>
+        <v>344</v>
       </c>
     </row>
     <row r="12" spans="1:18" x14ac:dyDescent="0.25">
@@ -2298,25 +2299,25 @@
         <v>95</v>
       </c>
       <c r="L12" s="21" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="M12" s="21" t="s">
-        <v>343</v>
+        <v>336</v>
       </c>
       <c r="N12" s="1" t="s">
-        <v>347</v>
+        <v>340</v>
       </c>
       <c r="O12" s="1" t="s">
-        <v>289</v>
+        <v>282</v>
       </c>
       <c r="P12" s="1" t="s">
-        <v>288</v>
+        <v>281</v>
       </c>
       <c r="Q12" s="21" t="s">
-        <v>317</v>
+        <v>310</v>
       </c>
       <c r="R12" s="1" t="s">
-        <v>362</v>
+        <v>355</v>
       </c>
     </row>
     <row r="13" spans="1:18" x14ac:dyDescent="0.25">
@@ -2342,22 +2343,22 @@
         <v>135</v>
       </c>
       <c r="L13" s="23" t="s">
-        <v>250</v>
+        <v>385</v>
       </c>
       <c r="M13" s="21" t="s">
-        <v>371</v>
+        <v>364</v>
       </c>
       <c r="O13" s="1" t="s">
-        <v>354</v>
+        <v>347</v>
       </c>
       <c r="P13" s="21" t="s">
-        <v>325</v>
+        <v>318</v>
       </c>
       <c r="Q13" s="21" t="s">
-        <v>318</v>
+        <v>311</v>
       </c>
       <c r="R13" s="1" t="s">
-        <v>352</v>
+        <v>345</v>
       </c>
     </row>
     <row r="14" spans="1:18" x14ac:dyDescent="0.25">
@@ -2383,22 +2384,22 @@
         <v>64</v>
       </c>
       <c r="L14" s="21" t="s">
-        <v>251</v>
+        <v>248</v>
       </c>
       <c r="M14" s="23" t="s">
-        <v>233</v>
+        <v>389</v>
       </c>
       <c r="O14" s="21" t="s">
-        <v>304</v>
+        <v>297</v>
       </c>
       <c r="P14" s="21" t="s">
-        <v>356</v>
+        <v>349</v>
       </c>
       <c r="Q14" s="1" t="s">
-        <v>319</v>
+        <v>312</v>
       </c>
       <c r="R14" s="21" t="s">
-        <v>350</v>
+        <v>343</v>
       </c>
     </row>
     <row r="15" spans="1:18" x14ac:dyDescent="0.25">
@@ -2424,13 +2425,13 @@
         <v>105</v>
       </c>
       <c r="L15" s="21" t="s">
-        <v>252</v>
+        <v>249</v>
       </c>
       <c r="O15" s="21" t="s">
-        <v>357</v>
+        <v>350</v>
       </c>
       <c r="Q15" s="21" t="s">
-        <v>320</v>
+        <v>313</v>
       </c>
     </row>
     <row r="16" spans="1:18" x14ac:dyDescent="0.25">
@@ -2441,10 +2442,10 @@
         <v>115</v>
       </c>
       <c r="L16" s="21" t="s">
-        <v>360</v>
+        <v>353</v>
       </c>
       <c r="Q16" s="1" t="s">
-        <v>321</v>
+        <v>314</v>
       </c>
     </row>
     <row r="17" spans="1:18" x14ac:dyDescent="0.25">
@@ -2470,10 +2471,10 @@
         <v>137</v>
       </c>
       <c r="L17" s="21" t="s">
-        <v>262</v>
+        <v>256</v>
       </c>
       <c r="Q17" s="1" t="s">
-        <v>322</v>
+        <v>315</v>
       </c>
     </row>
     <row r="18" spans="1:18" x14ac:dyDescent="0.25">
@@ -2499,10 +2500,10 @@
         <v>136</v>
       </c>
       <c r="L18" s="21" t="s">
-        <v>263</v>
+        <v>257</v>
       </c>
       <c r="Q18" s="1" t="s">
-        <v>323</v>
+        <v>316</v>
       </c>
     </row>
     <row r="19" spans="1:18" x14ac:dyDescent="0.25">
@@ -2525,13 +2526,13 @@
         <v>166</v>
       </c>
       <c r="I19" s="3" t="s">
-        <v>363</v>
+        <v>356</v>
       </c>
       <c r="L19" s="21" t="s">
-        <v>353</v>
+        <v>346</v>
       </c>
       <c r="Q19" s="1" t="s">
-        <v>324</v>
+        <v>317</v>
       </c>
     </row>
     <row r="20" spans="1:18" x14ac:dyDescent="0.25">
@@ -2554,13 +2555,13 @@
         <v>166</v>
       </c>
       <c r="I20" s="3" t="s">
-        <v>364</v>
+        <v>357</v>
       </c>
       <c r="L20" s="21" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="Q20" s="21" t="s">
-        <v>355</v>
+        <v>348</v>
       </c>
     </row>
     <row r="21" spans="1:18" x14ac:dyDescent="0.25">
@@ -2568,10 +2569,10 @@
         <v>166</v>
       </c>
       <c r="I21" s="3" t="s">
-        <v>369</v>
+        <v>362</v>
       </c>
       <c r="L21" s="23" t="s">
-        <v>224</v>
+        <v>386</v>
       </c>
     </row>
     <row r="22" spans="1:18" x14ac:dyDescent="0.25">
@@ -2594,10 +2595,10 @@
         <v>166</v>
       </c>
       <c r="I22" s="3" t="s">
-        <v>370</v>
+        <v>363</v>
       </c>
       <c r="L22" s="21" t="s">
-        <v>257</v>
+        <v>254</v>
       </c>
     </row>
     <row r="23" spans="1:18" x14ac:dyDescent="0.25">
@@ -2620,7 +2621,7 @@
         <v>166</v>
       </c>
       <c r="I23" s="3" t="s">
-        <v>365</v>
+        <v>358</v>
       </c>
     </row>
     <row r="24" spans="1:18" x14ac:dyDescent="0.25">
@@ -2643,7 +2644,7 @@
         <v>166</v>
       </c>
       <c r="I24" s="3" t="s">
-        <v>366</v>
+        <v>359</v>
       </c>
     </row>
     <row r="25" spans="1:18" x14ac:dyDescent="0.25">
@@ -2666,34 +2667,34 @@
         <v>166</v>
       </c>
       <c r="I25" s="5" t="s">
-        <v>367</v>
+        <v>360</v>
       </c>
       <c r="J25" s="1" t="s">
-        <v>372</v>
+        <v>365</v>
       </c>
       <c r="K25" s="1" t="s">
-        <v>373</v>
+        <v>366</v>
       </c>
       <c r="L25" s="1" t="s">
-        <v>382</v>
+        <v>375</v>
       </c>
       <c r="M25" s="1" t="s">
+        <v>376</v>
+      </c>
+      <c r="N25" s="1" t="s">
+        <v>380</v>
+      </c>
+      <c r="O25" s="1" t="s">
+        <v>377</v>
+      </c>
+      <c r="P25" s="1" t="s">
         <v>383</v>
       </c>
-      <c r="N25" s="1" t="s">
-        <v>387</v>
-      </c>
-      <c r="O25" s="1" t="s">
-        <v>384</v>
-      </c>
-      <c r="P25" s="1" t="s">
-        <v>392</v>
-      </c>
       <c r="Q25" s="1" t="s">
-        <v>385</v>
+        <v>378</v>
       </c>
       <c r="R25" s="1" t="s">
-        <v>386</v>
+        <v>379</v>
       </c>
     </row>
     <row r="26" spans="1:18" x14ac:dyDescent="0.25">
@@ -2702,7 +2703,7 @@
         <v>166</v>
       </c>
       <c r="I26" s="5" t="s">
-        <v>368</v>
+        <v>361</v>
       </c>
       <c r="J26" s="20" t="s">
         <v>222</v>
@@ -2750,31 +2751,31 @@
       </c>
       <c r="I27" s="19"/>
       <c r="J27" s="21" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="K27" s="21" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="L27" s="21" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="M27" s="21" t="s">
-        <v>264</v>
+        <v>258</v>
       </c>
       <c r="N27" s="21" t="s">
-        <v>277</v>
+        <v>270</v>
       </c>
       <c r="O27" s="21" t="s">
-        <v>291</v>
+        <v>284</v>
       </c>
       <c r="P27" s="1" t="s">
-        <v>309</v>
+        <v>302</v>
       </c>
       <c r="Q27" s="1" t="s">
-        <v>326</v>
+        <v>319</v>
       </c>
       <c r="R27" s="1" t="s">
-        <v>332</v>
+        <v>325</v>
       </c>
     </row>
     <row r="28" spans="1:18" x14ac:dyDescent="0.25">
@@ -2795,31 +2796,31 @@
       </c>
       <c r="I28" s="19"/>
       <c r="J28" s="21" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="K28" s="21" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="L28" s="21" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="M28" s="21" t="s">
-        <v>265</v>
+        <v>259</v>
       </c>
       <c r="N28" s="21" t="s">
-        <v>278</v>
+        <v>271</v>
       </c>
       <c r="O28" s="21" t="s">
-        <v>292</v>
+        <v>285</v>
       </c>
       <c r="P28" s="1" t="s">
-        <v>306</v>
+        <v>299</v>
       </c>
       <c r="Q28" s="21" t="s">
-        <v>327</v>
+        <v>320</v>
       </c>
       <c r="R28" s="1" t="s">
-        <v>333</v>
+        <v>326</v>
       </c>
     </row>
     <row r="29" spans="1:18" x14ac:dyDescent="0.25">
@@ -2840,31 +2841,31 @@
       </c>
       <c r="I29" s="19"/>
       <c r="J29" s="21" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="K29" s="21" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="L29" s="21" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
       <c r="M29" s="21" t="s">
-        <v>266</v>
+        <v>260</v>
       </c>
       <c r="N29" s="21" t="s">
-        <v>279</v>
+        <v>272</v>
       </c>
       <c r="O29" s="1" t="s">
-        <v>293</v>
+        <v>286</v>
       </c>
       <c r="P29" s="21" t="s">
-        <v>307</v>
+        <v>300</v>
       </c>
       <c r="Q29" s="1" t="s">
-        <v>328</v>
+        <v>321</v>
       </c>
       <c r="R29" s="1" t="s">
-        <v>334</v>
+        <v>327</v>
       </c>
     </row>
     <row r="30" spans="1:18" x14ac:dyDescent="0.25">
@@ -2885,56 +2886,56 @@
       </c>
       <c r="I30" s="19"/>
       <c r="J30" s="21" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="K30" s="21" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="L30" s="21" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
       <c r="M30" s="21" t="s">
-        <v>267</v>
+        <v>261</v>
       </c>
       <c r="N30" s="21" t="s">
-        <v>280</v>
+        <v>273</v>
       </c>
       <c r="O30" s="1" t="s">
-        <v>294</v>
+        <v>287</v>
       </c>
       <c r="P30" s="1" t="s">
-        <v>305</v>
+        <v>298</v>
       </c>
       <c r="Q30" s="1" t="s">
-        <v>329</v>
+        <v>322</v>
       </c>
       <c r="R30" s="1" t="s">
-        <v>335</v>
+        <v>328</v>
       </c>
     </row>
     <row r="31" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B31" s="16"/>
       <c r="I31" s="19"/>
       <c r="J31" s="21" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="M31" s="21" t="s">
-        <v>268</v>
+        <v>262</v>
       </c>
       <c r="N31" s="21" t="s">
-        <v>273</v>
+        <v>266</v>
       </c>
       <c r="O31" s="21" t="s">
-        <v>295</v>
+        <v>288</v>
       </c>
       <c r="P31" s="21" t="s">
-        <v>308</v>
+        <v>301</v>
       </c>
       <c r="Q31" s="1" t="s">
-        <v>330</v>
+        <v>323</v>
       </c>
       <c r="R31" s="1" t="s">
-        <v>336</v>
+        <v>329</v>
       </c>
     </row>
     <row r="32" spans="1:18" x14ac:dyDescent="0.25">
@@ -2956,16 +2957,16 @@
       <c r="H32" s="19"/>
       <c r="I32" s="19"/>
       <c r="N32" s="1" t="s">
-        <v>274</v>
+        <v>267</v>
       </c>
       <c r="O32" s="1" t="s">
-        <v>296</v>
+        <v>289</v>
       </c>
       <c r="Q32" s="21" t="s">
-        <v>331</v>
+        <v>324</v>
       </c>
       <c r="R32" s="1" t="s">
-        <v>337</v>
+        <v>330</v>
       </c>
     </row>
     <row r="33" spans="1:18" x14ac:dyDescent="0.25">
@@ -2987,10 +2988,10 @@
       <c r="H33" s="19"/>
       <c r="I33" s="19"/>
       <c r="N33" s="21" t="s">
-        <v>275</v>
+        <v>268</v>
       </c>
       <c r="R33" s="1" t="s">
-        <v>338</v>
+        <v>331</v>
       </c>
     </row>
     <row r="34" spans="1:18" x14ac:dyDescent="0.25">
@@ -3012,13 +3013,13 @@
       <c r="H34" s="19"/>
       <c r="I34" s="19"/>
       <c r="J34" s="22" t="s">
-        <v>393</v>
+        <v>384</v>
       </c>
       <c r="N34" s="21" t="s">
-        <v>276</v>
+        <v>269</v>
       </c>
       <c r="R34" s="1" t="s">
-        <v>339</v>
+        <v>332</v>
       </c>
     </row>
     <row r="35" spans="1:18" x14ac:dyDescent="0.25">
@@ -3040,7 +3041,7 @@
       <c r="H35" s="19"/>
       <c r="I35" s="19"/>
       <c r="J35" s="1" t="s">
-        <v>389</v>
+        <v>382</v>
       </c>
     </row>
     <row r="36" spans="1:18" x14ac:dyDescent="0.25">
@@ -3069,7 +3070,7 @@
       <c r="H37" s="19"/>
       <c r="I37" s="19"/>
       <c r="J37" s="1" t="s">
-        <v>391</v>
+        <v>393</v>
       </c>
     </row>
     <row r="38" spans="1:18" x14ac:dyDescent="0.25">
@@ -3090,7 +3091,7 @@
       </c>
       <c r="I38" s="19"/>
       <c r="J38" s="1" t="s">
-        <v>378</v>
+        <v>371</v>
       </c>
     </row>
     <row r="39" spans="1:18" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Asset List Update 14-12-2015
</commit_message>
<xml_diff>
--- a/Algemeen/Asset List Game-Lab 1.xlsx
+++ b/Algemeen/Asset List Game-Lab 1.xlsx
@@ -1162,9 +1162,6 @@
     <t>50 Fahrettin|40 Sven|30 Rief</t>
   </si>
   <si>
-    <t xml:space="preserve">10 Anthony| 0 Michiel| 26 Roos </t>
-  </si>
-  <si>
     <t>350 Fahrettin|210 Sven|180 Rief</t>
   </si>
   <si>
@@ -1192,16 +1189,19 @@
     <t>Enemy_TermietGeneral_2 (37) 6/8</t>
   </si>
   <si>
-    <t>Enemy_ZwarteWeduwe_5 (49) 4/8</t>
-  </si>
-  <si>
-    <t xml:space="preserve">58 Anthony| 26 Michiel| 0 Roos </t>
-  </si>
-  <si>
-    <t xml:space="preserve">318 Anthony | 147 Michiel | 167 Roos </t>
-  </si>
-  <si>
-    <t>Artist Points Behaald: 662 / 875</t>
+    <t>Enemy_ZwarteWeduwe_5 (49) 3/8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">58 Anthony| 19 Michiel| 0 Roos </t>
+  </si>
+  <si>
+    <t xml:space="preserve">14 Anthony| 0 Michiel| 26 Roos </t>
+  </si>
+  <si>
+    <t xml:space="preserve">322 Anthony | 140 Michiel | 167 Roos </t>
+  </si>
+  <si>
+    <t>Artist Points Behaald: 659 / 875</t>
   </si>
 </sst>
 </file>
@@ -1722,7 +1722,7 @@
   <dimension ref="A1:R593"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="J1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="N21" sqref="N21"/>
+      <selection activeCell="N20" sqref="N20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1894,10 +1894,10 @@
         <v>370</v>
       </c>
       <c r="N3" s="1" t="s">
+        <v>391</v>
+      </c>
+      <c r="O3" s="1" t="s">
         <v>392</v>
-      </c>
-      <c r="O3" s="1" t="s">
-        <v>381</v>
       </c>
       <c r="P3" s="1" t="s">
         <v>372</v>
@@ -2000,7 +2000,7 @@
         <v>231</v>
       </c>
       <c r="N5" s="23" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="O5" s="1" t="s">
         <v>274</v>
@@ -2038,7 +2038,7 @@
         <v>230</v>
       </c>
       <c r="N6" s="23" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="O6" s="1" t="s">
         <v>275</v>
@@ -2085,7 +2085,7 @@
         <v>242</v>
       </c>
       <c r="M7" s="23" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="N7" s="21" t="s">
         <v>263</v>
@@ -2182,7 +2182,7 @@
         <v>244</v>
       </c>
       <c r="M9" s="23" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="N9" s="21" t="s">
         <v>354</v>
@@ -2234,7 +2234,7 @@
       <c r="N10" s="1" t="s">
         <v>265</v>
       </c>
-      <c r="O10" s="1" t="s">
+      <c r="O10" s="21" t="s">
         <v>279</v>
       </c>
       <c r="P10" s="1" t="s">
@@ -2343,7 +2343,7 @@
         <v>135</v>
       </c>
       <c r="L13" s="23" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="M13" s="21" t="s">
         <v>364</v>
@@ -2387,7 +2387,7 @@
         <v>248</v>
       </c>
       <c r="M14" s="23" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="O14" s="21" t="s">
         <v>297</v>
@@ -2572,7 +2572,7 @@
         <v>362</v>
       </c>
       <c r="L21" s="23" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
     </row>
     <row r="22" spans="1:18" x14ac:dyDescent="0.25">
@@ -2688,7 +2688,7 @@
         <v>377</v>
       </c>
       <c r="P25" s="1" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="Q25" s="1" t="s">
         <v>378</v>
@@ -3013,7 +3013,7 @@
       <c r="H34" s="19"/>
       <c r="I34" s="19"/>
       <c r="J34" s="22" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="N34" s="21" t="s">
         <v>269</v>
@@ -3041,7 +3041,7 @@
       <c r="H35" s="19"/>
       <c r="I35" s="19"/>
       <c r="J35" s="1" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
     </row>
     <row r="36" spans="1:18" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Tutorial 9.1 Bug fixes met save en load en rechter muisknop op charpannel items + asset list update 16-12-2015
</commit_message>
<xml_diff>
--- a/Algemeen/Asset List Game-Lab 1.xlsx
+++ b/Algemeen/Asset List Game-Lab 1.xlsx
@@ -1195,13 +1195,13 @@
     <t xml:space="preserve">58 Anthony| 19 Michiel| 0 Roos </t>
   </si>
   <si>
-    <t xml:space="preserve">14 Anthony| 0 Michiel| 26 Roos </t>
-  </si>
-  <si>
-    <t xml:space="preserve">322 Anthony | 140 Michiel | 167 Roos </t>
-  </si>
-  <si>
-    <t>Artist Points Behaald: 659 / 875</t>
+    <t xml:space="preserve">21 Anthony| 0 Michiel| 26 Roos </t>
+  </si>
+  <si>
+    <t xml:space="preserve">329 Anthony | 140 Michiel | 167 Roos </t>
+  </si>
+  <si>
+    <t>Artist Points Behaald: 666 / 875</t>
   </si>
 </sst>
 </file>
@@ -2263,7 +2263,7 @@
       <c r="N11" s="21" t="s">
         <v>283</v>
       </c>
-      <c r="O11" s="1" t="s">
+      <c r="O11" s="21" t="s">
         <v>280</v>
       </c>
       <c r="P11" s="1" t="s">

</xml_diff>

<commit_message>
EINDELIJK KLAAR MET ALLE SCRIPTS!!!!
</commit_message>
<xml_diff>
--- a/Algemeen/Asset List Game-Lab 1.xlsx
+++ b/Algemeen/Asset List Game-Lab 1.xlsx
@@ -1150,18 +1150,12 @@
     <t>75 Fahrettin|40 Sven|0 Rief</t>
   </si>
   <si>
-    <t>25 Fahrettin|0 Sven|15 Rief</t>
-  </si>
-  <si>
     <t>60 Fahrettin|0 Sven|0 Rief</t>
   </si>
   <si>
     <t>0 Fahrettin|0 Sven|0 Rief</t>
   </si>
   <si>
-    <t>50 Fahrettin|40 Sven|30 Rief</t>
-  </si>
-  <si>
     <t>Characters_SoldierAnt_4 (51) 6/8</t>
   </si>
   <si>
@@ -1198,10 +1192,16 @@
     <t>0 Fahrettin|25 Sven|30 Rief</t>
   </si>
   <si>
-    <t>Development Points: 755 / 875</t>
-  </si>
-  <si>
-    <t>350 Fahrettin|210 Sven|195 Rief</t>
+    <t>60 Fahrettin|40 Sven|30 Rief</t>
+  </si>
+  <si>
+    <t>65 Fahrettin|0 Sven|15 Rief</t>
+  </si>
+  <si>
+    <t>400 Fahrettin|210 Sven|195 Rief</t>
+  </si>
+  <si>
+    <t>Development Points: 805 / 875</t>
   </si>
 </sst>
 </file>
@@ -1722,7 +1722,7 @@
   <dimension ref="A1:R593"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="J1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J36" sqref="J36"/>
+      <selection activeCell="K16" sqref="K16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1894,10 +1894,10 @@
         <v>370</v>
       </c>
       <c r="N3" s="1" t="s">
-        <v>388</v>
+        <v>386</v>
       </c>
       <c r="O3" s="1" t="s">
-        <v>389</v>
+        <v>387</v>
       </c>
       <c r="P3" s="1" t="s">
         <v>372</v>
@@ -2000,7 +2000,7 @@
         <v>231</v>
       </c>
       <c r="N5" s="23" t="s">
-        <v>386</v>
+        <v>384</v>
       </c>
       <c r="O5" s="1" t="s">
         <v>274</v>
@@ -2038,7 +2038,7 @@
         <v>230</v>
       </c>
       <c r="N6" s="23" t="s">
-        <v>387</v>
+        <v>385</v>
       </c>
       <c r="O6" s="1" t="s">
         <v>275</v>
@@ -2085,7 +2085,7 @@
         <v>242</v>
       </c>
       <c r="M7" s="23" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
       <c r="N7" s="21" t="s">
         <v>263</v>
@@ -2182,7 +2182,7 @@
         <v>244</v>
       </c>
       <c r="M9" s="23" t="s">
-        <v>384</v>
+        <v>382</v>
       </c>
       <c r="N9" s="21" t="s">
         <v>354</v>
@@ -2343,7 +2343,7 @@
         <v>135</v>
       </c>
       <c r="L13" s="23" t="s">
-        <v>381</v>
+        <v>379</v>
       </c>
       <c r="M13" s="21" t="s">
         <v>364</v>
@@ -2387,7 +2387,7 @@
         <v>248</v>
       </c>
       <c r="M14" s="23" t="s">
-        <v>385</v>
+        <v>383</v>
       </c>
       <c r="O14" s="21" t="s">
         <v>297</v>
@@ -2572,7 +2572,7 @@
         <v>362</v>
       </c>
       <c r="L21" s="23" t="s">
-        <v>382</v>
+        <v>380</v>
       </c>
     </row>
     <row r="22" spans="1:18" x14ac:dyDescent="0.25">
@@ -2682,19 +2682,19 @@
         <v>376</v>
       </c>
       <c r="N25" s="1" t="s">
-        <v>380</v>
+        <v>391</v>
       </c>
       <c r="O25" s="1" t="s">
+        <v>392</v>
+      </c>
+      <c r="P25" s="1" t="s">
+        <v>390</v>
+      </c>
+      <c r="Q25" s="1" t="s">
         <v>377</v>
       </c>
-      <c r="P25" s="1" t="s">
-        <v>392</v>
-      </c>
-      <c r="Q25" s="1" t="s">
+      <c r="R25" s="1" t="s">
         <v>378</v>
-      </c>
-      <c r="R25" s="1" t="s">
-        <v>379</v>
       </c>
     </row>
     <row r="26" spans="1:18" x14ac:dyDescent="0.25">
@@ -2956,10 +2956,10 @@
       </c>
       <c r="H32" s="19"/>
       <c r="I32" s="19"/>
-      <c r="N32" s="1" t="s">
+      <c r="N32" s="21" t="s">
         <v>267</v>
       </c>
-      <c r="O32" s="1" t="s">
+      <c r="O32" s="21" t="s">
         <v>289</v>
       </c>
       <c r="Q32" s="21" t="s">
@@ -3013,7 +3013,7 @@
       <c r="H34" s="19"/>
       <c r="I34" s="19"/>
       <c r="J34" s="22" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="N34" s="21" t="s">
         <v>269</v>
@@ -3041,14 +3041,14 @@
       <c r="H35" s="19"/>
       <c r="I35" s="19"/>
       <c r="J35" s="1" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
     </row>
     <row r="36" spans="1:18" x14ac:dyDescent="0.25">
       <c r="H36" s="19"/>
       <c r="I36" s="19"/>
       <c r="J36" s="22" t="s">
-        <v>391</v>
+        <v>389</v>
       </c>
     </row>
     <row r="37" spans="1:18" x14ac:dyDescent="0.25">
@@ -3070,7 +3070,7 @@
       <c r="H37" s="19"/>
       <c r="I37" s="19"/>
       <c r="J37" s="1" t="s">
-        <v>390</v>
+        <v>388</v>
       </c>
     </row>
     <row r="38" spans="1:18" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Asset list update & meer grassprieten voor collision
</commit_message>
<xml_diff>
--- a/Algemeen/Asset List Game-Lab 1.xlsx
+++ b/Algemeen/Asset List Game-Lab 1.xlsx
@@ -1180,15 +1180,6 @@
     <t xml:space="preserve">58 Anthony| 19 Michiel| 0 Roos </t>
   </si>
   <si>
-    <t xml:space="preserve">21 Anthony| 0 Michiel| 26 Roos </t>
-  </si>
-  <si>
-    <t xml:space="preserve">329 Anthony | 140 Michiel | 167 Roos </t>
-  </si>
-  <si>
-    <t>Artist Points Behaald: 666 / 875</t>
-  </si>
-  <si>
     <t>0 Fahrettin|25 Sven|30 Rief</t>
   </si>
   <si>
@@ -1202,6 +1193,15 @@
   </si>
   <si>
     <t>Development Points: 805 / 875</t>
+  </si>
+  <si>
+    <t xml:space="preserve">21 Anthony| 0 Michiel| 43 Roos </t>
+  </si>
+  <si>
+    <t xml:space="preserve">329 Anthony | 140 Michiel | 184 Roos </t>
+  </si>
+  <si>
+    <t>Artist Points Behaald: 683 / 875</t>
   </si>
 </sst>
 </file>
@@ -1722,7 +1722,7 @@
   <dimension ref="A1:R593"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="J1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K16" sqref="K16"/>
+      <selection activeCell="K33" sqref="K33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1897,7 +1897,7 @@
         <v>386</v>
       </c>
       <c r="O3" s="1" t="s">
-        <v>387</v>
+        <v>392</v>
       </c>
       <c r="P3" s="1" t="s">
         <v>372</v>
@@ -2002,7 +2002,7 @@
       <c r="N5" s="23" t="s">
         <v>384</v>
       </c>
-      <c r="O5" s="1" t="s">
+      <c r="O5" s="21" t="s">
         <v>274</v>
       </c>
       <c r="P5" s="1" t="s">
@@ -2682,13 +2682,13 @@
         <v>376</v>
       </c>
       <c r="N25" s="1" t="s">
-        <v>391</v>
+        <v>388</v>
       </c>
       <c r="O25" s="1" t="s">
-        <v>392</v>
+        <v>389</v>
       </c>
       <c r="P25" s="1" t="s">
-        <v>390</v>
+        <v>387</v>
       </c>
       <c r="Q25" s="1" t="s">
         <v>377</v>
@@ -3013,7 +3013,7 @@
       <c r="H34" s="19"/>
       <c r="I34" s="19"/>
       <c r="J34" s="22" t="s">
-        <v>394</v>
+        <v>391</v>
       </c>
       <c r="N34" s="21" t="s">
         <v>269</v>
@@ -3041,14 +3041,14 @@
       <c r="H35" s="19"/>
       <c r="I35" s="19"/>
       <c r="J35" s="1" t="s">
-        <v>393</v>
+        <v>390</v>
       </c>
     </row>
     <row r="36" spans="1:18" x14ac:dyDescent="0.25">
       <c r="H36" s="19"/>
       <c r="I36" s="19"/>
       <c r="J36" s="22" t="s">
-        <v>389</v>
+        <v>394</v>
       </c>
     </row>
     <row r="37" spans="1:18" x14ac:dyDescent="0.25">
@@ -3070,7 +3070,7 @@
       <c r="H37" s="19"/>
       <c r="I37" s="19"/>
       <c r="J37" s="1" t="s">
-        <v>388</v>
+        <v>393</v>
       </c>
     </row>
     <row r="38" spans="1:18" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Asset List Update 07-01-2016
</commit_message>
<xml_diff>
--- a/Algemeen/Asset List Game-Lab 1.xlsx
+++ b/Algemeen/Asset List Game-Lab 1.xlsx
@@ -847,9 +847,6 @@
     <t>Characters_CivilianAnt_5 (46)</t>
   </si>
   <si>
-    <t>Weapons_SlingShot_5 (13)</t>
-  </si>
-  <si>
     <t>Armor_BoomschorsSchild_1 (15)</t>
   </si>
   <si>
@@ -1138,9 +1135,6 @@
     <t xml:space="preserve">10 Anthony| 0 Michiel| 0 Roos </t>
   </si>
   <si>
-    <t xml:space="preserve">10 Anthony| 0 Michiel| 25 Roos </t>
-  </si>
-  <si>
     <t xml:space="preserve">12 Anthony| 0 Michiel| 0 Roos </t>
   </si>
   <si>
@@ -1192,16 +1186,22 @@
     <t>400 Fahrettin|210 Sven|195 Rief</t>
   </si>
   <si>
-    <t>Development Points: 805 / 875</t>
-  </si>
-  <si>
-    <t xml:space="preserve">21 Anthony| 0 Michiel| 43 Roos </t>
-  </si>
-  <si>
-    <t xml:space="preserve">329 Anthony | 140 Michiel | 184 Roos </t>
-  </si>
-  <si>
-    <t>Artist Points Behaald: 683 / 875</t>
+    <t>Weapons_SlingShot_5 (13) 2/5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">33 Anthony| 0 Michiel| 50 Roos </t>
+  </si>
+  <si>
+    <t xml:space="preserve">10 Anthony| 0 Michiel| 46 Roos </t>
+  </si>
+  <si>
+    <t xml:space="preserve">341 Anthony | 140 Michiel | 212 Roos </t>
+  </si>
+  <si>
+    <t>Development Points: 805 / 1000</t>
+  </si>
+  <si>
+    <t>Artist Points Behaald: 723 / 1000</t>
   </si>
 </sst>
 </file>
@@ -1722,7 +1722,7 @@
   <dimension ref="A1:R593"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="J1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K33" sqref="K33"/>
+      <selection activeCell="N20" sqref="N20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1882,31 +1882,31 @@
         <v>67</v>
       </c>
       <c r="J3" s="1" t="s">
+        <v>366</v>
+      </c>
+      <c r="K3" s="1" t="s">
         <v>367</v>
       </c>
-      <c r="K3" s="1" t="s">
+      <c r="L3" s="1" t="s">
         <v>368</v>
       </c>
-      <c r="L3" s="1" t="s">
+      <c r="M3" s="1" t="s">
         <v>369</v>
       </c>
-      <c r="M3" s="1" t="s">
-        <v>370</v>
-      </c>
       <c r="N3" s="1" t="s">
-        <v>386</v>
+        <v>384</v>
       </c>
       <c r="O3" s="1" t="s">
-        <v>392</v>
+        <v>390</v>
       </c>
       <c r="P3" s="1" t="s">
+        <v>371</v>
+      </c>
+      <c r="Q3" s="1" t="s">
+        <v>391</v>
+      </c>
+      <c r="R3" s="1" t="s">
         <v>372</v>
-      </c>
-      <c r="Q3" s="1" t="s">
-        <v>373</v>
-      </c>
-      <c r="R3" s="1" t="s">
-        <v>374</v>
       </c>
     </row>
     <row r="4" spans="1:18" x14ac:dyDescent="0.25">
@@ -1988,10 +1988,10 @@
         <v>152</v>
       </c>
       <c r="J5" s="21" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="K5" s="21" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="L5" s="21" t="s">
         <v>240</v>
@@ -2000,19 +2000,19 @@
         <v>231</v>
       </c>
       <c r="N5" s="23" t="s">
-        <v>384</v>
+        <v>382</v>
       </c>
       <c r="O5" s="21" t="s">
         <v>274</v>
       </c>
       <c r="P5" s="1" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="Q5" s="1" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="R5" s="1" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
     </row>
     <row r="6" spans="1:18" x14ac:dyDescent="0.25">
@@ -2038,19 +2038,19 @@
         <v>230</v>
       </c>
       <c r="N6" s="23" t="s">
-        <v>385</v>
+        <v>383</v>
       </c>
       <c r="O6" s="1" t="s">
         <v>275</v>
       </c>
       <c r="P6" s="1" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="Q6" s="1" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="R6" s="1" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
     </row>
     <row r="7" spans="1:18" x14ac:dyDescent="0.25">
@@ -2085,22 +2085,22 @@
         <v>242</v>
       </c>
       <c r="M7" s="23" t="s">
-        <v>381</v>
+        <v>379</v>
       </c>
       <c r="N7" s="21" t="s">
         <v>263</v>
       </c>
-      <c r="O7" s="1" t="s">
-        <v>276</v>
+      <c r="O7" s="23" t="s">
+        <v>389</v>
       </c>
       <c r="P7" s="1" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="Q7" s="1" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="R7" s="1" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
     </row>
     <row r="8" spans="1:18" x14ac:dyDescent="0.25">
@@ -2141,16 +2141,16 @@
         <v>264</v>
       </c>
       <c r="O8" s="21" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="P8" s="1" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="Q8" s="1" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="R8" s="1" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
     </row>
     <row r="9" spans="1:18" x14ac:dyDescent="0.25">
@@ -2182,22 +2182,22 @@
         <v>244</v>
       </c>
       <c r="M9" s="23" t="s">
-        <v>382</v>
+        <v>380</v>
       </c>
       <c r="N9" s="21" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="O9" s="21" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="P9" s="1" t="s">
-        <v>294</v>
-      </c>
-      <c r="Q9" s="1" t="s">
-        <v>307</v>
+        <v>293</v>
+      </c>
+      <c r="Q9" s="21" t="s">
+        <v>306</v>
       </c>
       <c r="R9" s="1" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
     </row>
     <row r="10" spans="1:18" x14ac:dyDescent="0.25">
@@ -2229,22 +2229,22 @@
         <v>245</v>
       </c>
       <c r="M10" s="21" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="N10" s="1" t="s">
         <v>265</v>
       </c>
       <c r="O10" s="21" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="P10" s="1" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="Q10" s="21" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="R10" s="1" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
     </row>
     <row r="11" spans="1:18" x14ac:dyDescent="0.25">
@@ -2258,22 +2258,22 @@
         <v>246</v>
       </c>
       <c r="M11" s="21" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="N11" s="21" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="O11" s="21" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="P11" s="1" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="Q11" s="21" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="R11" s="1" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
     </row>
     <row r="12" spans="1:18" x14ac:dyDescent="0.25">
@@ -2302,22 +2302,22 @@
         <v>247</v>
       </c>
       <c r="M12" s="21" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="N12" s="1" t="s">
-        <v>340</v>
-      </c>
-      <c r="O12" s="1" t="s">
-        <v>282</v>
+        <v>339</v>
+      </c>
+      <c r="O12" s="21" t="s">
+        <v>281</v>
       </c>
       <c r="P12" s="1" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="Q12" s="21" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="R12" s="1" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
     </row>
     <row r="13" spans="1:18" x14ac:dyDescent="0.25">
@@ -2343,22 +2343,22 @@
         <v>135</v>
       </c>
       <c r="L13" s="23" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
       <c r="M13" s="21" t="s">
-        <v>364</v>
-      </c>
-      <c r="O13" s="1" t="s">
-        <v>347</v>
+        <v>363</v>
+      </c>
+      <c r="O13" s="21" t="s">
+        <v>346</v>
       </c>
       <c r="P13" s="21" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="Q13" s="21" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="R13" s="1" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
     </row>
     <row r="14" spans="1:18" x14ac:dyDescent="0.25">
@@ -2387,19 +2387,19 @@
         <v>248</v>
       </c>
       <c r="M14" s="23" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
       <c r="O14" s="21" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="P14" s="21" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="Q14" s="1" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="R14" s="21" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
     </row>
     <row r="15" spans="1:18" x14ac:dyDescent="0.25">
@@ -2428,10 +2428,10 @@
         <v>249</v>
       </c>
       <c r="O15" s="21" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="Q15" s="21" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
     </row>
     <row r="16" spans="1:18" x14ac:dyDescent="0.25">
@@ -2442,10 +2442,10 @@
         <v>115</v>
       </c>
       <c r="L16" s="21" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="Q16" s="1" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
     </row>
     <row r="17" spans="1:18" x14ac:dyDescent="0.25">
@@ -2473,8 +2473,8 @@
       <c r="L17" s="21" t="s">
         <v>256</v>
       </c>
-      <c r="Q17" s="1" t="s">
-        <v>315</v>
+      <c r="Q17" s="21" t="s">
+        <v>314</v>
       </c>
     </row>
     <row r="18" spans="1:18" x14ac:dyDescent="0.25">
@@ -2503,7 +2503,7 @@
         <v>257</v>
       </c>
       <c r="Q18" s="1" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
     </row>
     <row r="19" spans="1:18" x14ac:dyDescent="0.25">
@@ -2526,13 +2526,13 @@
         <v>166</v>
       </c>
       <c r="I19" s="3" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="L19" s="21" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="Q19" s="1" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
     </row>
     <row r="20" spans="1:18" x14ac:dyDescent="0.25">
@@ -2555,13 +2555,13 @@
         <v>166</v>
       </c>
       <c r="I20" s="3" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="L20" s="21" t="s">
         <v>234</v>
       </c>
       <c r="Q20" s="21" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
     </row>
     <row r="21" spans="1:18" x14ac:dyDescent="0.25">
@@ -2569,10 +2569,10 @@
         <v>166</v>
       </c>
       <c r="I21" s="3" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="L21" s="23" t="s">
-        <v>380</v>
+        <v>378</v>
       </c>
     </row>
     <row r="22" spans="1:18" x14ac:dyDescent="0.25">
@@ -2595,7 +2595,7 @@
         <v>166</v>
       </c>
       <c r="I22" s="3" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="L22" s="21" t="s">
         <v>254</v>
@@ -2621,7 +2621,7 @@
         <v>166</v>
       </c>
       <c r="I23" s="3" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
     </row>
     <row r="24" spans="1:18" x14ac:dyDescent="0.25">
@@ -2644,7 +2644,7 @@
         <v>166</v>
       </c>
       <c r="I24" s="3" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
     </row>
     <row r="25" spans="1:18" x14ac:dyDescent="0.25">
@@ -2667,34 +2667,34 @@
         <v>166</v>
       </c>
       <c r="I25" s="5" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="J25" s="1" t="s">
+        <v>364</v>
+      </c>
+      <c r="K25" s="1" t="s">
         <v>365</v>
       </c>
-      <c r="K25" s="1" t="s">
-        <v>366</v>
-      </c>
       <c r="L25" s="1" t="s">
+        <v>373</v>
+      </c>
+      <c r="M25" s="1" t="s">
+        <v>374</v>
+      </c>
+      <c r="N25" s="1" t="s">
+        <v>386</v>
+      </c>
+      <c r="O25" s="1" t="s">
+        <v>387</v>
+      </c>
+      <c r="P25" s="1" t="s">
+        <v>385</v>
+      </c>
+      <c r="Q25" s="1" t="s">
         <v>375</v>
       </c>
-      <c r="M25" s="1" t="s">
+      <c r="R25" s="1" t="s">
         <v>376</v>
-      </c>
-      <c r="N25" s="1" t="s">
-        <v>388</v>
-      </c>
-      <c r="O25" s="1" t="s">
-        <v>389</v>
-      </c>
-      <c r="P25" s="1" t="s">
-        <v>387</v>
-      </c>
-      <c r="Q25" s="1" t="s">
-        <v>377</v>
-      </c>
-      <c r="R25" s="1" t="s">
-        <v>378</v>
       </c>
     </row>
     <row r="26" spans="1:18" x14ac:dyDescent="0.25">
@@ -2703,7 +2703,7 @@
         <v>166</v>
       </c>
       <c r="I26" s="5" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="J26" s="20" t="s">
         <v>222</v>
@@ -2766,16 +2766,16 @@
         <v>270</v>
       </c>
       <c r="O27" s="21" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="P27" s="1" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="Q27" s="1" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="R27" s="1" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="28" spans="1:18" x14ac:dyDescent="0.25">
@@ -2811,16 +2811,16 @@
         <v>271</v>
       </c>
       <c r="O28" s="21" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="P28" s="21" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="Q28" s="21" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="R28" s="1" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
     </row>
     <row r="29" spans="1:18" x14ac:dyDescent="0.25">
@@ -2856,16 +2856,16 @@
         <v>272</v>
       </c>
       <c r="O29" s="1" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="P29" s="21" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="Q29" s="1" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="R29" s="1" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
     </row>
     <row r="30" spans="1:18" x14ac:dyDescent="0.25">
@@ -2901,16 +2901,16 @@
         <v>273</v>
       </c>
       <c r="O30" s="1" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="P30" s="1" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="Q30" s="1" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="R30" s="1" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
     </row>
     <row r="31" spans="1:18" x14ac:dyDescent="0.25">
@@ -2926,16 +2926,16 @@
         <v>266</v>
       </c>
       <c r="O31" s="21" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="P31" s="21" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="Q31" s="1" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="R31" s="1" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
     </row>
     <row r="32" spans="1:18" x14ac:dyDescent="0.25">
@@ -2960,13 +2960,13 @@
         <v>267</v>
       </c>
       <c r="O32" s="21" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="Q32" s="21" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="R32" s="1" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
     </row>
     <row r="33" spans="1:18" x14ac:dyDescent="0.25">
@@ -2991,7 +2991,7 @@
         <v>268</v>
       </c>
       <c r="R33" s="1" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
     </row>
     <row r="34" spans="1:18" x14ac:dyDescent="0.25">
@@ -3013,13 +3013,13 @@
       <c r="H34" s="19"/>
       <c r="I34" s="19"/>
       <c r="J34" s="22" t="s">
-        <v>391</v>
+        <v>393</v>
       </c>
       <c r="N34" s="21" t="s">
         <v>269</v>
       </c>
       <c r="R34" s="1" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
     </row>
     <row r="35" spans="1:18" x14ac:dyDescent="0.25">
@@ -3041,7 +3041,7 @@
       <c r="H35" s="19"/>
       <c r="I35" s="19"/>
       <c r="J35" s="1" t="s">
-        <v>390</v>
+        <v>388</v>
       </c>
     </row>
     <row r="36" spans="1:18" x14ac:dyDescent="0.25">
@@ -3070,7 +3070,7 @@
       <c r="H37" s="19"/>
       <c r="I37" s="19"/>
       <c r="J37" s="1" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
     </row>
     <row r="38" spans="1:18" x14ac:dyDescent="0.25">
@@ -3091,7 +3091,7 @@
       </c>
       <c r="I38" s="19"/>
       <c r="J38" s="1" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
     </row>
     <row r="39" spans="1:18" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Uren Registratie Roos aangepast & tot sprint 4 alle assets imported
</commit_message>
<xml_diff>
--- a/Algemeen/Asset List Game-Lab 1.xlsx
+++ b/Algemeen/Asset List Game-Lab 1.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1548" uniqueCount="395">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1549" uniqueCount="396">
   <si>
     <t>ID Code</t>
   </si>
@@ -1202,6 +1202,9 @@
   </si>
   <si>
     <t>Artist Points Behaald: 723 / 1000</t>
+  </si>
+  <si>
+    <t xml:space="preserve">24 Fahrettin </t>
   </si>
 </sst>
 </file>
@@ -1224,14 +1227,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color rgb="FF9C0006"/>
       <name val="Calibri"/>
@@ -1241,6 +1236,13 @@
     <font>
       <sz val="11"/>
       <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -1335,8 +1337,8 @@
   <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -1393,16 +1395,16 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="12" borderId="0" xfId="2" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="0" xfId="2" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="13" borderId="0" xfId="3" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="13" borderId="0" xfId="3" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1722,7 +1724,7 @@
   <dimension ref="A1:R593"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="J1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="N20" sqref="N20"/>
+      <selection activeCell="J13" sqref="J13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1934,31 +1936,31 @@
       <c r="I4" s="3" t="s">
         <v>151</v>
       </c>
-      <c r="J4" s="20" t="s">
+      <c r="J4" s="23" t="s">
         <v>221</v>
       </c>
-      <c r="K4" s="20" t="s">
+      <c r="K4" s="23" t="s">
         <v>221</v>
       </c>
-      <c r="L4" s="20" t="s">
+      <c r="L4" s="1" t="s">
+        <v>395</v>
+      </c>
+      <c r="M4" s="21" t="s">
         <v>221</v>
       </c>
-      <c r="M4" s="20" t="s">
+      <c r="N4" s="21" t="s">
         <v>221</v>
       </c>
-      <c r="N4" s="20" t="s">
+      <c r="O4" s="21" t="s">
         <v>221</v>
       </c>
-      <c r="O4" s="20" t="s">
+      <c r="P4" s="21" t="s">
         <v>221</v>
       </c>
-      <c r="P4" s="20" t="s">
+      <c r="Q4" s="21" t="s">
         <v>221</v>
       </c>
-      <c r="Q4" s="20" t="s">
-        <v>221</v>
-      </c>
-      <c r="R4" s="20" t="s">
+      <c r="R4" s="21" t="s">
         <v>221</v>
       </c>
     </row>
@@ -1987,22 +1989,22 @@
       <c r="I5" s="3" t="s">
         <v>152</v>
       </c>
-      <c r="J5" s="21" t="s">
+      <c r="J5" s="20" t="s">
         <v>351</v>
       </c>
-      <c r="K5" s="21" t="s">
+      <c r="K5" s="20" t="s">
         <v>341</v>
       </c>
       <c r="L5" s="21" t="s">
-        <v>240</v>
-      </c>
-      <c r="M5" s="21" t="s">
+        <v>221</v>
+      </c>
+      <c r="M5" s="20" t="s">
         <v>231</v>
       </c>
-      <c r="N5" s="23" t="s">
+      <c r="N5" s="22" t="s">
         <v>382</v>
       </c>
-      <c r="O5" s="21" t="s">
+      <c r="O5" s="20" t="s">
         <v>274</v>
       </c>
       <c r="P5" s="1" t="s">
@@ -2025,19 +2027,19 @@
       <c r="I6" s="3" t="s">
         <v>73</v>
       </c>
-      <c r="J6" s="21" t="s">
+      <c r="J6" s="20" t="s">
         <v>229</v>
       </c>
-      <c r="K6" s="21" t="s">
+      <c r="K6" s="20" t="s">
         <v>250</v>
       </c>
-      <c r="L6" s="21" t="s">
-        <v>241</v>
-      </c>
-      <c r="M6" s="21" t="s">
+      <c r="L6" s="20" t="s">
+        <v>240</v>
+      </c>
+      <c r="M6" s="20" t="s">
         <v>230</v>
       </c>
-      <c r="N6" s="23" t="s">
+      <c r="N6" s="22" t="s">
         <v>383</v>
       </c>
       <c r="O6" s="1" t="s">
@@ -2078,19 +2080,19 @@
       <c r="I7" s="3" t="s">
         <v>75</v>
       </c>
-      <c r="J7" s="21" t="s">
+      <c r="J7" s="20" t="s">
         <v>232</v>
       </c>
-      <c r="L7" s="21" t="s">
-        <v>242</v>
-      </c>
-      <c r="M7" s="23" t="s">
+      <c r="L7" s="20" t="s">
+        <v>241</v>
+      </c>
+      <c r="M7" s="22" t="s">
         <v>379</v>
       </c>
-      <c r="N7" s="21" t="s">
+      <c r="N7" s="20" t="s">
         <v>263</v>
       </c>
-      <c r="O7" s="23" t="s">
+      <c r="O7" s="22" t="s">
         <v>389</v>
       </c>
       <c r="P7" s="1" t="s">
@@ -2128,19 +2130,19 @@
       <c r="I8" s="3" t="s">
         <v>150</v>
       </c>
-      <c r="J8" s="21" t="s">
+      <c r="J8" s="20" t="s">
         <v>233</v>
       </c>
-      <c r="L8" s="21" t="s">
-        <v>243</v>
-      </c>
-      <c r="M8" s="21" t="s">
+      <c r="L8" s="20" t="s">
+        <v>242</v>
+      </c>
+      <c r="M8" s="20" t="s">
         <v>255</v>
       </c>
       <c r="N8" s="1" t="s">
         <v>264</v>
       </c>
-      <c r="O8" s="21" t="s">
+      <c r="O8" s="20" t="s">
         <v>276</v>
       </c>
       <c r="P8" s="1" t="s">
@@ -2178,22 +2180,22 @@
       <c r="I9" s="3" t="s">
         <v>134</v>
       </c>
-      <c r="L9" s="21" t="s">
-        <v>244</v>
-      </c>
-      <c r="M9" s="23" t="s">
+      <c r="L9" s="20" t="s">
+        <v>243</v>
+      </c>
+      <c r="M9" s="22" t="s">
         <v>380</v>
       </c>
-      <c r="N9" s="21" t="s">
+      <c r="N9" s="20" t="s">
         <v>353</v>
       </c>
-      <c r="O9" s="21" t="s">
+      <c r="O9" s="20" t="s">
         <v>277</v>
       </c>
       <c r="P9" s="1" t="s">
         <v>293</v>
       </c>
-      <c r="Q9" s="21" t="s">
+      <c r="Q9" s="20" t="s">
         <v>306</v>
       </c>
       <c r="R9" s="1" t="s">
@@ -2225,22 +2227,22 @@
       <c r="I10" s="3" t="s">
         <v>84</v>
       </c>
-      <c r="L10" s="21" t="s">
-        <v>245</v>
-      </c>
-      <c r="M10" s="21" t="s">
+      <c r="L10" s="20" t="s">
+        <v>244</v>
+      </c>
+      <c r="M10" s="20" t="s">
         <v>350</v>
       </c>
       <c r="N10" s="1" t="s">
         <v>265</v>
       </c>
-      <c r="O10" s="21" t="s">
+      <c r="O10" s="20" t="s">
         <v>278</v>
       </c>
       <c r="P10" s="1" t="s">
         <v>294</v>
       </c>
-      <c r="Q10" s="21" t="s">
+      <c r="Q10" s="20" t="s">
         <v>307</v>
       </c>
       <c r="R10" s="1" t="s">
@@ -2254,22 +2256,22 @@
       <c r="I11" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="L11" s="21" t="s">
-        <v>246</v>
-      </c>
-      <c r="M11" s="21" t="s">
+      <c r="L11" s="20" t="s">
+        <v>245</v>
+      </c>
+      <c r="M11" s="20" t="s">
         <v>338</v>
       </c>
-      <c r="N11" s="21" t="s">
+      <c r="N11" s="20" t="s">
         <v>282</v>
       </c>
-      <c r="O11" s="21" t="s">
+      <c r="O11" s="20" t="s">
         <v>279</v>
       </c>
       <c r="P11" s="1" t="s">
         <v>295</v>
       </c>
-      <c r="Q11" s="21" t="s">
+      <c r="Q11" s="20" t="s">
         <v>308</v>
       </c>
       <c r="R11" s="1" t="s">
@@ -2298,22 +2300,22 @@
       <c r="I12" s="3" t="s">
         <v>95</v>
       </c>
-      <c r="L12" s="21" t="s">
-        <v>247</v>
-      </c>
-      <c r="M12" s="21" t="s">
+      <c r="L12" s="20" t="s">
+        <v>246</v>
+      </c>
+      <c r="M12" s="20" t="s">
         <v>335</v>
       </c>
       <c r="N12" s="1" t="s">
         <v>339</v>
       </c>
-      <c r="O12" s="21" t="s">
+      <c r="O12" s="20" t="s">
         <v>281</v>
       </c>
       <c r="P12" s="1" t="s">
         <v>280</v>
       </c>
-      <c r="Q12" s="21" t="s">
+      <c r="Q12" s="20" t="s">
         <v>309</v>
       </c>
       <c r="R12" s="1" t="s">
@@ -2342,19 +2344,19 @@
       <c r="I13" s="3" t="s">
         <v>135</v>
       </c>
-      <c r="L13" s="23" t="s">
-        <v>377</v>
-      </c>
-      <c r="M13" s="21" t="s">
+      <c r="L13" s="20" t="s">
+        <v>247</v>
+      </c>
+      <c r="M13" s="20" t="s">
         <v>363</v>
       </c>
-      <c r="O13" s="21" t="s">
+      <c r="O13" s="20" t="s">
         <v>346</v>
       </c>
-      <c r="P13" s="21" t="s">
+      <c r="P13" s="20" t="s">
         <v>317</v>
       </c>
-      <c r="Q13" s="21" t="s">
+      <c r="Q13" s="20" t="s">
         <v>310</v>
       </c>
       <c r="R13" s="1" t="s">
@@ -2383,22 +2385,22 @@
       <c r="I14" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="L14" s="21" t="s">
-        <v>248</v>
-      </c>
-      <c r="M14" s="23" t="s">
+      <c r="L14" s="22" t="s">
+        <v>377</v>
+      </c>
+      <c r="M14" s="22" t="s">
         <v>381</v>
       </c>
-      <c r="O14" s="21" t="s">
+      <c r="O14" s="20" t="s">
         <v>296</v>
       </c>
-      <c r="P14" s="21" t="s">
+      <c r="P14" s="20" t="s">
         <v>348</v>
       </c>
       <c r="Q14" s="1" t="s">
         <v>311</v>
       </c>
-      <c r="R14" s="21" t="s">
+      <c r="R14" s="20" t="s">
         <v>342</v>
       </c>
     </row>
@@ -2424,13 +2426,13 @@
       <c r="I15" s="3" t="s">
         <v>105</v>
       </c>
-      <c r="L15" s="21" t="s">
-        <v>249</v>
-      </c>
-      <c r="O15" s="21" t="s">
+      <c r="L15" s="20" t="s">
+        <v>248</v>
+      </c>
+      <c r="O15" s="20" t="s">
         <v>349</v>
       </c>
-      <c r="Q15" s="21" t="s">
+      <c r="Q15" s="20" t="s">
         <v>312</v>
       </c>
     </row>
@@ -2441,8 +2443,8 @@
       <c r="I16" s="3" t="s">
         <v>115</v>
       </c>
-      <c r="L16" s="21" t="s">
-        <v>352</v>
+      <c r="L16" s="20" t="s">
+        <v>249</v>
       </c>
       <c r="Q16" s="1" t="s">
         <v>313</v>
@@ -2470,10 +2472,10 @@
       <c r="I17" s="3" t="s">
         <v>137</v>
       </c>
-      <c r="L17" s="21" t="s">
-        <v>256</v>
-      </c>
-      <c r="Q17" s="21" t="s">
+      <c r="L17" s="20" t="s">
+        <v>352</v>
+      </c>
+      <c r="Q17" s="20" t="s">
         <v>314</v>
       </c>
     </row>
@@ -2499,8 +2501,8 @@
       <c r="I18" s="3" t="s">
         <v>136</v>
       </c>
-      <c r="L18" s="21" t="s">
-        <v>257</v>
+      <c r="L18" s="20" t="s">
+        <v>256</v>
       </c>
       <c r="Q18" s="1" t="s">
         <v>315</v>
@@ -2528,8 +2530,8 @@
       <c r="I19" s="3" t="s">
         <v>355</v>
       </c>
-      <c r="L19" s="21" t="s">
-        <v>345</v>
+      <c r="L19" s="20" t="s">
+        <v>257</v>
       </c>
       <c r="Q19" s="1" t="s">
         <v>316</v>
@@ -2557,10 +2559,10 @@
       <c r="I20" s="3" t="s">
         <v>356</v>
       </c>
-      <c r="L20" s="21" t="s">
-        <v>234</v>
-      </c>
-      <c r="Q20" s="21" t="s">
+      <c r="L20" s="20" t="s">
+        <v>345</v>
+      </c>
+      <c r="Q20" s="20" t="s">
         <v>347</v>
       </c>
     </row>
@@ -2571,8 +2573,8 @@
       <c r="I21" s="3" t="s">
         <v>361</v>
       </c>
-      <c r="L21" s="23" t="s">
-        <v>378</v>
+      <c r="L21" s="20" t="s">
+        <v>234</v>
       </c>
     </row>
     <row r="22" spans="1:18" x14ac:dyDescent="0.25">
@@ -2597,8 +2599,8 @@
       <c r="I22" s="3" t="s">
         <v>362</v>
       </c>
-      <c r="L22" s="21" t="s">
-        <v>254</v>
+      <c r="L22" s="22" t="s">
+        <v>378</v>
       </c>
     </row>
     <row r="23" spans="1:18" x14ac:dyDescent="0.25">
@@ -2623,6 +2625,9 @@
       <c r="I23" s="3" t="s">
         <v>357</v>
       </c>
+      <c r="L23" s="20" t="s">
+        <v>254</v>
+      </c>
     </row>
     <row r="24" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A24" s="5" t="s">
@@ -2668,33 +2673,6 @@
       </c>
       <c r="I25" s="5" t="s">
         <v>359</v>
-      </c>
-      <c r="J25" s="1" t="s">
-        <v>364</v>
-      </c>
-      <c r="K25" s="1" t="s">
-        <v>365</v>
-      </c>
-      <c r="L25" s="1" t="s">
-        <v>373</v>
-      </c>
-      <c r="M25" s="1" t="s">
-        <v>374</v>
-      </c>
-      <c r="N25" s="1" t="s">
-        <v>386</v>
-      </c>
-      <c r="O25" s="1" t="s">
-        <v>387</v>
-      </c>
-      <c r="P25" s="1" t="s">
-        <v>385</v>
-      </c>
-      <c r="Q25" s="1" t="s">
-        <v>375</v>
-      </c>
-      <c r="R25" s="1" t="s">
-        <v>376</v>
       </c>
     </row>
     <row r="26" spans="1:18" x14ac:dyDescent="0.25">
@@ -2705,32 +2683,32 @@
       <c r="I26" s="5" t="s">
         <v>360</v>
       </c>
-      <c r="J26" s="20" t="s">
-        <v>222</v>
-      </c>
-      <c r="K26" s="20" t="s">
-        <v>222</v>
-      </c>
-      <c r="L26" s="20" t="s">
-        <v>222</v>
-      </c>
-      <c r="M26" s="20" t="s">
-        <v>222</v>
-      </c>
-      <c r="N26" s="20" t="s">
-        <v>222</v>
-      </c>
-      <c r="O26" s="20" t="s">
-        <v>222</v>
-      </c>
-      <c r="P26" s="20" t="s">
-        <v>222</v>
-      </c>
-      <c r="Q26" s="20" t="s">
-        <v>222</v>
-      </c>
-      <c r="R26" s="20" t="s">
-        <v>222</v>
+      <c r="J26" s="1" t="s">
+        <v>364</v>
+      </c>
+      <c r="K26" s="1" t="s">
+        <v>365</v>
+      </c>
+      <c r="L26" s="1" t="s">
+        <v>373</v>
+      </c>
+      <c r="M26" s="1" t="s">
+        <v>374</v>
+      </c>
+      <c r="N26" s="1" t="s">
+        <v>386</v>
+      </c>
+      <c r="O26" s="1" t="s">
+        <v>387</v>
+      </c>
+      <c r="P26" s="1" t="s">
+        <v>385</v>
+      </c>
+      <c r="Q26" s="1" t="s">
+        <v>375</v>
+      </c>
+      <c r="R26" s="1" t="s">
+        <v>376</v>
       </c>
     </row>
     <row r="27" spans="1:18" x14ac:dyDescent="0.25">
@@ -2750,32 +2728,32 @@
         <v>3</v>
       </c>
       <c r="I27" s="19"/>
-      <c r="J27" s="21" t="s">
-        <v>224</v>
-      </c>
-      <c r="K27" s="21" t="s">
-        <v>236</v>
+      <c r="J27" s="23" t="s">
+        <v>222</v>
+      </c>
+      <c r="K27" s="23" t="s">
+        <v>222</v>
       </c>
       <c r="L27" s="21" t="s">
-        <v>235</v>
+        <v>222</v>
       </c>
       <c r="M27" s="21" t="s">
-        <v>258</v>
+        <v>222</v>
       </c>
       <c r="N27" s="21" t="s">
-        <v>270</v>
+        <v>222</v>
       </c>
       <c r="O27" s="21" t="s">
-        <v>283</v>
-      </c>
-      <c r="P27" s="1" t="s">
-        <v>301</v>
-      </c>
-      <c r="Q27" s="1" t="s">
-        <v>318</v>
-      </c>
-      <c r="R27" s="1" t="s">
-        <v>324</v>
+        <v>222</v>
+      </c>
+      <c r="P27" s="21" t="s">
+        <v>222</v>
+      </c>
+      <c r="Q27" s="21" t="s">
+        <v>222</v>
+      </c>
+      <c r="R27" s="21" t="s">
+        <v>222</v>
       </c>
     </row>
     <row r="28" spans="1:18" x14ac:dyDescent="0.25">
@@ -2795,32 +2773,32 @@
         <v>3</v>
       </c>
       <c r="I28" s="19"/>
-      <c r="J28" s="21" t="s">
-        <v>225</v>
-      </c>
-      <c r="K28" s="21" t="s">
-        <v>237</v>
-      </c>
-      <c r="L28" s="21" t="s">
-        <v>252</v>
-      </c>
-      <c r="M28" s="21" t="s">
-        <v>259</v>
-      </c>
-      <c r="N28" s="21" t="s">
-        <v>271</v>
-      </c>
-      <c r="O28" s="21" t="s">
-        <v>284</v>
-      </c>
-      <c r="P28" s="21" t="s">
-        <v>298</v>
-      </c>
-      <c r="Q28" s="21" t="s">
-        <v>319</v>
+      <c r="J28" s="20" t="s">
+        <v>224</v>
+      </c>
+      <c r="K28" s="20" t="s">
+        <v>236</v>
+      </c>
+      <c r="L28" s="20" t="s">
+        <v>235</v>
+      </c>
+      <c r="M28" s="20" t="s">
+        <v>258</v>
+      </c>
+      <c r="N28" s="20" t="s">
+        <v>270</v>
+      </c>
+      <c r="O28" s="20" t="s">
+        <v>283</v>
+      </c>
+      <c r="P28" s="1" t="s">
+        <v>301</v>
+      </c>
+      <c r="Q28" s="1" t="s">
+        <v>318</v>
       </c>
       <c r="R28" s="1" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="29" spans="1:18" x14ac:dyDescent="0.25">
@@ -2840,32 +2818,32 @@
         <v>3</v>
       </c>
       <c r="I29" s="19"/>
-      <c r="J29" s="21" t="s">
-        <v>226</v>
-      </c>
-      <c r="K29" s="21" t="s">
-        <v>238</v>
-      </c>
-      <c r="L29" s="21" t="s">
-        <v>253</v>
-      </c>
-      <c r="M29" s="21" t="s">
-        <v>260</v>
-      </c>
-      <c r="N29" s="21" t="s">
-        <v>272</v>
-      </c>
-      <c r="O29" s="1" t="s">
-        <v>285</v>
-      </c>
-      <c r="P29" s="21" t="s">
-        <v>299</v>
-      </c>
-      <c r="Q29" s="1" t="s">
-        <v>320</v>
+      <c r="J29" s="20" t="s">
+        <v>225</v>
+      </c>
+      <c r="K29" s="20" t="s">
+        <v>237</v>
+      </c>
+      <c r="L29" s="20" t="s">
+        <v>252</v>
+      </c>
+      <c r="M29" s="20" t="s">
+        <v>259</v>
+      </c>
+      <c r="N29" s="20" t="s">
+        <v>271</v>
+      </c>
+      <c r="O29" s="20" t="s">
+        <v>284</v>
+      </c>
+      <c r="P29" s="20" t="s">
+        <v>298</v>
+      </c>
+      <c r="Q29" s="20" t="s">
+        <v>319</v>
       </c>
       <c r="R29" s="1" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
     </row>
     <row r="30" spans="1:18" x14ac:dyDescent="0.25">
@@ -2885,57 +2863,63 @@
         <v>3</v>
       </c>
       <c r="I30" s="19"/>
-      <c r="J30" s="21" t="s">
-        <v>227</v>
-      </c>
-      <c r="K30" s="21" t="s">
-        <v>239</v>
-      </c>
-      <c r="L30" s="21" t="s">
-        <v>251</v>
-      </c>
-      <c r="M30" s="21" t="s">
-        <v>261</v>
-      </c>
-      <c r="N30" s="21" t="s">
-        <v>273</v>
+      <c r="J30" s="20" t="s">
+        <v>226</v>
+      </c>
+      <c r="K30" s="20" t="s">
+        <v>238</v>
+      </c>
+      <c r="L30" s="20" t="s">
+        <v>253</v>
+      </c>
+      <c r="M30" s="20" t="s">
+        <v>260</v>
+      </c>
+      <c r="N30" s="20" t="s">
+        <v>272</v>
       </c>
       <c r="O30" s="1" t="s">
-        <v>286</v>
-      </c>
-      <c r="P30" s="1" t="s">
-        <v>297</v>
+        <v>285</v>
+      </c>
+      <c r="P30" s="20" t="s">
+        <v>299</v>
       </c>
       <c r="Q30" s="1" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="R30" s="1" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
     </row>
     <row r="31" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B31" s="16"/>
       <c r="I31" s="19"/>
-      <c r="J31" s="21" t="s">
-        <v>228</v>
-      </c>
-      <c r="M31" s="21" t="s">
-        <v>262</v>
-      </c>
-      <c r="N31" s="21" t="s">
-        <v>266</v>
-      </c>
-      <c r="O31" s="21" t="s">
-        <v>287</v>
-      </c>
-      <c r="P31" s="21" t="s">
-        <v>300</v>
+      <c r="J31" s="20" t="s">
+        <v>227</v>
+      </c>
+      <c r="K31" s="20" t="s">
+        <v>239</v>
+      </c>
+      <c r="L31" s="20" t="s">
+        <v>251</v>
+      </c>
+      <c r="M31" s="20" t="s">
+        <v>261</v>
+      </c>
+      <c r="N31" s="20" t="s">
+        <v>273</v>
+      </c>
+      <c r="O31" s="1" t="s">
+        <v>286</v>
+      </c>
+      <c r="P31" s="1" t="s">
+        <v>297</v>
       </c>
       <c r="Q31" s="1" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="R31" s="1" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
     </row>
     <row r="32" spans="1:18" x14ac:dyDescent="0.25">
@@ -2956,17 +2940,26 @@
       </c>
       <c r="H32" s="19"/>
       <c r="I32" s="19"/>
-      <c r="N32" s="21" t="s">
-        <v>267</v>
-      </c>
-      <c r="O32" s="21" t="s">
-        <v>288</v>
-      </c>
-      <c r="Q32" s="21" t="s">
-        <v>323</v>
+      <c r="J32" s="20" t="s">
+        <v>228</v>
+      </c>
+      <c r="M32" s="20" t="s">
+        <v>262</v>
+      </c>
+      <c r="N32" s="20" t="s">
+        <v>266</v>
+      </c>
+      <c r="O32" s="20" t="s">
+        <v>287</v>
+      </c>
+      <c r="P32" s="20" t="s">
+        <v>300</v>
+      </c>
+      <c r="Q32" s="1" t="s">
+        <v>322</v>
       </c>
       <c r="R32" s="1" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
     </row>
     <row r="33" spans="1:18" x14ac:dyDescent="0.25">
@@ -2987,11 +2980,17 @@
       </c>
       <c r="H33" s="19"/>
       <c r="I33" s="19"/>
-      <c r="N33" s="21" t="s">
-        <v>268</v>
+      <c r="N33" s="20" t="s">
+        <v>267</v>
+      </c>
+      <c r="O33" s="20" t="s">
+        <v>288</v>
+      </c>
+      <c r="Q33" s="20" t="s">
+        <v>323</v>
       </c>
       <c r="R33" s="1" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
     </row>
     <row r="34" spans="1:18" x14ac:dyDescent="0.25">
@@ -3012,14 +3011,11 @@
       </c>
       <c r="H34" s="19"/>
       <c r="I34" s="19"/>
-      <c r="J34" s="22" t="s">
-        <v>393</v>
-      </c>
-      <c r="N34" s="21" t="s">
-        <v>269</v>
+      <c r="N34" s="20" t="s">
+        <v>268</v>
       </c>
       <c r="R34" s="1" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
     </row>
     <row r="35" spans="1:18" x14ac:dyDescent="0.25">
@@ -3040,15 +3036,21 @@
       </c>
       <c r="H35" s="19"/>
       <c r="I35" s="19"/>
-      <c r="J35" s="1" t="s">
-        <v>388</v>
+      <c r="J35" s="21" t="s">
+        <v>393</v>
+      </c>
+      <c r="N35" s="20" t="s">
+        <v>269</v>
+      </c>
+      <c r="R35" s="1" t="s">
+        <v>331</v>
       </c>
     </row>
     <row r="36" spans="1:18" x14ac:dyDescent="0.25">
       <c r="H36" s="19"/>
       <c r="I36" s="19"/>
-      <c r="J36" s="22" t="s">
-        <v>394</v>
+      <c r="J36" s="1" t="s">
+        <v>388</v>
       </c>
     </row>
     <row r="37" spans="1:18" x14ac:dyDescent="0.25">
@@ -3069,8 +3071,8 @@
       </c>
       <c r="H37" s="19"/>
       <c r="I37" s="19"/>
-      <c r="J37" s="1" t="s">
-        <v>392</v>
+      <c r="J37" s="21" t="s">
+        <v>394</v>
       </c>
     </row>
     <row r="38" spans="1:18" x14ac:dyDescent="0.25">
@@ -3091,7 +3093,7 @@
       </c>
       <c r="I38" s="19"/>
       <c r="J38" s="1" t="s">
-        <v>370</v>
+        <v>392</v>
       </c>
     </row>
     <row r="39" spans="1:18" x14ac:dyDescent="0.25">
@@ -3111,6 +3113,9 @@
         <v>4</v>
       </c>
       <c r="I39" s="19"/>
+      <c r="J39" s="1" t="s">
+        <v>370</v>
+      </c>
     </row>
     <row r="40" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A40" s="5" t="s">

</xml_diff>

<commit_message>
11-01-2016 Uren Registratie & Update Asset List & Import Assets & Schuur in Tutorial Level
</commit_message>
<xml_diff>
--- a/Algemeen/Asset List Game-Lab 1.xlsx
+++ b/Algemeen/Asset List Game-Lab 1.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1549" uniqueCount="396">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1550" uniqueCount="397">
   <si>
     <t>ID Code</t>
   </si>
@@ -1205,6 +1205,9 @@
   </si>
   <si>
     <t xml:space="preserve">24 Fahrettin </t>
+  </si>
+  <si>
+    <t xml:space="preserve">3 Fahrettin </t>
   </si>
 </sst>
 </file>
@@ -1724,7 +1727,7 @@
   <dimension ref="A1:R593"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="J1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J13" sqref="J13"/>
+      <selection activeCell="O18" sqref="O18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1948,8 +1951,8 @@
       <c r="M4" s="21" t="s">
         <v>221</v>
       </c>
-      <c r="N4" s="21" t="s">
-        <v>221</v>
+      <c r="N4" s="1" t="s">
+        <v>396</v>
       </c>
       <c r="O4" s="21" t="s">
         <v>221</v>
@@ -2001,8 +2004,8 @@
       <c r="M5" s="20" t="s">
         <v>231</v>
       </c>
-      <c r="N5" s="22" t="s">
-        <v>382</v>
+      <c r="N5" s="21" t="s">
+        <v>221</v>
       </c>
       <c r="O5" s="20" t="s">
         <v>274</v>
@@ -2040,7 +2043,7 @@
         <v>230</v>
       </c>
       <c r="N6" s="22" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="O6" s="1" t="s">
         <v>275</v>
@@ -2089,10 +2092,10 @@
       <c r="M7" s="22" t="s">
         <v>379</v>
       </c>
-      <c r="N7" s="20" t="s">
-        <v>263</v>
-      </c>
-      <c r="O7" s="22" t="s">
+      <c r="N7" s="22" t="s">
+        <v>383</v>
+      </c>
+      <c r="O7" s="20" t="s">
         <v>389</v>
       </c>
       <c r="P7" s="1" t="s">
@@ -2139,8 +2142,8 @@
       <c r="M8" s="20" t="s">
         <v>255</v>
       </c>
-      <c r="N8" s="1" t="s">
-        <v>264</v>
+      <c r="N8" s="20" t="s">
+        <v>263</v>
       </c>
       <c r="O8" s="20" t="s">
         <v>276</v>
@@ -2186,8 +2189,8 @@
       <c r="M9" s="22" t="s">
         <v>380</v>
       </c>
-      <c r="N9" s="20" t="s">
-        <v>353</v>
+      <c r="N9" s="1" t="s">
+        <v>264</v>
       </c>
       <c r="O9" s="20" t="s">
         <v>277</v>
@@ -2233,8 +2236,8 @@
       <c r="M10" s="20" t="s">
         <v>350</v>
       </c>
-      <c r="N10" s="1" t="s">
-        <v>265</v>
+      <c r="N10" s="20" t="s">
+        <v>353</v>
       </c>
       <c r="O10" s="20" t="s">
         <v>278</v>
@@ -2262,8 +2265,8 @@
       <c r="M11" s="20" t="s">
         <v>338</v>
       </c>
-      <c r="N11" s="20" t="s">
-        <v>282</v>
+      <c r="N11" s="1" t="s">
+        <v>265</v>
       </c>
       <c r="O11" s="20" t="s">
         <v>279</v>
@@ -2306,8 +2309,8 @@
       <c r="M12" s="20" t="s">
         <v>335</v>
       </c>
-      <c r="N12" s="1" t="s">
-        <v>339</v>
+      <c r="N12" s="20" t="s">
+        <v>282</v>
       </c>
       <c r="O12" s="20" t="s">
         <v>281</v>
@@ -2349,6 +2352,9 @@
       </c>
       <c r="M13" s="20" t="s">
         <v>363</v>
+      </c>
+      <c r="N13" s="20" t="s">
+        <v>339</v>
       </c>
       <c r="O13" s="20" t="s">
         <v>346</v>
@@ -2734,13 +2740,13 @@
       <c r="K27" s="23" t="s">
         <v>222</v>
       </c>
-      <c r="L27" s="21" t="s">
+      <c r="L27" s="23" t="s">
         <v>222</v>
       </c>
-      <c r="M27" s="21" t="s">
+      <c r="M27" s="23" t="s">
         <v>222</v>
       </c>
-      <c r="N27" s="21" t="s">
+      <c r="N27" s="23" t="s">
         <v>222</v>
       </c>
       <c r="O27" s="21" t="s">

</xml_diff>

<commit_message>
Asset List Update & Import Alle Assets die tot nu toe af zijn
</commit_message>
<xml_diff>
--- a/Algemeen/Asset List Game-Lab 1.xlsx
+++ b/Algemeen/Asset List Game-Lab 1.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1550" uniqueCount="397">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1551" uniqueCount="397">
   <si>
     <t>ID Code</t>
   </si>
@@ -844,9 +844,6 @@
     <t>Building_FightPit_4 (17)</t>
   </si>
   <si>
-    <t>Characters_CivilianAnt_5 (46)</t>
-  </si>
-  <si>
     <t>Armor_BoomschorsSchild_1 (15)</t>
   </si>
   <si>
@@ -1132,12 +1129,6 @@
     <t xml:space="preserve">30 Fahrettin </t>
   </si>
   <si>
-    <t xml:space="preserve">10 Anthony| 0 Michiel| 0 Roos </t>
-  </si>
-  <si>
-    <t xml:space="preserve">12 Anthony| 0 Michiel| 0 Roos </t>
-  </si>
-  <si>
     <t>85 Fahrettin|0 Sven|75 Rief</t>
   </si>
   <si>
@@ -1174,40 +1165,49 @@
     <t xml:space="preserve">58 Anthony| 19 Michiel| 0 Roos </t>
   </si>
   <si>
-    <t>0 Fahrettin|25 Sven|30 Rief</t>
-  </si>
-  <si>
     <t>60 Fahrettin|40 Sven|30 Rief</t>
   </si>
   <si>
     <t>65 Fahrettin|0 Sven|15 Rief</t>
   </si>
   <si>
-    <t>400 Fahrettin|210 Sven|195 Rief</t>
-  </si>
-  <si>
     <t>Weapons_SlingShot_5 (13) 2/5</t>
   </si>
   <si>
-    <t xml:space="preserve">33 Anthony| 0 Michiel| 50 Roos </t>
-  </si>
-  <si>
-    <t xml:space="preserve">10 Anthony| 0 Michiel| 46 Roos </t>
-  </si>
-  <si>
-    <t xml:space="preserve">341 Anthony | 140 Michiel | 212 Roos </t>
-  </si>
-  <si>
-    <t>Development Points: 805 / 1000</t>
-  </si>
-  <si>
-    <t>Artist Points Behaald: 723 / 1000</t>
-  </si>
-  <si>
     <t xml:space="preserve">24 Fahrettin </t>
   </si>
   <si>
     <t xml:space="preserve">3 Fahrettin </t>
+  </si>
+  <si>
+    <t>0 Fahrettin|65 Sven|30 Rief</t>
+  </si>
+  <si>
+    <t>Characters_CivilianAnt_5 (46) 2/8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">52 Anthony| 0 Michiel| 50 Roos </t>
+  </si>
+  <si>
+    <t xml:space="preserve">10 Anthony| 0 Michiel| 27 Roos </t>
+  </si>
+  <si>
+    <t>400 Fahrettin|250 Sven|195 Rief</t>
+  </si>
+  <si>
+    <t>Development Points: 845 / 1125</t>
+  </si>
+  <si>
+    <t xml:space="preserve">12 Anthony| 0 Michiel| 7 Roos </t>
+  </si>
+  <si>
+    <t xml:space="preserve">10 Anthony| 0 Michiel| 57 Roos </t>
+  </si>
+  <si>
+    <t xml:space="preserve">360 Anthony | 140 Michiel | 257 Roos </t>
+  </si>
+  <si>
+    <t>Artist Points Behaald: 787 / 1125</t>
   </si>
 </sst>
 </file>
@@ -1727,7 +1727,7 @@
   <dimension ref="A1:R593"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="J1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="O18" sqref="O18"/>
+      <selection activeCell="N23" sqref="N23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1887,31 +1887,31 @@
         <v>67</v>
       </c>
       <c r="J3" s="1" t="s">
+        <v>365</v>
+      </c>
+      <c r="K3" s="1" t="s">
         <v>366</v>
       </c>
-      <c r="K3" s="1" t="s">
+      <c r="L3" s="1" t="s">
         <v>367</v>
       </c>
-      <c r="L3" s="1" t="s">
+      <c r="M3" s="1" t="s">
         <v>368</v>
       </c>
-      <c r="M3" s="1" t="s">
-        <v>369</v>
-      </c>
       <c r="N3" s="1" t="s">
-        <v>384</v>
+        <v>381</v>
       </c>
       <c r="O3" s="1" t="s">
+        <v>389</v>
+      </c>
+      <c r="P3" s="1" t="s">
         <v>390</v>
       </c>
-      <c r="P3" s="1" t="s">
-        <v>371</v>
-      </c>
       <c r="Q3" s="1" t="s">
-        <v>391</v>
+        <v>394</v>
       </c>
       <c r="R3" s="1" t="s">
-        <v>372</v>
+        <v>393</v>
       </c>
     </row>
     <row r="4" spans="1:18" x14ac:dyDescent="0.25">
@@ -1946,19 +1946,19 @@
         <v>221</v>
       </c>
       <c r="L4" s="1" t="s">
-        <v>395</v>
+        <v>385</v>
       </c>
       <c r="M4" s="21" t="s">
         <v>221</v>
       </c>
       <c r="N4" s="1" t="s">
-        <v>396</v>
+        <v>386</v>
       </c>
       <c r="O4" s="21" t="s">
         <v>221</v>
       </c>
-      <c r="P4" s="21" t="s">
-        <v>221</v>
+      <c r="P4" s="1" t="s">
+        <v>386</v>
       </c>
       <c r="Q4" s="21" t="s">
         <v>221</v>
@@ -1993,10 +1993,10 @@
         <v>152</v>
       </c>
       <c r="J5" s="20" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="K5" s="20" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="L5" s="21" t="s">
         <v>221</v>
@@ -2010,14 +2010,14 @@
       <c r="O5" s="20" t="s">
         <v>274</v>
       </c>
-      <c r="P5" s="1" t="s">
-        <v>289</v>
+      <c r="P5" s="21" t="s">
+        <v>221</v>
       </c>
       <c r="Q5" s="1" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="R5" s="1" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
     </row>
     <row r="6" spans="1:18" x14ac:dyDescent="0.25">
@@ -2043,19 +2043,19 @@
         <v>230</v>
       </c>
       <c r="N6" s="22" t="s">
-        <v>382</v>
-      </c>
-      <c r="O6" s="1" t="s">
-        <v>275</v>
+        <v>379</v>
+      </c>
+      <c r="O6" s="22" t="s">
+        <v>388</v>
       </c>
       <c r="P6" s="1" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="Q6" s="1" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="R6" s="1" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
     </row>
     <row r="7" spans="1:18" x14ac:dyDescent="0.25">
@@ -2090,22 +2090,22 @@
         <v>241</v>
       </c>
       <c r="M7" s="22" t="s">
-        <v>379</v>
+        <v>376</v>
       </c>
       <c r="N7" s="22" t="s">
-        <v>383</v>
+        <v>380</v>
       </c>
       <c r="O7" s="20" t="s">
-        <v>389</v>
+        <v>384</v>
       </c>
       <c r="P7" s="1" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="Q7" s="1" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="R7" s="1" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
     </row>
     <row r="8" spans="1:18" x14ac:dyDescent="0.25">
@@ -2146,16 +2146,16 @@
         <v>263</v>
       </c>
       <c r="O8" s="20" t="s">
-        <v>276</v>
-      </c>
-      <c r="P8" s="1" t="s">
-        <v>292</v>
+        <v>275</v>
+      </c>
+      <c r="P8" s="20" t="s">
+        <v>290</v>
       </c>
       <c r="Q8" s="1" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="R8" s="1" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
     </row>
     <row r="9" spans="1:18" x14ac:dyDescent="0.25">
@@ -2187,22 +2187,22 @@
         <v>243</v>
       </c>
       <c r="M9" s="22" t="s">
-        <v>380</v>
+        <v>377</v>
       </c>
       <c r="N9" s="1" t="s">
         <v>264</v>
       </c>
       <c r="O9" s="20" t="s">
-        <v>277</v>
-      </c>
-      <c r="P9" s="1" t="s">
-        <v>293</v>
+        <v>276</v>
+      </c>
+      <c r="P9" s="20" t="s">
+        <v>291</v>
       </c>
       <c r="Q9" s="20" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="R9" s="1" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
     </row>
     <row r="10" spans="1:18" x14ac:dyDescent="0.25">
@@ -2234,22 +2234,22 @@
         <v>244</v>
       </c>
       <c r="M10" s="20" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="N10" s="20" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="O10" s="20" t="s">
-        <v>278</v>
-      </c>
-      <c r="P10" s="1" t="s">
-        <v>294</v>
+        <v>277</v>
+      </c>
+      <c r="P10" s="20" t="s">
+        <v>292</v>
       </c>
       <c r="Q10" s="20" t="s">
-        <v>307</v>
-      </c>
-      <c r="R10" s="1" t="s">
-        <v>340</v>
+        <v>306</v>
+      </c>
+      <c r="R10" s="20" t="s">
+        <v>339</v>
       </c>
     </row>
     <row r="11" spans="1:18" x14ac:dyDescent="0.25">
@@ -2263,22 +2263,22 @@
         <v>245</v>
       </c>
       <c r="M11" s="20" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="N11" s="1" t="s">
         <v>265</v>
       </c>
       <c r="O11" s="20" t="s">
-        <v>279</v>
-      </c>
-      <c r="P11" s="1" t="s">
-        <v>295</v>
+        <v>278</v>
+      </c>
+      <c r="P11" s="20" t="s">
+        <v>293</v>
       </c>
       <c r="Q11" s="20" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="R11" s="1" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
     </row>
     <row r="12" spans="1:18" x14ac:dyDescent="0.25">
@@ -2307,22 +2307,22 @@
         <v>246</v>
       </c>
       <c r="M12" s="20" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="N12" s="20" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="O12" s="20" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="P12" s="1" t="s">
-        <v>280</v>
+        <v>294</v>
       </c>
       <c r="Q12" s="20" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="R12" s="1" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
     </row>
     <row r="13" spans="1:18" x14ac:dyDescent="0.25">
@@ -2351,22 +2351,22 @@
         <v>247</v>
       </c>
       <c r="M13" s="20" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="N13" s="20" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="O13" s="20" t="s">
-        <v>346</v>
-      </c>
-      <c r="P13" s="20" t="s">
-        <v>317</v>
+        <v>345</v>
+      </c>
+      <c r="P13" s="1" t="s">
+        <v>279</v>
       </c>
       <c r="Q13" s="20" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="R13" s="1" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
     </row>
     <row r="14" spans="1:18" x14ac:dyDescent="0.25">
@@ -2392,22 +2392,22 @@
         <v>64</v>
       </c>
       <c r="L14" s="22" t="s">
-        <v>377</v>
+        <v>374</v>
       </c>
       <c r="M14" s="22" t="s">
-        <v>381</v>
+        <v>378</v>
       </c>
       <c r="O14" s="20" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="P14" s="20" t="s">
-        <v>348</v>
+        <v>316</v>
       </c>
       <c r="Q14" s="1" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="R14" s="20" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
     </row>
     <row r="15" spans="1:18" x14ac:dyDescent="0.25">
@@ -2436,10 +2436,13 @@
         <v>248</v>
       </c>
       <c r="O15" s="20" t="s">
-        <v>349</v>
+        <v>348</v>
+      </c>
+      <c r="P15" s="20" t="s">
+        <v>347</v>
       </c>
       <c r="Q15" s="20" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
     </row>
     <row r="16" spans="1:18" x14ac:dyDescent="0.25">
@@ -2452,8 +2455,8 @@
       <c r="L16" s="20" t="s">
         <v>249</v>
       </c>
-      <c r="Q16" s="1" t="s">
-        <v>313</v>
+      <c r="Q16" s="20" t="s">
+        <v>312</v>
       </c>
     </row>
     <row r="17" spans="1:18" x14ac:dyDescent="0.25">
@@ -2479,10 +2482,10 @@
         <v>137</v>
       </c>
       <c r="L17" s="20" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="Q17" s="20" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
     </row>
     <row r="18" spans="1:18" x14ac:dyDescent="0.25">
@@ -2511,7 +2514,7 @@
         <v>256</v>
       </c>
       <c r="Q18" s="1" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
     </row>
     <row r="19" spans="1:18" x14ac:dyDescent="0.25">
@@ -2534,13 +2537,13 @@
         <v>166</v>
       </c>
       <c r="I19" s="3" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="L19" s="20" t="s">
         <v>257</v>
       </c>
       <c r="Q19" s="1" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
     </row>
     <row r="20" spans="1:18" x14ac:dyDescent="0.25">
@@ -2563,13 +2566,13 @@
         <v>166</v>
       </c>
       <c r="I20" s="3" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="L20" s="20" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="Q20" s="20" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
     </row>
     <row r="21" spans="1:18" x14ac:dyDescent="0.25">
@@ -2577,7 +2580,7 @@
         <v>166</v>
       </c>
       <c r="I21" s="3" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="L21" s="20" t="s">
         <v>234</v>
@@ -2603,10 +2606,10 @@
         <v>166</v>
       </c>
       <c r="I22" s="3" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="L22" s="22" t="s">
-        <v>378</v>
+        <v>375</v>
       </c>
     </row>
     <row r="23" spans="1:18" x14ac:dyDescent="0.25">
@@ -2629,7 +2632,7 @@
         <v>166</v>
       </c>
       <c r="I23" s="3" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="L23" s="20" t="s">
         <v>254</v>
@@ -2655,7 +2658,7 @@
         <v>166</v>
       </c>
       <c r="I24" s="3" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
     </row>
     <row r="25" spans="1:18" x14ac:dyDescent="0.25">
@@ -2678,7 +2681,7 @@
         <v>166</v>
       </c>
       <c r="I25" s="5" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
     </row>
     <row r="26" spans="1:18" x14ac:dyDescent="0.25">
@@ -2687,34 +2690,34 @@
         <v>166</v>
       </c>
       <c r="I26" s="5" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="J26" s="1" t="s">
+        <v>363</v>
+      </c>
+      <c r="K26" s="1" t="s">
         <v>364</v>
       </c>
-      <c r="K26" s="1" t="s">
-        <v>365</v>
-      </c>
       <c r="L26" s="1" t="s">
+        <v>370</v>
+      </c>
+      <c r="M26" s="1" t="s">
+        <v>371</v>
+      </c>
+      <c r="N26" s="1" t="s">
+        <v>382</v>
+      </c>
+      <c r="O26" s="1" t="s">
+        <v>383</v>
+      </c>
+      <c r="P26" s="1" t="s">
+        <v>387</v>
+      </c>
+      <c r="Q26" s="1" t="s">
+        <v>372</v>
+      </c>
+      <c r="R26" s="1" t="s">
         <v>373</v>
-      </c>
-      <c r="M26" s="1" t="s">
-        <v>374</v>
-      </c>
-      <c r="N26" s="1" t="s">
-        <v>386</v>
-      </c>
-      <c r="O26" s="1" t="s">
-        <v>387</v>
-      </c>
-      <c r="P26" s="1" t="s">
-        <v>385</v>
-      </c>
-      <c r="Q26" s="1" t="s">
-        <v>375</v>
-      </c>
-      <c r="R26" s="1" t="s">
-        <v>376</v>
       </c>
     </row>
     <row r="27" spans="1:18" x14ac:dyDescent="0.25">
@@ -2795,16 +2798,16 @@
         <v>270</v>
       </c>
       <c r="O28" s="20" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="P28" s="1" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="Q28" s="1" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="R28" s="1" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
     </row>
     <row r="29" spans="1:18" x14ac:dyDescent="0.25">
@@ -2840,16 +2843,16 @@
         <v>271</v>
       </c>
       <c r="O29" s="20" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="P29" s="20" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="Q29" s="20" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="R29" s="1" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="30" spans="1:18" x14ac:dyDescent="0.25">
@@ -2885,16 +2888,16 @@
         <v>272</v>
       </c>
       <c r="O30" s="1" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="P30" s="20" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="Q30" s="1" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="R30" s="1" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
     </row>
     <row r="31" spans="1:18" x14ac:dyDescent="0.25">
@@ -2916,16 +2919,16 @@
         <v>273</v>
       </c>
       <c r="O31" s="1" t="s">
-        <v>286</v>
-      </c>
-      <c r="P31" s="1" t="s">
-        <v>297</v>
+        <v>285</v>
+      </c>
+      <c r="P31" s="20" t="s">
+        <v>296</v>
       </c>
       <c r="Q31" s="1" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="R31" s="1" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
     </row>
     <row r="32" spans="1:18" x14ac:dyDescent="0.25">
@@ -2956,16 +2959,16 @@
         <v>266</v>
       </c>
       <c r="O32" s="20" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="P32" s="20" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="Q32" s="1" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="R32" s="1" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
     </row>
     <row r="33" spans="1:18" x14ac:dyDescent="0.25">
@@ -2990,13 +2993,13 @@
         <v>267</v>
       </c>
       <c r="O33" s="20" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="Q33" s="20" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="R33" s="1" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
     </row>
     <row r="34" spans="1:18" x14ac:dyDescent="0.25">
@@ -3021,7 +3024,7 @@
         <v>268</v>
       </c>
       <c r="R34" s="1" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
     </row>
     <row r="35" spans="1:18" x14ac:dyDescent="0.25">
@@ -3043,20 +3046,20 @@
       <c r="H35" s="19"/>
       <c r="I35" s="19"/>
       <c r="J35" s="21" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="N35" s="20" t="s">
         <v>269</v>
       </c>
       <c r="R35" s="1" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
     </row>
     <row r="36" spans="1:18" x14ac:dyDescent="0.25">
       <c r="H36" s="19"/>
       <c r="I36" s="19"/>
       <c r="J36" s="1" t="s">
-        <v>388</v>
+        <v>391</v>
       </c>
     </row>
     <row r="37" spans="1:18" x14ac:dyDescent="0.25">
@@ -3078,7 +3081,7 @@
       <c r="H37" s="19"/>
       <c r="I37" s="19"/>
       <c r="J37" s="21" t="s">
-        <v>394</v>
+        <v>396</v>
       </c>
     </row>
     <row r="38" spans="1:18" x14ac:dyDescent="0.25">
@@ -3099,7 +3102,7 @@
       </c>
       <c r="I38" s="19"/>
       <c r="J38" s="1" t="s">
-        <v>392</v>
+        <v>395</v>
       </c>
     </row>
     <row r="39" spans="1:18" x14ac:dyDescent="0.25">
@@ -3120,7 +3123,7 @@
       </c>
       <c r="I39" s="19"/>
       <c r="J39" s="1" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
     </row>
     <row r="40" spans="1:18" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Asset List Update En Import De Assets
</commit_message>
<xml_diff>
--- a/Algemeen/Asset List Game-Lab 1.xlsx
+++ b/Algemeen/Asset List Game-Lab 1.xlsx
@@ -1141,27 +1141,6 @@
     <t>0 Fahrettin|0 Sven|0 Rief</t>
   </si>
   <si>
-    <t>Characters_SoldierAnt_4 (51) 6/8</t>
-  </si>
-  <si>
-    <t>Characters_Sara_1 (44) 5/8</t>
-  </si>
-  <si>
-    <t>Characters_Moeder_3 (40) 6/8</t>
-  </si>
-  <si>
-    <t>Enemy_VliegendHert_3 (49) 6/8</t>
-  </si>
-  <si>
-    <t>Enemy_TermietSoldier_1 (43) 6/8</t>
-  </si>
-  <si>
-    <t>Enemy_TermietGeneral_2 (37) 6/8</t>
-  </si>
-  <si>
-    <t>Enemy_ZwarteWeduwe_5 (49) 3/8</t>
-  </si>
-  <si>
     <t xml:space="preserve">58 Anthony| 19 Michiel| 0 Roos </t>
   </si>
   <si>
@@ -1183,15 +1162,6 @@
     <t>0 Fahrettin|65 Sven|30 Rief</t>
   </si>
   <si>
-    <t>Characters_CivilianAnt_5 (46) 2/8</t>
-  </si>
-  <si>
-    <t xml:space="preserve">52 Anthony| 0 Michiel| 50 Roos </t>
-  </si>
-  <si>
-    <t xml:space="preserve">10 Anthony| 0 Michiel| 27 Roos </t>
-  </si>
-  <si>
     <t>400 Fahrettin|250 Sven|195 Rief</t>
   </si>
   <si>
@@ -1204,10 +1174,40 @@
     <t xml:space="preserve">10 Anthony| 0 Michiel| 57 Roos </t>
   </si>
   <si>
-    <t xml:space="preserve">360 Anthony | 140 Michiel | 257 Roos </t>
-  </si>
-  <si>
-    <t>Artist Points Behaald: 787 / 1125</t>
+    <t xml:space="preserve">62 Anthony| 0 Michiel| 50 Roos </t>
+  </si>
+  <si>
+    <t xml:space="preserve">10 Anthony| 0 Michiel| 39 Roos </t>
+  </si>
+  <si>
+    <t xml:space="preserve">370 Anthony | 140 Michiel | 269 Roos </t>
+  </si>
+  <si>
+    <t>Artist Points Behaald: 809 / 1125</t>
+  </si>
+  <si>
+    <t>Characters_SoldierAnt_4 (45) 6/8</t>
+  </si>
+  <si>
+    <t>Characters_Sara_1 (29) 5/8</t>
+  </si>
+  <si>
+    <t>Characters_Moeder_3 (34) 6/8</t>
+  </si>
+  <si>
+    <t>Enemy_VliegendHert_3 (43) 6/8</t>
+  </si>
+  <si>
+    <t>Enemy_TermietSoldier_1 (37) 6/8</t>
+  </si>
+  <si>
+    <t>Enemy_TermietGeneral_2 (31) 6/8</t>
+  </si>
+  <si>
+    <t>Enemy_ZwarteWeduwe_5 (19) 3/8</t>
+  </si>
+  <si>
+    <t>Characters_CivilianAnt_5 (19) 3/8</t>
   </si>
 </sst>
 </file>
@@ -1727,7 +1727,7 @@
   <dimension ref="A1:R593"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="J1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="N23" sqref="N23"/>
+      <selection activeCell="N17" sqref="N17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1899,19 +1899,19 @@
         <v>368</v>
       </c>
       <c r="N3" s="1" t="s">
-        <v>381</v>
+        <v>374</v>
       </c>
       <c r="O3" s="1" t="s">
-        <v>389</v>
+        <v>385</v>
       </c>
       <c r="P3" s="1" t="s">
-        <v>390</v>
+        <v>386</v>
       </c>
       <c r="Q3" s="1" t="s">
-        <v>394</v>
+        <v>384</v>
       </c>
       <c r="R3" s="1" t="s">
-        <v>393</v>
+        <v>383</v>
       </c>
     </row>
     <row r="4" spans="1:18" x14ac:dyDescent="0.25">
@@ -1946,19 +1946,19 @@
         <v>221</v>
       </c>
       <c r="L4" s="1" t="s">
-        <v>385</v>
+        <v>378</v>
       </c>
       <c r="M4" s="21" t="s">
         <v>221</v>
       </c>
       <c r="N4" s="1" t="s">
-        <v>386</v>
+        <v>379</v>
       </c>
       <c r="O4" s="21" t="s">
         <v>221</v>
       </c>
       <c r="P4" s="1" t="s">
-        <v>386</v>
+        <v>379</v>
       </c>
       <c r="Q4" s="21" t="s">
         <v>221</v>
@@ -2043,10 +2043,10 @@
         <v>230</v>
       </c>
       <c r="N6" s="22" t="s">
-        <v>379</v>
+        <v>394</v>
       </c>
       <c r="O6" s="22" t="s">
-        <v>388</v>
+        <v>396</v>
       </c>
       <c r="P6" s="1" t="s">
         <v>288</v>
@@ -2090,13 +2090,13 @@
         <v>241</v>
       </c>
       <c r="M7" s="22" t="s">
-        <v>376</v>
+        <v>391</v>
       </c>
       <c r="N7" s="22" t="s">
-        <v>380</v>
+        <v>395</v>
       </c>
       <c r="O7" s="20" t="s">
-        <v>384</v>
+        <v>377</v>
       </c>
       <c r="P7" s="1" t="s">
         <v>289</v>
@@ -2187,7 +2187,7 @@
         <v>243</v>
       </c>
       <c r="M9" s="22" t="s">
-        <v>377</v>
+        <v>392</v>
       </c>
       <c r="N9" s="1" t="s">
         <v>264</v>
@@ -2315,7 +2315,7 @@
       <c r="O12" s="20" t="s">
         <v>280</v>
       </c>
-      <c r="P12" s="1" t="s">
+      <c r="P12" s="20" t="s">
         <v>294</v>
       </c>
       <c r="Q12" s="20" t="s">
@@ -2392,10 +2392,10 @@
         <v>64</v>
       </c>
       <c r="L14" s="22" t="s">
-        <v>374</v>
+        <v>389</v>
       </c>
       <c r="M14" s="22" t="s">
-        <v>378</v>
+        <v>393</v>
       </c>
       <c r="O14" s="20" t="s">
         <v>295</v>
@@ -2609,7 +2609,7 @@
         <v>361</v>
       </c>
       <c r="L22" s="22" t="s">
-        <v>375</v>
+        <v>390</v>
       </c>
     </row>
     <row r="23" spans="1:18" x14ac:dyDescent="0.25">
@@ -2705,13 +2705,13 @@
         <v>371</v>
       </c>
       <c r="N26" s="1" t="s">
-        <v>382</v>
+        <v>375</v>
       </c>
       <c r="O26" s="1" t="s">
-        <v>383</v>
+        <v>376</v>
       </c>
       <c r="P26" s="1" t="s">
-        <v>387</v>
+        <v>380</v>
       </c>
       <c r="Q26" s="1" t="s">
         <v>372</v>
@@ -3046,7 +3046,7 @@
       <c r="H35" s="19"/>
       <c r="I35" s="19"/>
       <c r="J35" s="21" t="s">
-        <v>392</v>
+        <v>382</v>
       </c>
       <c r="N35" s="20" t="s">
         <v>269</v>
@@ -3059,7 +3059,7 @@
       <c r="H36" s="19"/>
       <c r="I36" s="19"/>
       <c r="J36" s="1" t="s">
-        <v>391</v>
+        <v>381</v>
       </c>
     </row>
     <row r="37" spans="1:18" x14ac:dyDescent="0.25">
@@ -3081,7 +3081,7 @@
       <c r="H37" s="19"/>
       <c r="I37" s="19"/>
       <c r="J37" s="21" t="s">
-        <v>396</v>
+        <v>388</v>
       </c>
     </row>
     <row r="38" spans="1:18" x14ac:dyDescent="0.25">
@@ -3102,7 +3102,7 @@
       </c>
       <c r="I38" s="19"/>
       <c r="J38" s="1" t="s">
-        <v>395</v>
+        <v>387</v>
       </c>
     </row>
     <row r="39" spans="1:18" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Asset List Update & Import Asset & fix met loading screen
</commit_message>
<xml_diff>
--- a/Algemeen/Asset List Game-Lab 1.xlsx
+++ b/Algemeen/Asset List Game-Lab 1.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1551" uniqueCount="397">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1552" uniqueCount="397">
   <si>
     <t>ID Code</t>
   </si>
@@ -1126,9 +1126,6 @@
     <t xml:space="preserve">113 Anthony| 70 Michiel| 6 Roos </t>
   </si>
   <si>
-    <t xml:space="preserve">30 Fahrettin </t>
-  </si>
-  <si>
     <t>85 Fahrettin|0 Sven|75 Rief</t>
   </si>
   <si>
@@ -1171,21 +1168,12 @@
     <t xml:space="preserve">12 Anthony| 0 Michiel| 7 Roos </t>
   </si>
   <si>
-    <t xml:space="preserve">10 Anthony| 0 Michiel| 57 Roos </t>
-  </si>
-  <si>
     <t xml:space="preserve">62 Anthony| 0 Michiel| 50 Roos </t>
   </si>
   <si>
     <t xml:space="preserve">10 Anthony| 0 Michiel| 39 Roos </t>
   </si>
   <si>
-    <t xml:space="preserve">370 Anthony | 140 Michiel | 269 Roos </t>
-  </si>
-  <si>
-    <t>Artist Points Behaald: 809 / 1125</t>
-  </si>
-  <si>
     <t>Characters_SoldierAnt_4 (45) 6/8</t>
   </si>
   <si>
@@ -1208,6 +1196,18 @@
   </si>
   <si>
     <t>Characters_CivilianAnt_5 (19) 3/8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">10 Anthony| 0 Michiel| 66 Roos </t>
+  </si>
+  <si>
+    <t xml:space="preserve">370 Anthony | 140 Michiel | 278 Roos </t>
+  </si>
+  <si>
+    <t xml:space="preserve">33 Fahrettin </t>
+  </si>
+  <si>
+    <t>Artist Points Behaald: 821 / 1125</t>
   </si>
 </sst>
 </file>
@@ -1727,7 +1727,7 @@
   <dimension ref="A1:R593"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="J1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="N17" sqref="N17"/>
+      <selection activeCell="N20" sqref="N20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1899,19 +1899,19 @@
         <v>368</v>
       </c>
       <c r="N3" s="1" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="O3" s="1" t="s">
-        <v>385</v>
+        <v>383</v>
       </c>
       <c r="P3" s="1" t="s">
-        <v>386</v>
+        <v>384</v>
       </c>
       <c r="Q3" s="1" t="s">
-        <v>384</v>
+        <v>393</v>
       </c>
       <c r="R3" s="1" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
     </row>
     <row r="4" spans="1:18" x14ac:dyDescent="0.25">
@@ -1946,25 +1946,25 @@
         <v>221</v>
       </c>
       <c r="L4" s="1" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="M4" s="21" t="s">
         <v>221</v>
       </c>
       <c r="N4" s="1" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="O4" s="21" t="s">
         <v>221</v>
       </c>
       <c r="P4" s="1" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="Q4" s="21" t="s">
         <v>221</v>
       </c>
-      <c r="R4" s="21" t="s">
-        <v>221</v>
+      <c r="R4" s="1" t="s">
+        <v>378</v>
       </c>
     </row>
     <row r="5" spans="1:18" x14ac:dyDescent="0.25">
@@ -2013,11 +2013,11 @@
       <c r="P5" s="21" t="s">
         <v>221</v>
       </c>
-      <c r="Q5" s="1" t="s">
+      <c r="Q5" s="20" t="s">
         <v>301</v>
       </c>
-      <c r="R5" s="1" t="s">
-        <v>331</v>
+      <c r="R5" s="21" t="s">
+        <v>221</v>
       </c>
     </row>
     <row r="6" spans="1:18" x14ac:dyDescent="0.25">
@@ -2043,10 +2043,10 @@
         <v>230</v>
       </c>
       <c r="N6" s="22" t="s">
-        <v>394</v>
+        <v>390</v>
       </c>
       <c r="O6" s="22" t="s">
-        <v>396</v>
+        <v>392</v>
       </c>
       <c r="P6" s="1" t="s">
         <v>288</v>
@@ -2055,7 +2055,7 @@
         <v>302</v>
       </c>
       <c r="R6" s="1" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
     </row>
     <row r="7" spans="1:18" x14ac:dyDescent="0.25">
@@ -2090,13 +2090,13 @@
         <v>241</v>
       </c>
       <c r="M7" s="22" t="s">
+        <v>387</v>
+      </c>
+      <c r="N7" s="22" t="s">
         <v>391</v>
       </c>
-      <c r="N7" s="22" t="s">
-        <v>395</v>
-      </c>
       <c r="O7" s="20" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="P7" s="1" t="s">
         <v>289</v>
@@ -2105,7 +2105,7 @@
         <v>303</v>
       </c>
       <c r="R7" s="1" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
     </row>
     <row r="8" spans="1:18" x14ac:dyDescent="0.25">
@@ -2155,7 +2155,7 @@
         <v>304</v>
       </c>
       <c r="R8" s="1" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
     </row>
     <row r="9" spans="1:18" x14ac:dyDescent="0.25">
@@ -2187,7 +2187,7 @@
         <v>243</v>
       </c>
       <c r="M9" s="22" t="s">
-        <v>392</v>
+        <v>388</v>
       </c>
       <c r="N9" s="1" t="s">
         <v>264</v>
@@ -2202,7 +2202,7 @@
         <v>305</v>
       </c>
       <c r="R9" s="1" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
     </row>
     <row r="10" spans="1:18" x14ac:dyDescent="0.25">
@@ -2248,8 +2248,8 @@
       <c r="Q10" s="20" t="s">
         <v>306</v>
       </c>
-      <c r="R10" s="20" t="s">
-        <v>339</v>
+      <c r="R10" s="1" t="s">
+        <v>336</v>
       </c>
     </row>
     <row r="11" spans="1:18" x14ac:dyDescent="0.25">
@@ -2277,8 +2277,8 @@
       <c r="Q11" s="20" t="s">
         <v>307</v>
       </c>
-      <c r="R11" s="1" t="s">
-        <v>342</v>
+      <c r="R11" s="20" t="s">
+        <v>339</v>
       </c>
     </row>
     <row r="12" spans="1:18" x14ac:dyDescent="0.25">
@@ -2322,7 +2322,7 @@
         <v>308</v>
       </c>
       <c r="R12" s="1" t="s">
-        <v>353</v>
+        <v>342</v>
       </c>
     </row>
     <row r="13" spans="1:18" x14ac:dyDescent="0.25">
@@ -2365,8 +2365,8 @@
       <c r="Q13" s="20" t="s">
         <v>309</v>
       </c>
-      <c r="R13" s="1" t="s">
-        <v>343</v>
+      <c r="R13" s="20" t="s">
+        <v>353</v>
       </c>
     </row>
     <row r="14" spans="1:18" x14ac:dyDescent="0.25">
@@ -2392,10 +2392,10 @@
         <v>64</v>
       </c>
       <c r="L14" s="22" t="s">
+        <v>385</v>
+      </c>
+      <c r="M14" s="22" t="s">
         <v>389</v>
-      </c>
-      <c r="M14" s="22" t="s">
-        <v>393</v>
       </c>
       <c r="O14" s="20" t="s">
         <v>295</v>
@@ -2406,8 +2406,8 @@
       <c r="Q14" s="1" t="s">
         <v>310</v>
       </c>
-      <c r="R14" s="20" t="s">
-        <v>341</v>
+      <c r="R14" s="1" t="s">
+        <v>343</v>
       </c>
     </row>
     <row r="15" spans="1:18" x14ac:dyDescent="0.25">
@@ -2444,6 +2444,9 @@
       <c r="Q15" s="20" t="s">
         <v>311</v>
       </c>
+      <c r="R15" s="20" t="s">
+        <v>341</v>
+      </c>
     </row>
     <row r="16" spans="1:18" x14ac:dyDescent="0.25">
       <c r="H16" s="3" t="s">
@@ -2609,7 +2612,7 @@
         <v>361</v>
       </c>
       <c r="L22" s="22" t="s">
-        <v>390</v>
+        <v>386</v>
       </c>
     </row>
     <row r="23" spans="1:18" x14ac:dyDescent="0.25">
@@ -2699,25 +2702,25 @@
         <v>364</v>
       </c>
       <c r="L26" s="1" t="s">
+        <v>369</v>
+      </c>
+      <c r="M26" s="1" t="s">
         <v>370</v>
       </c>
-      <c r="M26" s="1" t="s">
+      <c r="N26" s="1" t="s">
+        <v>374</v>
+      </c>
+      <c r="O26" s="1" t="s">
+        <v>375</v>
+      </c>
+      <c r="P26" s="1" t="s">
+        <v>379</v>
+      </c>
+      <c r="Q26" s="1" t="s">
         <v>371</v>
       </c>
-      <c r="N26" s="1" t="s">
-        <v>375</v>
-      </c>
-      <c r="O26" s="1" t="s">
-        <v>376</v>
-      </c>
-      <c r="P26" s="1" t="s">
-        <v>380</v>
-      </c>
-      <c r="Q26" s="1" t="s">
+      <c r="R26" s="1" t="s">
         <v>372</v>
-      </c>
-      <c r="R26" s="1" t="s">
-        <v>373</v>
       </c>
     </row>
     <row r="27" spans="1:18" x14ac:dyDescent="0.25">
@@ -3046,7 +3049,7 @@
       <c r="H35" s="19"/>
       <c r="I35" s="19"/>
       <c r="J35" s="21" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="N35" s="20" t="s">
         <v>269</v>
@@ -3059,7 +3062,7 @@
       <c r="H36" s="19"/>
       <c r="I36" s="19"/>
       <c r="J36" s="1" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
     </row>
     <row r="37" spans="1:18" x14ac:dyDescent="0.25">
@@ -3081,7 +3084,7 @@
       <c r="H37" s="19"/>
       <c r="I37" s="19"/>
       <c r="J37" s="21" t="s">
-        <v>388</v>
+        <v>396</v>
       </c>
     </row>
     <row r="38" spans="1:18" x14ac:dyDescent="0.25">
@@ -3102,7 +3105,7 @@
       </c>
       <c r="I38" s="19"/>
       <c r="J38" s="1" t="s">
-        <v>387</v>
+        <v>394</v>
       </c>
     </row>
     <row r="39" spans="1:18" x14ac:dyDescent="0.25">
@@ -3123,7 +3126,7 @@
       </c>
       <c r="I39" s="19"/>
       <c r="J39" s="1" t="s">
-        <v>369</v>
+        <v>395</v>
       </c>
     </row>
     <row r="40" spans="1:18" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Asset List Update 14-01-2016
</commit_message>
<xml_diff>
--- a/Algemeen/Asset List Game-Lab 1.xlsx
+++ b/Algemeen/Asset List Game-Lab 1.xlsx
@@ -1132,12 +1132,6 @@
     <t>75 Fahrettin|40 Sven|0 Rief</t>
   </si>
   <si>
-    <t>60 Fahrettin|0 Sven|0 Rief</t>
-  </si>
-  <si>
-    <t>0 Fahrettin|0 Sven|0 Rief</t>
-  </si>
-  <si>
     <t xml:space="preserve">58 Anthony| 19 Michiel| 0 Roos </t>
   </si>
   <si>
@@ -1159,12 +1153,6 @@
     <t>0 Fahrettin|65 Sven|30 Rief</t>
   </si>
   <si>
-    <t>400 Fahrettin|250 Sven|195 Rief</t>
-  </si>
-  <si>
-    <t>Development Points: 845 / 1125</t>
-  </si>
-  <si>
     <t xml:space="preserve">12 Anthony| 0 Michiel| 7 Roos </t>
   </si>
   <si>
@@ -1208,6 +1196,18 @@
   </si>
   <si>
     <t>Artist Points Behaald: 821 / 1125</t>
+  </si>
+  <si>
+    <t>60 Fahrettin|0 Sven|15 Rief</t>
+  </si>
+  <si>
+    <t>0 Fahrettin|0 Sven|20 Rief</t>
+  </si>
+  <si>
+    <t>400 Fahrettin|250 Sven|230 Rief</t>
+  </si>
+  <si>
+    <t>Development Points: 880 / 1125</t>
   </si>
 </sst>
 </file>
@@ -1727,7 +1727,7 @@
   <dimension ref="A1:R593"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="J1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="N20" sqref="N20"/>
+      <selection activeCell="J18" sqref="J18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1899,19 +1899,19 @@
         <v>368</v>
       </c>
       <c r="N3" s="1" t="s">
-        <v>373</v>
+        <v>371</v>
       </c>
       <c r="O3" s="1" t="s">
-        <v>383</v>
+        <v>379</v>
       </c>
       <c r="P3" s="1" t="s">
-        <v>384</v>
+        <v>380</v>
       </c>
       <c r="Q3" s="1" t="s">
-        <v>393</v>
+        <v>389</v>
       </c>
       <c r="R3" s="1" t="s">
-        <v>382</v>
+        <v>378</v>
       </c>
     </row>
     <row r="4" spans="1:18" x14ac:dyDescent="0.25">
@@ -1946,25 +1946,25 @@
         <v>221</v>
       </c>
       <c r="L4" s="1" t="s">
-        <v>377</v>
+        <v>375</v>
       </c>
       <c r="M4" s="21" t="s">
         <v>221</v>
       </c>
       <c r="N4" s="1" t="s">
-        <v>378</v>
+        <v>376</v>
       </c>
       <c r="O4" s="21" t="s">
         <v>221</v>
       </c>
       <c r="P4" s="1" t="s">
-        <v>378</v>
+        <v>376</v>
       </c>
       <c r="Q4" s="21" t="s">
         <v>221</v>
       </c>
       <c r="R4" s="1" t="s">
-        <v>378</v>
+        <v>376</v>
       </c>
     </row>
     <row r="5" spans="1:18" x14ac:dyDescent="0.25">
@@ -2043,10 +2043,10 @@
         <v>230</v>
       </c>
       <c r="N6" s="22" t="s">
-        <v>390</v>
+        <v>386</v>
       </c>
       <c r="O6" s="22" t="s">
-        <v>392</v>
+        <v>388</v>
       </c>
       <c r="P6" s="1" t="s">
         <v>288</v>
@@ -2090,13 +2090,13 @@
         <v>241</v>
       </c>
       <c r="M7" s="22" t="s">
+        <v>383</v>
+      </c>
+      <c r="N7" s="22" t="s">
         <v>387</v>
       </c>
-      <c r="N7" s="22" t="s">
-        <v>391</v>
-      </c>
       <c r="O7" s="20" t="s">
-        <v>376</v>
+        <v>374</v>
       </c>
       <c r="P7" s="1" t="s">
         <v>289</v>
@@ -2187,7 +2187,7 @@
         <v>243</v>
       </c>
       <c r="M9" s="22" t="s">
-        <v>388</v>
+        <v>384</v>
       </c>
       <c r="N9" s="1" t="s">
         <v>264</v>
@@ -2392,10 +2392,10 @@
         <v>64</v>
       </c>
       <c r="L14" s="22" t="s">
+        <v>381</v>
+      </c>
+      <c r="M14" s="22" t="s">
         <v>385</v>
-      </c>
-      <c r="M14" s="22" t="s">
-        <v>389</v>
       </c>
       <c r="O14" s="20" t="s">
         <v>295</v>
@@ -2612,7 +2612,7 @@
         <v>361</v>
       </c>
       <c r="L22" s="22" t="s">
-        <v>386</v>
+        <v>382</v>
       </c>
     </row>
     <row r="23" spans="1:18" x14ac:dyDescent="0.25">
@@ -2708,19 +2708,19 @@
         <v>370</v>
       </c>
       <c r="N26" s="1" t="s">
-        <v>374</v>
+        <v>372</v>
       </c>
       <c r="O26" s="1" t="s">
-        <v>375</v>
+        <v>373</v>
       </c>
       <c r="P26" s="1" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
       <c r="Q26" s="1" t="s">
-        <v>371</v>
+        <v>393</v>
       </c>
       <c r="R26" s="1" t="s">
-        <v>372</v>
+        <v>394</v>
       </c>
     </row>
     <row r="27" spans="1:18" x14ac:dyDescent="0.25">
@@ -2896,7 +2896,7 @@
       <c r="P30" s="20" t="s">
         <v>298</v>
       </c>
-      <c r="Q30" s="1" t="s">
+      <c r="Q30" s="20" t="s">
         <v>319</v>
       </c>
       <c r="R30" s="1" t="s">
@@ -2927,10 +2927,10 @@
       <c r="P31" s="20" t="s">
         <v>296</v>
       </c>
-      <c r="Q31" s="1" t="s">
+      <c r="Q31" s="20" t="s">
         <v>320</v>
       </c>
-      <c r="R31" s="1" t="s">
+      <c r="R31" s="20" t="s">
         <v>326</v>
       </c>
     </row>
@@ -2967,10 +2967,10 @@
       <c r="P32" s="20" t="s">
         <v>299</v>
       </c>
-      <c r="Q32" s="1" t="s">
+      <c r="Q32" s="20" t="s">
         <v>321</v>
       </c>
-      <c r="R32" s="1" t="s">
+      <c r="R32" s="20" t="s">
         <v>327</v>
       </c>
     </row>
@@ -3001,7 +3001,7 @@
       <c r="Q33" s="20" t="s">
         <v>322</v>
       </c>
-      <c r="R33" s="1" t="s">
+      <c r="R33" s="20" t="s">
         <v>328</v>
       </c>
     </row>
@@ -3049,12 +3049,12 @@
       <c r="H35" s="19"/>
       <c r="I35" s="19"/>
       <c r="J35" s="21" t="s">
-        <v>381</v>
+        <v>396</v>
       </c>
       <c r="N35" s="20" t="s">
         <v>269</v>
       </c>
-      <c r="R35" s="1" t="s">
+      <c r="R35" s="20" t="s">
         <v>330</v>
       </c>
     </row>
@@ -3062,7 +3062,7 @@
       <c r="H36" s="19"/>
       <c r="I36" s="19"/>
       <c r="J36" s="1" t="s">
-        <v>380</v>
+        <v>395</v>
       </c>
     </row>
     <row r="37" spans="1:18" x14ac:dyDescent="0.25">
@@ -3084,7 +3084,7 @@
       <c r="H37" s="19"/>
       <c r="I37" s="19"/>
       <c r="J37" s="21" t="s">
-        <v>396</v>
+        <v>392</v>
       </c>
     </row>
     <row r="38" spans="1:18" x14ac:dyDescent="0.25">
@@ -3105,7 +3105,7 @@
       </c>
       <c r="I38" s="19"/>
       <c r="J38" s="1" t="s">
-        <v>394</v>
+        <v>390</v>
       </c>
     </row>
     <row r="39" spans="1:18" x14ac:dyDescent="0.25">
@@ -3126,7 +3126,7 @@
       </c>
       <c r="I39" s="19"/>
       <c r="J39" s="1" t="s">
-        <v>395</v>
+        <v>391</v>
       </c>
     </row>
     <row r="40" spans="1:18" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Uren Registratie 15-01-2016 & Asset list update & small fix met termiet
</commit_message>
<xml_diff>
--- a/Algemeen/Asset List Game-Lab 1.xlsx
+++ b/Algemeen/Asset List Game-Lab 1.xlsx
@@ -1156,9 +1156,6 @@
     <t xml:space="preserve">12 Anthony| 0 Michiel| 7 Roos </t>
   </si>
   <si>
-    <t xml:space="preserve">62 Anthony| 0 Michiel| 50 Roos </t>
-  </si>
-  <si>
     <t xml:space="preserve">10 Anthony| 0 Michiel| 39 Roos </t>
   </si>
   <si>
@@ -1183,21 +1180,12 @@
     <t>Enemy_ZwarteWeduwe_5 (19) 3/8</t>
   </si>
   <si>
-    <t>Characters_CivilianAnt_5 (19) 3/8</t>
-  </si>
-  <si>
     <t xml:space="preserve">10 Anthony| 0 Michiel| 66 Roos </t>
   </si>
   <si>
-    <t xml:space="preserve">370 Anthony | 140 Michiel | 278 Roos </t>
-  </si>
-  <si>
     <t xml:space="preserve">33 Fahrettin </t>
   </si>
   <si>
-    <t>Artist Points Behaald: 821 / 1125</t>
-  </si>
-  <si>
     <t>60 Fahrettin|0 Sven|15 Rief</t>
   </si>
   <si>
@@ -1208,6 +1196,18 @@
   </si>
   <si>
     <t>Development Points: 880 / 1125</t>
+  </si>
+  <si>
+    <t>Characters_CivilianAnt_5 (26) 4/8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">67 Anthony| 0 Michiel| 50 Roos </t>
+  </si>
+  <si>
+    <t xml:space="preserve">377 Anthony | 140 Michiel | 278 Roos </t>
+  </si>
+  <si>
+    <t>Artist Points Behaald: 828 / 1125</t>
   </si>
 </sst>
 </file>
@@ -1727,7 +1727,7 @@
   <dimension ref="A1:R593"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="J1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J18" sqref="J18"/>
+      <selection activeCell="M35" sqref="M35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1902,13 +1902,13 @@
         <v>371</v>
       </c>
       <c r="O3" s="1" t="s">
+        <v>394</v>
+      </c>
+      <c r="P3" s="1" t="s">
         <v>379</v>
       </c>
-      <c r="P3" s="1" t="s">
-        <v>380</v>
-      </c>
       <c r="Q3" s="1" t="s">
-        <v>389</v>
+        <v>387</v>
       </c>
       <c r="R3" s="1" t="s">
         <v>378</v>
@@ -2043,10 +2043,10 @@
         <v>230</v>
       </c>
       <c r="N6" s="22" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="O6" s="22" t="s">
-        <v>388</v>
+        <v>393</v>
       </c>
       <c r="P6" s="1" t="s">
         <v>288</v>
@@ -2090,10 +2090,10 @@
         <v>241</v>
       </c>
       <c r="M7" s="22" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="N7" s="22" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="O7" s="20" t="s">
         <v>374</v>
@@ -2187,7 +2187,7 @@
         <v>243</v>
       </c>
       <c r="M9" s="22" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="N9" s="1" t="s">
         <v>264</v>
@@ -2392,10 +2392,10 @@
         <v>64</v>
       </c>
       <c r="L14" s="22" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="M14" s="22" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="O14" s="20" t="s">
         <v>295</v>
@@ -2612,7 +2612,7 @@
         <v>361</v>
       </c>
       <c r="L22" s="22" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
     </row>
     <row r="23" spans="1:18" x14ac:dyDescent="0.25">
@@ -2717,10 +2717,10 @@
         <v>377</v>
       </c>
       <c r="Q26" s="1" t="s">
-        <v>393</v>
+        <v>389</v>
       </c>
       <c r="R26" s="1" t="s">
-        <v>394</v>
+        <v>390</v>
       </c>
     </row>
     <row r="27" spans="1:18" x14ac:dyDescent="0.25">
@@ -3049,7 +3049,7 @@
       <c r="H35" s="19"/>
       <c r="I35" s="19"/>
       <c r="J35" s="21" t="s">
-        <v>396</v>
+        <v>392</v>
       </c>
       <c r="N35" s="20" t="s">
         <v>269</v>
@@ -3062,7 +3062,7 @@
       <c r="H36" s="19"/>
       <c r="I36" s="19"/>
       <c r="J36" s="1" t="s">
-        <v>395</v>
+        <v>391</v>
       </c>
     </row>
     <row r="37" spans="1:18" x14ac:dyDescent="0.25">
@@ -3084,7 +3084,7 @@
       <c r="H37" s="19"/>
       <c r="I37" s="19"/>
       <c r="J37" s="21" t="s">
-        <v>392</v>
+        <v>396</v>
       </c>
     </row>
     <row r="38" spans="1:18" x14ac:dyDescent="0.25">
@@ -3105,7 +3105,7 @@
       </c>
       <c r="I38" s="19"/>
       <c r="J38" s="1" t="s">
-        <v>390</v>
+        <v>395</v>
       </c>
     </row>
     <row r="39" spans="1:18" x14ac:dyDescent="0.25">
@@ -3126,7 +3126,7 @@
       </c>
       <c r="I39" s="19"/>
       <c r="J39" s="1" t="s">
-        <v>391</v>
+        <v>388</v>
       </c>
     </row>
     <row r="40" spans="1:18" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
19-01-2016 Uren Registratie & Asset List Update
</commit_message>
<xml_diff>
--- a/Algemeen/Asset List Game-Lab 1.xlsx
+++ b/Algemeen/Asset List Game-Lab 1.xlsx
@@ -886,9 +886,6 @@
     <t>Characters_Vader_2 (40)</t>
   </si>
   <si>
-    <t>Enemy_Kakkerlak_4 (39)</t>
-  </si>
-  <si>
     <t>Platform_GroenPlatform_5 (7)</t>
   </si>
   <si>
@@ -1120,9 +1117,6 @@
     <t xml:space="preserve">12 Anthony| 0 Michiel| 20 Roos </t>
   </si>
   <si>
-    <t xml:space="preserve">61 Anthony| 51 Michiel| 74 Roos </t>
-  </si>
-  <si>
     <t xml:space="preserve">113 Anthony| 70 Michiel| 6 Roos </t>
   </si>
   <si>
@@ -1132,18 +1126,9 @@
     <t>75 Fahrettin|40 Sven|0 Rief</t>
   </si>
   <si>
-    <t xml:space="preserve">58 Anthony| 19 Michiel| 0 Roos </t>
-  </si>
-  <si>
     <t>60 Fahrettin|40 Sven|30 Rief</t>
   </si>
   <si>
-    <t>65 Fahrettin|0 Sven|15 Rief</t>
-  </si>
-  <si>
-    <t>Weapons_SlingShot_5 (13) 2/5</t>
-  </si>
-  <si>
     <t xml:space="preserve">24 Fahrettin </t>
   </si>
   <si>
@@ -1156,15 +1141,9 @@
     <t xml:space="preserve">12 Anthony| 0 Michiel| 7 Roos </t>
   </si>
   <si>
-    <t xml:space="preserve">10 Anthony| 0 Michiel| 39 Roos </t>
-  </si>
-  <si>
     <t>Characters_SoldierAnt_4 (45) 6/8</t>
   </si>
   <si>
-    <t>Characters_Sara_1 (29) 5/8</t>
-  </si>
-  <si>
     <t>Characters_Moeder_3 (34) 6/8</t>
   </si>
   <si>
@@ -1180,9 +1159,6 @@
     <t>Enemy_ZwarteWeduwe_5 (19) 3/8</t>
   </si>
   <si>
-    <t xml:space="preserve">10 Anthony| 0 Michiel| 66 Roos </t>
-  </si>
-  <si>
     <t xml:space="preserve">33 Fahrettin </t>
   </si>
   <si>
@@ -1192,22 +1168,46 @@
     <t>0 Fahrettin|0 Sven|20 Rief</t>
   </si>
   <si>
-    <t>400 Fahrettin|250 Sven|230 Rief</t>
-  </si>
-  <si>
-    <t>Development Points: 880 / 1125</t>
-  </si>
-  <si>
-    <t>Characters_CivilianAnt_5 (26) 4/8</t>
-  </si>
-  <si>
-    <t xml:space="preserve">67 Anthony| 0 Michiel| 50 Roos </t>
-  </si>
-  <si>
-    <t xml:space="preserve">377 Anthony | 140 Michiel | 278 Roos </t>
-  </si>
-  <si>
-    <t>Artist Points Behaald: 828 / 1125</t>
+    <t xml:space="preserve">60 Anthony| 19 Michiel| 0 Roos </t>
+  </si>
+  <si>
+    <t>Characters_Sara_1 (38) 6/8</t>
+  </si>
+  <si>
+    <t>Characters_CivilianAnt_5 (40) 6/8</t>
+  </si>
+  <si>
+    <t>Enemy_Kakkerlak_4 (20) 4/8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">61 Anthony| 67 Michiel| 74 Roos </t>
+  </si>
+  <si>
+    <t>65 Fahrettin|40 Sven|15 Rief</t>
+  </si>
+  <si>
+    <t>Weapons_SlingShot_5 (13)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">83 Anthony| 0 Michiel| 50 Roos </t>
+  </si>
+  <si>
+    <t xml:space="preserve">10 Anthony| 0 Michiel| 49 Roos </t>
+  </si>
+  <si>
+    <t xml:space="preserve">10 Anthony| 0 Michiel| 74 Roos </t>
+  </si>
+  <si>
+    <t>400 Fahrettin|290 Sven|230 Rief</t>
+  </si>
+  <si>
+    <t>Development Points: 920 / 1125</t>
+  </si>
+  <si>
+    <t xml:space="preserve">393 Anthony | 156 Michiel | 296 Roos </t>
+  </si>
+  <si>
+    <t>Artist Points Behaald: 878 / 1125</t>
   </si>
 </sst>
 </file>
@@ -1727,7 +1727,7 @@
   <dimension ref="A1:R593"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="J1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="M35" sqref="M35"/>
+      <selection activeCell="K35" sqref="K35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1887,31 +1887,31 @@
         <v>67</v>
       </c>
       <c r="J3" s="1" t="s">
+        <v>364</v>
+      </c>
+      <c r="K3" s="1" t="s">
         <v>365</v>
       </c>
-      <c r="K3" s="1" t="s">
+      <c r="L3" s="1" t="s">
+        <v>387</v>
+      </c>
+      <c r="M3" s="1" t="s">
         <v>366</v>
       </c>
-      <c r="L3" s="1" t="s">
-        <v>367</v>
-      </c>
-      <c r="M3" s="1" t="s">
-        <v>368</v>
-      </c>
       <c r="N3" s="1" t="s">
-        <v>371</v>
+        <v>383</v>
       </c>
       <c r="O3" s="1" t="s">
-        <v>394</v>
+        <v>390</v>
       </c>
       <c r="P3" s="1" t="s">
-        <v>379</v>
+        <v>391</v>
       </c>
       <c r="Q3" s="1" t="s">
-        <v>387</v>
+        <v>392</v>
       </c>
       <c r="R3" s="1" t="s">
-        <v>378</v>
+        <v>373</v>
       </c>
     </row>
     <row r="4" spans="1:18" x14ac:dyDescent="0.25">
@@ -1946,25 +1946,25 @@
         <v>221</v>
       </c>
       <c r="L4" s="1" t="s">
-        <v>375</v>
+        <v>370</v>
       </c>
       <c r="M4" s="21" t="s">
         <v>221</v>
       </c>
       <c r="N4" s="1" t="s">
-        <v>376</v>
+        <v>371</v>
       </c>
       <c r="O4" s="21" t="s">
         <v>221</v>
       </c>
       <c r="P4" s="1" t="s">
-        <v>376</v>
+        <v>371</v>
       </c>
       <c r="Q4" s="21" t="s">
         <v>221</v>
       </c>
       <c r="R4" s="1" t="s">
-        <v>376</v>
+        <v>371</v>
       </c>
     </row>
     <row r="5" spans="1:18" x14ac:dyDescent="0.25">
@@ -1993,10 +1993,10 @@
         <v>152</v>
       </c>
       <c r="J5" s="20" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="K5" s="20" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="L5" s="21" t="s">
         <v>221</v>
@@ -2014,7 +2014,7 @@
         <v>221</v>
       </c>
       <c r="Q5" s="20" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="R5" s="21" t="s">
         <v>221</v>
@@ -2043,19 +2043,19 @@
         <v>230</v>
       </c>
       <c r="N6" s="22" t="s">
+        <v>378</v>
+      </c>
+      <c r="O6" s="22" t="s">
         <v>385</v>
-      </c>
-      <c r="O6" s="22" t="s">
-        <v>393</v>
       </c>
       <c r="P6" s="1" t="s">
         <v>288</v>
       </c>
       <c r="Q6" s="1" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="R6" s="1" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
     </row>
     <row r="7" spans="1:18" x14ac:dyDescent="0.25">
@@ -2090,22 +2090,22 @@
         <v>241</v>
       </c>
       <c r="M7" s="22" t="s">
-        <v>382</v>
+        <v>375</v>
       </c>
       <c r="N7" s="22" t="s">
+        <v>379</v>
+      </c>
+      <c r="O7" s="20" t="s">
+        <v>389</v>
+      </c>
+      <c r="P7" s="22" t="s">
         <v>386</v>
       </c>
-      <c r="O7" s="20" t="s">
-        <v>374</v>
-      </c>
-      <c r="P7" s="1" t="s">
-        <v>289</v>
-      </c>
-      <c r="Q7" s="1" t="s">
-        <v>303</v>
+      <c r="Q7" s="20" t="s">
+        <v>302</v>
       </c>
       <c r="R7" s="1" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
     </row>
     <row r="8" spans="1:18" x14ac:dyDescent="0.25">
@@ -2149,13 +2149,13 @@
         <v>275</v>
       </c>
       <c r="P8" s="20" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="Q8" s="1" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="R8" s="1" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
     </row>
     <row r="9" spans="1:18" x14ac:dyDescent="0.25">
@@ -2187,7 +2187,7 @@
         <v>243</v>
       </c>
       <c r="M9" s="22" t="s">
-        <v>383</v>
+        <v>376</v>
       </c>
       <c r="N9" s="1" t="s">
         <v>264</v>
@@ -2196,13 +2196,13 @@
         <v>276</v>
       </c>
       <c r="P9" s="20" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="Q9" s="20" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="R9" s="1" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
     </row>
     <row r="10" spans="1:18" x14ac:dyDescent="0.25">
@@ -2234,22 +2234,22 @@
         <v>244</v>
       </c>
       <c r="M10" s="20" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="N10" s="20" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="O10" s="20" t="s">
         <v>277</v>
       </c>
       <c r="P10" s="20" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="Q10" s="20" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="R10" s="1" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
     </row>
     <row r="11" spans="1:18" x14ac:dyDescent="0.25">
@@ -2263,22 +2263,22 @@
         <v>245</v>
       </c>
       <c r="M11" s="20" t="s">
-        <v>337</v>
-      </c>
-      <c r="N11" s="1" t="s">
+        <v>336</v>
+      </c>
+      <c r="N11" s="20" t="s">
         <v>265</v>
       </c>
       <c r="O11" s="20" t="s">
         <v>278</v>
       </c>
       <c r="P11" s="20" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="Q11" s="20" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="R11" s="20" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
     </row>
     <row r="12" spans="1:18" x14ac:dyDescent="0.25">
@@ -2307,7 +2307,7 @@
         <v>246</v>
       </c>
       <c r="M12" s="20" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="N12" s="20" t="s">
         <v>281</v>
@@ -2316,13 +2316,13 @@
         <v>280</v>
       </c>
       <c r="P12" s="20" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="Q12" s="20" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="R12" s="1" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
     </row>
     <row r="13" spans="1:18" x14ac:dyDescent="0.25">
@@ -2351,22 +2351,22 @@
         <v>247</v>
       </c>
       <c r="M13" s="20" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="N13" s="20" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="O13" s="20" t="s">
-        <v>345</v>
-      </c>
-      <c r="P13" s="1" t="s">
+        <v>344</v>
+      </c>
+      <c r="P13" s="20" t="s">
         <v>279</v>
       </c>
       <c r="Q13" s="20" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="R13" s="20" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
     </row>
     <row r="14" spans="1:18" x14ac:dyDescent="0.25">
@@ -2392,22 +2392,22 @@
         <v>64</v>
       </c>
       <c r="L14" s="22" t="s">
-        <v>380</v>
+        <v>374</v>
       </c>
       <c r="M14" s="22" t="s">
-        <v>384</v>
+        <v>377</v>
       </c>
       <c r="O14" s="20" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="P14" s="20" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="Q14" s="1" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="R14" s="1" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
     </row>
     <row r="15" spans="1:18" x14ac:dyDescent="0.25">
@@ -2436,16 +2436,16 @@
         <v>248</v>
       </c>
       <c r="O15" s="20" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="P15" s="20" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="Q15" s="20" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="R15" s="20" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
     </row>
     <row r="16" spans="1:18" x14ac:dyDescent="0.25">
@@ -2459,7 +2459,7 @@
         <v>249</v>
       </c>
       <c r="Q16" s="20" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
     </row>
     <row r="17" spans="1:18" x14ac:dyDescent="0.25">
@@ -2485,10 +2485,10 @@
         <v>137</v>
       </c>
       <c r="L17" s="20" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="Q17" s="20" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
     </row>
     <row r="18" spans="1:18" x14ac:dyDescent="0.25">
@@ -2517,7 +2517,7 @@
         <v>256</v>
       </c>
       <c r="Q18" s="1" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
     </row>
     <row r="19" spans="1:18" x14ac:dyDescent="0.25">
@@ -2540,13 +2540,13 @@
         <v>166</v>
       </c>
       <c r="I19" s="3" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="L19" s="20" t="s">
         <v>257</v>
       </c>
       <c r="Q19" s="1" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
     </row>
     <row r="20" spans="1:18" x14ac:dyDescent="0.25">
@@ -2569,13 +2569,13 @@
         <v>166</v>
       </c>
       <c r="I20" s="3" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="L20" s="20" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="Q20" s="20" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
     </row>
     <row r="21" spans="1:18" x14ac:dyDescent="0.25">
@@ -2583,7 +2583,7 @@
         <v>166</v>
       </c>
       <c r="I21" s="3" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="L21" s="20" t="s">
         <v>234</v>
@@ -2609,10 +2609,10 @@
         <v>166</v>
       </c>
       <c r="I22" s="3" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="L22" s="22" t="s">
-        <v>381</v>
+        <v>384</v>
       </c>
     </row>
     <row r="23" spans="1:18" x14ac:dyDescent="0.25">
@@ -2635,7 +2635,7 @@
         <v>166</v>
       </c>
       <c r="I23" s="3" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="L23" s="20" t="s">
         <v>254</v>
@@ -2661,7 +2661,7 @@
         <v>166</v>
       </c>
       <c r="I24" s="3" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
     </row>
     <row r="25" spans="1:18" x14ac:dyDescent="0.25">
@@ -2684,7 +2684,7 @@
         <v>166</v>
       </c>
       <c r="I25" s="5" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
     </row>
     <row r="26" spans="1:18" x14ac:dyDescent="0.25">
@@ -2693,34 +2693,34 @@
         <v>166</v>
       </c>
       <c r="I26" s="5" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="J26" s="1" t="s">
+        <v>362</v>
+      </c>
+      <c r="K26" s="1" t="s">
         <v>363</v>
       </c>
-      <c r="K26" s="1" t="s">
-        <v>364</v>
-      </c>
       <c r="L26" s="1" t="s">
+        <v>367</v>
+      </c>
+      <c r="M26" s="1" t="s">
+        <v>368</v>
+      </c>
+      <c r="N26" s="1" t="s">
         <v>369</v>
       </c>
-      <c r="M26" s="1" t="s">
-        <v>370</v>
-      </c>
-      <c r="N26" s="1" t="s">
+      <c r="O26" s="1" t="s">
+        <v>388</v>
+      </c>
+      <c r="P26" s="1" t="s">
         <v>372</v>
       </c>
-      <c r="O26" s="1" t="s">
-        <v>373</v>
-      </c>
-      <c r="P26" s="1" t="s">
-        <v>377</v>
-      </c>
       <c r="Q26" s="1" t="s">
-        <v>389</v>
+        <v>381</v>
       </c>
       <c r="R26" s="1" t="s">
-        <v>390</v>
+        <v>382</v>
       </c>
     </row>
     <row r="27" spans="1:18" x14ac:dyDescent="0.25">
@@ -2755,7 +2755,7 @@
       <c r="N27" s="23" t="s">
         <v>222</v>
       </c>
-      <c r="O27" s="21" t="s">
+      <c r="O27" s="23" t="s">
         <v>222</v>
       </c>
       <c r="P27" s="21" t="s">
@@ -2804,13 +2804,13 @@
         <v>282</v>
       </c>
       <c r="P28" s="1" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="Q28" s="1" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="R28" s="1" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
     </row>
     <row r="29" spans="1:18" x14ac:dyDescent="0.25">
@@ -2849,13 +2849,13 @@
         <v>283</v>
       </c>
       <c r="P29" s="20" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="Q29" s="20" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="R29" s="1" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
     </row>
     <row r="30" spans="1:18" x14ac:dyDescent="0.25">
@@ -2890,17 +2890,17 @@
       <c r="N30" s="20" t="s">
         <v>272</v>
       </c>
-      <c r="O30" s="1" t="s">
+      <c r="O30" s="20" t="s">
         <v>284</v>
       </c>
       <c r="P30" s="20" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="Q30" s="20" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="R30" s="1" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="31" spans="1:18" x14ac:dyDescent="0.25">
@@ -2921,17 +2921,17 @@
       <c r="N31" s="20" t="s">
         <v>273</v>
       </c>
-      <c r="O31" s="1" t="s">
+      <c r="O31" s="20" t="s">
         <v>285</v>
       </c>
       <c r="P31" s="20" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="Q31" s="20" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="R31" s="20" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
     </row>
     <row r="32" spans="1:18" x14ac:dyDescent="0.25">
@@ -2965,13 +2965,13 @@
         <v>286</v>
       </c>
       <c r="P32" s="20" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="Q32" s="20" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="R32" s="20" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
     </row>
     <row r="33" spans="1:18" x14ac:dyDescent="0.25">
@@ -2999,10 +2999,10 @@
         <v>287</v>
       </c>
       <c r="Q33" s="20" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="R33" s="20" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
     </row>
     <row r="34" spans="1:18" x14ac:dyDescent="0.25">
@@ -3027,7 +3027,7 @@
         <v>268</v>
       </c>
       <c r="R34" s="1" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
     </row>
     <row r="35" spans="1:18" x14ac:dyDescent="0.25">
@@ -3049,20 +3049,20 @@
       <c r="H35" s="19"/>
       <c r="I35" s="19"/>
       <c r="J35" s="21" t="s">
-        <v>392</v>
+        <v>394</v>
       </c>
       <c r="N35" s="20" t="s">
         <v>269</v>
       </c>
       <c r="R35" s="20" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
     </row>
     <row r="36" spans="1:18" x14ac:dyDescent="0.25">
       <c r="H36" s="19"/>
       <c r="I36" s="19"/>
       <c r="J36" s="1" t="s">
-        <v>391</v>
+        <v>393</v>
       </c>
     </row>
     <row r="37" spans="1:18" x14ac:dyDescent="0.25">
@@ -3126,7 +3126,7 @@
       </c>
       <c r="I39" s="19"/>
       <c r="J39" s="1" t="s">
-        <v>388</v>
+        <v>380</v>
       </c>
     </row>
     <row r="40" spans="1:18" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Asset List Update & Import Skill UI
</commit_message>
<xml_diff>
--- a/Algemeen/Asset List Game-Lab 1.xlsx
+++ b/Algemeen/Asset List Game-Lab 1.xlsx
@@ -1195,19 +1195,19 @@
     <t xml:space="preserve">10 Anthony| 0 Michiel| 49 Roos </t>
   </si>
   <si>
-    <t xml:space="preserve">10 Anthony| 0 Michiel| 74 Roos </t>
-  </si>
-  <si>
-    <t>400 Fahrettin|290 Sven|230 Rief</t>
-  </si>
-  <si>
     <t>Development Points: 920 / 1125</t>
   </si>
   <si>
-    <t xml:space="preserve">393 Anthony | 156 Michiel | 296 Roos </t>
-  </si>
-  <si>
-    <t>Artist Points Behaald: 878 / 1125</t>
+    <t xml:space="preserve">10 Anthony| 0 Michiel| 78 Roos </t>
+  </si>
+  <si>
+    <t xml:space="preserve">393 Anthony | 156 Michiel | 300 Roos </t>
+  </si>
+  <si>
+    <t>400 Fahrettin | 290 Sven | 230 Rief</t>
+  </si>
+  <si>
+    <t>Artist Points Behaald: 882 / 1125</t>
   </si>
 </sst>
 </file>
@@ -1727,7 +1727,7 @@
   <dimension ref="A1:R593"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="J1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K35" sqref="K35"/>
+      <selection activeCell="J18" sqref="J18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1746,8 +1746,8 @@
     <col min="12" max="12" width="30.7109375" style="1" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="31.140625" style="1" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="32" style="1" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="30.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="30" style="1" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="30.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="29.7109375" style="1" bestFit="1" customWidth="1"/>
     <col min="17" max="18" width="30.42578125" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1908,7 +1908,7 @@
         <v>391</v>
       </c>
       <c r="Q3" s="1" t="s">
-        <v>392</v>
+        <v>393</v>
       </c>
       <c r="R3" s="1" t="s">
         <v>373</v>
@@ -2403,7 +2403,7 @@
       <c r="P14" s="20" t="s">
         <v>315</v>
       </c>
-      <c r="Q14" s="1" t="s">
+      <c r="Q14" s="20" t="s">
         <v>309</v>
       </c>
       <c r="R14" s="1" t="s">
@@ -3049,7 +3049,7 @@
       <c r="H35" s="19"/>
       <c r="I35" s="19"/>
       <c r="J35" s="21" t="s">
-        <v>394</v>
+        <v>392</v>
       </c>
       <c r="N35" s="20" t="s">
         <v>269</v>
@@ -3062,7 +3062,7 @@
       <c r="H36" s="19"/>
       <c r="I36" s="19"/>
       <c r="J36" s="1" t="s">
-        <v>393</v>
+        <v>395</v>
       </c>
     </row>
     <row r="37" spans="1:18" x14ac:dyDescent="0.25">
@@ -3105,7 +3105,7 @@
       </c>
       <c r="I38" s="19"/>
       <c r="J38" s="1" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
     </row>
     <row r="39" spans="1:18" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Aeet List Update & 21-01-2016 Uren Registratie
</commit_message>
<xml_diff>
--- a/Algemeen/Asset List Game-Lab 1.xlsx
+++ b/Algemeen/Asset List Game-Lab 1.xlsx
@@ -1198,16 +1198,16 @@
     <t>Development Points: 920 / 1125</t>
   </si>
   <si>
-    <t xml:space="preserve">10 Anthony| 0 Michiel| 78 Roos </t>
-  </si>
-  <si>
-    <t xml:space="preserve">393 Anthony | 156 Michiel | 300 Roos </t>
-  </si>
-  <si>
     <t>400 Fahrettin | 290 Sven | 230 Rief</t>
   </si>
   <si>
-    <t>Artist Points Behaald: 882 / 1125</t>
+    <t xml:space="preserve">10 Anthony| 0 Michiel| 101 Roos </t>
+  </si>
+  <si>
+    <t xml:space="preserve">393 Anthony | 156 Michiel | 323 Roos </t>
+  </si>
+  <si>
+    <t>Artist Points Behaald: 905 / 1125</t>
   </si>
 </sst>
 </file>
@@ -1727,7 +1727,7 @@
   <dimension ref="A1:R593"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="J1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J18" sqref="J18"/>
+      <selection activeCell="M35" sqref="M35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1908,7 +1908,7 @@
         <v>391</v>
       </c>
       <c r="Q3" s="1" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="R3" s="1" t="s">
         <v>373</v>
@@ -2151,7 +2151,7 @@
       <c r="P8" s="20" t="s">
         <v>289</v>
       </c>
-      <c r="Q8" s="1" t="s">
+      <c r="Q8" s="20" t="s">
         <v>303</v>
       </c>
       <c r="R8" s="1" t="s">
@@ -2545,7 +2545,7 @@
       <c r="L19" s="20" t="s">
         <v>257</v>
       </c>
-      <c r="Q19" s="1" t="s">
+      <c r="Q19" s="20" t="s">
         <v>314</v>
       </c>
     </row>
@@ -3062,7 +3062,7 @@
       <c r="H36" s="19"/>
       <c r="I36" s="19"/>
       <c r="J36" s="1" t="s">
-        <v>395</v>
+        <v>393</v>
       </c>
     </row>
     <row r="37" spans="1:18" x14ac:dyDescent="0.25">
@@ -3105,7 +3105,7 @@
       </c>
       <c r="I38" s="19"/>
       <c r="J38" s="1" t="s">
-        <v>394</v>
+        <v>395</v>
       </c>
     </row>
     <row r="39" spans="1:18" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Uren Registratie 22-01-2016 & Asset List Update & Import Eikeltje
</commit_message>
<xml_diff>
--- a/Algemeen/Asset List Game-Lab 1.xlsx
+++ b/Algemeen/Asset List Game-Lab 1.xlsx
@@ -1138,9 +1138,6 @@
     <t>0 Fahrettin|65 Sven|30 Rief</t>
   </si>
   <si>
-    <t xml:space="preserve">12 Anthony| 0 Michiel| 7 Roos </t>
-  </si>
-  <si>
     <t>Characters_SoldierAnt_4 (45) 6/8</t>
   </si>
   <si>
@@ -1204,10 +1201,13 @@
     <t xml:space="preserve">10 Anthony| 0 Michiel| 101 Roos </t>
   </si>
   <si>
-    <t xml:space="preserve">393 Anthony | 156 Michiel | 323 Roos </t>
-  </si>
-  <si>
-    <t>Artist Points Behaald: 905 / 1125</t>
+    <t xml:space="preserve">12 Anthony| 0 Michiel| 14 Roos </t>
+  </si>
+  <si>
+    <t xml:space="preserve">393 Anthony | 156 Michiel | 330 Roos </t>
+  </si>
+  <si>
+    <t>Artist Points Behaald: 912 / 1125</t>
   </si>
 </sst>
 </file>
@@ -1727,7 +1727,7 @@
   <dimension ref="A1:R593"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="J1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="M35" sqref="M35"/>
+      <selection activeCell="O20" sqref="O20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1893,25 +1893,25 @@
         <v>365</v>
       </c>
       <c r="L3" s="1" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="M3" s="1" t="s">
         <v>366</v>
       </c>
       <c r="N3" s="1" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="O3" s="1" t="s">
+        <v>389</v>
+      </c>
+      <c r="P3" s="1" t="s">
         <v>390</v>
       </c>
-      <c r="P3" s="1" t="s">
-        <v>391</v>
-      </c>
       <c r="Q3" s="1" t="s">
+        <v>393</v>
+      </c>
+      <c r="R3" s="1" t="s">
         <v>394</v>
-      </c>
-      <c r="R3" s="1" t="s">
-        <v>373</v>
       </c>
     </row>
     <row r="4" spans="1:18" x14ac:dyDescent="0.25">
@@ -2043,10 +2043,10 @@
         <v>230</v>
       </c>
       <c r="N6" s="22" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="O6" s="22" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="P6" s="1" t="s">
         <v>288</v>
@@ -2090,16 +2090,16 @@
         <v>241</v>
       </c>
       <c r="M7" s="22" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="N7" s="22" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="O7" s="20" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="P7" s="22" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="Q7" s="20" t="s">
         <v>302</v>
@@ -2154,7 +2154,7 @@
       <c r="Q8" s="20" t="s">
         <v>303</v>
       </c>
-      <c r="R8" s="1" t="s">
+      <c r="R8" s="20" t="s">
         <v>332</v>
       </c>
     </row>
@@ -2187,7 +2187,7 @@
         <v>243</v>
       </c>
       <c r="M9" s="22" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="N9" s="1" t="s">
         <v>264</v>
@@ -2392,10 +2392,10 @@
         <v>64</v>
       </c>
       <c r="L14" s="22" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="M14" s="22" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="O14" s="20" t="s">
         <v>294</v>
@@ -2612,7 +2612,7 @@
         <v>360</v>
       </c>
       <c r="L22" s="22" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
     </row>
     <row r="23" spans="1:18" x14ac:dyDescent="0.25">
@@ -2711,16 +2711,16 @@
         <v>369</v>
       </c>
       <c r="O26" s="1" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="P26" s="1" t="s">
         <v>372</v>
       </c>
       <c r="Q26" s="1" t="s">
+        <v>380</v>
+      </c>
+      <c r="R26" s="1" t="s">
         <v>381</v>
-      </c>
-      <c r="R26" s="1" t="s">
-        <v>382</v>
       </c>
     </row>
     <row r="27" spans="1:18" x14ac:dyDescent="0.25">
@@ -3049,7 +3049,7 @@
       <c r="H35" s="19"/>
       <c r="I35" s="19"/>
       <c r="J35" s="21" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="N35" s="20" t="s">
         <v>269</v>
@@ -3062,7 +3062,7 @@
       <c r="H36" s="19"/>
       <c r="I36" s="19"/>
       <c r="J36" s="1" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
     </row>
     <row r="37" spans="1:18" x14ac:dyDescent="0.25">
@@ -3126,7 +3126,7 @@
       </c>
       <c r="I39" s="19"/>
       <c r="J39" s="1" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
     </row>
     <row r="40" spans="1:18" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Import Scroll en Rocks & Asset-List Update
</commit_message>
<xml_diff>
--- a/Algemeen/Asset List Game-Lab 1.xlsx
+++ b/Algemeen/Asset List Game-Lab 1.xlsx
@@ -1195,19 +1195,19 @@
     <t>Characters_ArenaAnt_6 (43) 6/8</t>
   </si>
   <si>
-    <t xml:space="preserve">55 Anthony | 0 Michiel | 26 Roos </t>
-  </si>
-  <si>
     <t xml:space="preserve">61 Anthony | 60 Michiel | 74 Roos </t>
   </si>
   <si>
     <t xml:space="preserve">23 Anthony | 0 Michiel | 69 Roos </t>
   </si>
   <si>
-    <t xml:space="preserve">449 Anthony | 149 Michiel | 362 Roos </t>
-  </si>
-  <si>
-    <t>Artist Points Behaald: 993 / 1125</t>
+    <t xml:space="preserve">55 Anthony | 0 Michiel | 30 Roos </t>
+  </si>
+  <si>
+    <t xml:space="preserve">449 Anthony | 149 Michiel | 366 Roos </t>
+  </si>
+  <si>
+    <t>Artist Points Behaald: 997 / 1125</t>
   </si>
 </sst>
 </file>
@@ -1727,7 +1727,7 @@
   <dimension ref="A1:R593"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="J1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K19" sqref="K19"/>
+      <selection activeCell="N19" sqref="N19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1893,7 +1893,7 @@
         <v>381</v>
       </c>
       <c r="L3" s="1" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="M3" s="1" t="s">
         <v>382</v>
@@ -1905,13 +1905,13 @@
         <v>384</v>
       </c>
       <c r="P3" s="1" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="Q3" s="1" t="s">
         <v>385</v>
       </c>
       <c r="R3" s="1" t="s">
-        <v>392</v>
+        <v>394</v>
       </c>
     </row>
     <row r="4" spans="1:18" x14ac:dyDescent="0.25">
@@ -2054,7 +2054,7 @@
       <c r="Q6" s="1" t="s">
         <v>301</v>
       </c>
-      <c r="R6" s="1" t="s">
+      <c r="R6" s="20" t="s">
         <v>330</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Assets import & update asset list & sound fixes
</commit_message>
<xml_diff>
--- a/Algemeen/Asset List Game-Lab 1.xlsx
+++ b/Algemeen/Asset List Game-Lab 1.xlsx
@@ -1201,13 +1201,13 @@
     <t xml:space="preserve">23 Anthony | 0 Michiel | 69 Roos </t>
   </si>
   <si>
-    <t xml:space="preserve">55 Anthony | 0 Michiel | 30 Roos </t>
-  </si>
-  <si>
-    <t xml:space="preserve">449 Anthony | 149 Michiel | 366 Roos </t>
-  </si>
-  <si>
-    <t>Artist Points Behaald: 997 / 1125</t>
+    <t xml:space="preserve">55 Anthony | 0 Michiel | 37 Roos </t>
+  </si>
+  <si>
+    <t xml:space="preserve">449 Anthony | 149 Michiel | 373 Roos </t>
+  </si>
+  <si>
+    <t>Artist Points Behaald: 1004 / 1125</t>
   </si>
 </sst>
 </file>
@@ -1727,7 +1727,7 @@
   <dimension ref="A1:R593"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="J1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="N19" sqref="N19"/>
+      <selection activeCell="N20" sqref="N20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2104,7 +2104,7 @@
       <c r="Q7" s="20" t="s">
         <v>302</v>
       </c>
-      <c r="R7" s="1" t="s">
+      <c r="R7" s="20" t="s">
         <v>331</v>
       </c>
     </row>
@@ -2201,7 +2201,7 @@
       <c r="Q9" s="20" t="s">
         <v>304</v>
       </c>
-      <c r="R9" s="1" t="s">
+      <c r="R9" s="20" t="s">
         <v>334</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Import spinnenweb en deur en spinnenweb toegevoegd in laatste level
</commit_message>
<xml_diff>
--- a/Algemeen/Asset List Game-Lab 1.xlsx
+++ b/Algemeen/Asset List Game-Lab 1.xlsx
@@ -1024,9 +1024,6 @@
     <t>Water_WaterDruppel_1 (3)</t>
   </si>
   <si>
-    <t>Summons_VuurVlieg_1 (38)</t>
-  </si>
-  <si>
     <t>Weapons_Gladius_2 (4)</t>
   </si>
   <si>
@@ -1174,9 +1171,6 @@
     <t xml:space="preserve">83 Anthony | 0 Michiel | 50 Roos </t>
   </si>
   <si>
-    <t xml:space="preserve">10 Anthony | 0 Michiel | 101 Roos </t>
-  </si>
-  <si>
     <t>60 Fahrettin | 40 Sven | 30 Rief</t>
   </si>
   <si>
@@ -1201,13 +1195,19 @@
     <t xml:space="preserve">23 Anthony | 0 Michiel | 69 Roos </t>
   </si>
   <si>
-    <t xml:space="preserve">55 Anthony | 0 Michiel | 37 Roos </t>
-  </si>
-  <si>
-    <t xml:space="preserve">449 Anthony | 149 Michiel | 373 Roos </t>
-  </si>
-  <si>
-    <t>Artist Points Behaald: 1004 / 1125</t>
+    <t xml:space="preserve">10 Anthony | 0 Michiel | 123 Roos </t>
+  </si>
+  <si>
+    <t>Summons_VuurVlieg_1 (9) 2/7</t>
+  </si>
+  <si>
+    <t xml:space="preserve">64 Anthony | 0 Michiel | 37 Roos </t>
+  </si>
+  <si>
+    <t xml:space="preserve">458 Anthony | 149 Michiel | 395 Roos </t>
+  </si>
+  <si>
+    <t>Artist Points Behaald: 1035 / 1125</t>
   </si>
 </sst>
 </file>
@@ -1727,7 +1727,7 @@
   <dimension ref="A1:R593"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="J1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="N20" sqref="N20"/>
+      <selection activeCell="J17" sqref="J17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1887,28 +1887,28 @@
         <v>67</v>
       </c>
       <c r="J3" s="1" t="s">
+        <v>379</v>
+      </c>
+      <c r="K3" s="1" t="s">
         <v>380</v>
       </c>
-      <c r="K3" s="1" t="s">
+      <c r="L3" s="1" t="s">
+        <v>390</v>
+      </c>
+      <c r="M3" s="1" t="s">
         <v>381</v>
       </c>
-      <c r="L3" s="1" t="s">
+      <c r="N3" s="1" t="s">
+        <v>382</v>
+      </c>
+      <c r="O3" s="1" t="s">
+        <v>383</v>
+      </c>
+      <c r="P3" s="1" t="s">
+        <v>391</v>
+      </c>
+      <c r="Q3" s="1" t="s">
         <v>392</v>
-      </c>
-      <c r="M3" s="1" t="s">
-        <v>382</v>
-      </c>
-      <c r="N3" s="1" t="s">
-        <v>383</v>
-      </c>
-      <c r="O3" s="1" t="s">
-        <v>384</v>
-      </c>
-      <c r="P3" s="1" t="s">
-        <v>393</v>
-      </c>
-      <c r="Q3" s="1" t="s">
-        <v>385</v>
       </c>
       <c r="R3" s="1" t="s">
         <v>394</v>
@@ -1946,25 +1946,25 @@
         <v>221</v>
       </c>
       <c r="L4" s="1" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="M4" s="21" t="s">
         <v>221</v>
       </c>
       <c r="N4" s="1" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="O4" s="21" t="s">
         <v>221</v>
       </c>
       <c r="P4" s="1" t="s">
-        <v>362</v>
-      </c>
-      <c r="Q4" s="21" t="s">
+        <v>361</v>
+      </c>
+      <c r="Q4" s="23" t="s">
         <v>221</v>
       </c>
       <c r="R4" s="1" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
     </row>
     <row r="5" spans="1:18" x14ac:dyDescent="0.25">
@@ -1993,10 +1993,10 @@
         <v>152</v>
       </c>
       <c r="J5" s="20" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="K5" s="20" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="L5" s="21" t="s">
         <v>221</v>
@@ -2043,15 +2043,15 @@
         <v>230</v>
       </c>
       <c r="N6" s="22" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="O6" s="22" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="P6" s="1" t="s">
         <v>288</v>
       </c>
-      <c r="Q6" s="1" t="s">
+      <c r="Q6" s="20" t="s">
         <v>301</v>
       </c>
       <c r="R6" s="20" t="s">
@@ -2090,16 +2090,16 @@
         <v>241</v>
       </c>
       <c r="M7" s="22" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="N7" s="22" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="O7" s="20" t="s">
+        <v>371</v>
+      </c>
+      <c r="P7" s="22" t="s">
         <v>372</v>
-      </c>
-      <c r="P7" s="22" t="s">
-        <v>373</v>
       </c>
       <c r="Q7" s="20" t="s">
         <v>302</v>
@@ -2187,7 +2187,7 @@
         <v>243</v>
       </c>
       <c r="M9" s="22" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="N9" s="1" t="s">
         <v>264</v>
@@ -2234,10 +2234,10 @@
         <v>244</v>
       </c>
       <c r="M10" s="20" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="N10" s="20" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="O10" s="20" t="s">
         <v>277</v>
@@ -2248,8 +2248,8 @@
       <c r="Q10" s="20" t="s">
         <v>305</v>
       </c>
-      <c r="R10" s="1" t="s">
-        <v>335</v>
+      <c r="R10" s="22" t="s">
+        <v>393</v>
       </c>
     </row>
     <row r="11" spans="1:18" x14ac:dyDescent="0.25">
@@ -2263,7 +2263,7 @@
         <v>245</v>
       </c>
       <c r="M11" s="20" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="N11" s="20" t="s">
         <v>265</v>
@@ -2278,7 +2278,7 @@
         <v>306</v>
       </c>
       <c r="R11" s="20" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
     </row>
     <row r="12" spans="1:18" x14ac:dyDescent="0.25">
@@ -2322,7 +2322,7 @@
         <v>307</v>
       </c>
       <c r="R12" s="20" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
     </row>
     <row r="13" spans="1:18" x14ac:dyDescent="0.25">
@@ -2351,13 +2351,13 @@
         <v>247</v>
       </c>
       <c r="M13" s="20" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="N13" s="20" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="O13" s="20" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="P13" s="20" t="s">
         <v>279</v>
@@ -2366,7 +2366,7 @@
         <v>308</v>
       </c>
       <c r="R13" s="20" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
     </row>
     <row r="14" spans="1:18" x14ac:dyDescent="0.25">
@@ -2392,10 +2392,10 @@
         <v>64</v>
       </c>
       <c r="L14" s="22" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="M14" s="22" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="O14" s="20" t="s">
         <v>294</v>
@@ -2407,7 +2407,7 @@
         <v>309</v>
       </c>
       <c r="R14" s="22" t="s">
-        <v>391</v>
+        <v>389</v>
       </c>
     </row>
     <row r="15" spans="1:18" x14ac:dyDescent="0.25">
@@ -2436,16 +2436,16 @@
         <v>248</v>
       </c>
       <c r="O15" s="20" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="P15" s="20" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="Q15" s="20" t="s">
         <v>310</v>
       </c>
       <c r="R15" s="20" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
     </row>
     <row r="16" spans="1:18" x14ac:dyDescent="0.25">
@@ -2485,7 +2485,7 @@
         <v>137</v>
       </c>
       <c r="L17" s="20" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="Q17" s="20" t="s">
         <v>312</v>
@@ -2516,7 +2516,7 @@
       <c r="L18" s="20" t="s">
         <v>256</v>
       </c>
-      <c r="Q18" s="1" t="s">
+      <c r="Q18" s="20" t="s">
         <v>313</v>
       </c>
     </row>
@@ -2540,7 +2540,7 @@
         <v>166</v>
       </c>
       <c r="I19" s="3" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="L19" s="20" t="s">
         <v>257</v>
@@ -2569,13 +2569,13 @@
         <v>166</v>
       </c>
       <c r="I20" s="3" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="L20" s="20" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="Q20" s="20" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
     </row>
     <row r="21" spans="1:18" x14ac:dyDescent="0.25">
@@ -2583,7 +2583,7 @@
         <v>166</v>
       </c>
       <c r="I21" s="3" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="L21" s="20" t="s">
         <v>234</v>
@@ -2609,10 +2609,10 @@
         <v>166</v>
       </c>
       <c r="I22" s="3" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="L22" s="22" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
     </row>
     <row r="23" spans="1:18" x14ac:dyDescent="0.25">
@@ -2635,7 +2635,7 @@
         <v>166</v>
       </c>
       <c r="I23" s="3" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="L23" s="20" t="s">
         <v>254</v>
@@ -2661,7 +2661,7 @@
         <v>166</v>
       </c>
       <c r="I24" s="3" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
     </row>
     <row r="25" spans="1:18" x14ac:dyDescent="0.25">
@@ -2684,7 +2684,7 @@
         <v>166</v>
       </c>
       <c r="I25" s="5" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
     </row>
     <row r="26" spans="1:18" x14ac:dyDescent="0.25">
@@ -2693,34 +2693,34 @@
         <v>166</v>
       </c>
       <c r="I26" s="5" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="J26" s="1" t="s">
-        <v>390</v>
+        <v>388</v>
       </c>
       <c r="K26" s="1" t="s">
-        <v>389</v>
+        <v>387</v>
       </c>
       <c r="L26" s="1" t="s">
-        <v>388</v>
+        <v>386</v>
       </c>
       <c r="M26" s="1" t="s">
-        <v>387</v>
+        <v>385</v>
       </c>
       <c r="N26" s="1" t="s">
-        <v>386</v>
+        <v>384</v>
       </c>
       <c r="O26" s="1" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="P26" s="1" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="Q26" s="1" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="R26" s="1" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
     </row>
     <row r="27" spans="1:18" x14ac:dyDescent="0.25">
@@ -3049,7 +3049,7 @@
       <c r="H35" s="19"/>
       <c r="I35" s="19"/>
       <c r="J35" s="21" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="N35" s="20" t="s">
         <v>269</v>
@@ -3062,7 +3062,7 @@
       <c r="H36" s="19"/>
       <c r="I36" s="19"/>
       <c r="J36" s="1" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
     </row>
     <row r="37" spans="1:18" x14ac:dyDescent="0.25">
@@ -3126,7 +3126,7 @@
       </c>
       <c r="I39" s="19"/>
       <c r="J39" s="1" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
     </row>
     <row r="40" spans="1:18" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Asset List Update & Import Shrinkray & Import Weduwe
</commit_message>
<xml_diff>
--- a/Algemeen/Asset List Game-Lab 1.xlsx
+++ b/Algemeen/Asset List Game-Lab 1.xlsx
@@ -1120,9 +1120,6 @@
     <t>Enemy_TermietGeneral_2 (31) 6/8</t>
   </si>
   <si>
-    <t>Enemy_ZwarteWeduwe_5 (19) 3/8</t>
-  </si>
-  <si>
     <t xml:space="preserve">33 Fahrettin </t>
   </si>
   <si>
@@ -1165,9 +1162,6 @@
     <t xml:space="preserve">113 Anthony | 70 Michiel | 6 Roos </t>
   </si>
   <si>
-    <t xml:space="preserve">60 Anthony | 19 Michiel | 0 Roos </t>
-  </si>
-  <si>
     <t xml:space="preserve">83 Anthony | 0 Michiel | 50 Roos </t>
   </si>
   <si>
@@ -1204,10 +1198,16 @@
     <t xml:space="preserve">64 Anthony | 0 Michiel | 37 Roos </t>
   </si>
   <si>
-    <t xml:space="preserve">458 Anthony | 149 Michiel | 395 Roos </t>
-  </si>
-  <si>
-    <t>Artist Points Behaald: 1035 / 1125</t>
+    <t>Enemy_ZwarteWeduwe_5 (43) 6/8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">60 Anthony | 62 Michiel | 0 Roos </t>
+  </si>
+  <si>
+    <t xml:space="preserve">458 Anthony | 192 Michiel | 395 Roos </t>
+  </si>
+  <si>
+    <t>Artist Points Behaald: 1078 / 1125</t>
   </si>
 </sst>
 </file>
@@ -1727,7 +1727,7 @@
   <dimension ref="A1:R593"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="J1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J17" sqref="J17"/>
+      <selection activeCell="N18" sqref="N18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1887,31 +1887,31 @@
         <v>67</v>
       </c>
       <c r="J3" s="1" t="s">
+        <v>378</v>
+      </c>
+      <c r="K3" s="1" t="s">
         <v>379</v>
       </c>
-      <c r="K3" s="1" t="s">
+      <c r="L3" s="1" t="s">
+        <v>388</v>
+      </c>
+      <c r="M3" s="1" t="s">
         <v>380</v>
       </c>
-      <c r="L3" s="1" t="s">
+      <c r="N3" s="1" t="s">
+        <v>394</v>
+      </c>
+      <c r="O3" s="1" t="s">
+        <v>381</v>
+      </c>
+      <c r="P3" s="1" t="s">
+        <v>389</v>
+      </c>
+      <c r="Q3" s="1" t="s">
         <v>390</v>
       </c>
-      <c r="M3" s="1" t="s">
-        <v>381</v>
-      </c>
-      <c r="N3" s="1" t="s">
-        <v>382</v>
-      </c>
-      <c r="O3" s="1" t="s">
-        <v>383</v>
-      </c>
-      <c r="P3" s="1" t="s">
-        <v>391</v>
-      </c>
-      <c r="Q3" s="1" t="s">
+      <c r="R3" s="1" t="s">
         <v>392</v>
-      </c>
-      <c r="R3" s="1" t="s">
-        <v>394</v>
       </c>
     </row>
     <row r="4" spans="1:18" x14ac:dyDescent="0.25">
@@ -2046,7 +2046,7 @@
         <v>366</v>
       </c>
       <c r="O6" s="22" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="P6" s="1" t="s">
         <v>288</v>
@@ -2093,13 +2093,13 @@
         <v>363</v>
       </c>
       <c r="N7" s="22" t="s">
-        <v>367</v>
+        <v>393</v>
       </c>
       <c r="O7" s="20" t="s">
+        <v>370</v>
+      </c>
+      <c r="P7" s="22" t="s">
         <v>371</v>
-      </c>
-      <c r="P7" s="22" t="s">
-        <v>372</v>
       </c>
       <c r="Q7" s="20" t="s">
         <v>302</v>
@@ -2189,7 +2189,7 @@
       <c r="M9" s="22" t="s">
         <v>364</v>
       </c>
-      <c r="N9" s="1" t="s">
+      <c r="N9" s="20" t="s">
         <v>264</v>
       </c>
       <c r="O9" s="20" t="s">
@@ -2249,7 +2249,7 @@
         <v>305</v>
       </c>
       <c r="R10" s="22" t="s">
-        <v>393</v>
+        <v>391</v>
       </c>
     </row>
     <row r="11" spans="1:18" x14ac:dyDescent="0.25">
@@ -2407,7 +2407,7 @@
         <v>309</v>
       </c>
       <c r="R14" s="22" t="s">
-        <v>389</v>
+        <v>387</v>
       </c>
     </row>
     <row r="15" spans="1:18" x14ac:dyDescent="0.25">
@@ -2612,7 +2612,7 @@
         <v>358</v>
       </c>
       <c r="L22" s="22" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
     </row>
     <row r="23" spans="1:18" x14ac:dyDescent="0.25">
@@ -2696,31 +2696,31 @@
         <v>356</v>
       </c>
       <c r="J26" s="1" t="s">
-        <v>388</v>
+        <v>386</v>
       </c>
       <c r="K26" s="1" t="s">
-        <v>387</v>
+        <v>385</v>
       </c>
       <c r="L26" s="1" t="s">
-        <v>386</v>
+        <v>384</v>
       </c>
       <c r="M26" s="1" t="s">
-        <v>385</v>
+        <v>383</v>
       </c>
       <c r="N26" s="1" t="s">
-        <v>384</v>
+        <v>382</v>
       </c>
       <c r="O26" s="1" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="P26" s="1" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="Q26" s="1" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="R26" s="1" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
     </row>
     <row r="27" spans="1:18" x14ac:dyDescent="0.25">
@@ -3049,7 +3049,7 @@
       <c r="H35" s="19"/>
       <c r="I35" s="19"/>
       <c r="J35" s="21" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="N35" s="20" t="s">
         <v>269</v>
@@ -3062,7 +3062,7 @@
       <c r="H36" s="19"/>
       <c r="I36" s="19"/>
       <c r="J36" s="1" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
     </row>
     <row r="37" spans="1:18" x14ac:dyDescent="0.25">
@@ -3126,7 +3126,7 @@
       </c>
       <c r="I39" s="19"/>
       <c r="J39" s="1" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
     </row>
     <row r="40" spans="1:18" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Uren Registratie DONE & Import vuurvlieg & Assetlist update
</commit_message>
<xml_diff>
--- a/Algemeen/Asset List Game-Lab 1.xlsx
+++ b/Algemeen/Asset List Game-Lab 1.xlsx
@@ -1192,22 +1192,22 @@
     <t xml:space="preserve">10 Anthony | 0 Michiel | 123 Roos </t>
   </si>
   <si>
-    <t>Summons_VuurVlieg_1 (9) 2/7</t>
-  </si>
-  <si>
-    <t xml:space="preserve">64 Anthony | 0 Michiel | 37 Roos </t>
-  </si>
-  <si>
     <t>Enemy_ZwarteWeduwe_5 (43) 6/8</t>
   </si>
   <si>
     <t xml:space="preserve">60 Anthony | 62 Michiel | 0 Roos </t>
   </si>
   <si>
-    <t xml:space="preserve">458 Anthony | 192 Michiel | 395 Roos </t>
-  </si>
-  <si>
-    <t>Artist Points Behaald: 1078 / 1125</t>
+    <t>Summons_VuurVlieg_1 (37) 6/7</t>
+  </si>
+  <si>
+    <t xml:space="preserve">92 Anthony | 0 Michiel | 37 Roos </t>
+  </si>
+  <si>
+    <t xml:space="preserve">486 Anthony | 192 Michiel | 395 Roos </t>
+  </si>
+  <si>
+    <t>Artist Points Behaald: 1106 / 1125</t>
   </si>
 </sst>
 </file>
@@ -1726,8 +1726,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R593"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="J1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="N18" sqref="N18"/>
+    <sheetView tabSelected="1" topLeftCell="K1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="N19" sqref="N19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1899,7 +1899,7 @@
         <v>380</v>
       </c>
       <c r="N3" s="1" t="s">
-        <v>394</v>
+        <v>392</v>
       </c>
       <c r="O3" s="1" t="s">
         <v>381</v>
@@ -1911,7 +1911,7 @@
         <v>390</v>
       </c>
       <c r="R3" s="1" t="s">
-        <v>392</v>
+        <v>394</v>
       </c>
     </row>
     <row r="4" spans="1:18" x14ac:dyDescent="0.25">
@@ -2093,7 +2093,7 @@
         <v>363</v>
       </c>
       <c r="N7" s="22" t="s">
-        <v>393</v>
+        <v>391</v>
       </c>
       <c r="O7" s="20" t="s">
         <v>370</v>
@@ -2249,7 +2249,7 @@
         <v>305</v>
       </c>
       <c r="R10" s="22" t="s">
-        <v>391</v>
+        <v>393</v>
       </c>
     </row>
     <row r="11" spans="1:18" x14ac:dyDescent="0.25">

</xml_diff>